<commit_message>
Updating the mapping sheet
git-tfs-id: [http://developmentvlan:8585/tfs/vanrise.collection]$/;C54792
</commit_message>
<xml_diff>
--- a/SOM/Documents/SOM/SOM APIs Mapping Sheet.xlsx
+++ b/SOM/Documents/SOM/SOM APIs Mapping Sheet.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="293">
   <si>
     <t>GetTechnicalDetails</t>
   </si>
@@ -476,9 +476,6 @@
   </si>
   <si>
     <t>Get all telephony contracts for a specific customer, get the status details of each contract by calling get single contract for each. Then get the phone number by calling the method that gets resources of a contract</t>
-  </si>
-  <si>
-    <t>We can get rid of this call if the number can be got from directory number property in contractsSearchResponse</t>
   </si>
   <si>
     <t>Contracts should be filtered in BPM based on Rate Plan Id. Same for all similar calls for (Leased Line, ADSL and GSHDSL)</t>
@@ -644,10 +641,6 @@
     <t>GetPOSServices</t>
   </si>
   <si>
-    <t xml:space="preserve">ratePlanId
-</t>
-  </si>
-  <si>
     <t>ratePlanId
 switchId</t>
   </si>
@@ -656,9 +649,6 @@
   </si>
   <si>
     <t>L2S3139</t>
-  </si>
-  <si>
-    <t>Passing package id POS statically from SOM</t>
   </si>
   <si>
     <t>GetCoreServices</t>
@@ -938,6 +928,12 @@
   </si>
   <si>
     <t>added two new columns to include samples about request and response in JSON format. Started with TelephonySoftSuspend call</t>
+  </si>
+  <si>
+    <t>This call will return for now all services due to the lack of having a we service on BSCS that gets services per package</t>
+  </si>
+  <si>
+    <t>This is not needed in telephony because we can depened on contratsSearchResponse it has Directory Number</t>
   </si>
 </sst>
 </file>
@@ -1100,10 +1096,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1511,27 +1507,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>276</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B2" s="8">
         <v>43538</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D2" s="7">
         <v>1</v>
@@ -1539,13 +1535,13 @@
     </row>
     <row r="3" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B3" s="8">
         <v>43539</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D3" s="7">
         <v>1.1000000000000001</v>
@@ -1570,11 +1566,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O121"/>
+  <dimension ref="A1:O122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B110" sqref="B110:B112"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E28" sqref="E28:E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1597,13 +1593,13 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -1705,7 +1701,7 @@
         <v>141</v>
       </c>
       <c r="B4" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F4" t="s">
         <v>25</v>
@@ -2287,7 +2283,7 @@
         <v>69</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
@@ -2301,9 +2297,9 @@
         <v>98</v>
       </c>
       <c r="I22" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="J22" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="J22" s="20" t="s">
         <v>82</v>
       </c>
       <c r="K22" s="17" t="s">
@@ -2319,7 +2315,7 @@
         <v>67</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="75" x14ac:dyDescent="0.25">
@@ -2332,10 +2328,10 @@
       <c r="G23" s="17"/>
       <c r="H23" s="17"/>
       <c r="I23" s="14"/>
-      <c r="J23" s="19"/>
+      <c r="J23" s="20"/>
       <c r="K23" s="17"/>
       <c r="L23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M23" t="s">
         <v>83</v>
@@ -2344,7 +2340,7 @@
         <v>27</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -2355,7 +2351,7 @@
         <v>72</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D24" s="13"/>
       <c r="E24" s="13"/>
@@ -2443,7 +2439,7 @@
         <v>124</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -2483,7 +2479,7 @@
         <v>146</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D28" s="13"/>
       <c r="E28" s="13"/>
@@ -2515,7 +2511,7 @@
         <v>67</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -2540,7 +2536,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
       <c r="B30" s="10"/>
       <c r="C30" s="11"/>
@@ -2562,7 +2558,7 @@
         <v>67</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>151</v>
+        <v>292</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2573,7 +2569,7 @@
         <v>147</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D31" s="13"/>
       <c r="E31" s="13"/>
@@ -2587,7 +2583,7 @@
         <v>102</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J31" s="10" t="s">
         <v>82</v>
@@ -2649,7 +2645,7 @@
         <v>67</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
@@ -2660,7 +2656,7 @@
         <v>148</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D34" s="13"/>
       <c r="E34" s="13"/>
@@ -2674,7 +2670,7 @@
         <v>102</v>
       </c>
       <c r="I34" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J34" s="10" t="s">
         <v>82</v>
@@ -2736,7 +2732,7 @@
         <v>67</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
@@ -2747,7 +2743,7 @@
         <v>149</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D37" s="13"/>
       <c r="E37" s="13"/>
@@ -2761,7 +2757,7 @@
         <v>102</v>
       </c>
       <c r="I37" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J37" s="10" t="s">
         <v>82</v>
@@ -2831,7 +2827,7 @@
         <v>88</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
@@ -2871,7 +2867,7 @@
         <v>139</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D41" s="13"/>
       <c r="E41" s="13"/>
@@ -3048,7 +3044,7 @@
         <v>108</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
@@ -3088,7 +3084,7 @@
         <v>112</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
@@ -3128,7 +3124,7 @@
         <v>127</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
@@ -3168,7 +3164,7 @@
         <v>76</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
@@ -3211,7 +3207,7 @@
         <v>86</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F52" t="s">
         <v>25</v>
@@ -3393,8 +3389,8 @@
         <v>121</v>
       </c>
       <c r="C57" s="12"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="20"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19"/>
       <c r="F57" s="10" t="s">
         <v>25</v>
       </c>
@@ -3427,8 +3423,8 @@
       <c r="A58" s="10"/>
       <c r="B58" s="10"/>
       <c r="C58" s="12"/>
-      <c r="D58" s="20"/>
-      <c r="E58" s="20"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="19"/>
       <c r="F58" s="10"/>
       <c r="G58" s="10"/>
       <c r="H58" s="10"/>
@@ -3449,8 +3445,8 @@
       <c r="A59" s="10"/>
       <c r="B59" s="10"/>
       <c r="C59" s="12"/>
-      <c r="D59" s="20"/>
-      <c r="E59" s="20"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="19"/>
       <c r="F59" s="10"/>
       <c r="G59" s="10"/>
       <c r="H59" s="10"/>
@@ -3475,7 +3471,7 @@
         <v>141</v>
       </c>
       <c r="B60" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F60" t="s">
         <v>25</v>
@@ -3484,7 +3480,7 @@
         <v>27</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J60" t="s">
         <v>62</v>
@@ -3493,16 +3489,16 @@
         <v>119</v>
       </c>
       <c r="L60" t="s">
+        <v>169</v>
+      </c>
+      <c r="M60" t="s">
+        <v>66</v>
+      </c>
+      <c r="N60" t="s">
+        <v>67</v>
+      </c>
+      <c r="O60" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="M60" t="s">
-        <v>66</v>
-      </c>
-      <c r="N60" t="s">
-        <v>67</v>
-      </c>
-      <c r="O60" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="61" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -3510,19 +3506,19 @@
         <v>141</v>
       </c>
       <c r="B61" t="s">
+        <v>172</v>
+      </c>
+      <c r="F61" t="s">
+        <v>25</v>
+      </c>
+      <c r="G61" t="s">
+        <v>27</v>
+      </c>
+      <c r="H61" t="s">
+        <v>174</v>
+      </c>
+      <c r="I61" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="F61" t="s">
-        <v>25</v>
-      </c>
-      <c r="G61" t="s">
-        <v>27</v>
-      </c>
-      <c r="H61" t="s">
-        <v>175</v>
-      </c>
-      <c r="I61" s="1" t="s">
-        <v>174</v>
       </c>
       <c r="J61" t="s">
         <v>62</v>
@@ -3531,16 +3527,16 @@
         <v>119</v>
       </c>
       <c r="L61" t="s">
+        <v>175</v>
+      </c>
+      <c r="M61" t="s">
+        <v>66</v>
+      </c>
+      <c r="N61" t="s">
+        <v>67</v>
+      </c>
+      <c r="O61" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="M61" t="s">
-        <v>66</v>
-      </c>
-      <c r="N61" t="s">
-        <v>67</v>
-      </c>
-      <c r="O61" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="62" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -3548,10 +3544,10 @@
         <v>141</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D62" s="15"/>
       <c r="E62" s="15"/>
@@ -3562,10 +3558,10 @@
         <v>27</v>
       </c>
       <c r="H62" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="I62" s="12" t="s">
         <v>179</v>
-      </c>
-      <c r="I62" s="12" t="s">
-        <v>180</v>
       </c>
       <c r="J62" s="10" t="s">
         <v>82</v>
@@ -3574,7 +3570,7 @@
         <v>119</v>
       </c>
       <c r="L62" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M62" t="s">
         <v>26</v>
@@ -3583,7 +3579,7 @@
         <v>27</v>
       </c>
       <c r="O62" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="63" spans="1:15" ht="45" x14ac:dyDescent="0.25">
@@ -3599,16 +3595,16 @@
       <c r="J63" s="10"/>
       <c r="K63" s="10"/>
       <c r="L63" t="s">
+        <v>182</v>
+      </c>
+      <c r="M63" t="s">
+        <v>66</v>
+      </c>
+      <c r="N63" t="s">
+        <v>67</v>
+      </c>
+      <c r="O63" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="M63" t="s">
-        <v>66</v>
-      </c>
-      <c r="N63" t="s">
-        <v>67</v>
-      </c>
-      <c r="O63" s="1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="64" spans="1:15" ht="135" customHeight="1" x14ac:dyDescent="0.25">
@@ -3616,10 +3612,10 @@
         <v>141</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D64" s="15"/>
       <c r="E64" s="15"/>
@@ -3630,10 +3626,10 @@
         <v>27</v>
       </c>
       <c r="H64" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I64" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J64" s="10" t="s">
         <v>82</v>
@@ -3642,7 +3638,7 @@
         <v>120</v>
       </c>
       <c r="L64" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M64" t="s">
         <v>66</v>
@@ -3651,7 +3647,7 @@
         <v>67</v>
       </c>
       <c r="O64" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="65" spans="1:15" ht="90" x14ac:dyDescent="0.25">
@@ -3667,7 +3663,7 @@
       <c r="J65" s="10"/>
       <c r="K65" s="10"/>
       <c r="L65" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M65" t="s">
         <v>66</v>
@@ -3676,7 +3672,7 @@
         <v>67</v>
       </c>
       <c r="O65" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
@@ -3692,7 +3688,7 @@
       <c r="J66" s="10"/>
       <c r="K66" s="10"/>
       <c r="L66" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M66" t="s">
         <v>66</v>
@@ -3714,7 +3710,7 @@
       <c r="J67" s="10"/>
       <c r="K67" s="10"/>
       <c r="L67" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M67" t="s">
         <v>66</v>
@@ -3728,10 +3724,10 @@
         <v>141</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C68" s="14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D68" s="15"/>
       <c r="E68" s="15"/>
@@ -3742,10 +3738,10 @@
         <v>27</v>
       </c>
       <c r="H68" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I68" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J68" s="10" t="s">
         <v>82</v>
@@ -3754,7 +3750,7 @@
         <v>120</v>
       </c>
       <c r="L68" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M68" t="s">
         <v>66</v>
@@ -3763,7 +3759,7 @@
         <v>67</v>
       </c>
       <c r="O68" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
@@ -3779,7 +3775,7 @@
       <c r="J69" s="10"/>
       <c r="K69" s="10"/>
       <c r="L69" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M69" t="s">
         <v>66</v>
@@ -3801,7 +3797,7 @@
       <c r="J70" s="10"/>
       <c r="K70" s="10"/>
       <c r="L70" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M70" t="s">
         <v>66</v>
@@ -3823,7 +3819,7 @@
       <c r="J71" s="10"/>
       <c r="K71" s="10"/>
       <c r="L71" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M71" t="s">
         <v>66</v>
@@ -3837,10 +3833,10 @@
         <v>141</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D72" s="15"/>
       <c r="E72" s="15"/>
@@ -3851,10 +3847,10 @@
         <v>27</v>
       </c>
       <c r="H72" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I72" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J72" s="10" t="s">
         <v>82</v>
@@ -3863,7 +3859,7 @@
         <v>120</v>
       </c>
       <c r="L72" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M72" t="s">
         <v>66</v>
@@ -3885,7 +3881,7 @@
       <c r="J73" s="10"/>
       <c r="K73" s="10"/>
       <c r="L73" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M73" t="s">
         <v>66</v>
@@ -3907,7 +3903,7 @@
       <c r="J74" s="10"/>
       <c r="K74" s="10"/>
       <c r="L74" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M74" t="s">
         <v>66</v>
@@ -3929,7 +3925,7 @@
       <c r="J75" s="10"/>
       <c r="K75" s="10"/>
       <c r="L75" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M75" t="s">
         <v>66</v>
@@ -3938,27 +3934,24 @@
         <v>67</v>
       </c>
     </row>
-    <row r="76" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>141</v>
       </c>
       <c r="B76" t="s">
-        <v>200</v>
-      </c>
-      <c r="C76" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F76" t="s">
+        <v>25</v>
+      </c>
+      <c r="G76" t="s">
+        <v>27</v>
+      </c>
+      <c r="H76" t="s">
+        <v>202</v>
+      </c>
+      <c r="I76" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="F76" t="s">
-        <v>25</v>
-      </c>
-      <c r="G76" t="s">
-        <v>27</v>
-      </c>
-      <c r="H76" t="s">
-        <v>204</v>
-      </c>
-      <c r="I76" s="1" t="s">
-        <v>203</v>
       </c>
       <c r="J76" t="s">
         <v>62</v>
@@ -3967,7 +3960,7 @@
         <v>119</v>
       </c>
       <c r="L76" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M76" t="s">
         <v>66</v>
@@ -3976,7 +3969,7 @@
         <v>67</v>
       </c>
       <c r="O76" s="1" t="s">
-        <v>205</v>
+        <v>291</v>
       </c>
     </row>
     <row r="77" spans="1:15" ht="45" x14ac:dyDescent="0.25">
@@ -3984,10 +3977,10 @@
         <v>141</v>
       </c>
       <c r="B77" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F77" t="s">
         <v>25</v>
@@ -3996,7 +3989,7 @@
         <v>27</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="J77" t="s">
         <v>62</v>
@@ -4005,7 +3998,7 @@
         <v>119</v>
       </c>
       <c r="L77" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M77" t="s">
         <v>66</v>
@@ -4014,7 +4007,7 @@
         <v>67</v>
       </c>
       <c r="O77" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="78" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4022,10 +4015,10 @@
         <v>141</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C78" s="14" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D78" s="15"/>
       <c r="E78" s="15"/>
@@ -4036,10 +4029,10 @@
         <v>27</v>
       </c>
       <c r="H78" s="10" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I78" s="10" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="J78" s="10" t="s">
         <v>82</v>
@@ -4051,13 +4044,13 @@
         <v>47</v>
       </c>
       <c r="M78" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N78" t="s">
         <v>27</v>
       </c>
       <c r="O78" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="79" spans="1:15" ht="45" x14ac:dyDescent="0.25">
@@ -4073,16 +4066,16 @@
       <c r="J79" s="10"/>
       <c r="K79" s="10"/>
       <c r="L79" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="M79" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="N79" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O79" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="80" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -4098,7 +4091,7 @@
       <c r="J80" s="10"/>
       <c r="K80" s="10"/>
       <c r="L80" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M80" t="s">
         <v>83</v>
@@ -4107,7 +4100,7 @@
         <v>27</v>
       </c>
       <c r="O80" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="81" spans="1:15" ht="60" x14ac:dyDescent="0.25">
@@ -4132,7 +4125,7 @@
         <v>67</v>
       </c>
       <c r="O81" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
@@ -4162,10 +4155,10 @@
         <v>141</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C83" s="14" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D83" s="15"/>
       <c r="E83" s="15"/>
@@ -4177,7 +4170,7 @@
       </c>
       <c r="H83" s="10"/>
       <c r="I83" s="10" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="J83" s="10" t="s">
         <v>82</v>
@@ -4189,7 +4182,7 @@
         <v>47</v>
       </c>
       <c r="M83" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N83" t="s">
         <v>27</v>
@@ -4208,13 +4201,13 @@
       <c r="J84" s="10"/>
       <c r="K84" s="10"/>
       <c r="L84" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="M84" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="N84" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.25">
@@ -4230,7 +4223,7 @@
       <c r="J85" s="10"/>
       <c r="K85" s="10"/>
       <c r="L85" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M85" t="s">
         <v>83</v>
@@ -4283,7 +4276,7 @@
         <v>67</v>
       </c>
       <c r="O87" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="88" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4291,10 +4284,10 @@
         <v>141</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C88" s="14" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D88" s="15"/>
       <c r="E88" s="15"/>
@@ -4305,10 +4298,10 @@
         <v>27</v>
       </c>
       <c r="H88" s="10" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="I88" s="10" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="J88" s="10" t="s">
         <v>82</v>
@@ -4326,7 +4319,7 @@
         <v>27</v>
       </c>
       <c r="O88" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="89" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -4345,13 +4338,13 @@
         <v>47</v>
       </c>
       <c r="M89" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N89" t="s">
         <v>27</v>
       </c>
       <c r="O89" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="90" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -4367,7 +4360,7 @@
       <c r="J90" s="10"/>
       <c r="K90" s="10"/>
       <c r="L90" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M90" t="s">
         <v>26</v>
@@ -4376,7 +4369,7 @@
         <v>27</v>
       </c>
       <c r="O90" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="91" spans="1:15" ht="75" x14ac:dyDescent="0.25">
@@ -4392,7 +4385,7 @@
       <c r="J91" s="10"/>
       <c r="K91" s="10"/>
       <c r="L91" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M91" t="s">
         <v>83</v>
@@ -4401,7 +4394,7 @@
         <v>27</v>
       </c>
       <c r="O91" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
@@ -4453,10 +4446,10 @@
         <v>141</v>
       </c>
       <c r="B94" s="10" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C94" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D94" s="15"/>
       <c r="E94" s="15"/>
@@ -4467,10 +4460,10 @@
         <v>27</v>
       </c>
       <c r="H94" s="10" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="I94" s="10" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="J94" s="10" t="s">
         <v>82</v>
@@ -4479,7 +4472,7 @@
         <v>120</v>
       </c>
       <c r="L94" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="M94" t="s">
         <v>66</v>
@@ -4501,16 +4494,16 @@
       <c r="J95" s="10"/>
       <c r="K95" s="10"/>
       <c r="L95" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="M95" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="N95" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O95" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="96" spans="1:15" ht="45" x14ac:dyDescent="0.25">
@@ -4526,16 +4519,16 @@
       <c r="J96" s="10"/>
       <c r="K96" s="10"/>
       <c r="L96" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="M96" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N96" t="s">
         <v>27</v>
       </c>
       <c r="O96" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.25">
@@ -4543,10 +4536,10 @@
         <v>141</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C97" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D97" s="15"/>
       <c r="E97" s="15"/>
@@ -4557,10 +4550,10 @@
         <v>27</v>
       </c>
       <c r="H97" s="10" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="I97" s="10" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="J97" s="10" t="s">
         <v>82</v>
@@ -4569,7 +4562,7 @@
         <v>120</v>
       </c>
       <c r="L97" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="M97" t="s">
         <v>66</v>
@@ -4591,16 +4584,16 @@
       <c r="J98" s="10"/>
       <c r="K98" s="10"/>
       <c r="L98" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="M98" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N98" t="s">
         <v>27</v>
       </c>
       <c r="O98" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.25">
@@ -4608,7 +4601,7 @@
         <v>141</v>
       </c>
       <c r="B99" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F99" t="s">
         <v>25</v>
@@ -4617,10 +4610,10 @@
         <v>27</v>
       </c>
       <c r="H99" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
@@ -4628,10 +4621,10 @@
         <v>141</v>
       </c>
       <c r="B100" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F100" t="s">
         <v>25</v>
@@ -4640,7 +4633,7 @@
         <v>27</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="J100" t="s">
         <v>82</v>
@@ -4649,7 +4642,7 @@
         <v>120</v>
       </c>
       <c r="L100" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="M100" t="s">
         <v>66</v>
@@ -4658,7 +4651,7 @@
         <v>67</v>
       </c>
       <c r="O100" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.25">
@@ -4666,10 +4659,10 @@
         <v>141</v>
       </c>
       <c r="B101" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F101" t="s">
         <v>25</v>
@@ -4678,10 +4671,10 @@
         <v>27</v>
       </c>
       <c r="H101" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="J101" t="s">
         <v>82</v>
@@ -4690,7 +4683,7 @@
         <v>120</v>
       </c>
       <c r="L101" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="M101" t="s">
         <v>66</v>
@@ -4699,7 +4692,7 @@
         <v>67</v>
       </c>
       <c r="O101" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="102" spans="1:15" ht="60" x14ac:dyDescent="0.25">
@@ -4707,10 +4700,10 @@
         <v>141</v>
       </c>
       <c r="B102" s="10" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C102" s="14" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D102" s="15"/>
       <c r="E102" s="15"/>
@@ -4721,10 +4714,10 @@
         <v>27</v>
       </c>
       <c r="H102" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="I102" s="10" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="J102" s="10" t="s">
         <v>82</v>
@@ -4733,16 +4726,16 @@
         <v>120</v>
       </c>
       <c r="L102" t="s">
+        <v>253</v>
+      </c>
+      <c r="M102" t="s">
+        <v>66</v>
+      </c>
+      <c r="N102" t="s">
+        <v>67</v>
+      </c>
+      <c r="O102" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="M102" t="s">
-        <v>66</v>
-      </c>
-      <c r="N102" t="s">
-        <v>67</v>
-      </c>
-      <c r="O102" s="1" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.25">
@@ -4758,7 +4751,7 @@
       <c r="J103" s="10"/>
       <c r="K103" s="10"/>
       <c r="L103" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M103" t="s">
         <v>66</v>
@@ -4767,7 +4760,7 @@
         <v>67</v>
       </c>
       <c r="O103" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="104" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -4783,16 +4776,16 @@
       <c r="J104" s="10"/>
       <c r="K104" s="10"/>
       <c r="L104" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="M104" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N104" t="s">
         <v>27</v>
       </c>
       <c r="O104" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="105" spans="1:15" ht="45" x14ac:dyDescent="0.25">
@@ -4800,10 +4793,10 @@
         <v>141</v>
       </c>
       <c r="B105" s="10" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C105" s="14" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D105" s="15"/>
       <c r="E105" s="15"/>
@@ -4814,10 +4807,10 @@
         <v>27</v>
       </c>
       <c r="H105" s="10" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="I105" s="12" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="J105" s="10" t="s">
         <v>82</v>
@@ -4826,7 +4819,7 @@
         <v>120</v>
       </c>
       <c r="L105" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="M105" t="s">
         <v>66</v>
@@ -4835,7 +4828,7 @@
         <v>67</v>
       </c>
       <c r="O105" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="106" spans="1:15" ht="45" x14ac:dyDescent="0.25">
@@ -4851,7 +4844,7 @@
       <c r="J106" s="10"/>
       <c r="K106" s="10"/>
       <c r="L106" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="M106" t="s">
         <v>66</v>
@@ -4860,7 +4853,7 @@
         <v>67</v>
       </c>
       <c r="O106" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="107" spans="1:15" ht="60" x14ac:dyDescent="0.25">
@@ -4876,16 +4869,16 @@
       <c r="J107" s="10"/>
       <c r="K107" s="10"/>
       <c r="L107" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="M107" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="N107" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O107" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="108" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -4901,16 +4894,16 @@
       <c r="J108" s="10"/>
       <c r="K108" s="10"/>
       <c r="L108" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="M108" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N108" t="s">
         <v>27</v>
       </c>
       <c r="O108" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="109" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -4918,10 +4911,10 @@
         <v>141</v>
       </c>
       <c r="B109" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="F109" t="s">
         <v>25</v>
@@ -4930,7 +4923,7 @@
         <v>27</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="J109" t="s">
         <v>62</v>
@@ -4939,7 +4932,7 @@
         <v>119</v>
       </c>
       <c r="L109" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="M109" t="s">
         <v>66</v>
@@ -4948,7 +4941,7 @@
         <v>67</v>
       </c>
       <c r="O109" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="110" spans="1:15" ht="45" x14ac:dyDescent="0.25">
@@ -4956,10 +4949,10 @@
         <v>141</v>
       </c>
       <c r="B110" s="10" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C110" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D110" s="13"/>
       <c r="E110" s="13"/>
@@ -4971,7 +4964,7 @@
       </c>
       <c r="H110" s="10"/>
       <c r="I110" s="12" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="J110" s="10" t="s">
         <v>82</v>
@@ -4983,13 +4976,13 @@
         <v>47</v>
       </c>
       <c r="M110" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N110" t="s">
         <v>27</v>
       </c>
       <c r="O110" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="111" spans="1:15" ht="45" x14ac:dyDescent="0.25">
@@ -5005,16 +4998,16 @@
       <c r="J111" s="10"/>
       <c r="K111" s="10"/>
       <c r="L111" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="M111" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="N111" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O111" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.25">
@@ -5030,7 +5023,7 @@
       <c r="J112" s="10"/>
       <c r="K112" s="10"/>
       <c r="L112" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M112" t="s">
         <v>83</v>
@@ -5039,7 +5032,7 @@
         <v>27</v>
       </c>
       <c r="O112" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="113" spans="1:15" ht="45" x14ac:dyDescent="0.25">
@@ -5047,10 +5040,10 @@
         <v>141</v>
       </c>
       <c r="B113" s="10" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C113" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D113" s="13"/>
       <c r="E113" s="13"/>
@@ -5062,7 +5055,7 @@
       </c>
       <c r="H113" s="10"/>
       <c r="I113" s="12" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="J113" s="10" t="s">
         <v>82</v>
@@ -5074,13 +5067,13 @@
         <v>47</v>
       </c>
       <c r="M113" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N113" t="s">
         <v>27</v>
       </c>
       <c r="O113" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="114" spans="1:15" ht="45" x14ac:dyDescent="0.25">
@@ -5096,16 +5089,16 @@
       <c r="J114" s="10"/>
       <c r="K114" s="10"/>
       <c r="L114" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="M114" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="N114" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O114" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.25">
@@ -5121,7 +5114,7 @@
       <c r="J115" s="10"/>
       <c r="K115" s="10"/>
       <c r="L115" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M115" t="s">
         <v>83</v>
@@ -5130,7 +5123,7 @@
         <v>27</v>
       </c>
       <c r="O115" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="116" spans="1:15" ht="45" x14ac:dyDescent="0.25">
@@ -5138,10 +5131,10 @@
         <v>141</v>
       </c>
       <c r="B116" s="10" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C116" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D116" s="13"/>
       <c r="E116" s="13"/>
@@ -5153,7 +5146,7 @@
       </c>
       <c r="H116" s="10"/>
       <c r="I116" s="12" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="J116" s="10" t="s">
         <v>82</v>
@@ -5165,13 +5158,13 @@
         <v>47</v>
       </c>
       <c r="M116" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N116" t="s">
         <v>27</v>
       </c>
       <c r="O116" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="117" spans="1:15" ht="45" x14ac:dyDescent="0.25">
@@ -5187,16 +5180,16 @@
       <c r="J117" s="10"/>
       <c r="K117" s="10"/>
       <c r="L117" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="M117" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="N117" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O117" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.25">
@@ -5212,7 +5205,7 @@
       <c r="J118" s="10"/>
       <c r="K118" s="10"/>
       <c r="L118" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M118" t="s">
         <v>83</v>
@@ -5221,7 +5214,7 @@
         <v>27</v>
       </c>
       <c r="O118" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="119" spans="1:15" ht="45" x14ac:dyDescent="0.25">
@@ -5229,10 +5222,10 @@
         <v>141</v>
       </c>
       <c r="B119" s="10" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C119" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D119" s="13"/>
       <c r="E119" s="13"/>
@@ -5244,7 +5237,7 @@
       </c>
       <c r="H119" s="10"/>
       <c r="I119" s="12" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="J119" s="10" t="s">
         <v>82</v>
@@ -5256,13 +5249,13 @@
         <v>47</v>
       </c>
       <c r="M119" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N119" t="s">
         <v>27</v>
       </c>
       <c r="O119" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="120" spans="1:15" ht="45" x14ac:dyDescent="0.25">
@@ -5278,16 +5271,16 @@
       <c r="J120" s="10"/>
       <c r="K120" s="10"/>
       <c r="L120" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="M120" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="N120" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O120" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.25">
@@ -5303,7 +5296,7 @@
       <c r="J121" s="10"/>
       <c r="K121" s="10"/>
       <c r="L121" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M121" t="s">
         <v>83</v>
@@ -5312,7 +5305,12 @@
         <v>27</v>
       </c>
       <c r="O121" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -5351,25 +5349,15 @@
     <mergeCell ref="G113:G115"/>
     <mergeCell ref="H113:H115"/>
     <mergeCell ref="I113:I115"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="B34:B36"/>
     <mergeCell ref="D34:D36"/>
     <mergeCell ref="D37:D39"/>
     <mergeCell ref="D41:D47"/>
     <mergeCell ref="D57:D59"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="D64:D67"/>
-    <mergeCell ref="D68:D71"/>
-    <mergeCell ref="D72:D75"/>
-    <mergeCell ref="D78:D82"/>
-    <mergeCell ref="D83:D87"/>
-    <mergeCell ref="D88:D93"/>
-    <mergeCell ref="D94:D96"/>
-    <mergeCell ref="D97:D98"/>
-    <mergeCell ref="D102:D104"/>
-    <mergeCell ref="D105:D108"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="E37:E39"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
     <mergeCell ref="F22:F23"/>
     <mergeCell ref="G22:G23"/>
     <mergeCell ref="I22:I23"/>
@@ -5391,7 +5379,7 @@
     <mergeCell ref="E31:E33"/>
     <mergeCell ref="G24:G26"/>
     <mergeCell ref="F28:F30"/>
-    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="G28:G30"/>
     <mergeCell ref="K22:K23"/>
     <mergeCell ref="K41:K47"/>
     <mergeCell ref="J41:J47"/>
@@ -5416,6 +5404,12 @@
     <mergeCell ref="I37:I39"/>
     <mergeCell ref="J37:J39"/>
     <mergeCell ref="K37:K39"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="F31:F33"/>
     <mergeCell ref="K57:K59"/>
     <mergeCell ref="J57:J59"/>
     <mergeCell ref="I57:I59"/>
@@ -5430,23 +5424,8 @@
     <mergeCell ref="F57:F59"/>
     <mergeCell ref="B57:B59"/>
     <mergeCell ref="A57:A59"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="F34:F36"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="F37:F39"/>
-    <mergeCell ref="C41:C47"/>
-    <mergeCell ref="C57:C59"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="C37:C39"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="G28:G30"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="F31:F33"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="E37:E39"/>
     <mergeCell ref="G34:G36"/>
     <mergeCell ref="G37:G39"/>
     <mergeCell ref="A28:A30"/>
@@ -5460,6 +5439,15 @@
     <mergeCell ref="F62:F63"/>
     <mergeCell ref="G62:G63"/>
     <mergeCell ref="E62:E63"/>
+    <mergeCell ref="F34:F36"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="F37:F39"/>
+    <mergeCell ref="C41:C47"/>
+    <mergeCell ref="C57:C59"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="C37:C39"/>
+    <mergeCell ref="D62:D63"/>
     <mergeCell ref="G68:G71"/>
     <mergeCell ref="H68:H71"/>
     <mergeCell ref="I68:I71"/>
@@ -5480,6 +5468,8 @@
     <mergeCell ref="G64:G67"/>
     <mergeCell ref="E64:E67"/>
     <mergeCell ref="E68:E71"/>
+    <mergeCell ref="D64:D67"/>
+    <mergeCell ref="D68:D71"/>
     <mergeCell ref="G78:G82"/>
     <mergeCell ref="F78:F82"/>
     <mergeCell ref="C78:C82"/>
@@ -5500,6 +5490,8 @@
     <mergeCell ref="G72:G75"/>
     <mergeCell ref="E72:E75"/>
     <mergeCell ref="E78:E82"/>
+    <mergeCell ref="D72:D75"/>
+    <mergeCell ref="D78:D82"/>
     <mergeCell ref="F83:F87"/>
     <mergeCell ref="B83:B87"/>
     <mergeCell ref="A83:A87"/>
@@ -5520,6 +5512,8 @@
     <mergeCell ref="G83:G87"/>
     <mergeCell ref="E83:E87"/>
     <mergeCell ref="E88:E93"/>
+    <mergeCell ref="D83:D87"/>
+    <mergeCell ref="D88:D93"/>
     <mergeCell ref="F94:F96"/>
     <mergeCell ref="B94:B96"/>
     <mergeCell ref="A94:A96"/>
@@ -5530,6 +5524,7 @@
     <mergeCell ref="H94:H96"/>
     <mergeCell ref="G94:G96"/>
     <mergeCell ref="E94:E96"/>
+    <mergeCell ref="D94:D96"/>
     <mergeCell ref="F97:F98"/>
     <mergeCell ref="B97:B98"/>
     <mergeCell ref="A97:A98"/>
@@ -5550,6 +5545,8 @@
     <mergeCell ref="G97:G98"/>
     <mergeCell ref="E97:E98"/>
     <mergeCell ref="E102:E104"/>
+    <mergeCell ref="D97:D98"/>
+    <mergeCell ref="D102:D104"/>
     <mergeCell ref="H105:H108"/>
     <mergeCell ref="G105:G108"/>
     <mergeCell ref="F105:F108"/>
@@ -5560,6 +5557,7 @@
     <mergeCell ref="J105:J108"/>
     <mergeCell ref="I105:I108"/>
     <mergeCell ref="E105:E108"/>
+    <mergeCell ref="D105:D108"/>
     <mergeCell ref="A110:A112"/>
     <mergeCell ref="H110:H112"/>
     <mergeCell ref="G110:G112"/>

</xml_diff>

<commit_message>
Updating Som APIs Mapping
git-tfs-id: [http://developmentvlan:8585/tfs/vanrise.collection]$/;C55352
</commit_message>
<xml_diff>
--- a/SOM/Documents/SOM/SOM APIs Mapping Sheet.xlsx
+++ b/SOM/Documents/SOM/SOM APIs Mapping Sheet.xlsx
@@ -11,7 +11,7 @@
     <sheet name="API Calls" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'API Calls'!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'API Calls'!$A$1:$R$1</definedName>
   </definedNames>
   <calcPr calcId="152511" calcMode="manual"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="302">
   <si>
     <t>GetTechnicalDetails</t>
   </si>
@@ -935,12 +935,39 @@
   <si>
     <t>This is not needed in telephony because we can depened on contratsSearchResponse it has Directory Number</t>
   </si>
+  <si>
+    <t>MappingSheetResources\GetCallDetails\usageDataRecordsReadRequest.txt</t>
+  </si>
+  <si>
+    <t>MappingSheetResources\GetCallDetails\GetCallDetailsRequest.txt</t>
+  </si>
+  <si>
+    <t>MappingSheetResources\GetCallDetails\GetCallDetailsResponse.txt</t>
+  </si>
+  <si>
+    <t>Request Mapping</t>
+  </si>
+  <si>
+    <t>Response Mapping</t>
+  </si>
+  <si>
+    <t>MappingSheetResources\GetCallDetails\usageDataRecordsReadResponse.txt</t>
+  </si>
+  <si>
+    <t>Issues on Bug Tracker</t>
+  </si>
+  <si>
+    <t>We should ask Ericson to increase the limit of calls more than 50. We need to make sure also that MOC is the correct call type. Also make sure of the response we are getting if it is correct, check the issue on bug tracker #28</t>
+  </si>
+  <si>
+    <t>http://94.130.97.86:8888/edit_bug.aspx?id=28</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -967,6 +994,14 @@
     <font>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1043,11 +1078,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1101,9 +1137,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1566,11 +1609,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O122"/>
+  <dimension ref="A1:R122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E28" sqref="E28:E30"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q54" sqref="Q54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1585,10 +1628,11 @@
     <col min="12" max="12" width="38" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="36.7109375" style="1" customWidth="1"/>
+    <col min="15" max="17" width="22.42578125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="36.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -1628,11 +1672,20 @@
       <c r="N1" t="s">
         <v>63</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="R1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>141</v>
       </c>
@@ -1664,7 +1717,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>141</v>
       </c>
@@ -1696,7 +1749,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>141</v>
       </c>
@@ -1728,7 +1781,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>141</v>
       </c>
@@ -1760,7 +1813,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>141</v>
       </c>
@@ -1792,7 +1845,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>141</v>
       </c>
@@ -1824,7 +1877,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>141</v>
       </c>
@@ -1856,7 +1909,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>141</v>
       </c>
@@ -1888,7 +1941,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>141</v>
       </c>
@@ -1920,7 +1973,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>141</v>
       </c>
@@ -1952,7 +2005,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>141</v>
       </c>
@@ -1984,7 +2037,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>141</v>
       </c>
@@ -2016,7 +2069,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>141</v>
       </c>
@@ -2048,7 +2101,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>141</v>
       </c>
@@ -2080,7 +2133,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>141</v>
       </c>
@@ -2112,7 +2165,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>141</v>
       </c>
@@ -2144,7 +2197,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>141</v>
       </c>
@@ -2176,7 +2229,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>141</v>
       </c>
@@ -2208,7 +2261,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>141</v>
       </c>
@@ -2240,7 +2293,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>141</v>
       </c>
@@ -2275,7 +2328,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>141</v>
       </c>
@@ -2314,11 +2367,11 @@
       <c r="N22" t="s">
         <v>67</v>
       </c>
-      <c r="O22" s="1" t="s">
+      <c r="R22" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="17"/>
       <c r="C23" s="11"/>
@@ -2339,11 +2392,11 @@
       <c r="N23" t="s">
         <v>27</v>
       </c>
-      <c r="O23" s="1" t="s">
+      <c r="R23" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>141</v>
       </c>
@@ -2382,9 +2435,9 @@
       <c r="N24" t="s">
         <v>67</v>
       </c>
-      <c r="O24"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R24"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
       <c r="C25" s="11"/>
@@ -2406,7 +2459,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="10"/>
       <c r="C26" s="11"/>
@@ -2427,11 +2480,11 @@
       <c r="N26" t="s">
         <v>67</v>
       </c>
-      <c r="O26" s="1" t="s">
+      <c r="R26" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>141</v>
       </c>
@@ -2471,7 +2524,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>141</v>
       </c>
@@ -2510,11 +2563,11 @@
       <c r="N28" t="s">
         <v>67</v>
       </c>
-      <c r="O28" s="1" t="s">
+      <c r="R28" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
       <c r="C29" s="11"/>
@@ -2536,7 +2589,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
       <c r="B30" s="10"/>
       <c r="C30" s="11"/>
@@ -2557,11 +2610,11 @@
       <c r="N30" t="s">
         <v>67</v>
       </c>
-      <c r="O30" s="1" t="s">
+      <c r="R30" s="1" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>141</v>
       </c>
@@ -2601,7 +2654,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="10"/>
       <c r="C32" s="11"/>
@@ -2623,7 +2676,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
       <c r="B33" s="10"/>
       <c r="C33" s="11"/>
@@ -2644,11 +2697,11 @@
       <c r="N33" t="s">
         <v>67</v>
       </c>
-      <c r="O33" s="1" t="s">
+      <c r="R33" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>141</v>
       </c>
@@ -2688,7 +2741,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
       <c r="B35" s="10"/>
       <c r="C35" s="11"/>
@@ -2710,7 +2763,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
       <c r="B36" s="10"/>
       <c r="C36" s="11"/>
@@ -2731,11 +2784,11 @@
       <c r="N36" t="s">
         <v>67</v>
       </c>
-      <c r="O36" s="1" t="s">
+      <c r="R36" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>141</v>
       </c>
@@ -2775,7 +2828,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
       <c r="B38" s="10"/>
       <c r="C38" s="11"/>
@@ -2797,7 +2850,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
       <c r="B39" s="10"/>
       <c r="C39" s="11"/>
@@ -2819,7 +2872,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>141</v>
       </c>
@@ -2855,11 +2908,11 @@
       <c r="N40" t="s">
         <v>67</v>
       </c>
-      <c r="O40" s="1" t="s">
+      <c r="R40" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
         <v>141</v>
       </c>
@@ -2899,7 +2952,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="10"/>
       <c r="C42" s="11"/>
@@ -2921,7 +2974,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="B43" s="10"/>
       <c r="C43" s="11"/>
@@ -2942,9 +2995,9 @@
       <c r="N43" t="s">
         <v>67</v>
       </c>
-      <c r="O43"/>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R43"/>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="B44" s="10"/>
       <c r="C44" s="11"/>
@@ -2965,9 +3018,9 @@
       <c r="N44" t="s">
         <v>67</v>
       </c>
-      <c r="O44"/>
-    </row>
-    <row r="45" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="R44"/>
+    </row>
+    <row r="45" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="10"/>
       <c r="C45" s="11"/>
@@ -2988,11 +3041,11 @@
       <c r="N45" t="s">
         <v>67</v>
       </c>
-      <c r="O45" s="1" t="s">
+      <c r="R45" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="10"/>
       <c r="C46" s="11"/>
@@ -3014,7 +3067,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="B47" s="10"/>
       <c r="C47" s="11"/>
@@ -3036,7 +3089,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>141</v>
       </c>
@@ -3076,7 +3129,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>141</v>
       </c>
@@ -3116,7 +3169,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>141</v>
       </c>
@@ -3156,7 +3209,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>141</v>
       </c>
@@ -3195,11 +3248,11 @@
       <c r="N51" t="s">
         <v>67</v>
       </c>
-      <c r="O51" s="2" t="s">
+      <c r="R51" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>141</v>
       </c>
@@ -3236,9 +3289,9 @@
       <c r="N52" t="s">
         <v>67</v>
       </c>
-      <c r="O52"/>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R52"/>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>141</v>
       </c>
@@ -3273,13 +3326,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" ht="90" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>141</v>
       </c>
       <c r="B54" t="s">
         <v>79</v>
       </c>
+      <c r="D54" s="22" t="s">
+        <v>294</v>
+      </c>
+      <c r="E54" s="22" t="s">
+        <v>295</v>
+      </c>
       <c r="F54" t="s">
         <v>25</v>
       </c>
@@ -3307,8 +3366,20 @@
       <c r="N54" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" ht="105" x14ac:dyDescent="0.25">
+      <c r="O54" s="21" t="s">
+        <v>293</v>
+      </c>
+      <c r="P54" s="21" t="s">
+        <v>298</v>
+      </c>
+      <c r="Q54" s="21" t="s">
+        <v>301</v>
+      </c>
+      <c r="R54" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" ht="105" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>141</v>
       </c>
@@ -3342,11 +3413,11 @@
       <c r="N55" t="s">
         <v>67</v>
       </c>
-      <c r="O55" s="1" t="s">
+      <c r="R55" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>141</v>
       </c>
@@ -3381,7 +3452,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
         <v>141</v>
       </c>
@@ -3419,7 +3490,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="10"/>
       <c r="B58" s="10"/>
       <c r="C58" s="12"/>
@@ -3441,7 +3512,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="10"/>
       <c r="B59" s="10"/>
       <c r="C59" s="12"/>
@@ -3462,11 +3533,11 @@
       <c r="N59" t="s">
         <v>67</v>
       </c>
-      <c r="O59" s="2" t="s">
+      <c r="R59" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="60" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>141</v>
       </c>
@@ -3497,11 +3568,11 @@
       <c r="N60" t="s">
         <v>67</v>
       </c>
-      <c r="O60" s="1" t="s">
+      <c r="R60" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="61" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>141</v>
       </c>
@@ -3535,11 +3606,11 @@
       <c r="N61" t="s">
         <v>67</v>
       </c>
-      <c r="O61" s="1" t="s">
+      <c r="R61" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="17" t="s">
         <v>141</v>
       </c>
@@ -3578,11 +3649,11 @@
       <c r="N62" t="s">
         <v>27</v>
       </c>
-      <c r="O62" s="1" t="s">
+      <c r="R62" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="17"/>
       <c r="B63" s="17"/>
       <c r="C63" s="14"/>
@@ -3603,11 +3674,11 @@
       <c r="N63" t="s">
         <v>67</v>
       </c>
-      <c r="O63" s="1" t="s">
+      <c r="R63" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
         <v>141</v>
       </c>
@@ -3646,11 +3717,11 @@
       <c r="N64" t="s">
         <v>67</v>
       </c>
-      <c r="O64" s="1" t="s">
+      <c r="R64" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="90" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" ht="90" x14ac:dyDescent="0.25">
       <c r="A65" s="10"/>
       <c r="B65" s="10"/>
       <c r="C65" s="14"/>
@@ -3671,11 +3742,11 @@
       <c r="N65" t="s">
         <v>67</v>
       </c>
-      <c r="O65" s="1" t="s">
+      <c r="R65" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="10"/>
       <c r="B66" s="10"/>
       <c r="C66" s="14"/>
@@ -3697,7 +3768,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="10"/>
       <c r="B67" s="10"/>
       <c r="C67" s="14"/>
@@ -3719,7 +3790,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
         <v>141</v>
       </c>
@@ -3758,11 +3829,11 @@
       <c r="N68" t="s">
         <v>67</v>
       </c>
-      <c r="O68" s="1" t="s">
+      <c r="R68" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="10"/>
       <c r="B69" s="10"/>
       <c r="C69" s="14"/>
@@ -3784,7 +3855,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="10"/>
       <c r="B70" s="10"/>
       <c r="C70" s="14"/>
@@ -3806,7 +3877,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" s="10"/>
       <c r="B71" s="10"/>
       <c r="C71" s="14"/>
@@ -3828,7 +3899,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
         <v>141</v>
       </c>
@@ -3868,7 +3939,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" s="10"/>
       <c r="B73" s="10"/>
       <c r="C73" s="14"/>
@@ -3890,7 +3961,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" s="10"/>
       <c r="B74" s="10"/>
       <c r="C74" s="14"/>
@@ -3912,7 +3983,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" s="10"/>
       <c r="B75" s="10"/>
       <c r="C75" s="14"/>
@@ -3934,7 +4005,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="76" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>141</v>
       </c>
@@ -3968,11 +4039,11 @@
       <c r="N76" t="s">
         <v>67</v>
       </c>
-      <c r="O76" s="1" t="s">
+      <c r="R76" s="1" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="77" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>141</v>
       </c>
@@ -4006,11 +4077,11 @@
       <c r="N77" t="s">
         <v>67</v>
       </c>
-      <c r="O77" s="1" t="s">
+      <c r="R77" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
         <v>141</v>
       </c>
@@ -4049,11 +4120,11 @@
       <c r="N78" t="s">
         <v>27</v>
       </c>
-      <c r="O78" s="1" t="s">
+      <c r="R78" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="10"/>
       <c r="B79" s="10"/>
       <c r="C79" s="14"/>
@@ -4074,11 +4145,11 @@
       <c r="N79" t="s">
         <v>212</v>
       </c>
-      <c r="O79" s="1" t="s">
+      <c r="R79" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="10"/>
       <c r="B80" s="10"/>
       <c r="C80" s="14"/>
@@ -4099,11 +4170,11 @@
       <c r="N80" t="s">
         <v>27</v>
       </c>
-      <c r="O80" s="1" t="s">
+      <c r="R80" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A81" s="10"/>
       <c r="B81" s="10"/>
       <c r="C81" s="14"/>
@@ -4124,11 +4195,11 @@
       <c r="N81" t="s">
         <v>67</v>
       </c>
-      <c r="O81" s="1" t="s">
+      <c r="R81" s="1" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" s="10"/>
       <c r="B82" s="10"/>
       <c r="C82" s="14"/>
@@ -4150,7 +4221,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="83" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="16" t="s">
         <v>141</v>
       </c>
@@ -4188,7 +4259,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" s="16"/>
       <c r="B84" s="10"/>
       <c r="C84" s="14"/>
@@ -4210,7 +4281,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" s="16"/>
       <c r="B85" s="10"/>
       <c r="C85" s="14"/>
@@ -4232,7 +4303,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" s="16"/>
       <c r="B86" s="10"/>
       <c r="C86" s="14"/>
@@ -4254,7 +4325,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="87" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A87" s="16"/>
       <c r="B87" s="10"/>
       <c r="C87" s="14"/>
@@ -4275,11 +4346,11 @@
       <c r="N87" t="s">
         <v>67</v>
       </c>
-      <c r="O87" s="1" t="s">
+      <c r="R87" s="1" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="88" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="10" t="s">
         <v>141</v>
       </c>
@@ -4318,11 +4389,11 @@
       <c r="N88" t="s">
         <v>27</v>
       </c>
-      <c r="O88" s="1" t="s">
+      <c r="R88" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="89" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="10"/>
       <c r="B89" s="10"/>
       <c r="C89" s="14"/>
@@ -4343,11 +4414,11 @@
       <c r="N89" t="s">
         <v>27</v>
       </c>
-      <c r="O89" s="1" t="s">
+      <c r="R89" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="90" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="10"/>
       <c r="B90" s="10"/>
       <c r="C90" s="14"/>
@@ -4368,11 +4439,11 @@
       <c r="N90" t="s">
         <v>27</v>
       </c>
-      <c r="O90" s="1" t="s">
+      <c r="R90" s="1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="91" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A91" s="10"/>
       <c r="B91" s="10"/>
       <c r="C91" s="14"/>
@@ -4393,11 +4464,11 @@
       <c r="N91" t="s">
         <v>27</v>
       </c>
-      <c r="O91" s="1" t="s">
+      <c r="R91" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" s="10"/>
       <c r="B92" s="10"/>
       <c r="C92" s="14"/>
@@ -4419,7 +4490,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" s="10"/>
       <c r="B93" s="10"/>
       <c r="C93" s="14"/>
@@ -4441,7 +4512,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" s="10" t="s">
         <v>141</v>
       </c>
@@ -4481,7 +4552,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="95" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A95" s="10"/>
       <c r="B95" s="10"/>
       <c r="C95" s="14"/>
@@ -4502,11 +4573,11 @@
       <c r="N95" t="s">
         <v>212</v>
       </c>
-      <c r="O95" s="1" t="s">
+      <c r="R95" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="96" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="10"/>
       <c r="B96" s="10"/>
       <c r="C96" s="14"/>
@@ -4527,11 +4598,11 @@
       <c r="N96" t="s">
         <v>27</v>
       </c>
-      <c r="O96" s="1" t="s">
+      <c r="R96" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" s="10" t="s">
         <v>141</v>
       </c>
@@ -4571,7 +4642,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="98" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A98" s="10"/>
       <c r="B98" s="10"/>
       <c r="C98" s="14"/>
@@ -4592,11 +4663,11 @@
       <c r="N98" t="s">
         <v>27</v>
       </c>
-      <c r="O98" s="1" t="s">
+      <c r="R98" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>141</v>
       </c>
@@ -4616,7 +4687,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>141</v>
       </c>
@@ -4650,11 +4721,11 @@
       <c r="N100" t="s">
         <v>67</v>
       </c>
-      <c r="O100" s="1" t="s">
+      <c r="R100" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>141</v>
       </c>
@@ -4691,11 +4762,11 @@
       <c r="N101" t="s">
         <v>67</v>
       </c>
-      <c r="O101" s="1" t="s">
+      <c r="R101" s="1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="102" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A102" s="10" t="s">
         <v>141</v>
       </c>
@@ -4734,11 +4805,11 @@
       <c r="N102" t="s">
         <v>67</v>
       </c>
-      <c r="O102" s="1" t="s">
+      <c r="R102" s="1" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103" s="10"/>
       <c r="B103" s="10"/>
       <c r="C103" s="14"/>
@@ -4759,11 +4830,11 @@
       <c r="N103" t="s">
         <v>67</v>
       </c>
-      <c r="O103" s="1" t="s">
+      <c r="R103" s="1" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="104" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="10"/>
       <c r="B104" s="10"/>
       <c r="C104" s="14"/>
@@ -4784,11 +4855,11 @@
       <c r="N104" t="s">
         <v>27</v>
       </c>
-      <c r="O104" s="1" t="s">
+      <c r="R104" s="1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="105" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A105" s="10" t="s">
         <v>141</v>
       </c>
@@ -4827,11 +4898,11 @@
       <c r="N105" t="s">
         <v>67</v>
       </c>
-      <c r="O105" s="1" t="s">
+      <c r="R105" s="1" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="106" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A106" s="10"/>
       <c r="B106" s="10"/>
       <c r="C106" s="14"/>
@@ -4852,11 +4923,11 @@
       <c r="N106" t="s">
         <v>67</v>
       </c>
-      <c r="O106" s="1" t="s">
+      <c r="R106" s="1" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="107" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A107" s="10"/>
       <c r="B107" s="10"/>
       <c r="C107" s="14"/>
@@ -4877,11 +4948,11 @@
       <c r="N107" t="s">
         <v>212</v>
       </c>
-      <c r="O107" s="1" t="s">
+      <c r="R107" s="1" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="108" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="10"/>
       <c r="B108" s="10"/>
       <c r="C108" s="14"/>
@@ -4902,11 +4973,11 @@
       <c r="N108" t="s">
         <v>27</v>
       </c>
-      <c r="O108" s="1" t="s">
+      <c r="R108" s="1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="109" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>141</v>
       </c>
@@ -4940,11 +5011,11 @@
       <c r="N109" t="s">
         <v>67</v>
       </c>
-      <c r="O109" s="1" t="s">
+      <c r="R109" s="1" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="110" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A110" s="10" t="s">
         <v>141</v>
       </c>
@@ -4981,11 +5052,11 @@
       <c r="N110" t="s">
         <v>27</v>
       </c>
-      <c r="O110" s="1" t="s">
+      <c r="R110" s="1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="111" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A111" s="10"/>
       <c r="B111" s="10"/>
       <c r="C111" s="11"/>
@@ -5006,11 +5077,11 @@
       <c r="N111" t="s">
         <v>212</v>
       </c>
-      <c r="O111" s="1" t="s">
+      <c r="R111" s="1" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A112" s="10"/>
       <c r="B112" s="10"/>
       <c r="C112" s="11"/>
@@ -5031,11 +5102,11 @@
       <c r="N112" t="s">
         <v>27</v>
       </c>
-      <c r="O112" s="1" t="s">
+      <c r="R112" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="113" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A113" s="10" t="s">
         <v>141</v>
       </c>
@@ -5072,11 +5143,11 @@
       <c r="N113" t="s">
         <v>27</v>
       </c>
-      <c r="O113" s="1" t="s">
+      <c r="R113" s="1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="114" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A114" s="10"/>
       <c r="B114" s="10"/>
       <c r="C114" s="11"/>
@@ -5097,11 +5168,11 @@
       <c r="N114" t="s">
         <v>212</v>
       </c>
-      <c r="O114" s="1" t="s">
+      <c r="R114" s="1" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A115" s="10"/>
       <c r="B115" s="10"/>
       <c r="C115" s="11"/>
@@ -5122,11 +5193,11 @@
       <c r="N115" t="s">
         <v>27</v>
       </c>
-      <c r="O115" s="1" t="s">
+      <c r="R115" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="116" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A116" s="10" t="s">
         <v>141</v>
       </c>
@@ -5163,11 +5234,11 @@
       <c r="N116" t="s">
         <v>27</v>
       </c>
-      <c r="O116" s="1" t="s">
+      <c r="R116" s="1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="117" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A117" s="10"/>
       <c r="B117" s="10"/>
       <c r="C117" s="11"/>
@@ -5188,11 +5259,11 @@
       <c r="N117" t="s">
         <v>212</v>
       </c>
-      <c r="O117" s="1" t="s">
+      <c r="R117" s="1" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A118" s="10"/>
       <c r="B118" s="10"/>
       <c r="C118" s="11"/>
@@ -5213,11 +5284,11 @@
       <c r="N118" t="s">
         <v>27</v>
       </c>
-      <c r="O118" s="1" t="s">
+      <c r="R118" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="119" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A119" s="10" t="s">
         <v>141</v>
       </c>
@@ -5254,11 +5325,11 @@
       <c r="N119" t="s">
         <v>27</v>
       </c>
-      <c r="O119" s="1" t="s">
+      <c r="R119" s="1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="120" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A120" s="10"/>
       <c r="B120" s="10"/>
       <c r="C120" s="11"/>
@@ -5279,11 +5350,11 @@
       <c r="N120" t="s">
         <v>212</v>
       </c>
-      <c r="O120" s="1" t="s">
+      <c r="R120" s="1" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A121" s="10"/>
       <c r="B121" s="10"/>
       <c r="C121" s="11"/>
@@ -5304,17 +5375,17 @@
       <c r="N121" t="s">
         <v>27</v>
       </c>
-      <c r="O121" s="1" t="s">
+      <c r="R121" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>141</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O1"/>
+  <autoFilter ref="A1:R1"/>
   <mergeCells count="253">
     <mergeCell ref="A119:A121"/>
     <mergeCell ref="B119:B121"/>
@@ -5358,6 +5429,10 @@
     <mergeCell ref="D37:D39"/>
     <mergeCell ref="D41:D47"/>
     <mergeCell ref="D57:D59"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="B31:B33"/>
     <mergeCell ref="F22:F23"/>
     <mergeCell ref="G22:G23"/>
     <mergeCell ref="I22:I23"/>
@@ -5380,6 +5455,8 @@
     <mergeCell ref="G24:G26"/>
     <mergeCell ref="F28:F30"/>
     <mergeCell ref="G28:G30"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="F31:F33"/>
     <mergeCell ref="K22:K23"/>
     <mergeCell ref="K41:K47"/>
     <mergeCell ref="J41:J47"/>
@@ -5404,12 +5481,6 @@
     <mergeCell ref="I37:I39"/>
     <mergeCell ref="J37:J39"/>
     <mergeCell ref="K37:K39"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="F31:F33"/>
     <mergeCell ref="K57:K59"/>
     <mergeCell ref="J57:J59"/>
     <mergeCell ref="I57:I59"/>
@@ -5570,15 +5641,22 @@
     <mergeCell ref="D110:D112"/>
     <mergeCell ref="E110:E112"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="O54" r:id="rId1"/>
+    <hyperlink ref="D54" r:id="rId2"/>
+    <hyperlink ref="E54" r:id="rId3"/>
+    <hyperlink ref="P54" r:id="rId4"/>
+    <hyperlink ref="Q54" r:id="rId5"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId6"/>
+  <drawing r:id="rId7"/>
+  <legacyDrawing r:id="rId8"/>
   <oleObjects>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="1025" r:id="rId4">
-          <objectPr defaultSize="0" r:id="rId5">
+        <oleObject progId="Packager Shell Object" shapeId="1025" r:id="rId9">
+          <objectPr defaultSize="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>3</xdr:col>
@@ -5597,13 +5675,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="1025" r:id="rId4"/>
+        <oleObject progId="Packager Shell Object" shapeId="1025" r:id="rId9"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="1026" r:id="rId6">
-          <objectPr defaultSize="0" r:id="rId7">
+        <oleObject progId="Packager Shell Object" shapeId="1026" r:id="rId11">
+          <objectPr defaultSize="0" r:id="rId12">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -5622,7 +5700,7 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="1026" r:id="rId6"/>
+        <oleObject progId="Packager Shell Object" shapeId="1026" r:id="rId11"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </oleObjects>

</xml_diff>

<commit_message>
Addign user story column to SOM API Mapping
git-tfs-id: [http://developmentvlan:8585/tfs/vanrise.collection]$/;C55356
</commit_message>
<xml_diff>
--- a/SOM/Documents/SOM/SOM APIs Mapping Sheet.xlsx
+++ b/SOM/Documents/SOM/SOM APIs Mapping Sheet.xlsx
@@ -9,9 +9,10 @@
   <sheets>
     <sheet name="Revision History" sheetId="5" r:id="rId1"/>
     <sheet name="API Calls" sheetId="4" r:id="rId2"/>
+    <sheet name="Tables" sheetId="6" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'API Calls'!$A$1:$S$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'API Calls'!$A$1:$U$1</definedName>
   </definedNames>
   <calcPr calcId="152511" calcMode="manual"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="312">
   <si>
     <t>GetTechnicalDetails</t>
   </si>
@@ -967,6 +968,30 @@
   </si>
   <si>
     <t>Post</t>
+  </si>
+  <si>
+    <t>Related User Story</t>
+  </si>
+  <si>
+    <t>http://192.168.110.185:8585/tfs/web/UI/Pages/WorkItems/WorkItemEdit.aspx?id=6963&amp;pguid=81f5a887-a9da-41fc-8c45-50b4cb40e1ea</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>On Hold</t>
+  </si>
+  <si>
+    <t>Requires Confirmation</t>
   </si>
 </sst>
 </file>
@@ -1089,7 +1114,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1117,10 +1142,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1135,20 +1157,27 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -1615,11 +1644,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S121"/>
+  <dimension ref="A1:U121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A122" sqref="A122"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1635,11 +1664,12 @@
     <col min="13" max="13" width="38" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="22.42578125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="36.7109375" style="1" customWidth="1"/>
+    <col min="16" max="19" width="22.42578125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="19.85546875" style="12" customWidth="1"/>
+    <col min="21" max="21" width="36.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -1691,11 +1721,17 @@
       <c r="R1" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="T1" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="U1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>141</v>
       </c>
@@ -1727,7 +1763,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>141</v>
       </c>
@@ -1759,7 +1795,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>141</v>
       </c>
@@ -1791,7 +1827,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>141</v>
       </c>
@@ -1823,7 +1859,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>141</v>
       </c>
@@ -1855,7 +1891,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>141</v>
       </c>
@@ -1887,7 +1923,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>141</v>
       </c>
@@ -1919,7 +1955,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>141</v>
       </c>
@@ -1951,7 +1987,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>141</v>
       </c>
@@ -1983,7 +2019,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>141</v>
       </c>
@@ -2015,7 +2051,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>141</v>
       </c>
@@ -2047,7 +2083,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>141</v>
       </c>
@@ -2079,7 +2115,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>141</v>
       </c>
@@ -2111,7 +2147,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>141</v>
       </c>
@@ -2143,7 +2179,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>141</v>
       </c>
@@ -2175,7 +2211,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>141</v>
       </c>
@@ -2207,7 +2243,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>141</v>
       </c>
@@ -2239,7 +2275,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>141</v>
       </c>
@@ -2271,7 +2307,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>141</v>
       </c>
@@ -2303,7 +2339,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>141</v>
       </c>
@@ -2338,35 +2374,35 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B22" s="20" t="s">
+    <row r="22" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B22" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="15" t="s">
+      <c r="C22" s="20"/>
+      <c r="D22" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="H22" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="I22" s="20" t="s">
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="I22" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="J22" s="18" t="s">
+      <c r="J22" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="K22" s="12" t="s">
+      <c r="K22" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="L22" s="20" t="s">
+      <c r="L22" s="18" t="s">
         <v>120</v>
       </c>
       <c r="M22" t="s">
@@ -2378,23 +2414,23 @@
       <c r="O22" t="s">
         <v>67</v>
       </c>
-      <c r="S22" s="1" t="s">
+      <c r="U22" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="20"/>
+    <row r="23" spans="1:21" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="18"/>
       <c r="M23" t="s">
         <v>157</v>
       </c>
@@ -2404,39 +2440,39 @@
       <c r="O23" t="s">
         <v>27</v>
       </c>
-      <c r="S23" s="1" t="s">
+      <c r="U23" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B24" s="14" t="s">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B24" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="15" t="s">
+      <c r="C24" s="17"/>
+      <c r="D24" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I24" s="16" t="s">
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="J24" s="14" t="s">
+      <c r="J24" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="K24" s="14" t="s">
+      <c r="K24" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="L24" s="21" t="s">
+      <c r="L24" s="22" t="s">
         <v>120</v>
       </c>
       <c r="M24" t="s">
@@ -2448,21 +2484,21 @@
       <c r="O24" t="s">
         <v>67</v>
       </c>
-      <c r="S24"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="21"/>
+      <c r="U24"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="22"/>
       <c r="M25" t="s">
         <v>73</v>
       </c>
@@ -2473,19 +2509,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="21"/>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" s="13"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="22"/>
       <c r="M26" t="s">
         <v>135</v>
       </c>
@@ -2495,11 +2531,11 @@
       <c r="O26" t="s">
         <v>67</v>
       </c>
-      <c r="S26" s="1" t="s">
+      <c r="U26" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>141</v>
       </c>
@@ -2539,35 +2575,35 @@
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B28" s="14" t="s">
+    <row r="28" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B28" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="15" t="s">
+      <c r="C28" s="17"/>
+      <c r="D28" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H28" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I28" s="14" t="s">
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I28" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="J28" s="16" t="s">
+      <c r="J28" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="K28" s="14" t="s">
+      <c r="K28" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="L28" s="14" t="s">
+      <c r="L28" s="13" t="s">
         <v>119</v>
       </c>
       <c r="M28" t="s">
@@ -2579,23 +2615,23 @@
       <c r="O28" t="s">
         <v>67</v>
       </c>
-      <c r="S28" s="1" t="s">
+      <c r="U28" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
       <c r="M29" t="s">
         <v>85</v>
       </c>
@@ -2606,19 +2642,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="16"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
+    <row r="30" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
       <c r="M30" t="s">
         <v>90</v>
       </c>
@@ -2628,39 +2664,39 @@
       <c r="O30" t="s">
         <v>67</v>
       </c>
-      <c r="S30" s="1" t="s">
+      <c r="U30" s="1" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B31" s="14" t="s">
+    <row r="31" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B31" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="15" t="s">
+      <c r="C31" s="17"/>
+      <c r="D31" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H31" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I31" s="14" t="s">
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I31" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="J31" s="16" t="s">
+      <c r="J31" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="K31" s="14" t="s">
+      <c r="K31" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="L31" s="14" t="s">
+      <c r="L31" s="13" t="s">
         <v>119</v>
       </c>
       <c r="M31" t="s">
@@ -2673,19 +2709,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="16"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
+    <row r="32" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
       <c r="M32" t="s">
         <v>85</v>
       </c>
@@ -2696,19 +2732,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="16"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
+    <row r="33" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="13"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
       <c r="M33" t="s">
         <v>90</v>
       </c>
@@ -2718,39 +2754,39 @@
       <c r="O33" t="s">
         <v>67</v>
       </c>
-      <c r="S33" s="1" t="s">
+      <c r="U33" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B34" s="14" t="s">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B34" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="15" t="s">
+      <c r="C34" s="17"/>
+      <c r="D34" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H34" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I34" s="14" t="s">
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I34" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="J34" s="16" t="s">
+      <c r="J34" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="K34" s="14" t="s">
+      <c r="K34" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="L34" s="14" t="s">
+      <c r="L34" s="13" t="s">
         <v>119</v>
       </c>
       <c r="M34" t="s">
@@ -2763,19 +2799,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="16"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35" s="13"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
       <c r="M35" t="s">
         <v>85</v>
       </c>
@@ -2786,19 +2822,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="16"/>
-      <c r="K36" s="14"/>
-      <c r="L36" s="14"/>
+    <row r="36" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
       <c r="M36" t="s">
         <v>90</v>
       </c>
@@ -2808,39 +2844,39 @@
       <c r="O36" t="s">
         <v>67</v>
       </c>
-      <c r="S36" s="1" t="s">
+      <c r="U36" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B37" s="14" t="s">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B37" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="15" t="s">
+      <c r="C37" s="17"/>
+      <c r="D37" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H37" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I37" s="14" t="s">
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H37" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I37" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="J37" s="16" t="s">
+      <c r="J37" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="K37" s="14" t="s">
+      <c r="K37" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="L37" s="14" t="s">
+      <c r="L37" s="13" t="s">
         <v>119</v>
       </c>
       <c r="M37" t="s">
@@ -2853,19 +2889,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="16"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38" s="13"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
       <c r="M38" t="s">
         <v>85</v>
       </c>
@@ -2876,19 +2912,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="16"/>
-      <c r="K39" s="14"/>
-      <c r="L39" s="14"/>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39" s="13"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="15"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
       <c r="M39" t="s">
         <v>90</v>
       </c>
@@ -2899,7 +2935,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>141</v>
       </c>
@@ -2935,39 +2971,39 @@
       <c r="O40" t="s">
         <v>67</v>
       </c>
-      <c r="S40" s="1" t="s">
+      <c r="U40" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B41" s="14" t="s">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B41" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="C41" s="13"/>
-      <c r="D41" s="15" t="s">
+      <c r="C41" s="17"/>
+      <c r="D41" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H41" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I41" s="14" t="s">
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I41" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="J41" s="16" t="s">
+      <c r="J41" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="K41" s="14" t="s">
+      <c r="K41" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="L41" s="14" t="s">
+      <c r="L41" s="13" t="s">
         <v>119</v>
       </c>
       <c r="M41" t="s">
@@ -2980,19 +3016,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="16"/>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A42" s="13"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="15"/>
+      <c r="K42" s="13"/>
+      <c r="L42" s="13"/>
       <c r="M42" t="s">
         <v>90</v>
       </c>
@@ -3003,19 +3039,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="17"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="16"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A43" s="13"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="15"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="13"/>
       <c r="M43" t="s">
         <v>91</v>
       </c>
@@ -3025,21 +3061,21 @@
       <c r="O43" t="s">
         <v>67</v>
       </c>
-      <c r="S43"/>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
-      <c r="B44" s="14"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="16"/>
-      <c r="K44" s="14"/>
-      <c r="L44" s="14"/>
+      <c r="U43"/>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A44" s="13"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="15"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="13"/>
       <c r="M44" t="s">
         <v>93</v>
       </c>
@@ -3049,21 +3085,21 @@
       <c r="O44" t="s">
         <v>67</v>
       </c>
-      <c r="S44"/>
-    </row>
-    <row r="45" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="14"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="17"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
-      <c r="J45" s="16"/>
-      <c r="K45" s="14"/>
-      <c r="L45" s="14"/>
+      <c r="U44"/>
+    </row>
+    <row r="45" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="13"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="15"/>
+      <c r="K45" s="13"/>
+      <c r="L45" s="13"/>
       <c r="M45" t="s">
         <v>81</v>
       </c>
@@ -3073,23 +3109,23 @@
       <c r="O45" t="s">
         <v>67</v>
       </c>
-      <c r="S45" s="1" t="s">
+      <c r="U45" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="16"/>
-      <c r="K46" s="14"/>
-      <c r="L46" s="14"/>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A46" s="13"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="15"/>
+      <c r="K46" s="13"/>
+      <c r="L46" s="13"/>
       <c r="M46" t="s">
         <v>126</v>
       </c>
@@ -3100,19 +3136,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
-      <c r="B47" s="14"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="14"/>
-      <c r="J47" s="16"/>
-      <c r="K47" s="14"/>
-      <c r="L47" s="14"/>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A47" s="13"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="15"/>
+      <c r="K47" s="13"/>
+      <c r="L47" s="13"/>
       <c r="M47" t="s">
         <v>47</v>
       </c>
@@ -3123,7 +3159,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>141</v>
       </c>
@@ -3163,7 +3199,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>141</v>
       </c>
@@ -3203,7 +3239,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>141</v>
       </c>
@@ -3243,7 +3279,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>141</v>
       </c>
@@ -3282,11 +3318,11 @@
       <c r="O51" t="s">
         <v>67</v>
       </c>
-      <c r="S51" s="2" t="s">
+      <c r="U51" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>141</v>
       </c>
@@ -3323,9 +3359,9 @@
       <c r="O52" t="s">
         <v>67</v>
       </c>
-      <c r="S52"/>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U52"/>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>141</v>
       </c>
@@ -3360,8 +3396,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="90" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="54" spans="1:21" ht="90" x14ac:dyDescent="0.25">
+      <c r="A54" s="24" t="s">
         <v>141</v>
       </c>
       <c r="B54" t="s">
@@ -3412,11 +3448,17 @@
       <c r="R54" s="10" t="s">
         <v>301</v>
       </c>
-      <c r="S54" s="1" t="s">
+      <c r="S54" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="T54" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="U54" s="1" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="105" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" ht="105" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>141</v>
       </c>
@@ -3450,11 +3492,11 @@
       <c r="O55" t="s">
         <v>67</v>
       </c>
-      <c r="S55" s="1" t="s">
+      <c r="U55" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>141</v>
       </c>
@@ -3489,33 +3531,33 @@
         <v>67</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A57" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B57" s="14" t="s">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A57" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B57" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="C57" s="13"/>
-      <c r="D57" s="16"/>
-      <c r="E57" s="22"/>
-      <c r="F57" s="22"/>
-      <c r="G57" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H57" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I57" s="14" t="s">
+      <c r="C57" s="17"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="19"/>
+      <c r="G57" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H57" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I57" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="J57" s="16" t="s">
+      <c r="J57" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="K57" s="14" t="s">
+      <c r="K57" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="L57" s="21" t="s">
+      <c r="L57" s="22" t="s">
         <v>120</v>
       </c>
       <c r="M57" t="s">
@@ -3528,19 +3570,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A58" s="14"/>
-      <c r="B58" s="14"/>
-      <c r="C58" s="13"/>
-      <c r="D58" s="16"/>
-      <c r="E58" s="22"/>
-      <c r="F58" s="22"/>
-      <c r="G58" s="14"/>
-      <c r="H58" s="14"/>
-      <c r="I58" s="14"/>
-      <c r="J58" s="16"/>
-      <c r="K58" s="14"/>
-      <c r="L58" s="21"/>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A58" s="13"/>
+      <c r="B58" s="13"/>
+      <c r="C58" s="17"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="19"/>
+      <c r="F58" s="19"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="13"/>
+      <c r="J58" s="15"/>
+      <c r="K58" s="13"/>
+      <c r="L58" s="22"/>
       <c r="M58" t="s">
         <v>132</v>
       </c>
@@ -3551,19 +3593,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A59" s="14"/>
-      <c r="B59" s="14"/>
-      <c r="C59" s="13"/>
-      <c r="D59" s="16"/>
-      <c r="E59" s="22"/>
-      <c r="F59" s="22"/>
-      <c r="G59" s="14"/>
-      <c r="H59" s="14"/>
-      <c r="I59" s="14"/>
-      <c r="J59" s="16"/>
-      <c r="K59" s="14"/>
-      <c r="L59" s="21"/>
+    <row r="59" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="13"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="17"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="19"/>
+      <c r="F59" s="19"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="13"/>
+      <c r="J59" s="15"/>
+      <c r="K59" s="13"/>
+      <c r="L59" s="22"/>
       <c r="M59" t="s">
         <v>133</v>
       </c>
@@ -3573,11 +3615,11 @@
       <c r="O59" t="s">
         <v>67</v>
       </c>
-      <c r="S59" s="2" t="s">
+      <c r="U59" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>141</v>
       </c>
@@ -3608,11 +3650,11 @@
       <c r="O60" t="s">
         <v>67</v>
       </c>
-      <c r="S60" s="1" t="s">
+      <c r="U60" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>141</v>
       </c>
@@ -3646,39 +3688,39 @@
       <c r="O61" t="s">
         <v>67</v>
       </c>
-      <c r="S61" s="1" t="s">
+      <c r="U61" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="B62" s="20" t="s">
+    <row r="62" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="B62" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="C62" s="12"/>
-      <c r="D62" s="18" t="s">
+      <c r="C62" s="20"/>
+      <c r="D62" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="E62" s="19"/>
-      <c r="F62" s="19"/>
-      <c r="G62" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="H62" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="I62" s="14" t="s">
+      <c r="E62" s="23"/>
+      <c r="F62" s="23"/>
+      <c r="G62" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="H62" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="I62" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="J62" s="16" t="s">
+      <c r="J62" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="K62" s="14" t="s">
+      <c r="K62" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="L62" s="14" t="s">
+      <c r="L62" s="13" t="s">
         <v>119</v>
       </c>
       <c r="M62" t="s">
@@ -3690,23 +3732,23 @@
       <c r="O62" t="s">
         <v>27</v>
       </c>
-      <c r="S62" s="1" t="s">
+      <c r="U62" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A63" s="20"/>
-      <c r="B63" s="20"/>
-      <c r="C63" s="12"/>
-      <c r="D63" s="18"/>
-      <c r="E63" s="19"/>
-      <c r="F63" s="19"/>
-      <c r="G63" s="20"/>
-      <c r="H63" s="20"/>
-      <c r="I63" s="14"/>
-      <c r="J63" s="16"/>
-      <c r="K63" s="14"/>
-      <c r="L63" s="14"/>
+    <row r="63" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A63" s="18"/>
+      <c r="B63" s="18"/>
+      <c r="C63" s="20"/>
+      <c r="D63" s="21"/>
+      <c r="E63" s="23"/>
+      <c r="F63" s="23"/>
+      <c r="G63" s="18"/>
+      <c r="H63" s="18"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="15"/>
+      <c r="K63" s="13"/>
+      <c r="L63" s="13"/>
       <c r="M63" t="s">
         <v>182</v>
       </c>
@@ -3716,39 +3758,39 @@
       <c r="O63" t="s">
         <v>67</v>
       </c>
-      <c r="S63" s="1" t="s">
+      <c r="U63" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B64" s="14" t="s">
+    <row r="64" spans="1:21" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B64" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="C64" s="13"/>
-      <c r="D64" s="18" t="s">
+      <c r="C64" s="17"/>
+      <c r="D64" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="E64" s="19"/>
-      <c r="F64" s="19"/>
-      <c r="G64" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H64" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I64" s="14" t="s">
+      <c r="E64" s="23"/>
+      <c r="F64" s="23"/>
+      <c r="G64" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H64" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I64" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="J64" s="14" t="s">
+      <c r="J64" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="K64" s="14" t="s">
+      <c r="K64" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="L64" s="14" t="s">
+      <c r="L64" s="13" t="s">
         <v>120</v>
       </c>
       <c r="M64" t="s">
@@ -3760,23 +3802,23 @@
       <c r="O64" t="s">
         <v>67</v>
       </c>
-      <c r="S64" s="1" t="s">
+      <c r="U64" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="90" x14ac:dyDescent="0.25">
-      <c r="A65" s="14"/>
-      <c r="B65" s="14"/>
-      <c r="C65" s="13"/>
-      <c r="D65" s="18"/>
-      <c r="E65" s="19"/>
-      <c r="F65" s="19"/>
-      <c r="G65" s="14"/>
-      <c r="H65" s="14"/>
-      <c r="I65" s="14"/>
-      <c r="J65" s="14"/>
-      <c r="K65" s="14"/>
-      <c r="L65" s="14"/>
+    <row r="65" spans="1:21" ht="90" x14ac:dyDescent="0.25">
+      <c r="A65" s="13"/>
+      <c r="B65" s="13"/>
+      <c r="C65" s="17"/>
+      <c r="D65" s="21"/>
+      <c r="E65" s="23"/>
+      <c r="F65" s="23"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="13"/>
+      <c r="I65" s="13"/>
+      <c r="J65" s="13"/>
+      <c r="K65" s="13"/>
+      <c r="L65" s="13"/>
       <c r="M65" t="s">
         <v>187</v>
       </c>
@@ -3786,23 +3828,23 @@
       <c r="O65" t="s">
         <v>67</v>
       </c>
-      <c r="S65" s="1" t="s">
+      <c r="U65" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A66" s="14"/>
-      <c r="B66" s="14"/>
-      <c r="C66" s="13"/>
-      <c r="D66" s="18"/>
-      <c r="E66" s="19"/>
-      <c r="F66" s="19"/>
-      <c r="G66" s="14"/>
-      <c r="H66" s="14"/>
-      <c r="I66" s="14"/>
-      <c r="J66" s="14"/>
-      <c r="K66" s="14"/>
-      <c r="L66" s="14"/>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A66" s="13"/>
+      <c r="B66" s="13"/>
+      <c r="C66" s="17"/>
+      <c r="D66" s="21"/>
+      <c r="E66" s="23"/>
+      <c r="F66" s="23"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="13"/>
+      <c r="I66" s="13"/>
+      <c r="J66" s="13"/>
+      <c r="K66" s="13"/>
+      <c r="L66" s="13"/>
       <c r="M66" t="s">
         <v>190</v>
       </c>
@@ -3813,19 +3855,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A67" s="14"/>
-      <c r="B67" s="14"/>
-      <c r="C67" s="13"/>
-      <c r="D67" s="18"/>
-      <c r="E67" s="19"/>
-      <c r="F67" s="19"/>
-      <c r="G67" s="14"/>
-      <c r="H67" s="14"/>
-      <c r="I67" s="14"/>
-      <c r="J67" s="14"/>
-      <c r="K67" s="14"/>
-      <c r="L67" s="14"/>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A67" s="13"/>
+      <c r="B67" s="13"/>
+      <c r="C67" s="17"/>
+      <c r="D67" s="21"/>
+      <c r="E67" s="23"/>
+      <c r="F67" s="23"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="13"/>
+      <c r="I67" s="13"/>
+      <c r="J67" s="13"/>
+      <c r="K67" s="13"/>
+      <c r="L67" s="13"/>
       <c r="M67" t="s">
         <v>191</v>
       </c>
@@ -3836,35 +3878,35 @@
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B68" s="14" t="s">
+    <row r="68" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B68" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="C68" s="13"/>
-      <c r="D68" s="18" t="s">
+      <c r="C68" s="17"/>
+      <c r="D68" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="E68" s="19"/>
-      <c r="F68" s="19"/>
-      <c r="G68" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H68" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I68" s="14" t="s">
+      <c r="E68" s="23"/>
+      <c r="F68" s="23"/>
+      <c r="G68" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H68" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I68" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="J68" s="14" t="s">
+      <c r="J68" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="K68" s="14" t="s">
+      <c r="K68" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="L68" s="14" t="s">
+      <c r="L68" s="13" t="s">
         <v>120</v>
       </c>
       <c r="M68" t="s">
@@ -3876,23 +3918,23 @@
       <c r="O68" t="s">
         <v>67</v>
       </c>
-      <c r="S68" s="1" t="s">
+      <c r="U68" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A69" s="14"/>
-      <c r="B69" s="14"/>
-      <c r="C69" s="13"/>
-      <c r="D69" s="18"/>
-      <c r="E69" s="19"/>
-      <c r="F69" s="19"/>
-      <c r="G69" s="14"/>
-      <c r="H69" s="14"/>
-      <c r="I69" s="14"/>
-      <c r="J69" s="14"/>
-      <c r="K69" s="14"/>
-      <c r="L69" s="14"/>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A69" s="13"/>
+      <c r="B69" s="13"/>
+      <c r="C69" s="17"/>
+      <c r="D69" s="21"/>
+      <c r="E69" s="23"/>
+      <c r="F69" s="23"/>
+      <c r="G69" s="13"/>
+      <c r="H69" s="13"/>
+      <c r="I69" s="13"/>
+      <c r="J69" s="13"/>
+      <c r="K69" s="13"/>
+      <c r="L69" s="13"/>
       <c r="M69" t="s">
         <v>187</v>
       </c>
@@ -3903,19 +3945,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A70" s="14"/>
-      <c r="B70" s="14"/>
-      <c r="C70" s="13"/>
-      <c r="D70" s="18"/>
-      <c r="E70" s="19"/>
-      <c r="F70" s="19"/>
-      <c r="G70" s="14"/>
-      <c r="H70" s="14"/>
-      <c r="I70" s="14"/>
-      <c r="J70" s="14"/>
-      <c r="K70" s="14"/>
-      <c r="L70" s="14"/>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A70" s="13"/>
+      <c r="B70" s="13"/>
+      <c r="C70" s="17"/>
+      <c r="D70" s="21"/>
+      <c r="E70" s="23"/>
+      <c r="F70" s="23"/>
+      <c r="G70" s="13"/>
+      <c r="H70" s="13"/>
+      <c r="I70" s="13"/>
+      <c r="J70" s="13"/>
+      <c r="K70" s="13"/>
+      <c r="L70" s="13"/>
       <c r="M70" t="s">
         <v>190</v>
       </c>
@@ -3926,19 +3968,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A71" s="14"/>
-      <c r="B71" s="14"/>
-      <c r="C71" s="13"/>
-      <c r="D71" s="18"/>
-      <c r="E71" s="19"/>
-      <c r="F71" s="19"/>
-      <c r="G71" s="14"/>
-      <c r="H71" s="14"/>
-      <c r="I71" s="14"/>
-      <c r="J71" s="14"/>
-      <c r="K71" s="14"/>
-      <c r="L71" s="14"/>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A71" s="13"/>
+      <c r="B71" s="13"/>
+      <c r="C71" s="17"/>
+      <c r="D71" s="21"/>
+      <c r="E71" s="23"/>
+      <c r="F71" s="23"/>
+      <c r="G71" s="13"/>
+      <c r="H71" s="13"/>
+      <c r="I71" s="13"/>
+      <c r="J71" s="13"/>
+      <c r="K71" s="13"/>
+      <c r="L71" s="13"/>
       <c r="M71" t="s">
         <v>191</v>
       </c>
@@ -3949,35 +3991,35 @@
         <v>67</v>
       </c>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A72" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B72" s="14" t="s">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A72" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B72" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="C72" s="13"/>
-      <c r="D72" s="18" t="s">
+      <c r="C72" s="17"/>
+      <c r="D72" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="E72" s="19"/>
-      <c r="F72" s="19"/>
-      <c r="G72" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H72" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I72" s="14" t="s">
+      <c r="E72" s="23"/>
+      <c r="F72" s="23"/>
+      <c r="G72" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H72" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I72" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="J72" s="14" t="s">
+      <c r="J72" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="K72" s="14" t="s">
+      <c r="K72" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="L72" s="14" t="s">
+      <c r="L72" s="13" t="s">
         <v>120</v>
       </c>
       <c r="M72" t="s">
@@ -3990,19 +4032,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A73" s="14"/>
-      <c r="B73" s="14"/>
-      <c r="C73" s="13"/>
-      <c r="D73" s="18"/>
-      <c r="E73" s="19"/>
-      <c r="F73" s="19"/>
-      <c r="G73" s="14"/>
-      <c r="H73" s="14"/>
-      <c r="I73" s="14"/>
-      <c r="J73" s="14"/>
-      <c r="K73" s="14"/>
-      <c r="L73" s="14"/>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A73" s="13"/>
+      <c r="B73" s="13"/>
+      <c r="C73" s="17"/>
+      <c r="D73" s="21"/>
+      <c r="E73" s="23"/>
+      <c r="F73" s="23"/>
+      <c r="G73" s="13"/>
+      <c r="H73" s="13"/>
+      <c r="I73" s="13"/>
+      <c r="J73" s="13"/>
+      <c r="K73" s="13"/>
+      <c r="L73" s="13"/>
       <c r="M73" t="s">
         <v>187</v>
       </c>
@@ -4013,19 +4055,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A74" s="14"/>
-      <c r="B74" s="14"/>
-      <c r="C74" s="13"/>
-      <c r="D74" s="18"/>
-      <c r="E74" s="19"/>
-      <c r="F74" s="19"/>
-      <c r="G74" s="14"/>
-      <c r="H74" s="14"/>
-      <c r="I74" s="14"/>
-      <c r="J74" s="14"/>
-      <c r="K74" s="14"/>
-      <c r="L74" s="14"/>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A74" s="13"/>
+      <c r="B74" s="13"/>
+      <c r="C74" s="17"/>
+      <c r="D74" s="21"/>
+      <c r="E74" s="23"/>
+      <c r="F74" s="23"/>
+      <c r="G74" s="13"/>
+      <c r="H74" s="13"/>
+      <c r="I74" s="13"/>
+      <c r="J74" s="13"/>
+      <c r="K74" s="13"/>
+      <c r="L74" s="13"/>
       <c r="M74" t="s">
         <v>190</v>
       </c>
@@ -4036,19 +4078,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A75" s="14"/>
-      <c r="B75" s="14"/>
-      <c r="C75" s="13"/>
-      <c r="D75" s="18"/>
-      <c r="E75" s="19"/>
-      <c r="F75" s="19"/>
-      <c r="G75" s="14"/>
-      <c r="H75" s="14"/>
-      <c r="I75" s="14"/>
-      <c r="J75" s="14"/>
-      <c r="K75" s="14"/>
-      <c r="L75" s="14"/>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A75" s="13"/>
+      <c r="B75" s="13"/>
+      <c r="C75" s="17"/>
+      <c r="D75" s="21"/>
+      <c r="E75" s="23"/>
+      <c r="F75" s="23"/>
+      <c r="G75" s="13"/>
+      <c r="H75" s="13"/>
+      <c r="I75" s="13"/>
+      <c r="J75" s="13"/>
+      <c r="K75" s="13"/>
+      <c r="L75" s="13"/>
       <c r="M75" t="s">
         <v>191</v>
       </c>
@@ -4059,7 +4101,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="76" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>141</v>
       </c>
@@ -4093,11 +4135,11 @@
       <c r="O76" t="s">
         <v>67</v>
       </c>
-      <c r="S76" s="1" t="s">
+      <c r="U76" s="1" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="77" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>141</v>
       </c>
@@ -4131,39 +4173,39 @@
       <c r="O77" t="s">
         <v>67</v>
       </c>
-      <c r="S77" s="1" t="s">
+      <c r="U77" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="78" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B78" s="14" t="s">
+    <row r="78" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B78" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="C78" s="13"/>
-      <c r="D78" s="18" t="s">
+      <c r="C78" s="17"/>
+      <c r="D78" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="E78" s="19"/>
-      <c r="F78" s="19"/>
-      <c r="G78" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H78" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I78" s="14" t="s">
+      <c r="E78" s="23"/>
+      <c r="F78" s="23"/>
+      <c r="G78" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H78" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I78" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="J78" s="14" t="s">
+      <c r="J78" s="13" t="s">
         <v>210</v>
       </c>
-      <c r="K78" s="14" t="s">
+      <c r="K78" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="L78" s="14" t="s">
+      <c r="L78" s="13" t="s">
         <v>120</v>
       </c>
       <c r="M78" t="s">
@@ -4175,23 +4217,23 @@
       <c r="O78" t="s">
         <v>27</v>
       </c>
-      <c r="S78" s="1" t="s">
+      <c r="U78" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="79" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A79" s="14"/>
-      <c r="B79" s="14"/>
-      <c r="C79" s="13"/>
-      <c r="D79" s="18"/>
-      <c r="E79" s="19"/>
-      <c r="F79" s="19"/>
-      <c r="G79" s="14"/>
-      <c r="H79" s="14"/>
-      <c r="I79" s="14"/>
-      <c r="J79" s="14"/>
-      <c r="K79" s="14"/>
-      <c r="L79" s="14"/>
+    <row r="79" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A79" s="13"/>
+      <c r="B79" s="13"/>
+      <c r="C79" s="17"/>
+      <c r="D79" s="21"/>
+      <c r="E79" s="23"/>
+      <c r="F79" s="23"/>
+      <c r="G79" s="13"/>
+      <c r="H79" s="13"/>
+      <c r="I79" s="13"/>
+      <c r="J79" s="13"/>
+      <c r="K79" s="13"/>
+      <c r="L79" s="13"/>
       <c r="M79" t="s">
         <v>212</v>
       </c>
@@ -4201,23 +4243,23 @@
       <c r="O79" t="s">
         <v>212</v>
       </c>
-      <c r="S79" s="1" t="s">
+      <c r="U79" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="80" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="14"/>
-      <c r="B80" s="14"/>
-      <c r="C80" s="13"/>
-      <c r="D80" s="18"/>
-      <c r="E80" s="19"/>
-      <c r="F80" s="19"/>
-      <c r="G80" s="14"/>
-      <c r="H80" s="14"/>
-      <c r="I80" s="14"/>
-      <c r="J80" s="14"/>
-      <c r="K80" s="14"/>
-      <c r="L80" s="14"/>
+    <row r="80" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="13"/>
+      <c r="B80" s="13"/>
+      <c r="C80" s="17"/>
+      <c r="D80" s="21"/>
+      <c r="E80" s="23"/>
+      <c r="F80" s="23"/>
+      <c r="G80" s="13"/>
+      <c r="H80" s="13"/>
+      <c r="I80" s="13"/>
+      <c r="J80" s="13"/>
+      <c r="K80" s="13"/>
+      <c r="L80" s="13"/>
       <c r="M80" t="s">
         <v>214</v>
       </c>
@@ -4227,23 +4269,23 @@
       <c r="O80" t="s">
         <v>27</v>
       </c>
-      <c r="S80" s="1" t="s">
+      <c r="U80" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="81" spans="1:19" ht="60" x14ac:dyDescent="0.25">
-      <c r="A81" s="14"/>
-      <c r="B81" s="14"/>
-      <c r="C81" s="13"/>
-      <c r="D81" s="18"/>
-      <c r="E81" s="19"/>
-      <c r="F81" s="19"/>
-      <c r="G81" s="14"/>
-      <c r="H81" s="14"/>
-      <c r="I81" s="14"/>
-      <c r="J81" s="14"/>
-      <c r="K81" s="14"/>
-      <c r="L81" s="14"/>
+    <row r="81" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+      <c r="A81" s="13"/>
+      <c r="B81" s="13"/>
+      <c r="C81" s="17"/>
+      <c r="D81" s="21"/>
+      <c r="E81" s="23"/>
+      <c r="F81" s="23"/>
+      <c r="G81" s="13"/>
+      <c r="H81" s="13"/>
+      <c r="I81" s="13"/>
+      <c r="J81" s="13"/>
+      <c r="K81" s="13"/>
+      <c r="L81" s="13"/>
       <c r="M81" t="s">
         <v>132</v>
       </c>
@@ -4253,23 +4295,23 @@
       <c r="O81" t="s">
         <v>67</v>
       </c>
-      <c r="S81" s="1" t="s">
+      <c r="U81" s="1" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A82" s="14"/>
-      <c r="B82" s="14"/>
-      <c r="C82" s="13"/>
-      <c r="D82" s="18"/>
-      <c r="E82" s="19"/>
-      <c r="F82" s="19"/>
-      <c r="G82" s="14"/>
-      <c r="H82" s="14"/>
-      <c r="I82" s="14"/>
-      <c r="J82" s="14"/>
-      <c r="K82" s="14"/>
-      <c r="L82" s="14"/>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A82" s="13"/>
+      <c r="B82" s="13"/>
+      <c r="C82" s="17"/>
+      <c r="D82" s="21"/>
+      <c r="E82" s="23"/>
+      <c r="F82" s="23"/>
+      <c r="G82" s="13"/>
+      <c r="H82" s="13"/>
+      <c r="I82" s="13"/>
+      <c r="J82" s="13"/>
+      <c r="K82" s="13"/>
+      <c r="L82" s="13"/>
       <c r="M82" t="s">
         <v>133</v>
       </c>
@@ -4280,33 +4322,33 @@
         <v>67</v>
       </c>
     </row>
-    <row r="83" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B83" s="14" t="s">
+    <row r="83" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B83" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="C83" s="13"/>
-      <c r="D83" s="18" t="s">
+      <c r="C83" s="17"/>
+      <c r="D83" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="E83" s="19"/>
-      <c r="F83" s="19"/>
-      <c r="G83" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H83" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I83" s="14"/>
-      <c r="J83" s="14" t="s">
+      <c r="E83" s="23"/>
+      <c r="F83" s="23"/>
+      <c r="G83" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H83" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I83" s="13"/>
+      <c r="J83" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="K83" s="14" t="s">
+      <c r="K83" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="L83" s="14" t="s">
+      <c r="L83" s="13" t="s">
         <v>120</v>
       </c>
       <c r="M83" t="s">
@@ -4319,19 +4361,19 @@
         <v>27</v>
       </c>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A84" s="13"/>
-      <c r="B84" s="14"/>
-      <c r="C84" s="13"/>
-      <c r="D84" s="18"/>
-      <c r="E84" s="19"/>
-      <c r="F84" s="19"/>
-      <c r="G84" s="14"/>
-      <c r="H84" s="14"/>
-      <c r="I84" s="14"/>
-      <c r="J84" s="14"/>
-      <c r="K84" s="14"/>
-      <c r="L84" s="14"/>
+    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A84" s="17"/>
+      <c r="B84" s="13"/>
+      <c r="C84" s="17"/>
+      <c r="D84" s="21"/>
+      <c r="E84" s="23"/>
+      <c r="F84" s="23"/>
+      <c r="G84" s="13"/>
+      <c r="H84" s="13"/>
+      <c r="I84" s="13"/>
+      <c r="J84" s="13"/>
+      <c r="K84" s="13"/>
+      <c r="L84" s="13"/>
       <c r="M84" t="s">
         <v>212</v>
       </c>
@@ -4342,19 +4384,19 @@
         <v>212</v>
       </c>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A85" s="13"/>
-      <c r="B85" s="14"/>
-      <c r="C85" s="13"/>
-      <c r="D85" s="18"/>
-      <c r="E85" s="19"/>
-      <c r="F85" s="19"/>
-      <c r="G85" s="14"/>
-      <c r="H85" s="14"/>
-      <c r="I85" s="14"/>
-      <c r="J85" s="14"/>
-      <c r="K85" s="14"/>
-      <c r="L85" s="14"/>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A85" s="17"/>
+      <c r="B85" s="13"/>
+      <c r="C85" s="17"/>
+      <c r="D85" s="21"/>
+      <c r="E85" s="23"/>
+      <c r="F85" s="23"/>
+      <c r="G85" s="13"/>
+      <c r="H85" s="13"/>
+      <c r="I85" s="13"/>
+      <c r="J85" s="13"/>
+      <c r="K85" s="13"/>
+      <c r="L85" s="13"/>
       <c r="M85" t="s">
         <v>214</v>
       </c>
@@ -4365,19 +4407,19 @@
         <v>27</v>
       </c>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A86" s="13"/>
-      <c r="B86" s="14"/>
-      <c r="C86" s="13"/>
-      <c r="D86" s="18"/>
-      <c r="E86" s="19"/>
-      <c r="F86" s="19"/>
-      <c r="G86" s="14"/>
-      <c r="H86" s="14"/>
-      <c r="I86" s="14"/>
-      <c r="J86" s="14"/>
-      <c r="K86" s="14"/>
-      <c r="L86" s="14"/>
+    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A86" s="17"/>
+      <c r="B86" s="13"/>
+      <c r="C86" s="17"/>
+      <c r="D86" s="21"/>
+      <c r="E86" s="23"/>
+      <c r="F86" s="23"/>
+      <c r="G86" s="13"/>
+      <c r="H86" s="13"/>
+      <c r="I86" s="13"/>
+      <c r="J86" s="13"/>
+      <c r="K86" s="13"/>
+      <c r="L86" s="13"/>
       <c r="M86" t="s">
         <v>132</v>
       </c>
@@ -4388,19 +4430,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="87" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A87" s="13"/>
-      <c r="B87" s="14"/>
-      <c r="C87" s="13"/>
-      <c r="D87" s="18"/>
-      <c r="E87" s="19"/>
-      <c r="F87" s="19"/>
-      <c r="G87" s="14"/>
-      <c r="H87" s="14"/>
-      <c r="I87" s="14"/>
-      <c r="J87" s="14"/>
-      <c r="K87" s="14"/>
-      <c r="L87" s="14"/>
+    <row r="87" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A87" s="17"/>
+      <c r="B87" s="13"/>
+      <c r="C87" s="17"/>
+      <c r="D87" s="21"/>
+      <c r="E87" s="23"/>
+      <c r="F87" s="23"/>
+      <c r="G87" s="13"/>
+      <c r="H87" s="13"/>
+      <c r="I87" s="13"/>
+      <c r="J87" s="13"/>
+      <c r="K87" s="13"/>
+      <c r="L87" s="13"/>
       <c r="M87" t="s">
         <v>133</v>
       </c>
@@ -4410,39 +4452,39 @@
       <c r="O87" t="s">
         <v>67</v>
       </c>
-      <c r="S87" s="1" t="s">
+      <c r="U87" s="1" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="88" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B88" s="14" t="s">
+    <row r="88" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B88" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="C88" s="13"/>
-      <c r="D88" s="18" t="s">
+      <c r="C88" s="17"/>
+      <c r="D88" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="E88" s="19"/>
-      <c r="F88" s="19"/>
-      <c r="G88" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H88" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I88" s="14" t="s">
+      <c r="E88" s="23"/>
+      <c r="F88" s="23"/>
+      <c r="G88" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H88" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I88" s="13" t="s">
         <v>224</v>
       </c>
-      <c r="J88" s="14" t="s">
+      <c r="J88" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="K88" s="14" t="s">
+      <c r="K88" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="L88" s="14" t="s">
+      <c r="L88" s="13" t="s">
         <v>120</v>
       </c>
       <c r="M88" t="s">
@@ -4454,23 +4496,23 @@
       <c r="O88" t="s">
         <v>27</v>
       </c>
-      <c r="S88" s="1" t="s">
+      <c r="U88" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="89" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="14"/>
-      <c r="B89" s="14"/>
-      <c r="C89" s="13"/>
-      <c r="D89" s="18"/>
-      <c r="E89" s="19"/>
-      <c r="F89" s="19"/>
-      <c r="G89" s="14"/>
-      <c r="H89" s="14"/>
-      <c r="I89" s="14"/>
-      <c r="J89" s="14"/>
-      <c r="K89" s="14"/>
-      <c r="L89" s="14"/>
+    <row r="89" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="13"/>
+      <c r="B89" s="13"/>
+      <c r="C89" s="17"/>
+      <c r="D89" s="21"/>
+      <c r="E89" s="23"/>
+      <c r="F89" s="23"/>
+      <c r="G89" s="13"/>
+      <c r="H89" s="13"/>
+      <c r="I89" s="13"/>
+      <c r="J89" s="13"/>
+      <c r="K89" s="13"/>
+      <c r="L89" s="13"/>
       <c r="M89" t="s">
         <v>47</v>
       </c>
@@ -4480,23 +4522,23 @@
       <c r="O89" t="s">
         <v>27</v>
       </c>
-      <c r="S89" s="1" t="s">
+      <c r="U89" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="90" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="14"/>
-      <c r="B90" s="14"/>
-      <c r="C90" s="13"/>
-      <c r="D90" s="18"/>
-      <c r="E90" s="19"/>
-      <c r="F90" s="19"/>
-      <c r="G90" s="14"/>
-      <c r="H90" s="14"/>
-      <c r="I90" s="14"/>
-      <c r="J90" s="14"/>
-      <c r="K90" s="14"/>
-      <c r="L90" s="14"/>
+    <row r="90" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" s="13"/>
+      <c r="B90" s="13"/>
+      <c r="C90" s="17"/>
+      <c r="D90" s="21"/>
+      <c r="E90" s="23"/>
+      <c r="F90" s="23"/>
+      <c r="G90" s="13"/>
+      <c r="H90" s="13"/>
+      <c r="I90" s="13"/>
+      <c r="J90" s="13"/>
+      <c r="K90" s="13"/>
+      <c r="L90" s="13"/>
       <c r="M90" t="s">
         <v>180</v>
       </c>
@@ -4506,23 +4548,23 @@
       <c r="O90" t="s">
         <v>27</v>
       </c>
-      <c r="S90" s="1" t="s">
+      <c r="U90" s="1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="91" spans="1:19" ht="75" x14ac:dyDescent="0.25">
-      <c r="A91" s="14"/>
-      <c r="B91" s="14"/>
-      <c r="C91" s="13"/>
-      <c r="D91" s="18"/>
-      <c r="E91" s="19"/>
-      <c r="F91" s="19"/>
-      <c r="G91" s="14"/>
-      <c r="H91" s="14"/>
-      <c r="I91" s="14"/>
-      <c r="J91" s="14"/>
-      <c r="K91" s="14"/>
-      <c r="L91" s="14"/>
+    <row r="91" spans="1:21" ht="75" x14ac:dyDescent="0.25">
+      <c r="A91" s="13"/>
+      <c r="B91" s="13"/>
+      <c r="C91" s="17"/>
+      <c r="D91" s="21"/>
+      <c r="E91" s="23"/>
+      <c r="F91" s="23"/>
+      <c r="G91" s="13"/>
+      <c r="H91" s="13"/>
+      <c r="I91" s="13"/>
+      <c r="J91" s="13"/>
+      <c r="K91" s="13"/>
+      <c r="L91" s="13"/>
       <c r="M91" t="s">
         <v>214</v>
       </c>
@@ -4532,23 +4574,23 @@
       <c r="O91" t="s">
         <v>27</v>
       </c>
-      <c r="S91" s="1" t="s">
+      <c r="U91" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A92" s="14"/>
-      <c r="B92" s="14"/>
-      <c r="C92" s="13"/>
-      <c r="D92" s="18"/>
-      <c r="E92" s="19"/>
-      <c r="F92" s="19"/>
-      <c r="G92" s="14"/>
-      <c r="H92" s="14"/>
-      <c r="I92" s="14"/>
-      <c r="J92" s="14"/>
-      <c r="K92" s="14"/>
-      <c r="L92" s="14"/>
+    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A92" s="13"/>
+      <c r="B92" s="13"/>
+      <c r="C92" s="17"/>
+      <c r="D92" s="21"/>
+      <c r="E92" s="23"/>
+      <c r="F92" s="23"/>
+      <c r="G92" s="13"/>
+      <c r="H92" s="13"/>
+      <c r="I92" s="13"/>
+      <c r="J92" s="13"/>
+      <c r="K92" s="13"/>
+      <c r="L92" s="13"/>
       <c r="M92" t="s">
         <v>132</v>
       </c>
@@ -4559,19 +4601,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A93" s="14"/>
-      <c r="B93" s="14"/>
-      <c r="C93" s="13"/>
-      <c r="D93" s="18"/>
-      <c r="E93" s="19"/>
-      <c r="F93" s="19"/>
-      <c r="G93" s="14"/>
-      <c r="H93" s="14"/>
-      <c r="I93" s="14"/>
-      <c r="J93" s="14"/>
-      <c r="K93" s="14"/>
-      <c r="L93" s="14"/>
+    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A93" s="13"/>
+      <c r="B93" s="13"/>
+      <c r="C93" s="17"/>
+      <c r="D93" s="21"/>
+      <c r="E93" s="23"/>
+      <c r="F93" s="23"/>
+      <c r="G93" s="13"/>
+      <c r="H93" s="13"/>
+      <c r="I93" s="13"/>
+      <c r="J93" s="13"/>
+      <c r="K93" s="13"/>
+      <c r="L93" s="13"/>
       <c r="M93" t="s">
         <v>133</v>
       </c>
@@ -4582,35 +4624,35 @@
         <v>67</v>
       </c>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A94" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B94" s="14" t="s">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A94" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B94" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="C94" s="13"/>
-      <c r="D94" s="18" t="s">
+      <c r="C94" s="17"/>
+      <c r="D94" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="E94" s="19"/>
-      <c r="F94" s="19"/>
-      <c r="G94" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H94" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I94" s="14" t="s">
+      <c r="E94" s="23"/>
+      <c r="F94" s="23"/>
+      <c r="G94" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H94" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I94" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="J94" s="14" t="s">
+      <c r="J94" s="13" t="s">
         <v>234</v>
       </c>
-      <c r="K94" s="14" t="s">
+      <c r="K94" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="L94" s="14" t="s">
+      <c r="L94" s="13" t="s">
         <v>120</v>
       </c>
       <c r="M94" t="s">
@@ -4623,19 +4665,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="95" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A95" s="14"/>
-      <c r="B95" s="14"/>
-      <c r="C95" s="13"/>
-      <c r="D95" s="18"/>
-      <c r="E95" s="19"/>
-      <c r="F95" s="19"/>
-      <c r="G95" s="14"/>
-      <c r="H95" s="14"/>
-      <c r="I95" s="14"/>
-      <c r="J95" s="14"/>
-      <c r="K95" s="14"/>
-      <c r="L95" s="14"/>
+    <row r="95" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A95" s="13"/>
+      <c r="B95" s="13"/>
+      <c r="C95" s="17"/>
+      <c r="D95" s="21"/>
+      <c r="E95" s="23"/>
+      <c r="F95" s="23"/>
+      <c r="G95" s="13"/>
+      <c r="H95" s="13"/>
+      <c r="I95" s="13"/>
+      <c r="J95" s="13"/>
+      <c r="K95" s="13"/>
+      <c r="L95" s="13"/>
       <c r="M95" t="s">
         <v>212</v>
       </c>
@@ -4645,23 +4687,23 @@
       <c r="O95" t="s">
         <v>212</v>
       </c>
-      <c r="S95" s="1" t="s">
+      <c r="U95" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="96" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A96" s="14"/>
-      <c r="B96" s="14"/>
-      <c r="C96" s="13"/>
-      <c r="D96" s="18"/>
-      <c r="E96" s="19"/>
-      <c r="F96" s="19"/>
-      <c r="G96" s="14"/>
-      <c r="H96" s="14"/>
-      <c r="I96" s="14"/>
-      <c r="J96" s="14"/>
-      <c r="K96" s="14"/>
-      <c r="L96" s="14"/>
+    <row r="96" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A96" s="13"/>
+      <c r="B96" s="13"/>
+      <c r="C96" s="17"/>
+      <c r="D96" s="21"/>
+      <c r="E96" s="23"/>
+      <c r="F96" s="23"/>
+      <c r="G96" s="13"/>
+      <c r="H96" s="13"/>
+      <c r="I96" s="13"/>
+      <c r="J96" s="13"/>
+      <c r="K96" s="13"/>
+      <c r="L96" s="13"/>
       <c r="M96" t="s">
         <v>212</v>
       </c>
@@ -4671,39 +4713,39 @@
       <c r="O96" t="s">
         <v>27</v>
       </c>
-      <c r="S96" s="1" t="s">
+      <c r="U96" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A97" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B97" s="14" t="s">
+    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A97" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B97" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="C97" s="13"/>
-      <c r="D97" s="18" t="s">
+      <c r="C97" s="17"/>
+      <c r="D97" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="E97" s="19"/>
-      <c r="F97" s="19"/>
-      <c r="G97" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H97" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I97" s="14" t="s">
+      <c r="E97" s="23"/>
+      <c r="F97" s="23"/>
+      <c r="G97" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H97" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I97" s="13" t="s">
         <v>240</v>
       </c>
-      <c r="J97" s="14" t="s">
+      <c r="J97" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="K97" s="14" t="s">
+      <c r="K97" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="L97" s="14" t="s">
+      <c r="L97" s="13" t="s">
         <v>120</v>
       </c>
       <c r="M97" t="s">
@@ -4716,19 +4758,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="98" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A98" s="14"/>
-      <c r="B98" s="14"/>
-      <c r="C98" s="13"/>
-      <c r="D98" s="18"/>
-      <c r="E98" s="19"/>
-      <c r="F98" s="19"/>
-      <c r="G98" s="14"/>
-      <c r="H98" s="14"/>
-      <c r="I98" s="14"/>
-      <c r="J98" s="14"/>
-      <c r="K98" s="14"/>
-      <c r="L98" s="14"/>
+    <row r="98" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A98" s="13"/>
+      <c r="B98" s="13"/>
+      <c r="C98" s="17"/>
+      <c r="D98" s="21"/>
+      <c r="E98" s="23"/>
+      <c r="F98" s="23"/>
+      <c r="G98" s="13"/>
+      <c r="H98" s="13"/>
+      <c r="I98" s="13"/>
+      <c r="J98" s="13"/>
+      <c r="K98" s="13"/>
+      <c r="L98" s="13"/>
       <c r="M98" t="s">
         <v>212</v>
       </c>
@@ -4738,11 +4780,11 @@
       <c r="O98" t="s">
         <v>27</v>
       </c>
-      <c r="S98" s="1" t="s">
+      <c r="U98" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>141</v>
       </c>
@@ -4762,7 +4804,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>141</v>
       </c>
@@ -4796,11 +4838,11 @@
       <c r="O100" t="s">
         <v>67</v>
       </c>
-      <c r="S100" s="1" t="s">
+      <c r="U100" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>141</v>
       </c>
@@ -4837,39 +4879,39 @@
       <c r="O101" t="s">
         <v>67</v>
       </c>
-      <c r="S101" s="1" t="s">
+      <c r="U101" s="1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="102" spans="1:19" ht="60" x14ac:dyDescent="0.25">
-      <c r="A102" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B102" s="14" t="s">
+    <row r="102" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+      <c r="A102" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B102" s="13" t="s">
         <v>250</v>
       </c>
-      <c r="C102" s="13"/>
-      <c r="D102" s="18" t="s">
+      <c r="C102" s="17"/>
+      <c r="D102" s="21" t="s">
         <v>254</v>
       </c>
-      <c r="E102" s="19"/>
-      <c r="F102" s="19"/>
-      <c r="G102" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H102" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I102" s="14" t="s">
+      <c r="E102" s="23"/>
+      <c r="F102" s="23"/>
+      <c r="G102" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H102" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I102" s="13" t="s">
         <v>251</v>
       </c>
-      <c r="J102" s="14" t="s">
+      <c r="J102" s="13" t="s">
         <v>252</v>
       </c>
-      <c r="K102" s="14" t="s">
+      <c r="K102" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="L102" s="14" t="s">
+      <c r="L102" s="13" t="s">
         <v>120</v>
       </c>
       <c r="M102" t="s">
@@ -4881,23 +4923,23 @@
       <c r="O102" t="s">
         <v>67</v>
       </c>
-      <c r="S102" s="1" t="s">
+      <c r="U102" s="1" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A103" s="14"/>
-      <c r="B103" s="14"/>
-      <c r="C103" s="13"/>
-      <c r="D103" s="18"/>
-      <c r="E103" s="19"/>
-      <c r="F103" s="19"/>
-      <c r="G103" s="14"/>
-      <c r="H103" s="14"/>
-      <c r="I103" s="14"/>
-      <c r="J103" s="14"/>
-      <c r="K103" s="14"/>
-      <c r="L103" s="14"/>
+    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A103" s="13"/>
+      <c r="B103" s="13"/>
+      <c r="C103" s="17"/>
+      <c r="D103" s="21"/>
+      <c r="E103" s="23"/>
+      <c r="F103" s="23"/>
+      <c r="G103" s="13"/>
+      <c r="H103" s="13"/>
+      <c r="I103" s="13"/>
+      <c r="J103" s="13"/>
+      <c r="K103" s="13"/>
+      <c r="L103" s="13"/>
       <c r="M103" t="s">
         <v>187</v>
       </c>
@@ -4907,23 +4949,23 @@
       <c r="O103" t="s">
         <v>67</v>
       </c>
-      <c r="S103" s="1" t="s">
+      <c r="U103" s="1" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="104" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A104" s="14"/>
-      <c r="B104" s="14"/>
-      <c r="C104" s="13"/>
-      <c r="D104" s="18"/>
-      <c r="E104" s="19"/>
-      <c r="F104" s="19"/>
-      <c r="G104" s="14"/>
-      <c r="H104" s="14"/>
-      <c r="I104" s="14"/>
-      <c r="J104" s="14"/>
-      <c r="K104" s="14"/>
-      <c r="L104" s="14"/>
+    <row r="104" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A104" s="13"/>
+      <c r="B104" s="13"/>
+      <c r="C104" s="17"/>
+      <c r="D104" s="21"/>
+      <c r="E104" s="23"/>
+      <c r="F104" s="23"/>
+      <c r="G104" s="13"/>
+      <c r="H104" s="13"/>
+      <c r="I104" s="13"/>
+      <c r="J104" s="13"/>
+      <c r="K104" s="13"/>
+      <c r="L104" s="13"/>
       <c r="M104" t="s">
         <v>212</v>
       </c>
@@ -4933,39 +4975,39 @@
       <c r="O104" t="s">
         <v>27</v>
       </c>
-      <c r="S104" s="1" t="s">
+      <c r="U104" s="1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="105" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A105" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B105" s="14" t="s">
+    <row r="105" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A105" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B105" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="C105" s="13"/>
-      <c r="D105" s="18" t="s">
+      <c r="C105" s="17"/>
+      <c r="D105" s="21" t="s">
         <v>259</v>
       </c>
-      <c r="E105" s="19"/>
-      <c r="F105" s="19"/>
-      <c r="G105" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H105" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I105" s="14" t="s">
+      <c r="E105" s="23"/>
+      <c r="F105" s="23"/>
+      <c r="G105" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H105" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I105" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="J105" s="16" t="s">
+      <c r="J105" s="15" t="s">
         <v>265</v>
       </c>
-      <c r="K105" s="14" t="s">
+      <c r="K105" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="L105" s="14" t="s">
+      <c r="L105" s="13" t="s">
         <v>120</v>
       </c>
       <c r="M105" t="s">
@@ -4977,23 +5019,23 @@
       <c r="O105" t="s">
         <v>67</v>
       </c>
-      <c r="S105" s="1" t="s">
+      <c r="U105" s="1" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="106" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A106" s="14"/>
-      <c r="B106" s="14"/>
-      <c r="C106" s="13"/>
-      <c r="D106" s="18"/>
-      <c r="E106" s="19"/>
-      <c r="F106" s="19"/>
-      <c r="G106" s="14"/>
-      <c r="H106" s="14"/>
-      <c r="I106" s="14"/>
-      <c r="J106" s="16"/>
-      <c r="K106" s="14"/>
-      <c r="L106" s="14"/>
+    <row r="106" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A106" s="13"/>
+      <c r="B106" s="13"/>
+      <c r="C106" s="17"/>
+      <c r="D106" s="21"/>
+      <c r="E106" s="23"/>
+      <c r="F106" s="23"/>
+      <c r="G106" s="13"/>
+      <c r="H106" s="13"/>
+      <c r="I106" s="13"/>
+      <c r="J106" s="15"/>
+      <c r="K106" s="13"/>
+      <c r="L106" s="13"/>
       <c r="M106" t="s">
         <v>212</v>
       </c>
@@ -5003,23 +5045,23 @@
       <c r="O106" t="s">
         <v>67</v>
       </c>
-      <c r="S106" s="1" t="s">
+      <c r="U106" s="1" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="107" spans="1:19" ht="60" x14ac:dyDescent="0.25">
-      <c r="A107" s="14"/>
-      <c r="B107" s="14"/>
-      <c r="C107" s="13"/>
-      <c r="D107" s="18"/>
-      <c r="E107" s="19"/>
-      <c r="F107" s="19"/>
-      <c r="G107" s="14"/>
-      <c r="H107" s="14"/>
-      <c r="I107" s="14"/>
-      <c r="J107" s="16"/>
-      <c r="K107" s="14"/>
-      <c r="L107" s="14"/>
+    <row r="107" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+      <c r="A107" s="13"/>
+      <c r="B107" s="13"/>
+      <c r="C107" s="17"/>
+      <c r="D107" s="21"/>
+      <c r="E107" s="23"/>
+      <c r="F107" s="23"/>
+      <c r="G107" s="13"/>
+      <c r="H107" s="13"/>
+      <c r="I107" s="13"/>
+      <c r="J107" s="15"/>
+      <c r="K107" s="13"/>
+      <c r="L107" s="13"/>
       <c r="M107" t="s">
         <v>212</v>
       </c>
@@ -5029,23 +5071,23 @@
       <c r="O107" t="s">
         <v>212</v>
       </c>
-      <c r="S107" s="1" t="s">
+      <c r="U107" s="1" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="108" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A108" s="14"/>
-      <c r="B108" s="14"/>
-      <c r="C108" s="13"/>
-      <c r="D108" s="18"/>
-      <c r="E108" s="19"/>
-      <c r="F108" s="19"/>
-      <c r="G108" s="14"/>
-      <c r="H108" s="14"/>
-      <c r="I108" s="14"/>
-      <c r="J108" s="16"/>
-      <c r="K108" s="14"/>
-      <c r="L108" s="14"/>
+    <row r="108" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A108" s="13"/>
+      <c r="B108" s="13"/>
+      <c r="C108" s="17"/>
+      <c r="D108" s="21"/>
+      <c r="E108" s="23"/>
+      <c r="F108" s="23"/>
+      <c r="G108" s="13"/>
+      <c r="H108" s="13"/>
+      <c r="I108" s="13"/>
+      <c r="J108" s="15"/>
+      <c r="K108" s="13"/>
+      <c r="L108" s="13"/>
       <c r="M108" t="s">
         <v>212</v>
       </c>
@@ -5055,11 +5097,11 @@
       <c r="O108" t="s">
         <v>27</v>
       </c>
-      <c r="S108" s="1" t="s">
+      <c r="U108" s="1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="109" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>141</v>
       </c>
@@ -5093,37 +5135,37 @@
       <c r="O109" t="s">
         <v>67</v>
       </c>
-      <c r="S109" s="1" t="s">
+      <c r="U109" s="1" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="110" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A110" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B110" s="14" t="s">
+    <row r="110" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A110" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B110" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="C110" s="13"/>
-      <c r="D110" s="15" t="s">
+      <c r="C110" s="17"/>
+      <c r="D110" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="E110" s="17"/>
-      <c r="F110" s="17"/>
-      <c r="G110" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H110" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I110" s="14"/>
-      <c r="J110" s="16" t="s">
+      <c r="E110" s="16"/>
+      <c r="F110" s="16"/>
+      <c r="G110" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H110" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I110" s="13"/>
+      <c r="J110" s="15" t="s">
         <v>271</v>
       </c>
-      <c r="K110" s="14" t="s">
+      <c r="K110" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="L110" s="14" t="s">
+      <c r="L110" s="13" t="s">
         <v>120</v>
       </c>
       <c r="M110" t="s">
@@ -5135,23 +5177,23 @@
       <c r="O110" t="s">
         <v>27</v>
       </c>
-      <c r="S110" s="1" t="s">
+      <c r="U110" s="1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="111" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A111" s="14"/>
-      <c r="B111" s="14"/>
-      <c r="C111" s="13"/>
-      <c r="D111" s="15"/>
-      <c r="E111" s="17"/>
-      <c r="F111" s="17"/>
-      <c r="G111" s="14"/>
-      <c r="H111" s="14"/>
-      <c r="I111" s="14"/>
-      <c r="J111" s="16"/>
-      <c r="K111" s="14"/>
-      <c r="L111" s="14"/>
+    <row r="111" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A111" s="13"/>
+      <c r="B111" s="13"/>
+      <c r="C111" s="17"/>
+      <c r="D111" s="14"/>
+      <c r="E111" s="16"/>
+      <c r="F111" s="16"/>
+      <c r="G111" s="13"/>
+      <c r="H111" s="13"/>
+      <c r="I111" s="13"/>
+      <c r="J111" s="15"/>
+      <c r="K111" s="13"/>
+      <c r="L111" s="13"/>
       <c r="M111" t="s">
         <v>212</v>
       </c>
@@ -5161,23 +5203,23 @@
       <c r="O111" t="s">
         <v>212</v>
       </c>
-      <c r="S111" s="1" t="s">
+      <c r="U111" s="1" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A112" s="14"/>
-      <c r="B112" s="14"/>
-      <c r="C112" s="13"/>
-      <c r="D112" s="15"/>
-      <c r="E112" s="17"/>
-      <c r="F112" s="17"/>
-      <c r="G112" s="14"/>
-      <c r="H112" s="14"/>
-      <c r="I112" s="14"/>
-      <c r="J112" s="16"/>
-      <c r="K112" s="14"/>
-      <c r="L112" s="14"/>
+    <row r="112" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A112" s="13"/>
+      <c r="B112" s="13"/>
+      <c r="C112" s="17"/>
+      <c r="D112" s="14"/>
+      <c r="E112" s="16"/>
+      <c r="F112" s="16"/>
+      <c r="G112" s="13"/>
+      <c r="H112" s="13"/>
+      <c r="I112" s="13"/>
+      <c r="J112" s="15"/>
+      <c r="K112" s="13"/>
+      <c r="L112" s="13"/>
       <c r="M112" t="s">
         <v>214</v>
       </c>
@@ -5187,37 +5229,37 @@
       <c r="O112" t="s">
         <v>27</v>
       </c>
-      <c r="S112" s="1" t="s">
+      <c r="U112" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="113" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A113" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B113" s="14" t="s">
+    <row r="113" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A113" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B113" s="13" t="s">
         <v>281</v>
       </c>
-      <c r="C113" s="13"/>
-      <c r="D113" s="15" t="s">
+      <c r="C113" s="17"/>
+      <c r="D113" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="E113" s="17"/>
-      <c r="F113" s="17"/>
-      <c r="G113" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H113" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I113" s="14"/>
-      <c r="J113" s="16" t="s">
+      <c r="E113" s="16"/>
+      <c r="F113" s="16"/>
+      <c r="G113" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H113" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I113" s="13"/>
+      <c r="J113" s="15" t="s">
         <v>286</v>
       </c>
-      <c r="K113" s="14" t="s">
+      <c r="K113" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="L113" s="14" t="s">
+      <c r="L113" s="13" t="s">
         <v>120</v>
       </c>
       <c r="M113" t="s">
@@ -5229,23 +5271,23 @@
       <c r="O113" t="s">
         <v>27</v>
       </c>
-      <c r="S113" s="1" t="s">
+      <c r="U113" s="1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="114" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A114" s="14"/>
-      <c r="B114" s="14"/>
-      <c r="C114" s="13"/>
-      <c r="D114" s="15"/>
-      <c r="E114" s="17"/>
-      <c r="F114" s="17"/>
-      <c r="G114" s="14"/>
-      <c r="H114" s="14"/>
-      <c r="I114" s="14"/>
-      <c r="J114" s="16"/>
-      <c r="K114" s="14"/>
-      <c r="L114" s="14"/>
+    <row r="114" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A114" s="13"/>
+      <c r="B114" s="13"/>
+      <c r="C114" s="17"/>
+      <c r="D114" s="14"/>
+      <c r="E114" s="16"/>
+      <c r="F114" s="16"/>
+      <c r="G114" s="13"/>
+      <c r="H114" s="13"/>
+      <c r="I114" s="13"/>
+      <c r="J114" s="15"/>
+      <c r="K114" s="13"/>
+      <c r="L114" s="13"/>
       <c r="M114" t="s">
         <v>212</v>
       </c>
@@ -5255,23 +5297,23 @@
       <c r="O114" t="s">
         <v>212</v>
       </c>
-      <c r="S114" s="1" t="s">
+      <c r="U114" s="1" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A115" s="14"/>
-      <c r="B115" s="14"/>
-      <c r="C115" s="13"/>
-      <c r="D115" s="15"/>
-      <c r="E115" s="17"/>
-      <c r="F115" s="17"/>
-      <c r="G115" s="14"/>
-      <c r="H115" s="14"/>
-      <c r="I115" s="14"/>
-      <c r="J115" s="16"/>
-      <c r="K115" s="14"/>
-      <c r="L115" s="14"/>
+    <row r="115" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A115" s="13"/>
+      <c r="B115" s="13"/>
+      <c r="C115" s="17"/>
+      <c r="D115" s="14"/>
+      <c r="E115" s="16"/>
+      <c r="F115" s="16"/>
+      <c r="G115" s="13"/>
+      <c r="H115" s="13"/>
+      <c r="I115" s="13"/>
+      <c r="J115" s="15"/>
+      <c r="K115" s="13"/>
+      <c r="L115" s="13"/>
       <c r="M115" t="s">
         <v>214</v>
       </c>
@@ -5281,37 +5323,37 @@
       <c r="O115" t="s">
         <v>27</v>
       </c>
-      <c r="S115" s="1" t="s">
+      <c r="U115" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="116" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A116" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B116" s="14" t="s">
+    <row r="116" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A116" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B116" s="13" t="s">
         <v>282</v>
       </c>
-      <c r="C116" s="13"/>
-      <c r="D116" s="15" t="s">
+      <c r="C116" s="17"/>
+      <c r="D116" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="E116" s="17"/>
-      <c r="F116" s="17"/>
-      <c r="G116" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H116" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I116" s="14"/>
-      <c r="J116" s="16" t="s">
+      <c r="E116" s="16"/>
+      <c r="F116" s="16"/>
+      <c r="G116" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H116" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I116" s="13"/>
+      <c r="J116" s="15" t="s">
         <v>285</v>
       </c>
-      <c r="K116" s="14" t="s">
+      <c r="K116" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="L116" s="14" t="s">
+      <c r="L116" s="13" t="s">
         <v>120</v>
       </c>
       <c r="M116" t="s">
@@ -5323,23 +5365,23 @@
       <c r="O116" t="s">
         <v>27</v>
       </c>
-      <c r="S116" s="1" t="s">
+      <c r="U116" s="1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="117" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A117" s="14"/>
-      <c r="B117" s="14"/>
-      <c r="C117" s="13"/>
-      <c r="D117" s="15"/>
-      <c r="E117" s="17"/>
-      <c r="F117" s="17"/>
-      <c r="G117" s="14"/>
-      <c r="H117" s="14"/>
-      <c r="I117" s="14"/>
-      <c r="J117" s="16"/>
-      <c r="K117" s="14"/>
-      <c r="L117" s="14"/>
+    <row r="117" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A117" s="13"/>
+      <c r="B117" s="13"/>
+      <c r="C117" s="17"/>
+      <c r="D117" s="14"/>
+      <c r="E117" s="16"/>
+      <c r="F117" s="16"/>
+      <c r="G117" s="13"/>
+      <c r="H117" s="13"/>
+      <c r="I117" s="13"/>
+      <c r="J117" s="15"/>
+      <c r="K117" s="13"/>
+      <c r="L117" s="13"/>
       <c r="M117" t="s">
         <v>212</v>
       </c>
@@ -5349,23 +5391,23 @@
       <c r="O117" t="s">
         <v>212</v>
       </c>
-      <c r="S117" s="1" t="s">
+      <c r="U117" s="1" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A118" s="14"/>
-      <c r="B118" s="14"/>
-      <c r="C118" s="13"/>
-      <c r="D118" s="15"/>
-      <c r="E118" s="17"/>
-      <c r="F118" s="17"/>
-      <c r="G118" s="14"/>
-      <c r="H118" s="14"/>
-      <c r="I118" s="14"/>
-      <c r="J118" s="16"/>
-      <c r="K118" s="14"/>
-      <c r="L118" s="14"/>
+    <row r="118" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A118" s="13"/>
+      <c r="B118" s="13"/>
+      <c r="C118" s="17"/>
+      <c r="D118" s="14"/>
+      <c r="E118" s="16"/>
+      <c r="F118" s="16"/>
+      <c r="G118" s="13"/>
+      <c r="H118" s="13"/>
+      <c r="I118" s="13"/>
+      <c r="J118" s="15"/>
+      <c r="K118" s="13"/>
+      <c r="L118" s="13"/>
       <c r="M118" t="s">
         <v>214</v>
       </c>
@@ -5375,37 +5417,37 @@
       <c r="O118" t="s">
         <v>27</v>
       </c>
-      <c r="S118" s="1" t="s">
+      <c r="U118" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="119" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A119" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B119" s="14" t="s">
+    <row r="119" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A119" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B119" s="13" t="s">
         <v>283</v>
       </c>
-      <c r="C119" s="13"/>
-      <c r="D119" s="15" t="s">
+      <c r="C119" s="17"/>
+      <c r="D119" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="E119" s="17"/>
-      <c r="F119" s="17"/>
-      <c r="G119" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H119" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I119" s="14"/>
-      <c r="J119" s="16" t="s">
+      <c r="E119" s="16"/>
+      <c r="F119" s="16"/>
+      <c r="G119" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H119" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I119" s="13"/>
+      <c r="J119" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="K119" s="14" t="s">
+      <c r="K119" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="L119" s="14" t="s">
+      <c r="L119" s="13" t="s">
         <v>120</v>
       </c>
       <c r="M119" t="s">
@@ -5417,23 +5459,23 @@
       <c r="O119" t="s">
         <v>27</v>
       </c>
-      <c r="S119" s="1" t="s">
+      <c r="U119" s="1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="120" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A120" s="14"/>
-      <c r="B120" s="14"/>
-      <c r="C120" s="13"/>
-      <c r="D120" s="15"/>
-      <c r="E120" s="17"/>
-      <c r="F120" s="17"/>
-      <c r="G120" s="14"/>
-      <c r="H120" s="14"/>
-      <c r="I120" s="14"/>
-      <c r="J120" s="16"/>
-      <c r="K120" s="14"/>
-      <c r="L120" s="14"/>
+    <row r="120" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A120" s="13"/>
+      <c r="B120" s="13"/>
+      <c r="C120" s="17"/>
+      <c r="D120" s="14"/>
+      <c r="E120" s="16"/>
+      <c r="F120" s="16"/>
+      <c r="G120" s="13"/>
+      <c r="H120" s="13"/>
+      <c r="I120" s="13"/>
+      <c r="J120" s="15"/>
+      <c r="K120" s="13"/>
+      <c r="L120" s="13"/>
       <c r="M120" t="s">
         <v>212</v>
       </c>
@@ -5443,23 +5485,23 @@
       <c r="O120" t="s">
         <v>212</v>
       </c>
-      <c r="S120" s="1" t="s">
+      <c r="U120" s="1" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A121" s="14"/>
-      <c r="B121" s="14"/>
-      <c r="C121" s="13"/>
-      <c r="D121" s="15"/>
-      <c r="E121" s="17"/>
-      <c r="F121" s="17"/>
-      <c r="G121" s="14"/>
-      <c r="H121" s="14"/>
-      <c r="I121" s="14"/>
-      <c r="J121" s="16"/>
-      <c r="K121" s="14"/>
-      <c r="L121" s="14"/>
+    <row r="121" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A121" s="13"/>
+      <c r="B121" s="13"/>
+      <c r="C121" s="17"/>
+      <c r="D121" s="14"/>
+      <c r="E121" s="16"/>
+      <c r="F121" s="16"/>
+      <c r="G121" s="13"/>
+      <c r="H121" s="13"/>
+      <c r="I121" s="13"/>
+      <c r="J121" s="15"/>
+      <c r="K121" s="13"/>
+      <c r="L121" s="13"/>
       <c r="M121" t="s">
         <v>214</v>
       </c>
@@ -5469,25 +5511,253 @@
       <c r="O121" t="s">
         <v>27</v>
       </c>
-      <c r="S121" s="1" t="s">
+      <c r="U121" s="1" t="s">
         <v>280</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:S1"/>
+  <autoFilter ref="A1:U1"/>
   <mergeCells count="276">
-    <mergeCell ref="A119:A121"/>
-    <mergeCell ref="B119:B121"/>
-    <mergeCell ref="D119:D121"/>
-    <mergeCell ref="G119:G121"/>
-    <mergeCell ref="H119:H121"/>
-    <mergeCell ref="I119:I121"/>
-    <mergeCell ref="J119:J121"/>
-    <mergeCell ref="K119:K121"/>
-    <mergeCell ref="L119:L121"/>
-    <mergeCell ref="E119:E121"/>
-    <mergeCell ref="F119:F121"/>
-    <mergeCell ref="C119:C121"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="C64:C67"/>
+    <mergeCell ref="C68:C71"/>
+    <mergeCell ref="C72:C75"/>
+    <mergeCell ref="C78:C82"/>
+    <mergeCell ref="C83:C87"/>
+    <mergeCell ref="C88:C93"/>
+    <mergeCell ref="C94:C96"/>
+    <mergeCell ref="C97:C98"/>
+    <mergeCell ref="A110:A112"/>
+    <mergeCell ref="I110:I112"/>
+    <mergeCell ref="H110:H112"/>
+    <mergeCell ref="G110:G112"/>
+    <mergeCell ref="D110:D112"/>
+    <mergeCell ref="B110:B112"/>
+    <mergeCell ref="L110:L112"/>
+    <mergeCell ref="K110:K112"/>
+    <mergeCell ref="J110:J112"/>
+    <mergeCell ref="E110:E112"/>
+    <mergeCell ref="F110:F112"/>
+    <mergeCell ref="C110:C112"/>
+    <mergeCell ref="I105:I108"/>
+    <mergeCell ref="H105:H108"/>
+    <mergeCell ref="G105:G108"/>
+    <mergeCell ref="B105:B108"/>
+    <mergeCell ref="A105:A108"/>
+    <mergeCell ref="D105:D108"/>
+    <mergeCell ref="L105:L108"/>
+    <mergeCell ref="K105:K108"/>
+    <mergeCell ref="J105:J108"/>
+    <mergeCell ref="F105:F108"/>
+    <mergeCell ref="E105:E108"/>
+    <mergeCell ref="C105:C108"/>
+    <mergeCell ref="G97:G98"/>
+    <mergeCell ref="B97:B98"/>
+    <mergeCell ref="A97:A98"/>
+    <mergeCell ref="D97:D98"/>
+    <mergeCell ref="L102:L104"/>
+    <mergeCell ref="K102:K104"/>
+    <mergeCell ref="J102:J104"/>
+    <mergeCell ref="I102:I104"/>
+    <mergeCell ref="H102:H104"/>
+    <mergeCell ref="G102:G104"/>
+    <mergeCell ref="D102:D104"/>
+    <mergeCell ref="B102:B104"/>
+    <mergeCell ref="A102:A104"/>
+    <mergeCell ref="L97:L98"/>
+    <mergeCell ref="K97:K98"/>
+    <mergeCell ref="J97:J98"/>
+    <mergeCell ref="I97:I98"/>
+    <mergeCell ref="H97:H98"/>
+    <mergeCell ref="F97:F98"/>
+    <mergeCell ref="F102:F104"/>
+    <mergeCell ref="E97:E98"/>
+    <mergeCell ref="E102:E104"/>
+    <mergeCell ref="C102:C104"/>
+    <mergeCell ref="G94:G96"/>
+    <mergeCell ref="B94:B96"/>
+    <mergeCell ref="A94:A96"/>
+    <mergeCell ref="D94:D96"/>
+    <mergeCell ref="L94:L96"/>
+    <mergeCell ref="K94:K96"/>
+    <mergeCell ref="J94:J96"/>
+    <mergeCell ref="I94:I96"/>
+    <mergeCell ref="H94:H96"/>
+    <mergeCell ref="F94:F96"/>
+    <mergeCell ref="E94:E96"/>
+    <mergeCell ref="G83:G87"/>
+    <mergeCell ref="B83:B87"/>
+    <mergeCell ref="A83:A87"/>
+    <mergeCell ref="D83:D87"/>
+    <mergeCell ref="L88:L93"/>
+    <mergeCell ref="K88:K93"/>
+    <mergeCell ref="J88:J93"/>
+    <mergeCell ref="I88:I93"/>
+    <mergeCell ref="H88:H93"/>
+    <mergeCell ref="G88:G93"/>
+    <mergeCell ref="A88:A93"/>
+    <mergeCell ref="B88:B93"/>
+    <mergeCell ref="D88:D93"/>
+    <mergeCell ref="L83:L87"/>
+    <mergeCell ref="K83:K87"/>
+    <mergeCell ref="J83:J87"/>
+    <mergeCell ref="I83:I87"/>
+    <mergeCell ref="H83:H87"/>
+    <mergeCell ref="F83:F87"/>
+    <mergeCell ref="F88:F93"/>
+    <mergeCell ref="E83:E87"/>
+    <mergeCell ref="E88:E93"/>
+    <mergeCell ref="H78:H82"/>
+    <mergeCell ref="G78:G82"/>
+    <mergeCell ref="D78:D82"/>
+    <mergeCell ref="B78:B82"/>
+    <mergeCell ref="A78:A82"/>
+    <mergeCell ref="I72:I75"/>
+    <mergeCell ref="J72:J75"/>
+    <mergeCell ref="K72:K75"/>
+    <mergeCell ref="L72:L75"/>
+    <mergeCell ref="L78:L82"/>
+    <mergeCell ref="K78:K82"/>
+    <mergeCell ref="J78:J82"/>
+    <mergeCell ref="I78:I82"/>
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="D72:D75"/>
+    <mergeCell ref="G72:G75"/>
+    <mergeCell ref="H72:H75"/>
+    <mergeCell ref="F72:F75"/>
+    <mergeCell ref="F78:F82"/>
+    <mergeCell ref="E72:E75"/>
+    <mergeCell ref="E78:E82"/>
+    <mergeCell ref="H68:H71"/>
+    <mergeCell ref="I68:I71"/>
+    <mergeCell ref="J68:J71"/>
+    <mergeCell ref="K68:K71"/>
+    <mergeCell ref="L68:L71"/>
+    <mergeCell ref="G64:G67"/>
+    <mergeCell ref="B64:B67"/>
+    <mergeCell ref="A64:A67"/>
+    <mergeCell ref="D64:D67"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="D68:D71"/>
+    <mergeCell ref="G68:G71"/>
+    <mergeCell ref="L64:L67"/>
+    <mergeCell ref="K64:K67"/>
+    <mergeCell ref="J64:J67"/>
+    <mergeCell ref="I64:I67"/>
+    <mergeCell ref="H64:H67"/>
+    <mergeCell ref="F64:F67"/>
+    <mergeCell ref="F68:F71"/>
+    <mergeCell ref="E64:E67"/>
+    <mergeCell ref="E68:E71"/>
+    <mergeCell ref="F34:F36"/>
+    <mergeCell ref="F37:F39"/>
+    <mergeCell ref="H34:H36"/>
+    <mergeCell ref="H37:H39"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="I62:I63"/>
+    <mergeCell ref="J62:J63"/>
+    <mergeCell ref="K62:K63"/>
+    <mergeCell ref="L62:L63"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="G62:G63"/>
+    <mergeCell ref="H62:H63"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="G34:G36"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="G37:G39"/>
+    <mergeCell ref="D41:D47"/>
+    <mergeCell ref="D57:D59"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="D37:D39"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="L57:L59"/>
+    <mergeCell ref="K57:K59"/>
+    <mergeCell ref="J57:J59"/>
+    <mergeCell ref="I57:I59"/>
+    <mergeCell ref="H57:H59"/>
+    <mergeCell ref="H41:H47"/>
+    <mergeCell ref="G41:G47"/>
+    <mergeCell ref="B41:B47"/>
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="F41:F47"/>
+    <mergeCell ref="F57:F59"/>
+    <mergeCell ref="G57:G59"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="C41:C47"/>
+    <mergeCell ref="C57:C59"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="L41:L47"/>
+    <mergeCell ref="K41:K47"/>
+    <mergeCell ref="J41:J47"/>
+    <mergeCell ref="I41:I47"/>
+    <mergeCell ref="L28:L30"/>
+    <mergeCell ref="K28:K30"/>
+    <mergeCell ref="J28:J30"/>
+    <mergeCell ref="I28:I30"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="L24:L26"/>
+    <mergeCell ref="K24:K26"/>
+    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="K31:K33"/>
+    <mergeCell ref="L31:L33"/>
+    <mergeCell ref="I34:I36"/>
+    <mergeCell ref="J34:J36"/>
+    <mergeCell ref="K34:K36"/>
+    <mergeCell ref="L34:L36"/>
+    <mergeCell ref="I37:I39"/>
+    <mergeCell ref="J37:J39"/>
+    <mergeCell ref="K37:K39"/>
+    <mergeCell ref="L37:L39"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="H31:H33"/>
+    <mergeCell ref="I31:I33"/>
+    <mergeCell ref="J31:J33"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="E28:E30"/>
+    <mergeCell ref="E31:E33"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="F28:F30"/>
+    <mergeCell ref="F31:F33"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="G28:G30"/>
+    <mergeCell ref="H28:H30"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="G31:G33"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="E37:E39"/>
+    <mergeCell ref="E41:E47"/>
+    <mergeCell ref="E57:E59"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="C37:C39"/>
     <mergeCell ref="K113:K115"/>
     <mergeCell ref="L113:L115"/>
     <mergeCell ref="A116:A118"/>
@@ -5512,246 +5782,18 @@
     <mergeCell ref="J113:J115"/>
     <mergeCell ref="C113:C115"/>
     <mergeCell ref="C116:C118"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="E37:E39"/>
-    <mergeCell ref="E41:E47"/>
-    <mergeCell ref="E57:E59"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="C37:C39"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="H31:H33"/>
-    <mergeCell ref="I31:I33"/>
-    <mergeCell ref="J31:J33"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="E28:E30"/>
-    <mergeCell ref="E31:E33"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="F28:F30"/>
-    <mergeCell ref="F31:F33"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="G28:G30"/>
-    <mergeCell ref="H28:H30"/>
-    <mergeCell ref="G24:G26"/>
-    <mergeCell ref="G31:G33"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="L41:L47"/>
-    <mergeCell ref="K41:K47"/>
-    <mergeCell ref="J41:J47"/>
-    <mergeCell ref="I41:I47"/>
-    <mergeCell ref="L28:L30"/>
-    <mergeCell ref="K28:K30"/>
-    <mergeCell ref="J28:J30"/>
-    <mergeCell ref="I28:I30"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="L24:L26"/>
-    <mergeCell ref="K24:K26"/>
-    <mergeCell ref="J24:J26"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="K31:K33"/>
-    <mergeCell ref="L31:L33"/>
-    <mergeCell ref="I34:I36"/>
-    <mergeCell ref="J34:J36"/>
-    <mergeCell ref="K34:K36"/>
-    <mergeCell ref="L34:L36"/>
-    <mergeCell ref="I37:I39"/>
-    <mergeCell ref="J37:J39"/>
-    <mergeCell ref="K37:K39"/>
-    <mergeCell ref="L37:L39"/>
-    <mergeCell ref="L57:L59"/>
-    <mergeCell ref="K57:K59"/>
-    <mergeCell ref="J57:J59"/>
-    <mergeCell ref="I57:I59"/>
-    <mergeCell ref="H57:H59"/>
-    <mergeCell ref="H41:H47"/>
-    <mergeCell ref="G41:G47"/>
-    <mergeCell ref="B41:B47"/>
-    <mergeCell ref="A41:A47"/>
-    <mergeCell ref="F41:F47"/>
-    <mergeCell ref="F57:F59"/>
-    <mergeCell ref="G57:G59"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="C41:C47"/>
-    <mergeCell ref="C57:C59"/>
-    <mergeCell ref="F34:F36"/>
-    <mergeCell ref="F37:F39"/>
-    <mergeCell ref="H34:H36"/>
-    <mergeCell ref="H37:H39"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="I62:I63"/>
-    <mergeCell ref="J62:J63"/>
-    <mergeCell ref="K62:K63"/>
-    <mergeCell ref="L62:L63"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="G62:G63"/>
-    <mergeCell ref="H62:H63"/>
-    <mergeCell ref="F62:F63"/>
-    <mergeCell ref="G34:G36"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="G37:G39"/>
-    <mergeCell ref="D41:D47"/>
-    <mergeCell ref="D57:D59"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="D37:D39"/>
-    <mergeCell ref="E62:E63"/>
-    <mergeCell ref="H68:H71"/>
-    <mergeCell ref="I68:I71"/>
-    <mergeCell ref="J68:J71"/>
-    <mergeCell ref="K68:K71"/>
-    <mergeCell ref="L68:L71"/>
-    <mergeCell ref="G64:G67"/>
-    <mergeCell ref="B64:B67"/>
-    <mergeCell ref="A64:A67"/>
-    <mergeCell ref="D64:D67"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="D68:D71"/>
-    <mergeCell ref="G68:G71"/>
-    <mergeCell ref="L64:L67"/>
-    <mergeCell ref="K64:K67"/>
-    <mergeCell ref="J64:J67"/>
-    <mergeCell ref="I64:I67"/>
-    <mergeCell ref="H64:H67"/>
-    <mergeCell ref="F64:F67"/>
-    <mergeCell ref="F68:F71"/>
-    <mergeCell ref="E64:E67"/>
-    <mergeCell ref="E68:E71"/>
-    <mergeCell ref="H78:H82"/>
-    <mergeCell ref="G78:G82"/>
-    <mergeCell ref="D78:D82"/>
-    <mergeCell ref="B78:B82"/>
-    <mergeCell ref="A78:A82"/>
-    <mergeCell ref="I72:I75"/>
-    <mergeCell ref="J72:J75"/>
-    <mergeCell ref="K72:K75"/>
-    <mergeCell ref="L72:L75"/>
-    <mergeCell ref="L78:L82"/>
-    <mergeCell ref="K78:K82"/>
-    <mergeCell ref="J78:J82"/>
-    <mergeCell ref="I78:I82"/>
-    <mergeCell ref="A72:A75"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="D72:D75"/>
-    <mergeCell ref="G72:G75"/>
-    <mergeCell ref="H72:H75"/>
-    <mergeCell ref="F72:F75"/>
-    <mergeCell ref="F78:F82"/>
-    <mergeCell ref="E72:E75"/>
-    <mergeCell ref="E78:E82"/>
-    <mergeCell ref="G83:G87"/>
-    <mergeCell ref="B83:B87"/>
-    <mergeCell ref="A83:A87"/>
-    <mergeCell ref="D83:D87"/>
-    <mergeCell ref="L88:L93"/>
-    <mergeCell ref="K88:K93"/>
-    <mergeCell ref="J88:J93"/>
-    <mergeCell ref="I88:I93"/>
-    <mergeCell ref="H88:H93"/>
-    <mergeCell ref="G88:G93"/>
-    <mergeCell ref="A88:A93"/>
-    <mergeCell ref="B88:B93"/>
-    <mergeCell ref="D88:D93"/>
-    <mergeCell ref="L83:L87"/>
-    <mergeCell ref="K83:K87"/>
-    <mergeCell ref="J83:J87"/>
-    <mergeCell ref="I83:I87"/>
-    <mergeCell ref="H83:H87"/>
-    <mergeCell ref="F83:F87"/>
-    <mergeCell ref="F88:F93"/>
-    <mergeCell ref="E83:E87"/>
-    <mergeCell ref="E88:E93"/>
-    <mergeCell ref="G94:G96"/>
-    <mergeCell ref="B94:B96"/>
-    <mergeCell ref="A94:A96"/>
-    <mergeCell ref="D94:D96"/>
-    <mergeCell ref="L94:L96"/>
-    <mergeCell ref="K94:K96"/>
-    <mergeCell ref="J94:J96"/>
-    <mergeCell ref="I94:I96"/>
-    <mergeCell ref="H94:H96"/>
-    <mergeCell ref="F94:F96"/>
-    <mergeCell ref="E94:E96"/>
-    <mergeCell ref="G97:G98"/>
-    <mergeCell ref="B97:B98"/>
-    <mergeCell ref="A97:A98"/>
-    <mergeCell ref="D97:D98"/>
-    <mergeCell ref="L102:L104"/>
-    <mergeCell ref="K102:K104"/>
-    <mergeCell ref="J102:J104"/>
-    <mergeCell ref="I102:I104"/>
-    <mergeCell ref="H102:H104"/>
-    <mergeCell ref="G102:G104"/>
-    <mergeCell ref="D102:D104"/>
-    <mergeCell ref="B102:B104"/>
-    <mergeCell ref="A102:A104"/>
-    <mergeCell ref="L97:L98"/>
-    <mergeCell ref="K97:K98"/>
-    <mergeCell ref="J97:J98"/>
-    <mergeCell ref="I97:I98"/>
-    <mergeCell ref="H97:H98"/>
-    <mergeCell ref="F97:F98"/>
-    <mergeCell ref="F102:F104"/>
-    <mergeCell ref="E97:E98"/>
-    <mergeCell ref="E102:E104"/>
-    <mergeCell ref="C102:C104"/>
-    <mergeCell ref="I105:I108"/>
-    <mergeCell ref="H105:H108"/>
-    <mergeCell ref="G105:G108"/>
-    <mergeCell ref="B105:B108"/>
-    <mergeCell ref="A105:A108"/>
-    <mergeCell ref="D105:D108"/>
-    <mergeCell ref="L105:L108"/>
-    <mergeCell ref="K105:K108"/>
-    <mergeCell ref="J105:J108"/>
-    <mergeCell ref="F105:F108"/>
-    <mergeCell ref="E105:E108"/>
-    <mergeCell ref="C105:C108"/>
-    <mergeCell ref="A110:A112"/>
-    <mergeCell ref="I110:I112"/>
-    <mergeCell ref="H110:H112"/>
-    <mergeCell ref="G110:G112"/>
-    <mergeCell ref="D110:D112"/>
-    <mergeCell ref="B110:B112"/>
-    <mergeCell ref="L110:L112"/>
-    <mergeCell ref="K110:K112"/>
-    <mergeCell ref="J110:J112"/>
-    <mergeCell ref="E110:E112"/>
-    <mergeCell ref="F110:F112"/>
-    <mergeCell ref="C110:C112"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="C64:C67"/>
-    <mergeCell ref="C68:C71"/>
-    <mergeCell ref="C72:C75"/>
-    <mergeCell ref="C78:C82"/>
-    <mergeCell ref="C83:C87"/>
-    <mergeCell ref="C88:C93"/>
-    <mergeCell ref="C94:C96"/>
-    <mergeCell ref="C97:C98"/>
+    <mergeCell ref="A119:A121"/>
+    <mergeCell ref="B119:B121"/>
+    <mergeCell ref="D119:D121"/>
+    <mergeCell ref="G119:G121"/>
+    <mergeCell ref="H119:H121"/>
+    <mergeCell ref="I119:I121"/>
+    <mergeCell ref="J119:J121"/>
+    <mergeCell ref="K119:K121"/>
+    <mergeCell ref="L119:L121"/>
+    <mergeCell ref="E119:E121"/>
+    <mergeCell ref="F119:F121"/>
+    <mergeCell ref="C119:C121"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="P54" r:id="rId1"/>
@@ -5759,16 +5801,17 @@
     <hyperlink ref="F54" r:id="rId3"/>
     <hyperlink ref="Q54" r:id="rId4"/>
     <hyperlink ref="R54" r:id="rId5"/>
+    <hyperlink ref="S54" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId6"/>
-  <drawing r:id="rId7"/>
-  <legacyDrawing r:id="rId8"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId7"/>
+  <drawing r:id="rId8"/>
+  <legacyDrawing r:id="rId9"/>
   <oleObjects>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="1025" r:id="rId9">
-          <objectPr defaultSize="0" r:id="rId10">
+        <oleObject progId="Packager Shell Object" shapeId="1025" r:id="rId10">
+          <objectPr defaultSize="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -5787,13 +5830,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="1025" r:id="rId9"/>
+        <oleObject progId="Packager Shell Object" shapeId="1025" r:id="rId10"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="1026" r:id="rId11">
-          <objectPr defaultSize="0" r:id="rId12">
+        <oleObject progId="Packager Shell Object" shapeId="1026" r:id="rId12">
+          <objectPr defaultSize="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>5</xdr:col>
@@ -5812,9 +5855,65 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="1026" r:id="rId11"/>
+        <oleObject progId="Packager Shell Object" shapeId="1026" r:id="rId12"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </oleObjects>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Tables!$F$13:$F$17</xm:f>
+          </x14:formula1>
+          <xm:sqref>T1:T1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="F13:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="13" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="14" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="15" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="16" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>309</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updating the status in SOM APIs Mapping
git-tfs-id: [http://developmentvlan:8585/tfs/vanrise.collection]$/;C55357
</commit_message>
<xml_diff>
--- a/SOM/Documents/SOM/SOM APIs Mapping Sheet.xlsx
+++ b/SOM/Documents/SOM/SOM APIs Mapping Sheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="315">
   <si>
     <t>GetTechnicalDetails</t>
   </si>
@@ -991,7 +991,16 @@
     <t>On Hold</t>
   </si>
   <si>
-    <t>Requires Confirmation</t>
+    <t>Pending BSCS</t>
+  </si>
+  <si>
+    <t>Pending CRM</t>
+  </si>
+  <si>
+    <t>Pending Xata</t>
+  </si>
+  <si>
+    <t>Pending EDA</t>
   </si>
 </sst>
 </file>
@@ -1144,6 +1153,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1157,27 +1173,20 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -1646,9 +1655,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A54" sqref="A54"/>
+      <selection pane="bottomLeft" activeCell="T54" sqref="T54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2375,34 +2384,34 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B22" s="18" t="s">
+      <c r="A22" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B22" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="14" t="s">
+      <c r="C22" s="14"/>
+      <c r="D22" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="H22" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="I22" s="18" t="s">
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="I22" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="J22" s="21" t="s">
+      <c r="J22" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="K22" s="20" t="s">
+      <c r="K22" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="L22" s="18" t="s">
+      <c r="L22" s="22" t="s">
         <v>120</v>
       </c>
       <c r="M22" t="s">
@@ -2419,18 +2428,18 @@
       </c>
     </row>
     <row r="23" spans="1:21" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="21"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="18"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="22"/>
       <c r="M23" t="s">
         <v>157</v>
       </c>
@@ -2445,34 +2454,34 @@
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B24" s="13" t="s">
+      <c r="A24" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B24" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="14" t="s">
+      <c r="C24" s="15"/>
+      <c r="D24" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H24" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I24" s="15" t="s">
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="J24" s="13" t="s">
+      <c r="J24" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="K24" s="13" t="s">
+      <c r="K24" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L24" s="22" t="s">
+      <c r="L24" s="23" t="s">
         <v>120</v>
       </c>
       <c r="M24" t="s">
@@ -2487,18 +2496,18 @@
       <c r="U24"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="22"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="23"/>
       <c r="M25" t="s">
         <v>73</v>
       </c>
@@ -2510,18 +2519,18 @@
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="22"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="23"/>
       <c r="M26" t="s">
         <v>135</v>
       </c>
@@ -2576,34 +2585,34 @@
       </c>
     </row>
     <row r="28" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B28" s="13" t="s">
+      <c r="A28" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B28" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="14" t="s">
+      <c r="C28" s="15"/>
+      <c r="D28" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H28" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I28" s="13" t="s">
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I28" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="J28" s="15" t="s">
+      <c r="J28" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="K28" s="13" t="s">
+      <c r="K28" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L28" s="13" t="s">
+      <c r="L28" s="16" t="s">
         <v>119</v>
       </c>
       <c r="M28" t="s">
@@ -2620,18 +2629,18 @@
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
       <c r="M29" t="s">
         <v>85</v>
       </c>
@@ -2643,18 +2652,18 @@
       </c>
     </row>
     <row r="30" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
       <c r="M30" t="s">
         <v>90</v>
       </c>
@@ -2669,34 +2678,34 @@
       </c>
     </row>
     <row r="31" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B31" s="13" t="s">
+      <c r="A31" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B31" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="C31" s="17"/>
-      <c r="D31" s="14" t="s">
+      <c r="C31" s="15"/>
+      <c r="D31" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H31" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I31" s="13" t="s">
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I31" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="J31" s="15" t="s">
+      <c r="J31" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="K31" s="13" t="s">
+      <c r="K31" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L31" s="13" t="s">
+      <c r="L31" s="16" t="s">
         <v>119</v>
       </c>
       <c r="M31" t="s">
@@ -2710,18 +2719,18 @@
       </c>
     </row>
     <row r="32" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
+      <c r="A32" s="16"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="16"/>
       <c r="M32" t="s">
         <v>85</v>
       </c>
@@ -2733,18 +2742,18 @@
       </c>
     </row>
     <row r="33" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="15"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
       <c r="M33" t="s">
         <v>90</v>
       </c>
@@ -2759,34 +2768,34 @@
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B34" s="13" t="s">
+      <c r="A34" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B34" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="C34" s="17"/>
-      <c r="D34" s="14" t="s">
+      <c r="C34" s="15"/>
+      <c r="D34" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H34" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I34" s="13" t="s">
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H34" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I34" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="J34" s="15" t="s">
+      <c r="J34" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="K34" s="13" t="s">
+      <c r="K34" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L34" s="13" t="s">
+      <c r="L34" s="16" t="s">
         <v>119</v>
       </c>
       <c r="M34" t="s">
@@ -2800,18 +2809,18 @@
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
+      <c r="A35" s="16"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
       <c r="M35" t="s">
         <v>85</v>
       </c>
@@ -2823,18 +2832,18 @@
       </c>
     </row>
     <row r="36" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="13"/>
-      <c r="L36" s="13"/>
+      <c r="A36" s="16"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="16"/>
       <c r="M36" t="s">
         <v>90</v>
       </c>
@@ -2849,34 +2858,34 @@
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B37" s="13" t="s">
+      <c r="A37" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B37" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="C37" s="17"/>
-      <c r="D37" s="14" t="s">
+      <c r="C37" s="15"/>
+      <c r="D37" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H37" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I37" s="13" t="s">
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H37" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I37" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="J37" s="15" t="s">
+      <c r="J37" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="K37" s="13" t="s">
+      <c r="K37" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L37" s="13" t="s">
+      <c r="L37" s="16" t="s">
         <v>119</v>
       </c>
       <c r="M37" t="s">
@@ -2890,18 +2899,18 @@
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="13"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="13"/>
-      <c r="L38" s="13"/>
+      <c r="A38" s="16"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="16"/>
       <c r="M38" t="s">
         <v>85</v>
       </c>
@@ -2913,18 +2922,18 @@
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13"/>
-      <c r="J39" s="15"/>
-      <c r="K39" s="13"/>
-      <c r="L39" s="13"/>
+      <c r="A39" s="16"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="18"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="16"/>
       <c r="M39" t="s">
         <v>90</v>
       </c>
@@ -2976,34 +2985,34 @@
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B41" s="13" t="s">
+      <c r="A41" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B41" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="C41" s="17"/>
-      <c r="D41" s="14" t="s">
+      <c r="C41" s="15"/>
+      <c r="D41" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="E41" s="16"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H41" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I41" s="13" t="s">
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H41" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I41" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="J41" s="15" t="s">
+      <c r="J41" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="K41" s="13" t="s">
+      <c r="K41" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L41" s="13" t="s">
+      <c r="L41" s="16" t="s">
         <v>119</v>
       </c>
       <c r="M41" t="s">
@@ -3017,18 +3026,18 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="13"/>
-      <c r="B42" s="13"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="13"/>
-      <c r="J42" s="15"/>
-      <c r="K42" s="13"/>
-      <c r="L42" s="13"/>
+      <c r="A42" s="16"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="16"/>
+      <c r="J42" s="18"/>
+      <c r="K42" s="16"/>
+      <c r="L42" s="16"/>
       <c r="M42" t="s">
         <v>90</v>
       </c>
@@ -3040,18 +3049,18 @@
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A43" s="13"/>
-      <c r="B43" s="13"/>
-      <c r="C43" s="17"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
-      <c r="I43" s="13"/>
-      <c r="J43" s="15"/>
-      <c r="K43" s="13"/>
-      <c r="L43" s="13"/>
+      <c r="A43" s="16"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
+      <c r="J43" s="18"/>
+      <c r="K43" s="16"/>
+      <c r="L43" s="16"/>
       <c r="M43" t="s">
         <v>91</v>
       </c>
@@ -3064,18 +3073,18 @@
       <c r="U43"/>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A44" s="13"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="13"/>
-      <c r="J44" s="15"/>
-      <c r="K44" s="13"/>
-      <c r="L44" s="13"/>
+      <c r="A44" s="16"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="16"/>
+      <c r="J44" s="18"/>
+      <c r="K44" s="16"/>
+      <c r="L44" s="16"/>
       <c r="M44" t="s">
         <v>93</v>
       </c>
@@ -3088,18 +3097,18 @@
       <c r="U44"/>
     </row>
     <row r="45" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="13"/>
-      <c r="B45" s="13"/>
-      <c r="C45" s="17"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="16"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="13"/>
-      <c r="I45" s="13"/>
-      <c r="J45" s="15"/>
-      <c r="K45" s="13"/>
-      <c r="L45" s="13"/>
+      <c r="A45" s="16"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
+      <c r="J45" s="18"/>
+      <c r="K45" s="16"/>
+      <c r="L45" s="16"/>
       <c r="M45" t="s">
         <v>81</v>
       </c>
@@ -3114,18 +3123,18 @@
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A46" s="13"/>
-      <c r="B46" s="13"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="16"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="13"/>
-      <c r="I46" s="13"/>
-      <c r="J46" s="15"/>
-      <c r="K46" s="13"/>
-      <c r="L46" s="13"/>
+      <c r="A46" s="16"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="16"/>
+      <c r="J46" s="18"/>
+      <c r="K46" s="16"/>
+      <c r="L46" s="16"/>
       <c r="M46" t="s">
         <v>126</v>
       </c>
@@ -3137,18 +3146,18 @@
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="13"/>
-      <c r="B47" s="13"/>
-      <c r="C47" s="17"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="13"/>
-      <c r="I47" s="13"/>
-      <c r="J47" s="15"/>
-      <c r="K47" s="13"/>
-      <c r="L47" s="13"/>
+      <c r="A47" s="16"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
+      <c r="J47" s="18"/>
+      <c r="K47" s="16"/>
+      <c r="L47" s="16"/>
       <c r="M47" t="s">
         <v>47</v>
       </c>
@@ -3397,7 +3406,7 @@
       </c>
     </row>
     <row r="54" spans="1:21" ht="90" x14ac:dyDescent="0.25">
-      <c r="A54" s="24" t="s">
+      <c r="A54" s="13" t="s">
         <v>141</v>
       </c>
       <c r="B54" t="s">
@@ -3532,32 +3541,32 @@
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A57" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B57" s="13" t="s">
+      <c r="A57" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B57" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="C57" s="17"/>
-      <c r="D57" s="15"/>
-      <c r="E57" s="19"/>
-      <c r="F57" s="19"/>
-      <c r="G57" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H57" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I57" s="13" t="s">
+      <c r="C57" s="15"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="24"/>
+      <c r="F57" s="24"/>
+      <c r="G57" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H57" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I57" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="J57" s="15" t="s">
+      <c r="J57" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="K57" s="13" t="s">
+      <c r="K57" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L57" s="22" t="s">
+      <c r="L57" s="23" t="s">
         <v>120</v>
       </c>
       <c r="M57" t="s">
@@ -3571,18 +3580,18 @@
       </c>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A58" s="13"/>
-      <c r="B58" s="13"/>
-      <c r="C58" s="17"/>
-      <c r="D58" s="15"/>
-      <c r="E58" s="19"/>
-      <c r="F58" s="19"/>
-      <c r="G58" s="13"/>
-      <c r="H58" s="13"/>
-      <c r="I58" s="13"/>
-      <c r="J58" s="15"/>
-      <c r="K58" s="13"/>
-      <c r="L58" s="22"/>
+      <c r="A58" s="16"/>
+      <c r="B58" s="16"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="16"/>
+      <c r="H58" s="16"/>
+      <c r="I58" s="16"/>
+      <c r="J58" s="18"/>
+      <c r="K58" s="16"/>
+      <c r="L58" s="23"/>
       <c r="M58" t="s">
         <v>132</v>
       </c>
@@ -3594,18 +3603,18 @@
       </c>
     </row>
     <row r="59" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A59" s="13"/>
-      <c r="B59" s="13"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="15"/>
-      <c r="E59" s="19"/>
-      <c r="F59" s="19"/>
-      <c r="G59" s="13"/>
-      <c r="H59" s="13"/>
-      <c r="I59" s="13"/>
-      <c r="J59" s="15"/>
-      <c r="K59" s="13"/>
-      <c r="L59" s="22"/>
+      <c r="A59" s="16"/>
+      <c r="B59" s="16"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="24"/>
+      <c r="F59" s="24"/>
+      <c r="G59" s="16"/>
+      <c r="H59" s="16"/>
+      <c r="I59" s="16"/>
+      <c r="J59" s="18"/>
+      <c r="K59" s="16"/>
+      <c r="L59" s="23"/>
       <c r="M59" t="s">
         <v>133</v>
       </c>
@@ -3693,34 +3702,34 @@
       </c>
     </row>
     <row r="62" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="B62" s="18" t="s">
+      <c r="A62" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B62" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="C62" s="20"/>
-      <c r="D62" s="21" t="s">
+      <c r="C62" s="14"/>
+      <c r="D62" s="20" t="s">
         <v>200</v>
       </c>
-      <c r="E62" s="23"/>
-      <c r="F62" s="23"/>
-      <c r="G62" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="H62" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="I62" s="13" t="s">
+      <c r="E62" s="21"/>
+      <c r="F62" s="21"/>
+      <c r="G62" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H62" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="I62" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="J62" s="15" t="s">
+      <c r="J62" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="K62" s="13" t="s">
+      <c r="K62" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L62" s="13" t="s">
+      <c r="L62" s="16" t="s">
         <v>119</v>
       </c>
       <c r="M62" t="s">
@@ -3737,18 +3746,18 @@
       </c>
     </row>
     <row r="63" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A63" s="18"/>
-      <c r="B63" s="18"/>
-      <c r="C63" s="20"/>
-      <c r="D63" s="21"/>
-      <c r="E63" s="23"/>
-      <c r="F63" s="23"/>
-      <c r="G63" s="18"/>
-      <c r="H63" s="18"/>
-      <c r="I63" s="13"/>
-      <c r="J63" s="15"/>
-      <c r="K63" s="13"/>
-      <c r="L63" s="13"/>
+      <c r="A63" s="22"/>
+      <c r="B63" s="22"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="20"/>
+      <c r="E63" s="21"/>
+      <c r="F63" s="21"/>
+      <c r="G63" s="22"/>
+      <c r="H63" s="22"/>
+      <c r="I63" s="16"/>
+      <c r="J63" s="18"/>
+      <c r="K63" s="16"/>
+      <c r="L63" s="16"/>
       <c r="M63" t="s">
         <v>182</v>
       </c>
@@ -3763,34 +3772,34 @@
       </c>
     </row>
     <row r="64" spans="1:21" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B64" s="13" t="s">
+      <c r="A64" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B64" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="C64" s="17"/>
-      <c r="D64" s="21" t="s">
+      <c r="C64" s="15"/>
+      <c r="D64" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="E64" s="23"/>
-      <c r="F64" s="23"/>
-      <c r="G64" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H64" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I64" s="13" t="s">
+      <c r="E64" s="21"/>
+      <c r="F64" s="21"/>
+      <c r="G64" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H64" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I64" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="J64" s="13" t="s">
+      <c r="J64" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="K64" s="13" t="s">
+      <c r="K64" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L64" s="13" t="s">
+      <c r="L64" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M64" t="s">
@@ -3807,18 +3816,18 @@
       </c>
     </row>
     <row r="65" spans="1:21" ht="90" x14ac:dyDescent="0.25">
-      <c r="A65" s="13"/>
-      <c r="B65" s="13"/>
-      <c r="C65" s="17"/>
-      <c r="D65" s="21"/>
-      <c r="E65" s="23"/>
-      <c r="F65" s="23"/>
-      <c r="G65" s="13"/>
-      <c r="H65" s="13"/>
-      <c r="I65" s="13"/>
-      <c r="J65" s="13"/>
-      <c r="K65" s="13"/>
-      <c r="L65" s="13"/>
+      <c r="A65" s="16"/>
+      <c r="B65" s="16"/>
+      <c r="C65" s="15"/>
+      <c r="D65" s="20"/>
+      <c r="E65" s="21"/>
+      <c r="F65" s="21"/>
+      <c r="G65" s="16"/>
+      <c r="H65" s="16"/>
+      <c r="I65" s="16"/>
+      <c r="J65" s="16"/>
+      <c r="K65" s="16"/>
+      <c r="L65" s="16"/>
       <c r="M65" t="s">
         <v>187</v>
       </c>
@@ -3833,18 +3842,18 @@
       </c>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A66" s="13"/>
-      <c r="B66" s="13"/>
-      <c r="C66" s="17"/>
-      <c r="D66" s="21"/>
-      <c r="E66" s="23"/>
-      <c r="F66" s="23"/>
-      <c r="G66" s="13"/>
-      <c r="H66" s="13"/>
-      <c r="I66" s="13"/>
-      <c r="J66" s="13"/>
-      <c r="K66" s="13"/>
-      <c r="L66" s="13"/>
+      <c r="A66" s="16"/>
+      <c r="B66" s="16"/>
+      <c r="C66" s="15"/>
+      <c r="D66" s="20"/>
+      <c r="E66" s="21"/>
+      <c r="F66" s="21"/>
+      <c r="G66" s="16"/>
+      <c r="H66" s="16"/>
+      <c r="I66" s="16"/>
+      <c r="J66" s="16"/>
+      <c r="K66" s="16"/>
+      <c r="L66" s="16"/>
       <c r="M66" t="s">
         <v>190</v>
       </c>
@@ -3856,18 +3865,18 @@
       </c>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A67" s="13"/>
-      <c r="B67" s="13"/>
-      <c r="C67" s="17"/>
-      <c r="D67" s="21"/>
-      <c r="E67" s="23"/>
-      <c r="F67" s="23"/>
-      <c r="G67" s="13"/>
-      <c r="H67" s="13"/>
-      <c r="I67" s="13"/>
-      <c r="J67" s="13"/>
-      <c r="K67" s="13"/>
-      <c r="L67" s="13"/>
+      <c r="A67" s="16"/>
+      <c r="B67" s="16"/>
+      <c r="C67" s="15"/>
+      <c r="D67" s="20"/>
+      <c r="E67" s="21"/>
+      <c r="F67" s="21"/>
+      <c r="G67" s="16"/>
+      <c r="H67" s="16"/>
+      <c r="I67" s="16"/>
+      <c r="J67" s="16"/>
+      <c r="K67" s="16"/>
+      <c r="L67" s="16"/>
       <c r="M67" t="s">
         <v>191</v>
       </c>
@@ -3879,34 +3888,34 @@
       </c>
     </row>
     <row r="68" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B68" s="13" t="s">
+      <c r="A68" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B68" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="C68" s="17"/>
-      <c r="D68" s="21" t="s">
+      <c r="C68" s="15"/>
+      <c r="D68" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="E68" s="23"/>
-      <c r="F68" s="23"/>
-      <c r="G68" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H68" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I68" s="13" t="s">
+      <c r="E68" s="21"/>
+      <c r="F68" s="21"/>
+      <c r="G68" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H68" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I68" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="J68" s="13" t="s">
+      <c r="J68" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="K68" s="13" t="s">
+      <c r="K68" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L68" s="13" t="s">
+      <c r="L68" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M68" t="s">
@@ -3923,18 +3932,18 @@
       </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A69" s="13"/>
-      <c r="B69" s="13"/>
-      <c r="C69" s="17"/>
-      <c r="D69" s="21"/>
-      <c r="E69" s="23"/>
-      <c r="F69" s="23"/>
-      <c r="G69" s="13"/>
-      <c r="H69" s="13"/>
-      <c r="I69" s="13"/>
-      <c r="J69" s="13"/>
-      <c r="K69" s="13"/>
-      <c r="L69" s="13"/>
+      <c r="A69" s="16"/>
+      <c r="B69" s="16"/>
+      <c r="C69" s="15"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="21"/>
+      <c r="F69" s="21"/>
+      <c r="G69" s="16"/>
+      <c r="H69" s="16"/>
+      <c r="I69" s="16"/>
+      <c r="J69" s="16"/>
+      <c r="K69" s="16"/>
+      <c r="L69" s="16"/>
       <c r="M69" t="s">
         <v>187</v>
       </c>
@@ -3946,18 +3955,18 @@
       </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A70" s="13"/>
-      <c r="B70" s="13"/>
-      <c r="C70" s="17"/>
-      <c r="D70" s="21"/>
-      <c r="E70" s="23"/>
-      <c r="F70" s="23"/>
-      <c r="G70" s="13"/>
-      <c r="H70" s="13"/>
-      <c r="I70" s="13"/>
-      <c r="J70" s="13"/>
-      <c r="K70" s="13"/>
-      <c r="L70" s="13"/>
+      <c r="A70" s="16"/>
+      <c r="B70" s="16"/>
+      <c r="C70" s="15"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="21"/>
+      <c r="F70" s="21"/>
+      <c r="G70" s="16"/>
+      <c r="H70" s="16"/>
+      <c r="I70" s="16"/>
+      <c r="J70" s="16"/>
+      <c r="K70" s="16"/>
+      <c r="L70" s="16"/>
       <c r="M70" t="s">
         <v>190</v>
       </c>
@@ -3969,18 +3978,18 @@
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A71" s="13"/>
-      <c r="B71" s="13"/>
-      <c r="C71" s="17"/>
-      <c r="D71" s="21"/>
-      <c r="E71" s="23"/>
-      <c r="F71" s="23"/>
-      <c r="G71" s="13"/>
-      <c r="H71" s="13"/>
-      <c r="I71" s="13"/>
-      <c r="J71" s="13"/>
-      <c r="K71" s="13"/>
-      <c r="L71" s="13"/>
+      <c r="A71" s="16"/>
+      <c r="B71" s="16"/>
+      <c r="C71" s="15"/>
+      <c r="D71" s="20"/>
+      <c r="E71" s="21"/>
+      <c r="F71" s="21"/>
+      <c r="G71" s="16"/>
+      <c r="H71" s="16"/>
+      <c r="I71" s="16"/>
+      <c r="J71" s="16"/>
+      <c r="K71" s="16"/>
+      <c r="L71" s="16"/>
       <c r="M71" t="s">
         <v>191</v>
       </c>
@@ -3992,34 +4001,34 @@
       </c>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A72" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B72" s="13" t="s">
+      <c r="A72" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B72" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="C72" s="17"/>
-      <c r="D72" s="21" t="s">
+      <c r="C72" s="15"/>
+      <c r="D72" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="E72" s="23"/>
-      <c r="F72" s="23"/>
-      <c r="G72" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H72" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I72" s="13" t="s">
+      <c r="E72" s="21"/>
+      <c r="F72" s="21"/>
+      <c r="G72" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H72" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I72" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="J72" s="13" t="s">
+      <c r="J72" s="16" t="s">
         <v>198</v>
       </c>
-      <c r="K72" s="13" t="s">
+      <c r="K72" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L72" s="13" t="s">
+      <c r="L72" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M72" t="s">
@@ -4033,18 +4042,18 @@
       </c>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A73" s="13"/>
-      <c r="B73" s="13"/>
-      <c r="C73" s="17"/>
-      <c r="D73" s="21"/>
-      <c r="E73" s="23"/>
-      <c r="F73" s="23"/>
-      <c r="G73" s="13"/>
-      <c r="H73" s="13"/>
-      <c r="I73" s="13"/>
-      <c r="J73" s="13"/>
-      <c r="K73" s="13"/>
-      <c r="L73" s="13"/>
+      <c r="A73" s="16"/>
+      <c r="B73" s="16"/>
+      <c r="C73" s="15"/>
+      <c r="D73" s="20"/>
+      <c r="E73" s="21"/>
+      <c r="F73" s="21"/>
+      <c r="G73" s="16"/>
+      <c r="H73" s="16"/>
+      <c r="I73" s="16"/>
+      <c r="J73" s="16"/>
+      <c r="K73" s="16"/>
+      <c r="L73" s="16"/>
       <c r="M73" t="s">
         <v>187</v>
       </c>
@@ -4056,18 +4065,18 @@
       </c>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A74" s="13"/>
-      <c r="B74" s="13"/>
-      <c r="C74" s="17"/>
-      <c r="D74" s="21"/>
-      <c r="E74" s="23"/>
-      <c r="F74" s="23"/>
-      <c r="G74" s="13"/>
-      <c r="H74" s="13"/>
-      <c r="I74" s="13"/>
-      <c r="J74" s="13"/>
-      <c r="K74" s="13"/>
-      <c r="L74" s="13"/>
+      <c r="A74" s="16"/>
+      <c r="B74" s="16"/>
+      <c r="C74" s="15"/>
+      <c r="D74" s="20"/>
+      <c r="E74" s="21"/>
+      <c r="F74" s="21"/>
+      <c r="G74" s="16"/>
+      <c r="H74" s="16"/>
+      <c r="I74" s="16"/>
+      <c r="J74" s="16"/>
+      <c r="K74" s="16"/>
+      <c r="L74" s="16"/>
       <c r="M74" t="s">
         <v>190</v>
       </c>
@@ -4079,18 +4088,18 @@
       </c>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A75" s="13"/>
-      <c r="B75" s="13"/>
-      <c r="C75" s="17"/>
-      <c r="D75" s="21"/>
-      <c r="E75" s="23"/>
-      <c r="F75" s="23"/>
-      <c r="G75" s="13"/>
-      <c r="H75" s="13"/>
-      <c r="I75" s="13"/>
-      <c r="J75" s="13"/>
-      <c r="K75" s="13"/>
-      <c r="L75" s="13"/>
+      <c r="A75" s="16"/>
+      <c r="B75" s="16"/>
+      <c r="C75" s="15"/>
+      <c r="D75" s="20"/>
+      <c r="E75" s="21"/>
+      <c r="F75" s="21"/>
+      <c r="G75" s="16"/>
+      <c r="H75" s="16"/>
+      <c r="I75" s="16"/>
+      <c r="J75" s="16"/>
+      <c r="K75" s="16"/>
+      <c r="L75" s="16"/>
       <c r="M75" t="s">
         <v>191</v>
       </c>
@@ -4178,34 +4187,34 @@
       </c>
     </row>
     <row r="78" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B78" s="13" t="s">
+      <c r="A78" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B78" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="C78" s="17"/>
-      <c r="D78" s="21" t="s">
+      <c r="C78" s="15"/>
+      <c r="D78" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="E78" s="23"/>
-      <c r="F78" s="23"/>
-      <c r="G78" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H78" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I78" s="13" t="s">
+      <c r="E78" s="21"/>
+      <c r="F78" s="21"/>
+      <c r="G78" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H78" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I78" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="J78" s="13" t="s">
+      <c r="J78" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="K78" s="13" t="s">
+      <c r="K78" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L78" s="13" t="s">
+      <c r="L78" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M78" t="s">
@@ -4222,18 +4231,18 @@
       </c>
     </row>
     <row r="79" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A79" s="13"/>
-      <c r="B79" s="13"/>
-      <c r="C79" s="17"/>
-      <c r="D79" s="21"/>
-      <c r="E79" s="23"/>
-      <c r="F79" s="23"/>
-      <c r="G79" s="13"/>
-      <c r="H79" s="13"/>
-      <c r="I79" s="13"/>
-      <c r="J79" s="13"/>
-      <c r="K79" s="13"/>
-      <c r="L79" s="13"/>
+      <c r="A79" s="16"/>
+      <c r="B79" s="16"/>
+      <c r="C79" s="15"/>
+      <c r="D79" s="20"/>
+      <c r="E79" s="21"/>
+      <c r="F79" s="21"/>
+      <c r="G79" s="16"/>
+      <c r="H79" s="16"/>
+      <c r="I79" s="16"/>
+      <c r="J79" s="16"/>
+      <c r="K79" s="16"/>
+      <c r="L79" s="16"/>
       <c r="M79" t="s">
         <v>212</v>
       </c>
@@ -4248,18 +4257,18 @@
       </c>
     </row>
     <row r="80" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="13"/>
-      <c r="B80" s="13"/>
-      <c r="C80" s="17"/>
-      <c r="D80" s="21"/>
-      <c r="E80" s="23"/>
-      <c r="F80" s="23"/>
-      <c r="G80" s="13"/>
-      <c r="H80" s="13"/>
-      <c r="I80" s="13"/>
-      <c r="J80" s="13"/>
-      <c r="K80" s="13"/>
-      <c r="L80" s="13"/>
+      <c r="A80" s="16"/>
+      <c r="B80" s="16"/>
+      <c r="C80" s="15"/>
+      <c r="D80" s="20"/>
+      <c r="E80" s="21"/>
+      <c r="F80" s="21"/>
+      <c r="G80" s="16"/>
+      <c r="H80" s="16"/>
+      <c r="I80" s="16"/>
+      <c r="J80" s="16"/>
+      <c r="K80" s="16"/>
+      <c r="L80" s="16"/>
       <c r="M80" t="s">
         <v>214</v>
       </c>
@@ -4274,18 +4283,18 @@
       </c>
     </row>
     <row r="81" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A81" s="13"/>
-      <c r="B81" s="13"/>
-      <c r="C81" s="17"/>
-      <c r="D81" s="21"/>
-      <c r="E81" s="23"/>
-      <c r="F81" s="23"/>
-      <c r="G81" s="13"/>
-      <c r="H81" s="13"/>
-      <c r="I81" s="13"/>
-      <c r="J81" s="13"/>
-      <c r="K81" s="13"/>
-      <c r="L81" s="13"/>
+      <c r="A81" s="16"/>
+      <c r="B81" s="16"/>
+      <c r="C81" s="15"/>
+      <c r="D81" s="20"/>
+      <c r="E81" s="21"/>
+      <c r="F81" s="21"/>
+      <c r="G81" s="16"/>
+      <c r="H81" s="16"/>
+      <c r="I81" s="16"/>
+      <c r="J81" s="16"/>
+      <c r="K81" s="16"/>
+      <c r="L81" s="16"/>
       <c r="M81" t="s">
         <v>132</v>
       </c>
@@ -4300,18 +4309,18 @@
       </c>
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A82" s="13"/>
-      <c r="B82" s="13"/>
-      <c r="C82" s="17"/>
-      <c r="D82" s="21"/>
-      <c r="E82" s="23"/>
-      <c r="F82" s="23"/>
-      <c r="G82" s="13"/>
-      <c r="H82" s="13"/>
-      <c r="I82" s="13"/>
-      <c r="J82" s="13"/>
-      <c r="K82" s="13"/>
-      <c r="L82" s="13"/>
+      <c r="A82" s="16"/>
+      <c r="B82" s="16"/>
+      <c r="C82" s="15"/>
+      <c r="D82" s="20"/>
+      <c r="E82" s="21"/>
+      <c r="F82" s="21"/>
+      <c r="G82" s="16"/>
+      <c r="H82" s="16"/>
+      <c r="I82" s="16"/>
+      <c r="J82" s="16"/>
+      <c r="K82" s="16"/>
+      <c r="L82" s="16"/>
       <c r="M82" t="s">
         <v>133</v>
       </c>
@@ -4323,32 +4332,32 @@
       </c>
     </row>
     <row r="83" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B83" s="13" t="s">
+      <c r="A83" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B83" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="C83" s="17"/>
-      <c r="D83" s="21" t="s">
+      <c r="C83" s="15"/>
+      <c r="D83" s="20" t="s">
         <v>221</v>
       </c>
-      <c r="E83" s="23"/>
-      <c r="F83" s="23"/>
-      <c r="G83" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H83" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I83" s="13"/>
-      <c r="J83" s="13" t="s">
+      <c r="E83" s="21"/>
+      <c r="F83" s="21"/>
+      <c r="G83" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H83" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I83" s="16"/>
+      <c r="J83" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="K83" s="13" t="s">
+      <c r="K83" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L83" s="13" t="s">
+      <c r="L83" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M83" t="s">
@@ -4362,18 +4371,18 @@
       </c>
     </row>
     <row r="84" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A84" s="17"/>
-      <c r="B84" s="13"/>
-      <c r="C84" s="17"/>
-      <c r="D84" s="21"/>
-      <c r="E84" s="23"/>
-      <c r="F84" s="23"/>
-      <c r="G84" s="13"/>
-      <c r="H84" s="13"/>
-      <c r="I84" s="13"/>
-      <c r="J84" s="13"/>
-      <c r="K84" s="13"/>
-      <c r="L84" s="13"/>
+      <c r="A84" s="15"/>
+      <c r="B84" s="16"/>
+      <c r="C84" s="15"/>
+      <c r="D84" s="20"/>
+      <c r="E84" s="21"/>
+      <c r="F84" s="21"/>
+      <c r="G84" s="16"/>
+      <c r="H84" s="16"/>
+      <c r="I84" s="16"/>
+      <c r="J84" s="16"/>
+      <c r="K84" s="16"/>
+      <c r="L84" s="16"/>
       <c r="M84" t="s">
         <v>212</v>
       </c>
@@ -4385,18 +4394,18 @@
       </c>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A85" s="17"/>
-      <c r="B85" s="13"/>
-      <c r="C85" s="17"/>
-      <c r="D85" s="21"/>
-      <c r="E85" s="23"/>
-      <c r="F85" s="23"/>
-      <c r="G85" s="13"/>
-      <c r="H85" s="13"/>
-      <c r="I85" s="13"/>
-      <c r="J85" s="13"/>
-      <c r="K85" s="13"/>
-      <c r="L85" s="13"/>
+      <c r="A85" s="15"/>
+      <c r="B85" s="16"/>
+      <c r="C85" s="15"/>
+      <c r="D85" s="20"/>
+      <c r="E85" s="21"/>
+      <c r="F85" s="21"/>
+      <c r="G85" s="16"/>
+      <c r="H85" s="16"/>
+      <c r="I85" s="16"/>
+      <c r="J85" s="16"/>
+      <c r="K85" s="16"/>
+      <c r="L85" s="16"/>
       <c r="M85" t="s">
         <v>214</v>
       </c>
@@ -4408,18 +4417,18 @@
       </c>
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A86" s="17"/>
-      <c r="B86" s="13"/>
-      <c r="C86" s="17"/>
-      <c r="D86" s="21"/>
-      <c r="E86" s="23"/>
-      <c r="F86" s="23"/>
-      <c r="G86" s="13"/>
-      <c r="H86" s="13"/>
-      <c r="I86" s="13"/>
-      <c r="J86" s="13"/>
-      <c r="K86" s="13"/>
-      <c r="L86" s="13"/>
+      <c r="A86" s="15"/>
+      <c r="B86" s="16"/>
+      <c r="C86" s="15"/>
+      <c r="D86" s="20"/>
+      <c r="E86" s="21"/>
+      <c r="F86" s="21"/>
+      <c r="G86" s="16"/>
+      <c r="H86" s="16"/>
+      <c r="I86" s="16"/>
+      <c r="J86" s="16"/>
+      <c r="K86" s="16"/>
+      <c r="L86" s="16"/>
       <c r="M86" t="s">
         <v>132</v>
       </c>
@@ -4431,18 +4440,18 @@
       </c>
     </row>
     <row r="87" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A87" s="17"/>
-      <c r="B87" s="13"/>
-      <c r="C87" s="17"/>
-      <c r="D87" s="21"/>
-      <c r="E87" s="23"/>
-      <c r="F87" s="23"/>
-      <c r="G87" s="13"/>
-      <c r="H87" s="13"/>
-      <c r="I87" s="13"/>
-      <c r="J87" s="13"/>
-      <c r="K87" s="13"/>
-      <c r="L87" s="13"/>
+      <c r="A87" s="15"/>
+      <c r="B87" s="16"/>
+      <c r="C87" s="15"/>
+      <c r="D87" s="20"/>
+      <c r="E87" s="21"/>
+      <c r="F87" s="21"/>
+      <c r="G87" s="16"/>
+      <c r="H87" s="16"/>
+      <c r="I87" s="16"/>
+      <c r="J87" s="16"/>
+      <c r="K87" s="16"/>
+      <c r="L87" s="16"/>
       <c r="M87" t="s">
         <v>133</v>
       </c>
@@ -4457,34 +4466,34 @@
       </c>
     </row>
     <row r="88" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B88" s="13" t="s">
+      <c r="A88" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B88" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="C88" s="17"/>
-      <c r="D88" s="21" t="s">
+      <c r="C88" s="15"/>
+      <c r="D88" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="E88" s="23"/>
-      <c r="F88" s="23"/>
-      <c r="G88" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H88" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I88" s="13" t="s">
+      <c r="E88" s="21"/>
+      <c r="F88" s="21"/>
+      <c r="G88" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H88" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I88" s="16" t="s">
         <v>224</v>
       </c>
-      <c r="J88" s="13" t="s">
+      <c r="J88" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="K88" s="13" t="s">
+      <c r="K88" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L88" s="13" t="s">
+      <c r="L88" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M88" t="s">
@@ -4501,18 +4510,18 @@
       </c>
     </row>
     <row r="89" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="13"/>
-      <c r="B89" s="13"/>
-      <c r="C89" s="17"/>
-      <c r="D89" s="21"/>
-      <c r="E89" s="23"/>
-      <c r="F89" s="23"/>
-      <c r="G89" s="13"/>
-      <c r="H89" s="13"/>
-      <c r="I89" s="13"/>
-      <c r="J89" s="13"/>
-      <c r="K89" s="13"/>
-      <c r="L89" s="13"/>
+      <c r="A89" s="16"/>
+      <c r="B89" s="16"/>
+      <c r="C89" s="15"/>
+      <c r="D89" s="20"/>
+      <c r="E89" s="21"/>
+      <c r="F89" s="21"/>
+      <c r="G89" s="16"/>
+      <c r="H89" s="16"/>
+      <c r="I89" s="16"/>
+      <c r="J89" s="16"/>
+      <c r="K89" s="16"/>
+      <c r="L89" s="16"/>
       <c r="M89" t="s">
         <v>47</v>
       </c>
@@ -4527,18 +4536,18 @@
       </c>
     </row>
     <row r="90" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="13"/>
-      <c r="B90" s="13"/>
-      <c r="C90" s="17"/>
-      <c r="D90" s="21"/>
-      <c r="E90" s="23"/>
-      <c r="F90" s="23"/>
-      <c r="G90" s="13"/>
-      <c r="H90" s="13"/>
-      <c r="I90" s="13"/>
-      <c r="J90" s="13"/>
-      <c r="K90" s="13"/>
-      <c r="L90" s="13"/>
+      <c r="A90" s="16"/>
+      <c r="B90" s="16"/>
+      <c r="C90" s="15"/>
+      <c r="D90" s="20"/>
+      <c r="E90" s="21"/>
+      <c r="F90" s="21"/>
+      <c r="G90" s="16"/>
+      <c r="H90" s="16"/>
+      <c r="I90" s="16"/>
+      <c r="J90" s="16"/>
+      <c r="K90" s="16"/>
+      <c r="L90" s="16"/>
       <c r="M90" t="s">
         <v>180</v>
       </c>
@@ -4553,18 +4562,18 @@
       </c>
     </row>
     <row r="91" spans="1:21" ht="75" x14ac:dyDescent="0.25">
-      <c r="A91" s="13"/>
-      <c r="B91" s="13"/>
-      <c r="C91" s="17"/>
-      <c r="D91" s="21"/>
-      <c r="E91" s="23"/>
-      <c r="F91" s="23"/>
-      <c r="G91" s="13"/>
-      <c r="H91" s="13"/>
-      <c r="I91" s="13"/>
-      <c r="J91" s="13"/>
-      <c r="K91" s="13"/>
-      <c r="L91" s="13"/>
+      <c r="A91" s="16"/>
+      <c r="B91" s="16"/>
+      <c r="C91" s="15"/>
+      <c r="D91" s="20"/>
+      <c r="E91" s="21"/>
+      <c r="F91" s="21"/>
+      <c r="G91" s="16"/>
+      <c r="H91" s="16"/>
+      <c r="I91" s="16"/>
+      <c r="J91" s="16"/>
+      <c r="K91" s="16"/>
+      <c r="L91" s="16"/>
       <c r="M91" t="s">
         <v>214</v>
       </c>
@@ -4579,18 +4588,18 @@
       </c>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A92" s="13"/>
-      <c r="B92" s="13"/>
-      <c r="C92" s="17"/>
-      <c r="D92" s="21"/>
-      <c r="E92" s="23"/>
-      <c r="F92" s="23"/>
-      <c r="G92" s="13"/>
-      <c r="H92" s="13"/>
-      <c r="I92" s="13"/>
-      <c r="J92" s="13"/>
-      <c r="K92" s="13"/>
-      <c r="L92" s="13"/>
+      <c r="A92" s="16"/>
+      <c r="B92" s="16"/>
+      <c r="C92" s="15"/>
+      <c r="D92" s="20"/>
+      <c r="E92" s="21"/>
+      <c r="F92" s="21"/>
+      <c r="G92" s="16"/>
+      <c r="H92" s="16"/>
+      <c r="I92" s="16"/>
+      <c r="J92" s="16"/>
+      <c r="K92" s="16"/>
+      <c r="L92" s="16"/>
       <c r="M92" t="s">
         <v>132</v>
       </c>
@@ -4602,18 +4611,18 @@
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A93" s="13"/>
-      <c r="B93" s="13"/>
-      <c r="C93" s="17"/>
-      <c r="D93" s="21"/>
-      <c r="E93" s="23"/>
-      <c r="F93" s="23"/>
-      <c r="G93" s="13"/>
-      <c r="H93" s="13"/>
-      <c r="I93" s="13"/>
-      <c r="J93" s="13"/>
-      <c r="K93" s="13"/>
-      <c r="L93" s="13"/>
+      <c r="A93" s="16"/>
+      <c r="B93" s="16"/>
+      <c r="C93" s="15"/>
+      <c r="D93" s="20"/>
+      <c r="E93" s="21"/>
+      <c r="F93" s="21"/>
+      <c r="G93" s="16"/>
+      <c r="H93" s="16"/>
+      <c r="I93" s="16"/>
+      <c r="J93" s="16"/>
+      <c r="K93" s="16"/>
+      <c r="L93" s="16"/>
       <c r="M93" t="s">
         <v>133</v>
       </c>
@@ -4625,34 +4634,34 @@
       </c>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A94" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B94" s="13" t="s">
+      <c r="A94" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B94" s="16" t="s">
         <v>233</v>
       </c>
-      <c r="C94" s="17"/>
-      <c r="D94" s="21" t="s">
+      <c r="C94" s="15"/>
+      <c r="D94" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="E94" s="23"/>
-      <c r="F94" s="23"/>
-      <c r="G94" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H94" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I94" s="13" t="s">
+      <c r="E94" s="21"/>
+      <c r="F94" s="21"/>
+      <c r="G94" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H94" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I94" s="16" t="s">
         <v>232</v>
       </c>
-      <c r="J94" s="13" t="s">
+      <c r="J94" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="K94" s="13" t="s">
+      <c r="K94" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L94" s="13" t="s">
+      <c r="L94" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M94" t="s">
@@ -4666,18 +4675,18 @@
       </c>
     </row>
     <row r="95" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A95" s="13"/>
-      <c r="B95" s="13"/>
-      <c r="C95" s="17"/>
-      <c r="D95" s="21"/>
-      <c r="E95" s="23"/>
-      <c r="F95" s="23"/>
-      <c r="G95" s="13"/>
-      <c r="H95" s="13"/>
-      <c r="I95" s="13"/>
-      <c r="J95" s="13"/>
-      <c r="K95" s="13"/>
-      <c r="L95" s="13"/>
+      <c r="A95" s="16"/>
+      <c r="B95" s="16"/>
+      <c r="C95" s="15"/>
+      <c r="D95" s="20"/>
+      <c r="E95" s="21"/>
+      <c r="F95" s="21"/>
+      <c r="G95" s="16"/>
+      <c r="H95" s="16"/>
+      <c r="I95" s="16"/>
+      <c r="J95" s="16"/>
+      <c r="K95" s="16"/>
+      <c r="L95" s="16"/>
       <c r="M95" t="s">
         <v>212</v>
       </c>
@@ -4692,18 +4701,18 @@
       </c>
     </row>
     <row r="96" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A96" s="13"/>
-      <c r="B96" s="13"/>
-      <c r="C96" s="17"/>
-      <c r="D96" s="21"/>
-      <c r="E96" s="23"/>
-      <c r="F96" s="23"/>
-      <c r="G96" s="13"/>
-      <c r="H96" s="13"/>
-      <c r="I96" s="13"/>
-      <c r="J96" s="13"/>
-      <c r="K96" s="13"/>
-      <c r="L96" s="13"/>
+      <c r="A96" s="16"/>
+      <c r="B96" s="16"/>
+      <c r="C96" s="15"/>
+      <c r="D96" s="20"/>
+      <c r="E96" s="21"/>
+      <c r="F96" s="21"/>
+      <c r="G96" s="16"/>
+      <c r="H96" s="16"/>
+      <c r="I96" s="16"/>
+      <c r="J96" s="16"/>
+      <c r="K96" s="16"/>
+      <c r="L96" s="16"/>
       <c r="M96" t="s">
         <v>212</v>
       </c>
@@ -4718,34 +4727,34 @@
       </c>
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A97" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B97" s="13" t="s">
+      <c r="A97" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B97" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="C97" s="17"/>
-      <c r="D97" s="21" t="s">
+      <c r="C97" s="15"/>
+      <c r="D97" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="E97" s="23"/>
-      <c r="F97" s="23"/>
-      <c r="G97" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H97" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I97" s="13" t="s">
+      <c r="E97" s="21"/>
+      <c r="F97" s="21"/>
+      <c r="G97" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H97" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I97" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="J97" s="13" t="s">
+      <c r="J97" s="16" t="s">
         <v>241</v>
       </c>
-      <c r="K97" s="13" t="s">
+      <c r="K97" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L97" s="13" t="s">
+      <c r="L97" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M97" t="s">
@@ -4759,18 +4768,18 @@
       </c>
     </row>
     <row r="98" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A98" s="13"/>
-      <c r="B98" s="13"/>
-      <c r="C98" s="17"/>
-      <c r="D98" s="21"/>
-      <c r="E98" s="23"/>
-      <c r="F98" s="23"/>
-      <c r="G98" s="13"/>
-      <c r="H98" s="13"/>
-      <c r="I98" s="13"/>
-      <c r="J98" s="13"/>
-      <c r="K98" s="13"/>
-      <c r="L98" s="13"/>
+      <c r="A98" s="16"/>
+      <c r="B98" s="16"/>
+      <c r="C98" s="15"/>
+      <c r="D98" s="20"/>
+      <c r="E98" s="21"/>
+      <c r="F98" s="21"/>
+      <c r="G98" s="16"/>
+      <c r="H98" s="16"/>
+      <c r="I98" s="16"/>
+      <c r="J98" s="16"/>
+      <c r="K98" s="16"/>
+      <c r="L98" s="16"/>
       <c r="M98" t="s">
         <v>212</v>
       </c>
@@ -4884,34 +4893,34 @@
       </c>
     </row>
     <row r="102" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A102" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B102" s="13" t="s">
+      <c r="A102" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B102" s="16" t="s">
         <v>250</v>
       </c>
-      <c r="C102" s="17"/>
-      <c r="D102" s="21" t="s">
+      <c r="C102" s="15"/>
+      <c r="D102" s="20" t="s">
         <v>254</v>
       </c>
-      <c r="E102" s="23"/>
-      <c r="F102" s="23"/>
-      <c r="G102" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H102" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I102" s="13" t="s">
+      <c r="E102" s="21"/>
+      <c r="F102" s="21"/>
+      <c r="G102" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H102" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I102" s="16" t="s">
         <v>251</v>
       </c>
-      <c r="J102" s="13" t="s">
+      <c r="J102" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="K102" s="13" t="s">
+      <c r="K102" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L102" s="13" t="s">
+      <c r="L102" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M102" t="s">
@@ -4928,18 +4937,18 @@
       </c>
     </row>
     <row r="103" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A103" s="13"/>
-      <c r="B103" s="13"/>
-      <c r="C103" s="17"/>
-      <c r="D103" s="21"/>
-      <c r="E103" s="23"/>
-      <c r="F103" s="23"/>
-      <c r="G103" s="13"/>
-      <c r="H103" s="13"/>
-      <c r="I103" s="13"/>
-      <c r="J103" s="13"/>
-      <c r="K103" s="13"/>
-      <c r="L103" s="13"/>
+      <c r="A103" s="16"/>
+      <c r="B103" s="16"/>
+      <c r="C103" s="15"/>
+      <c r="D103" s="20"/>
+      <c r="E103" s="21"/>
+      <c r="F103" s="21"/>
+      <c r="G103" s="16"/>
+      <c r="H103" s="16"/>
+      <c r="I103" s="16"/>
+      <c r="J103" s="16"/>
+      <c r="K103" s="16"/>
+      <c r="L103" s="16"/>
       <c r="M103" t="s">
         <v>187</v>
       </c>
@@ -4954,18 +4963,18 @@
       </c>
     </row>
     <row r="104" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A104" s="13"/>
-      <c r="B104" s="13"/>
-      <c r="C104" s="17"/>
-      <c r="D104" s="21"/>
-      <c r="E104" s="23"/>
-      <c r="F104" s="23"/>
-      <c r="G104" s="13"/>
-      <c r="H104" s="13"/>
-      <c r="I104" s="13"/>
-      <c r="J104" s="13"/>
-      <c r="K104" s="13"/>
-      <c r="L104" s="13"/>
+      <c r="A104" s="16"/>
+      <c r="B104" s="16"/>
+      <c r="C104" s="15"/>
+      <c r="D104" s="20"/>
+      <c r="E104" s="21"/>
+      <c r="F104" s="21"/>
+      <c r="G104" s="16"/>
+      <c r="H104" s="16"/>
+      <c r="I104" s="16"/>
+      <c r="J104" s="16"/>
+      <c r="K104" s="16"/>
+      <c r="L104" s="16"/>
       <c r="M104" t="s">
         <v>212</v>
       </c>
@@ -4980,34 +4989,34 @@
       </c>
     </row>
     <row r="105" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A105" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B105" s="13" t="s">
+      <c r="A105" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B105" s="16" t="s">
         <v>258</v>
       </c>
-      <c r="C105" s="17"/>
-      <c r="D105" s="21" t="s">
+      <c r="C105" s="15"/>
+      <c r="D105" s="20" t="s">
         <v>259</v>
       </c>
-      <c r="E105" s="23"/>
-      <c r="F105" s="23"/>
-      <c r="G105" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H105" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I105" s="13" t="s">
+      <c r="E105" s="21"/>
+      <c r="F105" s="21"/>
+      <c r="G105" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H105" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I105" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="J105" s="15" t="s">
+      <c r="J105" s="18" t="s">
         <v>265</v>
       </c>
-      <c r="K105" s="13" t="s">
+      <c r="K105" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L105" s="13" t="s">
+      <c r="L105" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M105" t="s">
@@ -5024,18 +5033,18 @@
       </c>
     </row>
     <row r="106" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A106" s="13"/>
-      <c r="B106" s="13"/>
-      <c r="C106" s="17"/>
-      <c r="D106" s="21"/>
-      <c r="E106" s="23"/>
-      <c r="F106" s="23"/>
-      <c r="G106" s="13"/>
-      <c r="H106" s="13"/>
-      <c r="I106" s="13"/>
-      <c r="J106" s="15"/>
-      <c r="K106" s="13"/>
-      <c r="L106" s="13"/>
+      <c r="A106" s="16"/>
+      <c r="B106" s="16"/>
+      <c r="C106" s="15"/>
+      <c r="D106" s="20"/>
+      <c r="E106" s="21"/>
+      <c r="F106" s="21"/>
+      <c r="G106" s="16"/>
+      <c r="H106" s="16"/>
+      <c r="I106" s="16"/>
+      <c r="J106" s="18"/>
+      <c r="K106" s="16"/>
+      <c r="L106" s="16"/>
       <c r="M106" t="s">
         <v>212</v>
       </c>
@@ -5050,18 +5059,18 @@
       </c>
     </row>
     <row r="107" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A107" s="13"/>
-      <c r="B107" s="13"/>
-      <c r="C107" s="17"/>
-      <c r="D107" s="21"/>
-      <c r="E107" s="23"/>
-      <c r="F107" s="23"/>
-      <c r="G107" s="13"/>
-      <c r="H107" s="13"/>
-      <c r="I107" s="13"/>
-      <c r="J107" s="15"/>
-      <c r="K107" s="13"/>
-      <c r="L107" s="13"/>
+      <c r="A107" s="16"/>
+      <c r="B107" s="16"/>
+      <c r="C107" s="15"/>
+      <c r="D107" s="20"/>
+      <c r="E107" s="21"/>
+      <c r="F107" s="21"/>
+      <c r="G107" s="16"/>
+      <c r="H107" s="16"/>
+      <c r="I107" s="16"/>
+      <c r="J107" s="18"/>
+      <c r="K107" s="16"/>
+      <c r="L107" s="16"/>
       <c r="M107" t="s">
         <v>212</v>
       </c>
@@ -5076,18 +5085,18 @@
       </c>
     </row>
     <row r="108" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A108" s="13"/>
-      <c r="B108" s="13"/>
-      <c r="C108" s="17"/>
-      <c r="D108" s="21"/>
-      <c r="E108" s="23"/>
-      <c r="F108" s="23"/>
-      <c r="G108" s="13"/>
-      <c r="H108" s="13"/>
-      <c r="I108" s="13"/>
-      <c r="J108" s="15"/>
-      <c r="K108" s="13"/>
-      <c r="L108" s="13"/>
+      <c r="A108" s="16"/>
+      <c r="B108" s="16"/>
+      <c r="C108" s="15"/>
+      <c r="D108" s="20"/>
+      <c r="E108" s="21"/>
+      <c r="F108" s="21"/>
+      <c r="G108" s="16"/>
+      <c r="H108" s="16"/>
+      <c r="I108" s="16"/>
+      <c r="J108" s="18"/>
+      <c r="K108" s="16"/>
+      <c r="L108" s="16"/>
       <c r="M108" t="s">
         <v>212</v>
       </c>
@@ -5140,32 +5149,32 @@
       </c>
     </row>
     <row r="110" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A110" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B110" s="13" t="s">
+      <c r="A110" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B110" s="16" t="s">
         <v>270</v>
       </c>
-      <c r="C110" s="17"/>
-      <c r="D110" s="14" t="s">
+      <c r="C110" s="15"/>
+      <c r="D110" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="E110" s="16"/>
-      <c r="F110" s="16"/>
-      <c r="G110" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H110" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I110" s="13"/>
-      <c r="J110" s="15" t="s">
+      <c r="E110" s="19"/>
+      <c r="F110" s="19"/>
+      <c r="G110" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H110" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I110" s="16"/>
+      <c r="J110" s="18" t="s">
         <v>271</v>
       </c>
-      <c r="K110" s="13" t="s">
+      <c r="K110" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L110" s="13" t="s">
+      <c r="L110" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M110" t="s">
@@ -5182,18 +5191,18 @@
       </c>
     </row>
     <row r="111" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A111" s="13"/>
-      <c r="B111" s="13"/>
-      <c r="C111" s="17"/>
-      <c r="D111" s="14"/>
-      <c r="E111" s="16"/>
-      <c r="F111" s="16"/>
-      <c r="G111" s="13"/>
-      <c r="H111" s="13"/>
-      <c r="I111" s="13"/>
-      <c r="J111" s="15"/>
-      <c r="K111" s="13"/>
-      <c r="L111" s="13"/>
+      <c r="A111" s="16"/>
+      <c r="B111" s="16"/>
+      <c r="C111" s="15"/>
+      <c r="D111" s="17"/>
+      <c r="E111" s="19"/>
+      <c r="F111" s="19"/>
+      <c r="G111" s="16"/>
+      <c r="H111" s="16"/>
+      <c r="I111" s="16"/>
+      <c r="J111" s="18"/>
+      <c r="K111" s="16"/>
+      <c r="L111" s="16"/>
       <c r="M111" t="s">
         <v>212</v>
       </c>
@@ -5208,18 +5217,18 @@
       </c>
     </row>
     <row r="112" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A112" s="13"/>
-      <c r="B112" s="13"/>
-      <c r="C112" s="17"/>
-      <c r="D112" s="14"/>
-      <c r="E112" s="16"/>
-      <c r="F112" s="16"/>
-      <c r="G112" s="13"/>
-      <c r="H112" s="13"/>
-      <c r="I112" s="13"/>
-      <c r="J112" s="15"/>
-      <c r="K112" s="13"/>
-      <c r="L112" s="13"/>
+      <c r="A112" s="16"/>
+      <c r="B112" s="16"/>
+      <c r="C112" s="15"/>
+      <c r="D112" s="17"/>
+      <c r="E112" s="19"/>
+      <c r="F112" s="19"/>
+      <c r="G112" s="16"/>
+      <c r="H112" s="16"/>
+      <c r="I112" s="16"/>
+      <c r="J112" s="18"/>
+      <c r="K112" s="16"/>
+      <c r="L112" s="16"/>
       <c r="M112" t="s">
         <v>214</v>
       </c>
@@ -5234,32 +5243,32 @@
       </c>
     </row>
     <row r="113" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A113" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B113" s="13" t="s">
+      <c r="A113" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B113" s="16" t="s">
         <v>281</v>
       </c>
-      <c r="C113" s="17"/>
-      <c r="D113" s="14" t="s">
+      <c r="C113" s="15"/>
+      <c r="D113" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="E113" s="16"/>
-      <c r="F113" s="16"/>
-      <c r="G113" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H113" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I113" s="13"/>
-      <c r="J113" s="15" t="s">
+      <c r="E113" s="19"/>
+      <c r="F113" s="19"/>
+      <c r="G113" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H113" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I113" s="16"/>
+      <c r="J113" s="18" t="s">
         <v>286</v>
       </c>
-      <c r="K113" s="13" t="s">
+      <c r="K113" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L113" s="13" t="s">
+      <c r="L113" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M113" t="s">
@@ -5276,18 +5285,18 @@
       </c>
     </row>
     <row r="114" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A114" s="13"/>
-      <c r="B114" s="13"/>
-      <c r="C114" s="17"/>
-      <c r="D114" s="14"/>
-      <c r="E114" s="16"/>
-      <c r="F114" s="16"/>
-      <c r="G114" s="13"/>
-      <c r="H114" s="13"/>
-      <c r="I114" s="13"/>
-      <c r="J114" s="15"/>
-      <c r="K114" s="13"/>
-      <c r="L114" s="13"/>
+      <c r="A114" s="16"/>
+      <c r="B114" s="16"/>
+      <c r="C114" s="15"/>
+      <c r="D114" s="17"/>
+      <c r="E114" s="19"/>
+      <c r="F114" s="19"/>
+      <c r="G114" s="16"/>
+      <c r="H114" s="16"/>
+      <c r="I114" s="16"/>
+      <c r="J114" s="18"/>
+      <c r="K114" s="16"/>
+      <c r="L114" s="16"/>
       <c r="M114" t="s">
         <v>212</v>
       </c>
@@ -5302,18 +5311,18 @@
       </c>
     </row>
     <row r="115" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A115" s="13"/>
-      <c r="B115" s="13"/>
-      <c r="C115" s="17"/>
-      <c r="D115" s="14"/>
-      <c r="E115" s="16"/>
-      <c r="F115" s="16"/>
-      <c r="G115" s="13"/>
-      <c r="H115" s="13"/>
-      <c r="I115" s="13"/>
-      <c r="J115" s="15"/>
-      <c r="K115" s="13"/>
-      <c r="L115" s="13"/>
+      <c r="A115" s="16"/>
+      <c r="B115" s="16"/>
+      <c r="C115" s="15"/>
+      <c r="D115" s="17"/>
+      <c r="E115" s="19"/>
+      <c r="F115" s="19"/>
+      <c r="G115" s="16"/>
+      <c r="H115" s="16"/>
+      <c r="I115" s="16"/>
+      <c r="J115" s="18"/>
+      <c r="K115" s="16"/>
+      <c r="L115" s="16"/>
       <c r="M115" t="s">
         <v>214</v>
       </c>
@@ -5328,32 +5337,32 @@
       </c>
     </row>
     <row r="116" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A116" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B116" s="13" t="s">
+      <c r="A116" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B116" s="16" t="s">
         <v>282</v>
       </c>
-      <c r="C116" s="17"/>
-      <c r="D116" s="14" t="s">
+      <c r="C116" s="15"/>
+      <c r="D116" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="E116" s="16"/>
-      <c r="F116" s="16"/>
-      <c r="G116" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H116" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I116" s="13"/>
-      <c r="J116" s="15" t="s">
+      <c r="E116" s="19"/>
+      <c r="F116" s="19"/>
+      <c r="G116" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H116" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I116" s="16"/>
+      <c r="J116" s="18" t="s">
         <v>285</v>
       </c>
-      <c r="K116" s="13" t="s">
+      <c r="K116" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L116" s="13" t="s">
+      <c r="L116" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M116" t="s">
@@ -5370,18 +5379,18 @@
       </c>
     </row>
     <row r="117" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A117" s="13"/>
-      <c r="B117" s="13"/>
-      <c r="C117" s="17"/>
-      <c r="D117" s="14"/>
-      <c r="E117" s="16"/>
-      <c r="F117" s="16"/>
-      <c r="G117" s="13"/>
-      <c r="H117" s="13"/>
-      <c r="I117" s="13"/>
-      <c r="J117" s="15"/>
-      <c r="K117" s="13"/>
-      <c r="L117" s="13"/>
+      <c r="A117" s="16"/>
+      <c r="B117" s="16"/>
+      <c r="C117" s="15"/>
+      <c r="D117" s="17"/>
+      <c r="E117" s="19"/>
+      <c r="F117" s="19"/>
+      <c r="G117" s="16"/>
+      <c r="H117" s="16"/>
+      <c r="I117" s="16"/>
+      <c r="J117" s="18"/>
+      <c r="K117" s="16"/>
+      <c r="L117" s="16"/>
       <c r="M117" t="s">
         <v>212</v>
       </c>
@@ -5396,18 +5405,18 @@
       </c>
     </row>
     <row r="118" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A118" s="13"/>
-      <c r="B118" s="13"/>
-      <c r="C118" s="17"/>
-      <c r="D118" s="14"/>
-      <c r="E118" s="16"/>
-      <c r="F118" s="16"/>
-      <c r="G118" s="13"/>
-      <c r="H118" s="13"/>
-      <c r="I118" s="13"/>
-      <c r="J118" s="15"/>
-      <c r="K118" s="13"/>
-      <c r="L118" s="13"/>
+      <c r="A118" s="16"/>
+      <c r="B118" s="16"/>
+      <c r="C118" s="15"/>
+      <c r="D118" s="17"/>
+      <c r="E118" s="19"/>
+      <c r="F118" s="19"/>
+      <c r="G118" s="16"/>
+      <c r="H118" s="16"/>
+      <c r="I118" s="16"/>
+      <c r="J118" s="18"/>
+      <c r="K118" s="16"/>
+      <c r="L118" s="16"/>
       <c r="M118" t="s">
         <v>214</v>
       </c>
@@ -5422,32 +5431,32 @@
       </c>
     </row>
     <row r="119" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A119" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B119" s="13" t="s">
+      <c r="A119" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B119" s="16" t="s">
         <v>283</v>
       </c>
-      <c r="C119" s="17"/>
-      <c r="D119" s="14" t="s">
+      <c r="C119" s="15"/>
+      <c r="D119" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="E119" s="16"/>
-      <c r="F119" s="16"/>
-      <c r="G119" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H119" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I119" s="13"/>
-      <c r="J119" s="15" t="s">
+      <c r="E119" s="19"/>
+      <c r="F119" s="19"/>
+      <c r="G119" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H119" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I119" s="16"/>
+      <c r="J119" s="18" t="s">
         <v>284</v>
       </c>
-      <c r="K119" s="13" t="s">
+      <c r="K119" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L119" s="13" t="s">
+      <c r="L119" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M119" t="s">
@@ -5464,18 +5473,18 @@
       </c>
     </row>
     <row r="120" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A120" s="13"/>
-      <c r="B120" s="13"/>
-      <c r="C120" s="17"/>
-      <c r="D120" s="14"/>
-      <c r="E120" s="16"/>
-      <c r="F120" s="16"/>
-      <c r="G120" s="13"/>
-      <c r="H120" s="13"/>
-      <c r="I120" s="13"/>
-      <c r="J120" s="15"/>
-      <c r="K120" s="13"/>
-      <c r="L120" s="13"/>
+      <c r="A120" s="16"/>
+      <c r="B120" s="16"/>
+      <c r="C120" s="15"/>
+      <c r="D120" s="17"/>
+      <c r="E120" s="19"/>
+      <c r="F120" s="19"/>
+      <c r="G120" s="16"/>
+      <c r="H120" s="16"/>
+      <c r="I120" s="16"/>
+      <c r="J120" s="18"/>
+      <c r="K120" s="16"/>
+      <c r="L120" s="16"/>
       <c r="M120" t="s">
         <v>212</v>
       </c>
@@ -5490,18 +5499,18 @@
       </c>
     </row>
     <row r="121" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A121" s="13"/>
-      <c r="B121" s="13"/>
-      <c r="C121" s="17"/>
-      <c r="D121" s="14"/>
-      <c r="E121" s="16"/>
-      <c r="F121" s="16"/>
-      <c r="G121" s="13"/>
-      <c r="H121" s="13"/>
-      <c r="I121" s="13"/>
-      <c r="J121" s="15"/>
-      <c r="K121" s="13"/>
-      <c r="L121" s="13"/>
+      <c r="A121" s="16"/>
+      <c r="B121" s="16"/>
+      <c r="C121" s="15"/>
+      <c r="D121" s="17"/>
+      <c r="E121" s="19"/>
+      <c r="F121" s="19"/>
+      <c r="G121" s="16"/>
+      <c r="H121" s="16"/>
+      <c r="I121" s="16"/>
+      <c r="J121" s="18"/>
+      <c r="K121" s="16"/>
+      <c r="L121" s="16"/>
       <c r="M121" t="s">
         <v>214</v>
       </c>
@@ -5518,139 +5527,125 @@
   </sheetData>
   <autoFilter ref="A1:U1"/>
   <mergeCells count="276">
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="C64:C67"/>
-    <mergeCell ref="C68:C71"/>
-    <mergeCell ref="C72:C75"/>
-    <mergeCell ref="C78:C82"/>
-    <mergeCell ref="C83:C87"/>
-    <mergeCell ref="C88:C93"/>
-    <mergeCell ref="C94:C96"/>
-    <mergeCell ref="C97:C98"/>
-    <mergeCell ref="A110:A112"/>
-    <mergeCell ref="I110:I112"/>
-    <mergeCell ref="H110:H112"/>
-    <mergeCell ref="G110:G112"/>
-    <mergeCell ref="D110:D112"/>
-    <mergeCell ref="B110:B112"/>
-    <mergeCell ref="L110:L112"/>
-    <mergeCell ref="K110:K112"/>
-    <mergeCell ref="J110:J112"/>
-    <mergeCell ref="E110:E112"/>
-    <mergeCell ref="F110:F112"/>
-    <mergeCell ref="C110:C112"/>
-    <mergeCell ref="I105:I108"/>
-    <mergeCell ref="H105:H108"/>
-    <mergeCell ref="G105:G108"/>
-    <mergeCell ref="B105:B108"/>
-    <mergeCell ref="A105:A108"/>
-    <mergeCell ref="D105:D108"/>
-    <mergeCell ref="L105:L108"/>
-    <mergeCell ref="K105:K108"/>
-    <mergeCell ref="J105:J108"/>
-    <mergeCell ref="F105:F108"/>
-    <mergeCell ref="E105:E108"/>
-    <mergeCell ref="C105:C108"/>
-    <mergeCell ref="G97:G98"/>
-    <mergeCell ref="B97:B98"/>
-    <mergeCell ref="A97:A98"/>
-    <mergeCell ref="D97:D98"/>
-    <mergeCell ref="L102:L104"/>
-    <mergeCell ref="K102:K104"/>
-    <mergeCell ref="J102:J104"/>
-    <mergeCell ref="I102:I104"/>
-    <mergeCell ref="H102:H104"/>
-    <mergeCell ref="G102:G104"/>
-    <mergeCell ref="D102:D104"/>
-    <mergeCell ref="B102:B104"/>
-    <mergeCell ref="A102:A104"/>
-    <mergeCell ref="L97:L98"/>
-    <mergeCell ref="K97:K98"/>
-    <mergeCell ref="J97:J98"/>
-    <mergeCell ref="I97:I98"/>
-    <mergeCell ref="H97:H98"/>
-    <mergeCell ref="F97:F98"/>
-    <mergeCell ref="F102:F104"/>
-    <mergeCell ref="E97:E98"/>
-    <mergeCell ref="E102:E104"/>
-    <mergeCell ref="C102:C104"/>
-    <mergeCell ref="G94:G96"/>
-    <mergeCell ref="B94:B96"/>
-    <mergeCell ref="A94:A96"/>
-    <mergeCell ref="D94:D96"/>
-    <mergeCell ref="L94:L96"/>
-    <mergeCell ref="K94:K96"/>
-    <mergeCell ref="J94:J96"/>
-    <mergeCell ref="I94:I96"/>
-    <mergeCell ref="H94:H96"/>
-    <mergeCell ref="F94:F96"/>
-    <mergeCell ref="E94:E96"/>
-    <mergeCell ref="G83:G87"/>
-    <mergeCell ref="B83:B87"/>
-    <mergeCell ref="A83:A87"/>
-    <mergeCell ref="D83:D87"/>
-    <mergeCell ref="L88:L93"/>
-    <mergeCell ref="K88:K93"/>
-    <mergeCell ref="J88:J93"/>
-    <mergeCell ref="I88:I93"/>
-    <mergeCell ref="H88:H93"/>
-    <mergeCell ref="G88:G93"/>
-    <mergeCell ref="A88:A93"/>
-    <mergeCell ref="B88:B93"/>
-    <mergeCell ref="D88:D93"/>
-    <mergeCell ref="L83:L87"/>
-    <mergeCell ref="K83:K87"/>
-    <mergeCell ref="J83:J87"/>
-    <mergeCell ref="I83:I87"/>
-    <mergeCell ref="H83:H87"/>
-    <mergeCell ref="F83:F87"/>
-    <mergeCell ref="F88:F93"/>
-    <mergeCell ref="E83:E87"/>
-    <mergeCell ref="E88:E93"/>
-    <mergeCell ref="H78:H82"/>
-    <mergeCell ref="G78:G82"/>
-    <mergeCell ref="D78:D82"/>
-    <mergeCell ref="B78:B82"/>
-    <mergeCell ref="A78:A82"/>
-    <mergeCell ref="I72:I75"/>
-    <mergeCell ref="J72:J75"/>
-    <mergeCell ref="K72:K75"/>
-    <mergeCell ref="L72:L75"/>
-    <mergeCell ref="L78:L82"/>
-    <mergeCell ref="K78:K82"/>
-    <mergeCell ref="J78:J82"/>
-    <mergeCell ref="I78:I82"/>
-    <mergeCell ref="A72:A75"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="D72:D75"/>
-    <mergeCell ref="G72:G75"/>
-    <mergeCell ref="H72:H75"/>
-    <mergeCell ref="F72:F75"/>
-    <mergeCell ref="F78:F82"/>
-    <mergeCell ref="E72:E75"/>
-    <mergeCell ref="E78:E82"/>
-    <mergeCell ref="H68:H71"/>
-    <mergeCell ref="I68:I71"/>
-    <mergeCell ref="J68:J71"/>
-    <mergeCell ref="K68:K71"/>
-    <mergeCell ref="L68:L71"/>
-    <mergeCell ref="G64:G67"/>
-    <mergeCell ref="B64:B67"/>
-    <mergeCell ref="A64:A67"/>
-    <mergeCell ref="D64:D67"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="D68:D71"/>
-    <mergeCell ref="G68:G71"/>
-    <mergeCell ref="L64:L67"/>
-    <mergeCell ref="K64:K67"/>
-    <mergeCell ref="J64:J67"/>
-    <mergeCell ref="I64:I67"/>
-    <mergeCell ref="H64:H67"/>
-    <mergeCell ref="F64:F67"/>
-    <mergeCell ref="F68:F71"/>
-    <mergeCell ref="E64:E67"/>
-    <mergeCell ref="E68:E71"/>
+    <mergeCell ref="A119:A121"/>
+    <mergeCell ref="B119:B121"/>
+    <mergeCell ref="D119:D121"/>
+    <mergeCell ref="G119:G121"/>
+    <mergeCell ref="H119:H121"/>
+    <mergeCell ref="I119:I121"/>
+    <mergeCell ref="J119:J121"/>
+    <mergeCell ref="K119:K121"/>
+    <mergeCell ref="L119:L121"/>
+    <mergeCell ref="E119:E121"/>
+    <mergeCell ref="F119:F121"/>
+    <mergeCell ref="C119:C121"/>
+    <mergeCell ref="K113:K115"/>
+    <mergeCell ref="L113:L115"/>
+    <mergeCell ref="A116:A118"/>
+    <mergeCell ref="B116:B118"/>
+    <mergeCell ref="D116:D118"/>
+    <mergeCell ref="G116:G118"/>
+    <mergeCell ref="H116:H118"/>
+    <mergeCell ref="I116:I118"/>
+    <mergeCell ref="J116:J118"/>
+    <mergeCell ref="K116:K118"/>
+    <mergeCell ref="L116:L118"/>
+    <mergeCell ref="E113:E115"/>
+    <mergeCell ref="E116:E118"/>
+    <mergeCell ref="F113:F115"/>
+    <mergeCell ref="F116:F118"/>
+    <mergeCell ref="A113:A115"/>
+    <mergeCell ref="B113:B115"/>
+    <mergeCell ref="D113:D115"/>
+    <mergeCell ref="G113:G115"/>
+    <mergeCell ref="H113:H115"/>
+    <mergeCell ref="I113:I115"/>
+    <mergeCell ref="J113:J115"/>
+    <mergeCell ref="C113:C115"/>
+    <mergeCell ref="C116:C118"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="E37:E39"/>
+    <mergeCell ref="E41:E47"/>
+    <mergeCell ref="E57:E59"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="C37:C39"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="H31:H33"/>
+    <mergeCell ref="I31:I33"/>
+    <mergeCell ref="J31:J33"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="E28:E30"/>
+    <mergeCell ref="E31:E33"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="F28:F30"/>
+    <mergeCell ref="F31:F33"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="G28:G30"/>
+    <mergeCell ref="H28:H30"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="G31:G33"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="L41:L47"/>
+    <mergeCell ref="K41:K47"/>
+    <mergeCell ref="J41:J47"/>
+    <mergeCell ref="I41:I47"/>
+    <mergeCell ref="L28:L30"/>
+    <mergeCell ref="K28:K30"/>
+    <mergeCell ref="J28:J30"/>
+    <mergeCell ref="I28:I30"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="L24:L26"/>
+    <mergeCell ref="K24:K26"/>
+    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="K31:K33"/>
+    <mergeCell ref="L31:L33"/>
+    <mergeCell ref="I34:I36"/>
+    <mergeCell ref="J34:J36"/>
+    <mergeCell ref="K34:K36"/>
+    <mergeCell ref="L34:L36"/>
+    <mergeCell ref="I37:I39"/>
+    <mergeCell ref="J37:J39"/>
+    <mergeCell ref="K37:K39"/>
+    <mergeCell ref="L37:L39"/>
+    <mergeCell ref="L57:L59"/>
+    <mergeCell ref="K57:K59"/>
+    <mergeCell ref="J57:J59"/>
+    <mergeCell ref="I57:I59"/>
+    <mergeCell ref="H57:H59"/>
+    <mergeCell ref="H41:H47"/>
+    <mergeCell ref="G41:G47"/>
+    <mergeCell ref="B41:B47"/>
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="F41:F47"/>
+    <mergeCell ref="F57:F59"/>
+    <mergeCell ref="G57:G59"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="C41:C47"/>
+    <mergeCell ref="C57:C59"/>
     <mergeCell ref="F34:F36"/>
     <mergeCell ref="F37:F39"/>
     <mergeCell ref="H34:H36"/>
@@ -5675,125 +5670,139 @@
     <mergeCell ref="D34:D36"/>
     <mergeCell ref="D37:D39"/>
     <mergeCell ref="E62:E63"/>
-    <mergeCell ref="L57:L59"/>
-    <mergeCell ref="K57:K59"/>
-    <mergeCell ref="J57:J59"/>
-    <mergeCell ref="I57:I59"/>
-    <mergeCell ref="H57:H59"/>
-    <mergeCell ref="H41:H47"/>
-    <mergeCell ref="G41:G47"/>
-    <mergeCell ref="B41:B47"/>
-    <mergeCell ref="A41:A47"/>
-    <mergeCell ref="F41:F47"/>
-    <mergeCell ref="F57:F59"/>
-    <mergeCell ref="G57:G59"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="C41:C47"/>
-    <mergeCell ref="C57:C59"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="L41:L47"/>
-    <mergeCell ref="K41:K47"/>
-    <mergeCell ref="J41:J47"/>
-    <mergeCell ref="I41:I47"/>
-    <mergeCell ref="L28:L30"/>
-    <mergeCell ref="K28:K30"/>
-    <mergeCell ref="J28:J30"/>
-    <mergeCell ref="I28:I30"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="L24:L26"/>
-    <mergeCell ref="K24:K26"/>
-    <mergeCell ref="J24:J26"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="K31:K33"/>
-    <mergeCell ref="L31:L33"/>
-    <mergeCell ref="I34:I36"/>
-    <mergeCell ref="J34:J36"/>
-    <mergeCell ref="K34:K36"/>
-    <mergeCell ref="L34:L36"/>
-    <mergeCell ref="I37:I39"/>
-    <mergeCell ref="J37:J39"/>
-    <mergeCell ref="K37:K39"/>
-    <mergeCell ref="L37:L39"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="H31:H33"/>
-    <mergeCell ref="I31:I33"/>
-    <mergeCell ref="J31:J33"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="E28:E30"/>
-    <mergeCell ref="E31:E33"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="F28:F30"/>
-    <mergeCell ref="F31:F33"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="G28:G30"/>
-    <mergeCell ref="H28:H30"/>
-    <mergeCell ref="G24:G26"/>
-    <mergeCell ref="G31:G33"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="E37:E39"/>
-    <mergeCell ref="E41:E47"/>
-    <mergeCell ref="E57:E59"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="C37:C39"/>
-    <mergeCell ref="K113:K115"/>
-    <mergeCell ref="L113:L115"/>
-    <mergeCell ref="A116:A118"/>
-    <mergeCell ref="B116:B118"/>
-    <mergeCell ref="D116:D118"/>
-    <mergeCell ref="G116:G118"/>
-    <mergeCell ref="H116:H118"/>
-    <mergeCell ref="I116:I118"/>
-    <mergeCell ref="J116:J118"/>
-    <mergeCell ref="K116:K118"/>
-    <mergeCell ref="L116:L118"/>
-    <mergeCell ref="E113:E115"/>
-    <mergeCell ref="E116:E118"/>
-    <mergeCell ref="F113:F115"/>
-    <mergeCell ref="F116:F118"/>
-    <mergeCell ref="A113:A115"/>
-    <mergeCell ref="B113:B115"/>
-    <mergeCell ref="D113:D115"/>
-    <mergeCell ref="G113:G115"/>
-    <mergeCell ref="H113:H115"/>
-    <mergeCell ref="I113:I115"/>
-    <mergeCell ref="J113:J115"/>
-    <mergeCell ref="C113:C115"/>
-    <mergeCell ref="C116:C118"/>
-    <mergeCell ref="A119:A121"/>
-    <mergeCell ref="B119:B121"/>
-    <mergeCell ref="D119:D121"/>
-    <mergeCell ref="G119:G121"/>
-    <mergeCell ref="H119:H121"/>
-    <mergeCell ref="I119:I121"/>
-    <mergeCell ref="J119:J121"/>
-    <mergeCell ref="K119:K121"/>
-    <mergeCell ref="L119:L121"/>
-    <mergeCell ref="E119:E121"/>
-    <mergeCell ref="F119:F121"/>
-    <mergeCell ref="C119:C121"/>
+    <mergeCell ref="H68:H71"/>
+    <mergeCell ref="I68:I71"/>
+    <mergeCell ref="J68:J71"/>
+    <mergeCell ref="K68:K71"/>
+    <mergeCell ref="L68:L71"/>
+    <mergeCell ref="G64:G67"/>
+    <mergeCell ref="B64:B67"/>
+    <mergeCell ref="A64:A67"/>
+    <mergeCell ref="D64:D67"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="D68:D71"/>
+    <mergeCell ref="G68:G71"/>
+    <mergeCell ref="L64:L67"/>
+    <mergeCell ref="K64:K67"/>
+    <mergeCell ref="J64:J67"/>
+    <mergeCell ref="I64:I67"/>
+    <mergeCell ref="H64:H67"/>
+    <mergeCell ref="F64:F67"/>
+    <mergeCell ref="F68:F71"/>
+    <mergeCell ref="E64:E67"/>
+    <mergeCell ref="E68:E71"/>
+    <mergeCell ref="H78:H82"/>
+    <mergeCell ref="G78:G82"/>
+    <mergeCell ref="D78:D82"/>
+    <mergeCell ref="B78:B82"/>
+    <mergeCell ref="A78:A82"/>
+    <mergeCell ref="I72:I75"/>
+    <mergeCell ref="J72:J75"/>
+    <mergeCell ref="K72:K75"/>
+    <mergeCell ref="L72:L75"/>
+    <mergeCell ref="L78:L82"/>
+    <mergeCell ref="K78:K82"/>
+    <mergeCell ref="J78:J82"/>
+    <mergeCell ref="I78:I82"/>
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="D72:D75"/>
+    <mergeCell ref="G72:G75"/>
+    <mergeCell ref="H72:H75"/>
+    <mergeCell ref="F72:F75"/>
+    <mergeCell ref="F78:F82"/>
+    <mergeCell ref="E72:E75"/>
+    <mergeCell ref="E78:E82"/>
+    <mergeCell ref="G83:G87"/>
+    <mergeCell ref="B83:B87"/>
+    <mergeCell ref="A83:A87"/>
+    <mergeCell ref="D83:D87"/>
+    <mergeCell ref="L88:L93"/>
+    <mergeCell ref="K88:K93"/>
+    <mergeCell ref="J88:J93"/>
+    <mergeCell ref="I88:I93"/>
+    <mergeCell ref="H88:H93"/>
+    <mergeCell ref="G88:G93"/>
+    <mergeCell ref="A88:A93"/>
+    <mergeCell ref="B88:B93"/>
+    <mergeCell ref="D88:D93"/>
+    <mergeCell ref="L83:L87"/>
+    <mergeCell ref="K83:K87"/>
+    <mergeCell ref="J83:J87"/>
+    <mergeCell ref="I83:I87"/>
+    <mergeCell ref="H83:H87"/>
+    <mergeCell ref="F83:F87"/>
+    <mergeCell ref="F88:F93"/>
+    <mergeCell ref="E83:E87"/>
+    <mergeCell ref="E88:E93"/>
+    <mergeCell ref="G94:G96"/>
+    <mergeCell ref="B94:B96"/>
+    <mergeCell ref="A94:A96"/>
+    <mergeCell ref="D94:D96"/>
+    <mergeCell ref="L94:L96"/>
+    <mergeCell ref="K94:K96"/>
+    <mergeCell ref="J94:J96"/>
+    <mergeCell ref="I94:I96"/>
+    <mergeCell ref="H94:H96"/>
+    <mergeCell ref="F94:F96"/>
+    <mergeCell ref="E94:E96"/>
+    <mergeCell ref="G97:G98"/>
+    <mergeCell ref="B97:B98"/>
+    <mergeCell ref="A97:A98"/>
+    <mergeCell ref="D97:D98"/>
+    <mergeCell ref="L102:L104"/>
+    <mergeCell ref="K102:K104"/>
+    <mergeCell ref="J102:J104"/>
+    <mergeCell ref="I102:I104"/>
+    <mergeCell ref="H102:H104"/>
+    <mergeCell ref="G102:G104"/>
+    <mergeCell ref="D102:D104"/>
+    <mergeCell ref="B102:B104"/>
+    <mergeCell ref="A102:A104"/>
+    <mergeCell ref="L97:L98"/>
+    <mergeCell ref="K97:K98"/>
+    <mergeCell ref="J97:J98"/>
+    <mergeCell ref="I97:I98"/>
+    <mergeCell ref="H97:H98"/>
+    <mergeCell ref="F97:F98"/>
+    <mergeCell ref="F102:F104"/>
+    <mergeCell ref="E97:E98"/>
+    <mergeCell ref="E102:E104"/>
+    <mergeCell ref="C102:C104"/>
+    <mergeCell ref="I105:I108"/>
+    <mergeCell ref="H105:H108"/>
+    <mergeCell ref="G105:G108"/>
+    <mergeCell ref="B105:B108"/>
+    <mergeCell ref="A105:A108"/>
+    <mergeCell ref="D105:D108"/>
+    <mergeCell ref="L105:L108"/>
+    <mergeCell ref="K105:K108"/>
+    <mergeCell ref="J105:J108"/>
+    <mergeCell ref="F105:F108"/>
+    <mergeCell ref="E105:E108"/>
+    <mergeCell ref="C105:C108"/>
+    <mergeCell ref="A110:A112"/>
+    <mergeCell ref="I110:I112"/>
+    <mergeCell ref="H110:H112"/>
+    <mergeCell ref="G110:G112"/>
+    <mergeCell ref="D110:D112"/>
+    <mergeCell ref="B110:B112"/>
+    <mergeCell ref="L110:L112"/>
+    <mergeCell ref="K110:K112"/>
+    <mergeCell ref="J110:J112"/>
+    <mergeCell ref="E110:E112"/>
+    <mergeCell ref="F110:F112"/>
+    <mergeCell ref="C110:C112"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="C64:C67"/>
+    <mergeCell ref="C68:C71"/>
+    <mergeCell ref="C72:C75"/>
+    <mergeCell ref="C78:C82"/>
+    <mergeCell ref="C83:C87"/>
+    <mergeCell ref="C88:C93"/>
+    <mergeCell ref="C94:C96"/>
+    <mergeCell ref="C97:C98"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="P54" r:id="rId1"/>
@@ -5864,7 +5873,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Tables!$F$13:$F$17</xm:f>
+            <xm:f>Tables!$F$13:$F$20</xm:f>
           </x14:formula1>
           <xm:sqref>T1:T1048576</xm:sqref>
         </x14:dataValidation>
@@ -5876,7 +5885,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F13:F17"/>
+  <dimension ref="F13:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
@@ -5910,6 +5919,21 @@
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
         <v>309</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating Request Call Details
git-tfs-id: [http://developmentvlan:8585/tfs/vanrise.collection]$/;C55360
</commit_message>
<xml_diff>
--- a/SOM/Documents/SOM/SOM APIs Mapping Sheet.xlsx
+++ b/SOM/Documents/SOM/SOM APIs Mapping Sheet.xlsx
@@ -1155,12 +1155,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1173,19 +1167,25 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2384,34 +2384,34 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B22" s="22" t="s">
+      <c r="A22" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B22" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="17" t="s">
+      <c r="C22" s="21"/>
+      <c r="D22" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="H22" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="I22" s="22" t="s">
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I22" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="J22" s="20" t="s">
+      <c r="J22" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="K22" s="14" t="s">
+      <c r="K22" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="L22" s="22" t="s">
+      <c r="L22" s="19" t="s">
         <v>120</v>
       </c>
       <c r="M22" t="s">
@@ -2428,18 +2428,18 @@
       </c>
     </row>
     <row r="23" spans="1:21" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="22"/>
+      <c r="A23" s="14"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="19"/>
       <c r="M23" t="s">
         <v>157</v>
       </c>
@@ -2454,31 +2454,31 @@
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B24" s="16" t="s">
+      <c r="A24" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B24" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="17" t="s">
+      <c r="C24" s="18"/>
+      <c r="D24" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H24" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I24" s="18" t="s">
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="J24" s="16" t="s">
+      <c r="J24" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="K24" s="16" t="s">
+      <c r="K24" s="14" t="s">
         <v>82</v>
       </c>
       <c r="L24" s="23" t="s">
@@ -2496,17 +2496,17 @@
       <c r="U24"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16"/>
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
       <c r="L25" s="23"/>
       <c r="M25" t="s">
         <v>73</v>
@@ -2519,17 +2519,17 @@
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
       <c r="L26" s="23"/>
       <c r="M26" t="s">
         <v>135</v>
@@ -2585,34 +2585,34 @@
       </c>
     </row>
     <row r="28" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B28" s="16" t="s">
+      <c r="A28" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B28" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="17" t="s">
+      <c r="C28" s="18"/>
+      <c r="D28" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H28" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I28" s="16" t="s">
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I28" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="J28" s="18" t="s">
+      <c r="J28" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="K28" s="16" t="s">
+      <c r="K28" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="L28" s="16" t="s">
+      <c r="L28" s="14" t="s">
         <v>119</v>
       </c>
       <c r="M28" t="s">
@@ -2629,18 +2629,18 @@
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="16"/>
-      <c r="L29" s="16"/>
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
       <c r="M29" t="s">
         <v>85</v>
       </c>
@@ -2652,18 +2652,18 @@
       </c>
     </row>
     <row r="30" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="16"/>
-      <c r="L30" s="16"/>
+      <c r="A30" s="14"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
       <c r="M30" t="s">
         <v>90</v>
       </c>
@@ -2678,34 +2678,34 @@
       </c>
     </row>
     <row r="31" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B31" s="16" t="s">
+      <c r="A31" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B31" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="17" t="s">
+      <c r="C31" s="18"/>
+      <c r="D31" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H31" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I31" s="16" t="s">
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H31" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I31" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="J31" s="18" t="s">
+      <c r="J31" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="K31" s="16" t="s">
+      <c r="K31" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="L31" s="16" t="s">
+      <c r="L31" s="14" t="s">
         <v>119</v>
       </c>
       <c r="M31" t="s">
@@ -2719,18 +2719,18 @@
       </c>
     </row>
     <row r="32" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="16"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="16"/>
-      <c r="L32" s="16"/>
+      <c r="A32" s="14"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="16"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
       <c r="M32" t="s">
         <v>85</v>
       </c>
@@ -2742,18 +2742,18 @@
       </c>
     </row>
     <row r="33" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="16"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="16"/>
-      <c r="L33" s="16"/>
+      <c r="A33" s="14"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
       <c r="M33" t="s">
         <v>90</v>
       </c>
@@ -2768,34 +2768,34 @@
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B34" s="16" t="s">
+      <c r="A34" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B34" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="C34" s="15"/>
-      <c r="D34" s="17" t="s">
+      <c r="C34" s="18"/>
+      <c r="D34" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H34" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I34" s="16" t="s">
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H34" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I34" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="J34" s="18" t="s">
+      <c r="J34" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="K34" s="16" t="s">
+      <c r="K34" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="L34" s="16" t="s">
+      <c r="L34" s="14" t="s">
         <v>119</v>
       </c>
       <c r="M34" t="s">
@@ -2809,18 +2809,18 @@
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="18"/>
-      <c r="K35" s="16"/>
-      <c r="L35" s="16"/>
+      <c r="A35" s="14"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="16"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
       <c r="M35" t="s">
         <v>85</v>
       </c>
@@ -2832,18 +2832,18 @@
       </c>
     </row>
     <row r="36" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="16"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
-      <c r="I36" s="16"/>
-      <c r="J36" s="18"/>
-      <c r="K36" s="16"/>
-      <c r="L36" s="16"/>
+      <c r="A36" s="14"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
       <c r="M36" t="s">
         <v>90</v>
       </c>
@@ -2858,34 +2858,34 @@
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A37" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B37" s="16" t="s">
+      <c r="A37" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B37" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="C37" s="15"/>
-      <c r="D37" s="17" t="s">
+      <c r="C37" s="18"/>
+      <c r="D37" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H37" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I37" s="16" t="s">
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H37" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I37" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="J37" s="18" t="s">
+      <c r="J37" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="K37" s="16" t="s">
+      <c r="K37" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="L37" s="16" t="s">
+      <c r="L37" s="14" t="s">
         <v>119</v>
       </c>
       <c r="M37" t="s">
@@ -2899,18 +2899,18 @@
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="16"/>
-      <c r="B38" s="16"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
-      <c r="I38" s="16"/>
-      <c r="J38" s="18"/>
-      <c r="K38" s="16"/>
-      <c r="L38" s="16"/>
+      <c r="A38" s="14"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
       <c r="M38" t="s">
         <v>85</v>
       </c>
@@ -2922,18 +2922,18 @@
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A39" s="16"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
-      <c r="I39" s="16"/>
-      <c r="J39" s="18"/>
-      <c r="K39" s="16"/>
-      <c r="L39" s="16"/>
+      <c r="A39" s="14"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="14"/>
+      <c r="L39" s="14"/>
       <c r="M39" t="s">
         <v>90</v>
       </c>
@@ -2985,34 +2985,34 @@
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A41" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B41" s="16" t="s">
+      <c r="A41" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B41" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="C41" s="15"/>
-      <c r="D41" s="17" t="s">
+      <c r="C41" s="18"/>
+      <c r="D41" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H41" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I41" s="16" t="s">
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H41" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I41" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="J41" s="18" t="s">
+      <c r="J41" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="K41" s="16" t="s">
+      <c r="K41" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="L41" s="16" t="s">
+      <c r="L41" s="14" t="s">
         <v>119</v>
       </c>
       <c r="M41" t="s">
@@ -3026,18 +3026,18 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="16"/>
-      <c r="B42" s="16"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="16"/>
-      <c r="H42" s="16"/>
-      <c r="I42" s="16"/>
-      <c r="J42" s="18"/>
-      <c r="K42" s="16"/>
-      <c r="L42" s="16"/>
+      <c r="A42" s="14"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="16"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14"/>
       <c r="M42" t="s">
         <v>90</v>
       </c>
@@ -3049,18 +3049,18 @@
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A43" s="16"/>
-      <c r="B43" s="16"/>
-      <c r="C43" s="15"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="16"/>
-      <c r="H43" s="16"/>
-      <c r="I43" s="16"/>
-      <c r="J43" s="18"/>
-      <c r="K43" s="16"/>
-      <c r="L43" s="16"/>
+      <c r="A43" s="14"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="16"/>
+      <c r="K43" s="14"/>
+      <c r="L43" s="14"/>
       <c r="M43" t="s">
         <v>91</v>
       </c>
@@ -3073,18 +3073,18 @@
       <c r="U43"/>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A44" s="16"/>
-      <c r="B44" s="16"/>
-      <c r="C44" s="15"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="19"/>
-      <c r="G44" s="16"/>
-      <c r="H44" s="16"/>
-      <c r="I44" s="16"/>
-      <c r="J44" s="18"/>
-      <c r="K44" s="16"/>
-      <c r="L44" s="16"/>
+      <c r="A44" s="14"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="16"/>
+      <c r="K44" s="14"/>
+      <c r="L44" s="14"/>
       <c r="M44" t="s">
         <v>93</v>
       </c>
@@ -3097,18 +3097,18 @@
       <c r="U44"/>
     </row>
     <row r="45" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="16"/>
-      <c r="B45" s="16"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="16"/>
-      <c r="H45" s="16"/>
-      <c r="I45" s="16"/>
-      <c r="J45" s="18"/>
-      <c r="K45" s="16"/>
-      <c r="L45" s="16"/>
+      <c r="A45" s="14"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="14"/>
+      <c r="J45" s="16"/>
+      <c r="K45" s="14"/>
+      <c r="L45" s="14"/>
       <c r="M45" t="s">
         <v>81</v>
       </c>
@@ -3123,18 +3123,18 @@
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A46" s="16"/>
-      <c r="B46" s="16"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="19"/>
-      <c r="G46" s="16"/>
-      <c r="H46" s="16"/>
-      <c r="I46" s="16"/>
-      <c r="J46" s="18"/>
-      <c r="K46" s="16"/>
-      <c r="L46" s="16"/>
+      <c r="A46" s="14"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="16"/>
+      <c r="K46" s="14"/>
+      <c r="L46" s="14"/>
       <c r="M46" t="s">
         <v>126</v>
       </c>
@@ -3146,18 +3146,18 @@
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="16"/>
-      <c r="B47" s="16"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="19"/>
-      <c r="G47" s="16"/>
-      <c r="H47" s="16"/>
-      <c r="I47" s="16"/>
-      <c r="J47" s="18"/>
-      <c r="K47" s="16"/>
-      <c r="L47" s="16"/>
+      <c r="A47" s="14"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
+      <c r="J47" s="16"/>
+      <c r="K47" s="14"/>
+      <c r="L47" s="14"/>
       <c r="M47" t="s">
         <v>47</v>
       </c>
@@ -3461,7 +3461,7 @@
         <v>305</v>
       </c>
       <c r="T54" s="12" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="U54" s="1" t="s">
         <v>300</v>
@@ -3541,29 +3541,29 @@
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A57" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B57" s="16" t="s">
+      <c r="A57" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B57" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="C57" s="15"/>
-      <c r="D57" s="18"/>
-      <c r="E57" s="24"/>
-      <c r="F57" s="24"/>
-      <c r="G57" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H57" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I57" s="16" t="s">
+      <c r="C57" s="18"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H57" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I57" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="J57" s="18" t="s">
+      <c r="J57" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="K57" s="16" t="s">
+      <c r="K57" s="14" t="s">
         <v>82</v>
       </c>
       <c r="L57" s="23" t="s">
@@ -3580,17 +3580,17 @@
       </c>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A58" s="16"/>
-      <c r="B58" s="16"/>
-      <c r="C58" s="15"/>
-      <c r="D58" s="18"/>
-      <c r="E58" s="24"/>
-      <c r="F58" s="24"/>
-      <c r="G58" s="16"/>
-      <c r="H58" s="16"/>
-      <c r="I58" s="16"/>
-      <c r="J58" s="18"/>
-      <c r="K58" s="16"/>
+      <c r="A58" s="14"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="16"/>
+      <c r="E58" s="20"/>
+      <c r="F58" s="20"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="14"/>
+      <c r="J58" s="16"/>
+      <c r="K58" s="14"/>
       <c r="L58" s="23"/>
       <c r="M58" t="s">
         <v>132</v>
@@ -3603,17 +3603,17 @@
       </c>
     </row>
     <row r="59" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A59" s="16"/>
-      <c r="B59" s="16"/>
-      <c r="C59" s="15"/>
-      <c r="D59" s="18"/>
-      <c r="E59" s="24"/>
-      <c r="F59" s="24"/>
-      <c r="G59" s="16"/>
-      <c r="H59" s="16"/>
-      <c r="I59" s="16"/>
-      <c r="J59" s="18"/>
-      <c r="K59" s="16"/>
+      <c r="A59" s="14"/>
+      <c r="B59" s="14"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="16"/>
+      <c r="E59" s="20"/>
+      <c r="F59" s="20"/>
+      <c r="G59" s="14"/>
+      <c r="H59" s="14"/>
+      <c r="I59" s="14"/>
+      <c r="J59" s="16"/>
+      <c r="K59" s="14"/>
       <c r="L59" s="23"/>
       <c r="M59" t="s">
         <v>133</v>
@@ -3702,34 +3702,34 @@
       </c>
     </row>
     <row r="62" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="B62" s="22" t="s">
+      <c r="A62" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="B62" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="C62" s="14"/>
-      <c r="D62" s="20" t="s">
+      <c r="C62" s="21"/>
+      <c r="D62" s="22" t="s">
         <v>200</v>
       </c>
-      <c r="E62" s="21"/>
-      <c r="F62" s="21"/>
-      <c r="G62" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="H62" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="I62" s="16" t="s">
+      <c r="E62" s="24"/>
+      <c r="F62" s="24"/>
+      <c r="G62" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H62" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I62" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="J62" s="18" t="s">
+      <c r="J62" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="K62" s="16" t="s">
+      <c r="K62" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="L62" s="16" t="s">
+      <c r="L62" s="14" t="s">
         <v>119</v>
       </c>
       <c r="M62" t="s">
@@ -3746,18 +3746,18 @@
       </c>
     </row>
     <row r="63" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A63" s="22"/>
-      <c r="B63" s="22"/>
-      <c r="C63" s="14"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="21"/>
-      <c r="F63" s="21"/>
-      <c r="G63" s="22"/>
-      <c r="H63" s="22"/>
-      <c r="I63" s="16"/>
-      <c r="J63" s="18"/>
-      <c r="K63" s="16"/>
-      <c r="L63" s="16"/>
+      <c r="A63" s="19"/>
+      <c r="B63" s="19"/>
+      <c r="C63" s="21"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="24"/>
+      <c r="F63" s="24"/>
+      <c r="G63" s="19"/>
+      <c r="H63" s="19"/>
+      <c r="I63" s="14"/>
+      <c r="J63" s="16"/>
+      <c r="K63" s="14"/>
+      <c r="L63" s="14"/>
       <c r="M63" t="s">
         <v>182</v>
       </c>
@@ -3772,34 +3772,34 @@
       </c>
     </row>
     <row r="64" spans="1:21" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B64" s="16" t="s">
+      <c r="A64" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B64" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="C64" s="15"/>
-      <c r="D64" s="20" t="s">
+      <c r="C64" s="18"/>
+      <c r="D64" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="E64" s="21"/>
-      <c r="F64" s="21"/>
-      <c r="G64" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H64" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I64" s="16" t="s">
+      <c r="E64" s="24"/>
+      <c r="F64" s="24"/>
+      <c r="G64" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H64" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I64" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="J64" s="16" t="s">
+      <c r="J64" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="K64" s="16" t="s">
+      <c r="K64" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="L64" s="16" t="s">
+      <c r="L64" s="14" t="s">
         <v>120</v>
       </c>
       <c r="M64" t="s">
@@ -3816,18 +3816,18 @@
       </c>
     </row>
     <row r="65" spans="1:21" ht="90" x14ac:dyDescent="0.25">
-      <c r="A65" s="16"/>
-      <c r="B65" s="16"/>
-      <c r="C65" s="15"/>
-      <c r="D65" s="20"/>
-      <c r="E65" s="21"/>
-      <c r="F65" s="21"/>
-      <c r="G65" s="16"/>
-      <c r="H65" s="16"/>
-      <c r="I65" s="16"/>
-      <c r="J65" s="16"/>
-      <c r="K65" s="16"/>
-      <c r="L65" s="16"/>
+      <c r="A65" s="14"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="18"/>
+      <c r="D65" s="22"/>
+      <c r="E65" s="24"/>
+      <c r="F65" s="24"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14"/>
+      <c r="I65" s="14"/>
+      <c r="J65" s="14"/>
+      <c r="K65" s="14"/>
+      <c r="L65" s="14"/>
       <c r="M65" t="s">
         <v>187</v>
       </c>
@@ -3842,18 +3842,18 @@
       </c>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A66" s="16"/>
-      <c r="B66" s="16"/>
-      <c r="C66" s="15"/>
-      <c r="D66" s="20"/>
-      <c r="E66" s="21"/>
-      <c r="F66" s="21"/>
-      <c r="G66" s="16"/>
-      <c r="H66" s="16"/>
-      <c r="I66" s="16"/>
-      <c r="J66" s="16"/>
-      <c r="K66" s="16"/>
-      <c r="L66" s="16"/>
+      <c r="A66" s="14"/>
+      <c r="B66" s="14"/>
+      <c r="C66" s="18"/>
+      <c r="D66" s="22"/>
+      <c r="E66" s="24"/>
+      <c r="F66" s="24"/>
+      <c r="G66" s="14"/>
+      <c r="H66" s="14"/>
+      <c r="I66" s="14"/>
+      <c r="J66" s="14"/>
+      <c r="K66" s="14"/>
+      <c r="L66" s="14"/>
       <c r="M66" t="s">
         <v>190</v>
       </c>
@@ -3865,18 +3865,18 @@
       </c>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A67" s="16"/>
-      <c r="B67" s="16"/>
-      <c r="C67" s="15"/>
-      <c r="D67" s="20"/>
-      <c r="E67" s="21"/>
-      <c r="F67" s="21"/>
-      <c r="G67" s="16"/>
-      <c r="H67" s="16"/>
-      <c r="I67" s="16"/>
-      <c r="J67" s="16"/>
-      <c r="K67" s="16"/>
-      <c r="L67" s="16"/>
+      <c r="A67" s="14"/>
+      <c r="B67" s="14"/>
+      <c r="C67" s="18"/>
+      <c r="D67" s="22"/>
+      <c r="E67" s="24"/>
+      <c r="F67" s="24"/>
+      <c r="G67" s="14"/>
+      <c r="H67" s="14"/>
+      <c r="I67" s="14"/>
+      <c r="J67" s="14"/>
+      <c r="K67" s="14"/>
+      <c r="L67" s="14"/>
       <c r="M67" t="s">
         <v>191</v>
       </c>
@@ -3888,34 +3888,34 @@
       </c>
     </row>
     <row r="68" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B68" s="16" t="s">
+      <c r="A68" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B68" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="C68" s="15"/>
-      <c r="D68" s="20" t="s">
+      <c r="C68" s="18"/>
+      <c r="D68" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="E68" s="21"/>
-      <c r="F68" s="21"/>
-      <c r="G68" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H68" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I68" s="16" t="s">
+      <c r="E68" s="24"/>
+      <c r="F68" s="24"/>
+      <c r="G68" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H68" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I68" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="J68" s="16" t="s">
+      <c r="J68" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="K68" s="16" t="s">
+      <c r="K68" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="L68" s="16" t="s">
+      <c r="L68" s="14" t="s">
         <v>120</v>
       </c>
       <c r="M68" t="s">
@@ -3932,18 +3932,18 @@
       </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A69" s="16"/>
-      <c r="B69" s="16"/>
-      <c r="C69" s="15"/>
-      <c r="D69" s="20"/>
-      <c r="E69" s="21"/>
-      <c r="F69" s="21"/>
-      <c r="G69" s="16"/>
-      <c r="H69" s="16"/>
-      <c r="I69" s="16"/>
-      <c r="J69" s="16"/>
-      <c r="K69" s="16"/>
-      <c r="L69" s="16"/>
+      <c r="A69" s="14"/>
+      <c r="B69" s="14"/>
+      <c r="C69" s="18"/>
+      <c r="D69" s="22"/>
+      <c r="E69" s="24"/>
+      <c r="F69" s="24"/>
+      <c r="G69" s="14"/>
+      <c r="H69" s="14"/>
+      <c r="I69" s="14"/>
+      <c r="J69" s="14"/>
+      <c r="K69" s="14"/>
+      <c r="L69" s="14"/>
       <c r="M69" t="s">
         <v>187</v>
       </c>
@@ -3955,18 +3955,18 @@
       </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A70" s="16"/>
-      <c r="B70" s="16"/>
-      <c r="C70" s="15"/>
-      <c r="D70" s="20"/>
-      <c r="E70" s="21"/>
-      <c r="F70" s="21"/>
-      <c r="G70" s="16"/>
-      <c r="H70" s="16"/>
-      <c r="I70" s="16"/>
-      <c r="J70" s="16"/>
-      <c r="K70" s="16"/>
-      <c r="L70" s="16"/>
+      <c r="A70" s="14"/>
+      <c r="B70" s="14"/>
+      <c r="C70" s="18"/>
+      <c r="D70" s="22"/>
+      <c r="E70" s="24"/>
+      <c r="F70" s="24"/>
+      <c r="G70" s="14"/>
+      <c r="H70" s="14"/>
+      <c r="I70" s="14"/>
+      <c r="J70" s="14"/>
+      <c r="K70" s="14"/>
+      <c r="L70" s="14"/>
       <c r="M70" t="s">
         <v>190</v>
       </c>
@@ -3978,18 +3978,18 @@
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A71" s="16"/>
-      <c r="B71" s="16"/>
-      <c r="C71" s="15"/>
-      <c r="D71" s="20"/>
-      <c r="E71" s="21"/>
-      <c r="F71" s="21"/>
-      <c r="G71" s="16"/>
-      <c r="H71" s="16"/>
-      <c r="I71" s="16"/>
-      <c r="J71" s="16"/>
-      <c r="K71" s="16"/>
-      <c r="L71" s="16"/>
+      <c r="A71" s="14"/>
+      <c r="B71" s="14"/>
+      <c r="C71" s="18"/>
+      <c r="D71" s="22"/>
+      <c r="E71" s="24"/>
+      <c r="F71" s="24"/>
+      <c r="G71" s="14"/>
+      <c r="H71" s="14"/>
+      <c r="I71" s="14"/>
+      <c r="J71" s="14"/>
+      <c r="K71" s="14"/>
+      <c r="L71" s="14"/>
       <c r="M71" t="s">
         <v>191</v>
       </c>
@@ -4001,34 +4001,34 @@
       </c>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A72" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B72" s="16" t="s">
+      <c r="A72" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B72" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="C72" s="15"/>
-      <c r="D72" s="20" t="s">
+      <c r="C72" s="18"/>
+      <c r="D72" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="E72" s="21"/>
-      <c r="F72" s="21"/>
-      <c r="G72" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H72" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I72" s="16" t="s">
+      <c r="E72" s="24"/>
+      <c r="F72" s="24"/>
+      <c r="G72" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H72" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I72" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="J72" s="16" t="s">
+      <c r="J72" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="K72" s="16" t="s">
+      <c r="K72" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="L72" s="16" t="s">
+      <c r="L72" s="14" t="s">
         <v>120</v>
       </c>
       <c r="M72" t="s">
@@ -4042,18 +4042,18 @@
       </c>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A73" s="16"/>
-      <c r="B73" s="16"/>
-      <c r="C73" s="15"/>
-      <c r="D73" s="20"/>
-      <c r="E73" s="21"/>
-      <c r="F73" s="21"/>
-      <c r="G73" s="16"/>
-      <c r="H73" s="16"/>
-      <c r="I73" s="16"/>
-      <c r="J73" s="16"/>
-      <c r="K73" s="16"/>
-      <c r="L73" s="16"/>
+      <c r="A73" s="14"/>
+      <c r="B73" s="14"/>
+      <c r="C73" s="18"/>
+      <c r="D73" s="22"/>
+      <c r="E73" s="24"/>
+      <c r="F73" s="24"/>
+      <c r="G73" s="14"/>
+      <c r="H73" s="14"/>
+      <c r="I73" s="14"/>
+      <c r="J73" s="14"/>
+      <c r="K73" s="14"/>
+      <c r="L73" s="14"/>
       <c r="M73" t="s">
         <v>187</v>
       </c>
@@ -4065,18 +4065,18 @@
       </c>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A74" s="16"/>
-      <c r="B74" s="16"/>
-      <c r="C74" s="15"/>
-      <c r="D74" s="20"/>
-      <c r="E74" s="21"/>
-      <c r="F74" s="21"/>
-      <c r="G74" s="16"/>
-      <c r="H74" s="16"/>
-      <c r="I74" s="16"/>
-      <c r="J74" s="16"/>
-      <c r="K74" s="16"/>
-      <c r="L74" s="16"/>
+      <c r="A74" s="14"/>
+      <c r="B74" s="14"/>
+      <c r="C74" s="18"/>
+      <c r="D74" s="22"/>
+      <c r="E74" s="24"/>
+      <c r="F74" s="24"/>
+      <c r="G74" s="14"/>
+      <c r="H74" s="14"/>
+      <c r="I74" s="14"/>
+      <c r="J74" s="14"/>
+      <c r="K74" s="14"/>
+      <c r="L74" s="14"/>
       <c r="M74" t="s">
         <v>190</v>
       </c>
@@ -4088,18 +4088,18 @@
       </c>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A75" s="16"/>
-      <c r="B75" s="16"/>
-      <c r="C75" s="15"/>
-      <c r="D75" s="20"/>
-      <c r="E75" s="21"/>
-      <c r="F75" s="21"/>
-      <c r="G75" s="16"/>
-      <c r="H75" s="16"/>
-      <c r="I75" s="16"/>
-      <c r="J75" s="16"/>
-      <c r="K75" s="16"/>
-      <c r="L75" s="16"/>
+      <c r="A75" s="14"/>
+      <c r="B75" s="14"/>
+      <c r="C75" s="18"/>
+      <c r="D75" s="22"/>
+      <c r="E75" s="24"/>
+      <c r="F75" s="24"/>
+      <c r="G75" s="14"/>
+      <c r="H75" s="14"/>
+      <c r="I75" s="14"/>
+      <c r="J75" s="14"/>
+      <c r="K75" s="14"/>
+      <c r="L75" s="14"/>
       <c r="M75" t="s">
         <v>191</v>
       </c>
@@ -4187,34 +4187,34 @@
       </c>
     </row>
     <row r="78" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B78" s="16" t="s">
+      <c r="A78" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B78" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="C78" s="15"/>
-      <c r="D78" s="20" t="s">
+      <c r="C78" s="18"/>
+      <c r="D78" s="22" t="s">
         <v>208</v>
       </c>
-      <c r="E78" s="21"/>
-      <c r="F78" s="21"/>
-      <c r="G78" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H78" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I78" s="16" t="s">
+      <c r="E78" s="24"/>
+      <c r="F78" s="24"/>
+      <c r="G78" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H78" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I78" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="J78" s="16" t="s">
+      <c r="J78" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="K78" s="16" t="s">
+      <c r="K78" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="L78" s="16" t="s">
+      <c r="L78" s="14" t="s">
         <v>120</v>
       </c>
       <c r="M78" t="s">
@@ -4231,18 +4231,18 @@
       </c>
     </row>
     <row r="79" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A79" s="16"/>
-      <c r="B79" s="16"/>
-      <c r="C79" s="15"/>
-      <c r="D79" s="20"/>
-      <c r="E79" s="21"/>
-      <c r="F79" s="21"/>
-      <c r="G79" s="16"/>
-      <c r="H79" s="16"/>
-      <c r="I79" s="16"/>
-      <c r="J79" s="16"/>
-      <c r="K79" s="16"/>
-      <c r="L79" s="16"/>
+      <c r="A79" s="14"/>
+      <c r="B79" s="14"/>
+      <c r="C79" s="18"/>
+      <c r="D79" s="22"/>
+      <c r="E79" s="24"/>
+      <c r="F79" s="24"/>
+      <c r="G79" s="14"/>
+      <c r="H79" s="14"/>
+      <c r="I79" s="14"/>
+      <c r="J79" s="14"/>
+      <c r="K79" s="14"/>
+      <c r="L79" s="14"/>
       <c r="M79" t="s">
         <v>212</v>
       </c>
@@ -4257,18 +4257,18 @@
       </c>
     </row>
     <row r="80" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="16"/>
-      <c r="B80" s="16"/>
-      <c r="C80" s="15"/>
-      <c r="D80" s="20"/>
-      <c r="E80" s="21"/>
-      <c r="F80" s="21"/>
-      <c r="G80" s="16"/>
-      <c r="H80" s="16"/>
-      <c r="I80" s="16"/>
-      <c r="J80" s="16"/>
-      <c r="K80" s="16"/>
-      <c r="L80" s="16"/>
+      <c r="A80" s="14"/>
+      <c r="B80" s="14"/>
+      <c r="C80" s="18"/>
+      <c r="D80" s="22"/>
+      <c r="E80" s="24"/>
+      <c r="F80" s="24"/>
+      <c r="G80" s="14"/>
+      <c r="H80" s="14"/>
+      <c r="I80" s="14"/>
+      <c r="J80" s="14"/>
+      <c r="K80" s="14"/>
+      <c r="L80" s="14"/>
       <c r="M80" t="s">
         <v>214</v>
       </c>
@@ -4283,18 +4283,18 @@
       </c>
     </row>
     <row r="81" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A81" s="16"/>
-      <c r="B81" s="16"/>
-      <c r="C81" s="15"/>
-      <c r="D81" s="20"/>
-      <c r="E81" s="21"/>
-      <c r="F81" s="21"/>
-      <c r="G81" s="16"/>
-      <c r="H81" s="16"/>
-      <c r="I81" s="16"/>
-      <c r="J81" s="16"/>
-      <c r="K81" s="16"/>
-      <c r="L81" s="16"/>
+      <c r="A81" s="14"/>
+      <c r="B81" s="14"/>
+      <c r="C81" s="18"/>
+      <c r="D81" s="22"/>
+      <c r="E81" s="24"/>
+      <c r="F81" s="24"/>
+      <c r="G81" s="14"/>
+      <c r="H81" s="14"/>
+      <c r="I81" s="14"/>
+      <c r="J81" s="14"/>
+      <c r="K81" s="14"/>
+      <c r="L81" s="14"/>
       <c r="M81" t="s">
         <v>132</v>
       </c>
@@ -4309,18 +4309,18 @@
       </c>
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A82" s="16"/>
-      <c r="B82" s="16"/>
-      <c r="C82" s="15"/>
-      <c r="D82" s="20"/>
-      <c r="E82" s="21"/>
-      <c r="F82" s="21"/>
-      <c r="G82" s="16"/>
-      <c r="H82" s="16"/>
-      <c r="I82" s="16"/>
-      <c r="J82" s="16"/>
-      <c r="K82" s="16"/>
-      <c r="L82" s="16"/>
+      <c r="A82" s="14"/>
+      <c r="B82" s="14"/>
+      <c r="C82" s="18"/>
+      <c r="D82" s="22"/>
+      <c r="E82" s="24"/>
+      <c r="F82" s="24"/>
+      <c r="G82" s="14"/>
+      <c r="H82" s="14"/>
+      <c r="I82" s="14"/>
+      <c r="J82" s="14"/>
+      <c r="K82" s="14"/>
+      <c r="L82" s="14"/>
       <c r="M82" t="s">
         <v>133</v>
       </c>
@@ -4332,32 +4332,32 @@
       </c>
     </row>
     <row r="83" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="B83" s="16" t="s">
+      <c r="A83" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="B83" s="14" t="s">
         <v>217</v>
       </c>
-      <c r="C83" s="15"/>
-      <c r="D83" s="20" t="s">
+      <c r="C83" s="18"/>
+      <c r="D83" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="E83" s="21"/>
-      <c r="F83" s="21"/>
-      <c r="G83" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H83" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I83" s="16"/>
-      <c r="J83" s="16" t="s">
+      <c r="E83" s="24"/>
+      <c r="F83" s="24"/>
+      <c r="G83" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H83" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I83" s="14"/>
+      <c r="J83" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="K83" s="16" t="s">
+      <c r="K83" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="L83" s="16" t="s">
+      <c r="L83" s="14" t="s">
         <v>120</v>
       </c>
       <c r="M83" t="s">
@@ -4371,18 +4371,18 @@
       </c>
     </row>
     <row r="84" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A84" s="15"/>
-      <c r="B84" s="16"/>
-      <c r="C84" s="15"/>
-      <c r="D84" s="20"/>
-      <c r="E84" s="21"/>
-      <c r="F84" s="21"/>
-      <c r="G84" s="16"/>
-      <c r="H84" s="16"/>
-      <c r="I84" s="16"/>
-      <c r="J84" s="16"/>
-      <c r="K84" s="16"/>
-      <c r="L84" s="16"/>
+      <c r="A84" s="18"/>
+      <c r="B84" s="14"/>
+      <c r="C84" s="18"/>
+      <c r="D84" s="22"/>
+      <c r="E84" s="24"/>
+      <c r="F84" s="24"/>
+      <c r="G84" s="14"/>
+      <c r="H84" s="14"/>
+      <c r="I84" s="14"/>
+      <c r="J84" s="14"/>
+      <c r="K84" s="14"/>
+      <c r="L84" s="14"/>
       <c r="M84" t="s">
         <v>212</v>
       </c>
@@ -4394,18 +4394,18 @@
       </c>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A85" s="15"/>
-      <c r="B85" s="16"/>
-      <c r="C85" s="15"/>
-      <c r="D85" s="20"/>
-      <c r="E85" s="21"/>
-      <c r="F85" s="21"/>
-      <c r="G85" s="16"/>
-      <c r="H85" s="16"/>
-      <c r="I85" s="16"/>
-      <c r="J85" s="16"/>
-      <c r="K85" s="16"/>
-      <c r="L85" s="16"/>
+      <c r="A85" s="18"/>
+      <c r="B85" s="14"/>
+      <c r="C85" s="18"/>
+      <c r="D85" s="22"/>
+      <c r="E85" s="24"/>
+      <c r="F85" s="24"/>
+      <c r="G85" s="14"/>
+      <c r="H85" s="14"/>
+      <c r="I85" s="14"/>
+      <c r="J85" s="14"/>
+      <c r="K85" s="14"/>
+      <c r="L85" s="14"/>
       <c r="M85" t="s">
         <v>214</v>
       </c>
@@ -4417,18 +4417,18 @@
       </c>
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A86" s="15"/>
-      <c r="B86" s="16"/>
-      <c r="C86" s="15"/>
-      <c r="D86" s="20"/>
-      <c r="E86" s="21"/>
-      <c r="F86" s="21"/>
-      <c r="G86" s="16"/>
-      <c r="H86" s="16"/>
-      <c r="I86" s="16"/>
-      <c r="J86" s="16"/>
-      <c r="K86" s="16"/>
-      <c r="L86" s="16"/>
+      <c r="A86" s="18"/>
+      <c r="B86" s="14"/>
+      <c r="C86" s="18"/>
+      <c r="D86" s="22"/>
+      <c r="E86" s="24"/>
+      <c r="F86" s="24"/>
+      <c r="G86" s="14"/>
+      <c r="H86" s="14"/>
+      <c r="I86" s="14"/>
+      <c r="J86" s="14"/>
+      <c r="K86" s="14"/>
+      <c r="L86" s="14"/>
       <c r="M86" t="s">
         <v>132</v>
       </c>
@@ -4440,18 +4440,18 @@
       </c>
     </row>
     <row r="87" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A87" s="15"/>
-      <c r="B87" s="16"/>
-      <c r="C87" s="15"/>
-      <c r="D87" s="20"/>
-      <c r="E87" s="21"/>
-      <c r="F87" s="21"/>
-      <c r="G87" s="16"/>
-      <c r="H87" s="16"/>
-      <c r="I87" s="16"/>
-      <c r="J87" s="16"/>
-      <c r="K87" s="16"/>
-      <c r="L87" s="16"/>
+      <c r="A87" s="18"/>
+      <c r="B87" s="14"/>
+      <c r="C87" s="18"/>
+      <c r="D87" s="22"/>
+      <c r="E87" s="24"/>
+      <c r="F87" s="24"/>
+      <c r="G87" s="14"/>
+      <c r="H87" s="14"/>
+      <c r="I87" s="14"/>
+      <c r="J87" s="14"/>
+      <c r="K87" s="14"/>
+      <c r="L87" s="14"/>
       <c r="M87" t="s">
         <v>133</v>
       </c>
@@ -4466,34 +4466,34 @@
       </c>
     </row>
     <row r="88" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B88" s="16" t="s">
+      <c r="A88" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B88" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="C88" s="15"/>
-      <c r="D88" s="20" t="s">
+      <c r="C88" s="18"/>
+      <c r="D88" s="22" t="s">
         <v>225</v>
       </c>
-      <c r="E88" s="21"/>
-      <c r="F88" s="21"/>
-      <c r="G88" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H88" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I88" s="16" t="s">
+      <c r="E88" s="24"/>
+      <c r="F88" s="24"/>
+      <c r="G88" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H88" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I88" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="J88" s="16" t="s">
+      <c r="J88" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="K88" s="16" t="s">
+      <c r="K88" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="L88" s="16" t="s">
+      <c r="L88" s="14" t="s">
         <v>120</v>
       </c>
       <c r="M88" t="s">
@@ -4510,18 +4510,18 @@
       </c>
     </row>
     <row r="89" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="16"/>
-      <c r="B89" s="16"/>
-      <c r="C89" s="15"/>
-      <c r="D89" s="20"/>
-      <c r="E89" s="21"/>
-      <c r="F89" s="21"/>
-      <c r="G89" s="16"/>
-      <c r="H89" s="16"/>
-      <c r="I89" s="16"/>
-      <c r="J89" s="16"/>
-      <c r="K89" s="16"/>
-      <c r="L89" s="16"/>
+      <c r="A89" s="14"/>
+      <c r="B89" s="14"/>
+      <c r="C89" s="18"/>
+      <c r="D89" s="22"/>
+      <c r="E89" s="24"/>
+      <c r="F89" s="24"/>
+      <c r="G89" s="14"/>
+      <c r="H89" s="14"/>
+      <c r="I89" s="14"/>
+      <c r="J89" s="14"/>
+      <c r="K89" s="14"/>
+      <c r="L89" s="14"/>
       <c r="M89" t="s">
         <v>47</v>
       </c>
@@ -4536,18 +4536,18 @@
       </c>
     </row>
     <row r="90" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="16"/>
-      <c r="B90" s="16"/>
-      <c r="C90" s="15"/>
-      <c r="D90" s="20"/>
-      <c r="E90" s="21"/>
-      <c r="F90" s="21"/>
-      <c r="G90" s="16"/>
-      <c r="H90" s="16"/>
-      <c r="I90" s="16"/>
-      <c r="J90" s="16"/>
-      <c r="K90" s="16"/>
-      <c r="L90" s="16"/>
+      <c r="A90" s="14"/>
+      <c r="B90" s="14"/>
+      <c r="C90" s="18"/>
+      <c r="D90" s="22"/>
+      <c r="E90" s="24"/>
+      <c r="F90" s="24"/>
+      <c r="G90" s="14"/>
+      <c r="H90" s="14"/>
+      <c r="I90" s="14"/>
+      <c r="J90" s="14"/>
+      <c r="K90" s="14"/>
+      <c r="L90" s="14"/>
       <c r="M90" t="s">
         <v>180</v>
       </c>
@@ -4562,18 +4562,18 @@
       </c>
     </row>
     <row r="91" spans="1:21" ht="75" x14ac:dyDescent="0.25">
-      <c r="A91" s="16"/>
-      <c r="B91" s="16"/>
-      <c r="C91" s="15"/>
-      <c r="D91" s="20"/>
-      <c r="E91" s="21"/>
-      <c r="F91" s="21"/>
-      <c r="G91" s="16"/>
-      <c r="H91" s="16"/>
-      <c r="I91" s="16"/>
-      <c r="J91" s="16"/>
-      <c r="K91" s="16"/>
-      <c r="L91" s="16"/>
+      <c r="A91" s="14"/>
+      <c r="B91" s="14"/>
+      <c r="C91" s="18"/>
+      <c r="D91" s="22"/>
+      <c r="E91" s="24"/>
+      <c r="F91" s="24"/>
+      <c r="G91" s="14"/>
+      <c r="H91" s="14"/>
+      <c r="I91" s="14"/>
+      <c r="J91" s="14"/>
+      <c r="K91" s="14"/>
+      <c r="L91" s="14"/>
       <c r="M91" t="s">
         <v>214</v>
       </c>
@@ -4588,18 +4588,18 @@
       </c>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A92" s="16"/>
-      <c r="B92" s="16"/>
-      <c r="C92" s="15"/>
-      <c r="D92" s="20"/>
-      <c r="E92" s="21"/>
-      <c r="F92" s="21"/>
-      <c r="G92" s="16"/>
-      <c r="H92" s="16"/>
-      <c r="I92" s="16"/>
-      <c r="J92" s="16"/>
-      <c r="K92" s="16"/>
-      <c r="L92" s="16"/>
+      <c r="A92" s="14"/>
+      <c r="B92" s="14"/>
+      <c r="C92" s="18"/>
+      <c r="D92" s="22"/>
+      <c r="E92" s="24"/>
+      <c r="F92" s="24"/>
+      <c r="G92" s="14"/>
+      <c r="H92" s="14"/>
+      <c r="I92" s="14"/>
+      <c r="J92" s="14"/>
+      <c r="K92" s="14"/>
+      <c r="L92" s="14"/>
       <c r="M92" t="s">
         <v>132</v>
       </c>
@@ -4611,18 +4611,18 @@
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A93" s="16"/>
-      <c r="B93" s="16"/>
-      <c r="C93" s="15"/>
-      <c r="D93" s="20"/>
-      <c r="E93" s="21"/>
-      <c r="F93" s="21"/>
-      <c r="G93" s="16"/>
-      <c r="H93" s="16"/>
-      <c r="I93" s="16"/>
-      <c r="J93" s="16"/>
-      <c r="K93" s="16"/>
-      <c r="L93" s="16"/>
+      <c r="A93" s="14"/>
+      <c r="B93" s="14"/>
+      <c r="C93" s="18"/>
+      <c r="D93" s="22"/>
+      <c r="E93" s="24"/>
+      <c r="F93" s="24"/>
+      <c r="G93" s="14"/>
+      <c r="H93" s="14"/>
+      <c r="I93" s="14"/>
+      <c r="J93" s="14"/>
+      <c r="K93" s="14"/>
+      <c r="L93" s="14"/>
       <c r="M93" t="s">
         <v>133</v>
       </c>
@@ -4634,34 +4634,34 @@
       </c>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A94" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B94" s="16" t="s">
+      <c r="A94" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B94" s="14" t="s">
         <v>233</v>
       </c>
-      <c r="C94" s="15"/>
-      <c r="D94" s="20" t="s">
+      <c r="C94" s="18"/>
+      <c r="D94" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="E94" s="21"/>
-      <c r="F94" s="21"/>
-      <c r="G94" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H94" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I94" s="16" t="s">
+      <c r="E94" s="24"/>
+      <c r="F94" s="24"/>
+      <c r="G94" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H94" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I94" s="14" t="s">
         <v>232</v>
       </c>
-      <c r="J94" s="16" t="s">
+      <c r="J94" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="K94" s="16" t="s">
+      <c r="K94" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="L94" s="16" t="s">
+      <c r="L94" s="14" t="s">
         <v>120</v>
       </c>
       <c r="M94" t="s">
@@ -4675,18 +4675,18 @@
       </c>
     </row>
     <row r="95" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A95" s="16"/>
-      <c r="B95" s="16"/>
-      <c r="C95" s="15"/>
-      <c r="D95" s="20"/>
-      <c r="E95" s="21"/>
-      <c r="F95" s="21"/>
-      <c r="G95" s="16"/>
-      <c r="H95" s="16"/>
-      <c r="I95" s="16"/>
-      <c r="J95" s="16"/>
-      <c r="K95" s="16"/>
-      <c r="L95" s="16"/>
+      <c r="A95" s="14"/>
+      <c r="B95" s="14"/>
+      <c r="C95" s="18"/>
+      <c r="D95" s="22"/>
+      <c r="E95" s="24"/>
+      <c r="F95" s="24"/>
+      <c r="G95" s="14"/>
+      <c r="H95" s="14"/>
+      <c r="I95" s="14"/>
+      <c r="J95" s="14"/>
+      <c r="K95" s="14"/>
+      <c r="L95" s="14"/>
       <c r="M95" t="s">
         <v>212</v>
       </c>
@@ -4701,18 +4701,18 @@
       </c>
     </row>
     <row r="96" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A96" s="16"/>
-      <c r="B96" s="16"/>
-      <c r="C96" s="15"/>
-      <c r="D96" s="20"/>
-      <c r="E96" s="21"/>
-      <c r="F96" s="21"/>
-      <c r="G96" s="16"/>
-      <c r="H96" s="16"/>
-      <c r="I96" s="16"/>
-      <c r="J96" s="16"/>
-      <c r="K96" s="16"/>
-      <c r="L96" s="16"/>
+      <c r="A96" s="14"/>
+      <c r="B96" s="14"/>
+      <c r="C96" s="18"/>
+      <c r="D96" s="22"/>
+      <c r="E96" s="24"/>
+      <c r="F96" s="24"/>
+      <c r="G96" s="14"/>
+      <c r="H96" s="14"/>
+      <c r="I96" s="14"/>
+      <c r="J96" s="14"/>
+      <c r="K96" s="14"/>
+      <c r="L96" s="14"/>
       <c r="M96" t="s">
         <v>212</v>
       </c>
@@ -4727,34 +4727,34 @@
       </c>
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A97" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B97" s="16" t="s">
+      <c r="A97" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B97" s="14" t="s">
         <v>239</v>
       </c>
-      <c r="C97" s="15"/>
-      <c r="D97" s="20" t="s">
+      <c r="C97" s="18"/>
+      <c r="D97" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="E97" s="21"/>
-      <c r="F97" s="21"/>
-      <c r="G97" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H97" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I97" s="16" t="s">
+      <c r="E97" s="24"/>
+      <c r="F97" s="24"/>
+      <c r="G97" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H97" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I97" s="14" t="s">
         <v>240</v>
       </c>
-      <c r="J97" s="16" t="s">
+      <c r="J97" s="14" t="s">
         <v>241</v>
       </c>
-      <c r="K97" s="16" t="s">
+      <c r="K97" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="L97" s="16" t="s">
+      <c r="L97" s="14" t="s">
         <v>120</v>
       </c>
       <c r="M97" t="s">
@@ -4768,18 +4768,18 @@
       </c>
     </row>
     <row r="98" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A98" s="16"/>
-      <c r="B98" s="16"/>
-      <c r="C98" s="15"/>
-      <c r="D98" s="20"/>
-      <c r="E98" s="21"/>
-      <c r="F98" s="21"/>
-      <c r="G98" s="16"/>
-      <c r="H98" s="16"/>
-      <c r="I98" s="16"/>
-      <c r="J98" s="16"/>
-      <c r="K98" s="16"/>
-      <c r="L98" s="16"/>
+      <c r="A98" s="14"/>
+      <c r="B98" s="14"/>
+      <c r="C98" s="18"/>
+      <c r="D98" s="22"/>
+      <c r="E98" s="24"/>
+      <c r="F98" s="24"/>
+      <c r="G98" s="14"/>
+      <c r="H98" s="14"/>
+      <c r="I98" s="14"/>
+      <c r="J98" s="14"/>
+      <c r="K98" s="14"/>
+      <c r="L98" s="14"/>
       <c r="M98" t="s">
         <v>212</v>
       </c>
@@ -4893,34 +4893,34 @@
       </c>
     </row>
     <row r="102" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A102" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B102" s="16" t="s">
+      <c r="A102" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B102" s="14" t="s">
         <v>250</v>
       </c>
-      <c r="C102" s="15"/>
-      <c r="D102" s="20" t="s">
+      <c r="C102" s="18"/>
+      <c r="D102" s="22" t="s">
         <v>254</v>
       </c>
-      <c r="E102" s="21"/>
-      <c r="F102" s="21"/>
-      <c r="G102" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H102" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I102" s="16" t="s">
+      <c r="E102" s="24"/>
+      <c r="F102" s="24"/>
+      <c r="G102" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H102" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I102" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="J102" s="16" t="s">
+      <c r="J102" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="K102" s="16" t="s">
+      <c r="K102" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="L102" s="16" t="s">
+      <c r="L102" s="14" t="s">
         <v>120</v>
       </c>
       <c r="M102" t="s">
@@ -4937,18 +4937,18 @@
       </c>
     </row>
     <row r="103" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A103" s="16"/>
-      <c r="B103" s="16"/>
-      <c r="C103" s="15"/>
-      <c r="D103" s="20"/>
-      <c r="E103" s="21"/>
-      <c r="F103" s="21"/>
-      <c r="G103" s="16"/>
-      <c r="H103" s="16"/>
-      <c r="I103" s="16"/>
-      <c r="J103" s="16"/>
-      <c r="K103" s="16"/>
-      <c r="L103" s="16"/>
+      <c r="A103" s="14"/>
+      <c r="B103" s="14"/>
+      <c r="C103" s="18"/>
+      <c r="D103" s="22"/>
+      <c r="E103" s="24"/>
+      <c r="F103" s="24"/>
+      <c r="G103" s="14"/>
+      <c r="H103" s="14"/>
+      <c r="I103" s="14"/>
+      <c r="J103" s="14"/>
+      <c r="K103" s="14"/>
+      <c r="L103" s="14"/>
       <c r="M103" t="s">
         <v>187</v>
       </c>
@@ -4963,18 +4963,18 @@
       </c>
     </row>
     <row r="104" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A104" s="16"/>
-      <c r="B104" s="16"/>
-      <c r="C104" s="15"/>
-      <c r="D104" s="20"/>
-      <c r="E104" s="21"/>
-      <c r="F104" s="21"/>
-      <c r="G104" s="16"/>
-      <c r="H104" s="16"/>
-      <c r="I104" s="16"/>
-      <c r="J104" s="16"/>
-      <c r="K104" s="16"/>
-      <c r="L104" s="16"/>
+      <c r="A104" s="14"/>
+      <c r="B104" s="14"/>
+      <c r="C104" s="18"/>
+      <c r="D104" s="22"/>
+      <c r="E104" s="24"/>
+      <c r="F104" s="24"/>
+      <c r="G104" s="14"/>
+      <c r="H104" s="14"/>
+      <c r="I104" s="14"/>
+      <c r="J104" s="14"/>
+      <c r="K104" s="14"/>
+      <c r="L104" s="14"/>
       <c r="M104" t="s">
         <v>212</v>
       </c>
@@ -4989,34 +4989,34 @@
       </c>
     </row>
     <row r="105" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A105" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B105" s="16" t="s">
+      <c r="A105" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B105" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="C105" s="15"/>
-      <c r="D105" s="20" t="s">
+      <c r="C105" s="18"/>
+      <c r="D105" s="22" t="s">
         <v>259</v>
       </c>
-      <c r="E105" s="21"/>
-      <c r="F105" s="21"/>
-      <c r="G105" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H105" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I105" s="16" t="s">
+      <c r="E105" s="24"/>
+      <c r="F105" s="24"/>
+      <c r="G105" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H105" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I105" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="J105" s="18" t="s">
+      <c r="J105" s="16" t="s">
         <v>265</v>
       </c>
-      <c r="K105" s="16" t="s">
+      <c r="K105" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="L105" s="16" t="s">
+      <c r="L105" s="14" t="s">
         <v>120</v>
       </c>
       <c r="M105" t="s">
@@ -5033,18 +5033,18 @@
       </c>
     </row>
     <row r="106" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A106" s="16"/>
-      <c r="B106" s="16"/>
-      <c r="C106" s="15"/>
-      <c r="D106" s="20"/>
-      <c r="E106" s="21"/>
-      <c r="F106" s="21"/>
-      <c r="G106" s="16"/>
-      <c r="H106" s="16"/>
-      <c r="I106" s="16"/>
-      <c r="J106" s="18"/>
-      <c r="K106" s="16"/>
-      <c r="L106" s="16"/>
+      <c r="A106" s="14"/>
+      <c r="B106" s="14"/>
+      <c r="C106" s="18"/>
+      <c r="D106" s="22"/>
+      <c r="E106" s="24"/>
+      <c r="F106" s="24"/>
+      <c r="G106" s="14"/>
+      <c r="H106" s="14"/>
+      <c r="I106" s="14"/>
+      <c r="J106" s="16"/>
+      <c r="K106" s="14"/>
+      <c r="L106" s="14"/>
       <c r="M106" t="s">
         <v>212</v>
       </c>
@@ -5059,18 +5059,18 @@
       </c>
     </row>
     <row r="107" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A107" s="16"/>
-      <c r="B107" s="16"/>
-      <c r="C107" s="15"/>
-      <c r="D107" s="20"/>
-      <c r="E107" s="21"/>
-      <c r="F107" s="21"/>
-      <c r="G107" s="16"/>
-      <c r="H107" s="16"/>
-      <c r="I107" s="16"/>
-      <c r="J107" s="18"/>
-      <c r="K107" s="16"/>
-      <c r="L107" s="16"/>
+      <c r="A107" s="14"/>
+      <c r="B107" s="14"/>
+      <c r="C107" s="18"/>
+      <c r="D107" s="22"/>
+      <c r="E107" s="24"/>
+      <c r="F107" s="24"/>
+      <c r="G107" s="14"/>
+      <c r="H107" s="14"/>
+      <c r="I107" s="14"/>
+      <c r="J107" s="16"/>
+      <c r="K107" s="14"/>
+      <c r="L107" s="14"/>
       <c r="M107" t="s">
         <v>212</v>
       </c>
@@ -5085,18 +5085,18 @@
       </c>
     </row>
     <row r="108" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A108" s="16"/>
-      <c r="B108" s="16"/>
-      <c r="C108" s="15"/>
-      <c r="D108" s="20"/>
-      <c r="E108" s="21"/>
-      <c r="F108" s="21"/>
-      <c r="G108" s="16"/>
-      <c r="H108" s="16"/>
-      <c r="I108" s="16"/>
-      <c r="J108" s="18"/>
-      <c r="K108" s="16"/>
-      <c r="L108" s="16"/>
+      <c r="A108" s="14"/>
+      <c r="B108" s="14"/>
+      <c r="C108" s="18"/>
+      <c r="D108" s="22"/>
+      <c r="E108" s="24"/>
+      <c r="F108" s="24"/>
+      <c r="G108" s="14"/>
+      <c r="H108" s="14"/>
+      <c r="I108" s="14"/>
+      <c r="J108" s="16"/>
+      <c r="K108" s="14"/>
+      <c r="L108" s="14"/>
       <c r="M108" t="s">
         <v>212</v>
       </c>
@@ -5149,32 +5149,32 @@
       </c>
     </row>
     <row r="110" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A110" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B110" s="16" t="s">
+      <c r="A110" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B110" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="C110" s="15"/>
-      <c r="D110" s="17" t="s">
+      <c r="C110" s="18"/>
+      <c r="D110" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="E110" s="19"/>
-      <c r="F110" s="19"/>
-      <c r="G110" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H110" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I110" s="16"/>
-      <c r="J110" s="18" t="s">
+      <c r="E110" s="17"/>
+      <c r="F110" s="17"/>
+      <c r="G110" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H110" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I110" s="14"/>
+      <c r="J110" s="16" t="s">
         <v>271</v>
       </c>
-      <c r="K110" s="16" t="s">
+      <c r="K110" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="L110" s="16" t="s">
+      <c r="L110" s="14" t="s">
         <v>120</v>
       </c>
       <c r="M110" t="s">
@@ -5191,18 +5191,18 @@
       </c>
     </row>
     <row r="111" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A111" s="16"/>
-      <c r="B111" s="16"/>
-      <c r="C111" s="15"/>
-      <c r="D111" s="17"/>
-      <c r="E111" s="19"/>
-      <c r="F111" s="19"/>
-      <c r="G111" s="16"/>
-      <c r="H111" s="16"/>
-      <c r="I111" s="16"/>
-      <c r="J111" s="18"/>
-      <c r="K111" s="16"/>
-      <c r="L111" s="16"/>
+      <c r="A111" s="14"/>
+      <c r="B111" s="14"/>
+      <c r="C111" s="18"/>
+      <c r="D111" s="15"/>
+      <c r="E111" s="17"/>
+      <c r="F111" s="17"/>
+      <c r="G111" s="14"/>
+      <c r="H111" s="14"/>
+      <c r="I111" s="14"/>
+      <c r="J111" s="16"/>
+      <c r="K111" s="14"/>
+      <c r="L111" s="14"/>
       <c r="M111" t="s">
         <v>212</v>
       </c>
@@ -5217,18 +5217,18 @@
       </c>
     </row>
     <row r="112" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A112" s="16"/>
-      <c r="B112" s="16"/>
-      <c r="C112" s="15"/>
-      <c r="D112" s="17"/>
-      <c r="E112" s="19"/>
-      <c r="F112" s="19"/>
-      <c r="G112" s="16"/>
-      <c r="H112" s="16"/>
-      <c r="I112" s="16"/>
-      <c r="J112" s="18"/>
-      <c r="K112" s="16"/>
-      <c r="L112" s="16"/>
+      <c r="A112" s="14"/>
+      <c r="B112" s="14"/>
+      <c r="C112" s="18"/>
+      <c r="D112" s="15"/>
+      <c r="E112" s="17"/>
+      <c r="F112" s="17"/>
+      <c r="G112" s="14"/>
+      <c r="H112" s="14"/>
+      <c r="I112" s="14"/>
+      <c r="J112" s="16"/>
+      <c r="K112" s="14"/>
+      <c r="L112" s="14"/>
       <c r="M112" t="s">
         <v>214</v>
       </c>
@@ -5243,32 +5243,32 @@
       </c>
     </row>
     <row r="113" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A113" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B113" s="16" t="s">
+      <c r="A113" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B113" s="14" t="s">
         <v>281</v>
       </c>
-      <c r="C113" s="15"/>
-      <c r="D113" s="17" t="s">
+      <c r="C113" s="18"/>
+      <c r="D113" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="E113" s="19"/>
-      <c r="F113" s="19"/>
-      <c r="G113" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H113" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I113" s="16"/>
-      <c r="J113" s="18" t="s">
+      <c r="E113" s="17"/>
+      <c r="F113" s="17"/>
+      <c r="G113" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H113" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I113" s="14"/>
+      <c r="J113" s="16" t="s">
         <v>286</v>
       </c>
-      <c r="K113" s="16" t="s">
+      <c r="K113" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="L113" s="16" t="s">
+      <c r="L113" s="14" t="s">
         <v>120</v>
       </c>
       <c r="M113" t="s">
@@ -5285,18 +5285,18 @@
       </c>
     </row>
     <row r="114" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A114" s="16"/>
-      <c r="B114" s="16"/>
-      <c r="C114" s="15"/>
-      <c r="D114" s="17"/>
-      <c r="E114" s="19"/>
-      <c r="F114" s="19"/>
-      <c r="G114" s="16"/>
-      <c r="H114" s="16"/>
-      <c r="I114" s="16"/>
-      <c r="J114" s="18"/>
-      <c r="K114" s="16"/>
-      <c r="L114" s="16"/>
+      <c r="A114" s="14"/>
+      <c r="B114" s="14"/>
+      <c r="C114" s="18"/>
+      <c r="D114" s="15"/>
+      <c r="E114" s="17"/>
+      <c r="F114" s="17"/>
+      <c r="G114" s="14"/>
+      <c r="H114" s="14"/>
+      <c r="I114" s="14"/>
+      <c r="J114" s="16"/>
+      <c r="K114" s="14"/>
+      <c r="L114" s="14"/>
       <c r="M114" t="s">
         <v>212</v>
       </c>
@@ -5311,18 +5311,18 @@
       </c>
     </row>
     <row r="115" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A115" s="16"/>
-      <c r="B115" s="16"/>
-      <c r="C115" s="15"/>
-      <c r="D115" s="17"/>
-      <c r="E115" s="19"/>
-      <c r="F115" s="19"/>
-      <c r="G115" s="16"/>
-      <c r="H115" s="16"/>
-      <c r="I115" s="16"/>
-      <c r="J115" s="18"/>
-      <c r="K115" s="16"/>
-      <c r="L115" s="16"/>
+      <c r="A115" s="14"/>
+      <c r="B115" s="14"/>
+      <c r="C115" s="18"/>
+      <c r="D115" s="15"/>
+      <c r="E115" s="17"/>
+      <c r="F115" s="17"/>
+      <c r="G115" s="14"/>
+      <c r="H115" s="14"/>
+      <c r="I115" s="14"/>
+      <c r="J115" s="16"/>
+      <c r="K115" s="14"/>
+      <c r="L115" s="14"/>
       <c r="M115" t="s">
         <v>214</v>
       </c>
@@ -5337,32 +5337,32 @@
       </c>
     </row>
     <row r="116" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A116" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B116" s="16" t="s">
+      <c r="A116" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B116" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="C116" s="15"/>
-      <c r="D116" s="17" t="s">
+      <c r="C116" s="18"/>
+      <c r="D116" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="E116" s="19"/>
-      <c r="F116" s="19"/>
-      <c r="G116" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H116" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I116" s="16"/>
-      <c r="J116" s="18" t="s">
+      <c r="E116" s="17"/>
+      <c r="F116" s="17"/>
+      <c r="G116" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H116" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I116" s="14"/>
+      <c r="J116" s="16" t="s">
         <v>285</v>
       </c>
-      <c r="K116" s="16" t="s">
+      <c r="K116" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="L116" s="16" t="s">
+      <c r="L116" s="14" t="s">
         <v>120</v>
       </c>
       <c r="M116" t="s">
@@ -5379,18 +5379,18 @@
       </c>
     </row>
     <row r="117" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A117" s="16"/>
-      <c r="B117" s="16"/>
-      <c r="C117" s="15"/>
-      <c r="D117" s="17"/>
-      <c r="E117" s="19"/>
-      <c r="F117" s="19"/>
-      <c r="G117" s="16"/>
-      <c r="H117" s="16"/>
-      <c r="I117" s="16"/>
-      <c r="J117" s="18"/>
-      <c r="K117" s="16"/>
-      <c r="L117" s="16"/>
+      <c r="A117" s="14"/>
+      <c r="B117" s="14"/>
+      <c r="C117" s="18"/>
+      <c r="D117" s="15"/>
+      <c r="E117" s="17"/>
+      <c r="F117" s="17"/>
+      <c r="G117" s="14"/>
+      <c r="H117" s="14"/>
+      <c r="I117" s="14"/>
+      <c r="J117" s="16"/>
+      <c r="K117" s="14"/>
+      <c r="L117" s="14"/>
       <c r="M117" t="s">
         <v>212</v>
       </c>
@@ -5405,18 +5405,18 @@
       </c>
     </row>
     <row r="118" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A118" s="16"/>
-      <c r="B118" s="16"/>
-      <c r="C118" s="15"/>
-      <c r="D118" s="17"/>
-      <c r="E118" s="19"/>
-      <c r="F118" s="19"/>
-      <c r="G118" s="16"/>
-      <c r="H118" s="16"/>
-      <c r="I118" s="16"/>
-      <c r="J118" s="18"/>
-      <c r="K118" s="16"/>
-      <c r="L118" s="16"/>
+      <c r="A118" s="14"/>
+      <c r="B118" s="14"/>
+      <c r="C118" s="18"/>
+      <c r="D118" s="15"/>
+      <c r="E118" s="17"/>
+      <c r="F118" s="17"/>
+      <c r="G118" s="14"/>
+      <c r="H118" s="14"/>
+      <c r="I118" s="14"/>
+      <c r="J118" s="16"/>
+      <c r="K118" s="14"/>
+      <c r="L118" s="14"/>
       <c r="M118" t="s">
         <v>214</v>
       </c>
@@ -5431,32 +5431,32 @@
       </c>
     </row>
     <row r="119" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A119" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B119" s="16" t="s">
+      <c r="A119" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B119" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="C119" s="15"/>
-      <c r="D119" s="17" t="s">
+      <c r="C119" s="18"/>
+      <c r="D119" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="E119" s="19"/>
-      <c r="F119" s="19"/>
-      <c r="G119" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H119" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I119" s="16"/>
-      <c r="J119" s="18" t="s">
+      <c r="E119" s="17"/>
+      <c r="F119" s="17"/>
+      <c r="G119" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H119" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I119" s="14"/>
+      <c r="J119" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="K119" s="16" t="s">
+      <c r="K119" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="L119" s="16" t="s">
+      <c r="L119" s="14" t="s">
         <v>120</v>
       </c>
       <c r="M119" t="s">
@@ -5473,18 +5473,18 @@
       </c>
     </row>
     <row r="120" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A120" s="16"/>
-      <c r="B120" s="16"/>
-      <c r="C120" s="15"/>
-      <c r="D120" s="17"/>
-      <c r="E120" s="19"/>
-      <c r="F120" s="19"/>
-      <c r="G120" s="16"/>
-      <c r="H120" s="16"/>
-      <c r="I120" s="16"/>
-      <c r="J120" s="18"/>
-      <c r="K120" s="16"/>
-      <c r="L120" s="16"/>
+      <c r="A120" s="14"/>
+      <c r="B120" s="14"/>
+      <c r="C120" s="18"/>
+      <c r="D120" s="15"/>
+      <c r="E120" s="17"/>
+      <c r="F120" s="17"/>
+      <c r="G120" s="14"/>
+      <c r="H120" s="14"/>
+      <c r="I120" s="14"/>
+      <c r="J120" s="16"/>
+      <c r="K120" s="14"/>
+      <c r="L120" s="14"/>
       <c r="M120" t="s">
         <v>212</v>
       </c>
@@ -5499,18 +5499,18 @@
       </c>
     </row>
     <row r="121" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A121" s="16"/>
-      <c r="B121" s="16"/>
-      <c r="C121" s="15"/>
-      <c r="D121" s="17"/>
-      <c r="E121" s="19"/>
-      <c r="F121" s="19"/>
-      <c r="G121" s="16"/>
-      <c r="H121" s="16"/>
-      <c r="I121" s="16"/>
-      <c r="J121" s="18"/>
-      <c r="K121" s="16"/>
-      <c r="L121" s="16"/>
+      <c r="A121" s="14"/>
+      <c r="B121" s="14"/>
+      <c r="C121" s="18"/>
+      <c r="D121" s="15"/>
+      <c r="E121" s="17"/>
+      <c r="F121" s="17"/>
+      <c r="G121" s="14"/>
+      <c r="H121" s="14"/>
+      <c r="I121" s="14"/>
+      <c r="J121" s="16"/>
+      <c r="K121" s="14"/>
+      <c r="L121" s="14"/>
       <c r="M121" t="s">
         <v>214</v>
       </c>
@@ -5527,18 +5527,246 @@
   </sheetData>
   <autoFilter ref="A1:U1"/>
   <mergeCells count="276">
-    <mergeCell ref="A119:A121"/>
-    <mergeCell ref="B119:B121"/>
-    <mergeCell ref="D119:D121"/>
-    <mergeCell ref="G119:G121"/>
-    <mergeCell ref="H119:H121"/>
-    <mergeCell ref="I119:I121"/>
-    <mergeCell ref="J119:J121"/>
-    <mergeCell ref="K119:K121"/>
-    <mergeCell ref="L119:L121"/>
-    <mergeCell ref="E119:E121"/>
-    <mergeCell ref="F119:F121"/>
-    <mergeCell ref="C119:C121"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="C64:C67"/>
+    <mergeCell ref="C68:C71"/>
+    <mergeCell ref="C72:C75"/>
+    <mergeCell ref="C78:C82"/>
+    <mergeCell ref="C83:C87"/>
+    <mergeCell ref="C88:C93"/>
+    <mergeCell ref="C94:C96"/>
+    <mergeCell ref="C97:C98"/>
+    <mergeCell ref="A110:A112"/>
+    <mergeCell ref="I110:I112"/>
+    <mergeCell ref="H110:H112"/>
+    <mergeCell ref="G110:G112"/>
+    <mergeCell ref="D110:D112"/>
+    <mergeCell ref="B110:B112"/>
+    <mergeCell ref="L110:L112"/>
+    <mergeCell ref="K110:K112"/>
+    <mergeCell ref="J110:J112"/>
+    <mergeCell ref="E110:E112"/>
+    <mergeCell ref="F110:F112"/>
+    <mergeCell ref="C110:C112"/>
+    <mergeCell ref="I105:I108"/>
+    <mergeCell ref="H105:H108"/>
+    <mergeCell ref="G105:G108"/>
+    <mergeCell ref="B105:B108"/>
+    <mergeCell ref="A105:A108"/>
+    <mergeCell ref="D105:D108"/>
+    <mergeCell ref="L105:L108"/>
+    <mergeCell ref="K105:K108"/>
+    <mergeCell ref="J105:J108"/>
+    <mergeCell ref="F105:F108"/>
+    <mergeCell ref="E105:E108"/>
+    <mergeCell ref="C105:C108"/>
+    <mergeCell ref="G97:G98"/>
+    <mergeCell ref="B97:B98"/>
+    <mergeCell ref="A97:A98"/>
+    <mergeCell ref="D97:D98"/>
+    <mergeCell ref="L102:L104"/>
+    <mergeCell ref="K102:K104"/>
+    <mergeCell ref="J102:J104"/>
+    <mergeCell ref="I102:I104"/>
+    <mergeCell ref="H102:H104"/>
+    <mergeCell ref="G102:G104"/>
+    <mergeCell ref="D102:D104"/>
+    <mergeCell ref="B102:B104"/>
+    <mergeCell ref="A102:A104"/>
+    <mergeCell ref="L97:L98"/>
+    <mergeCell ref="K97:K98"/>
+    <mergeCell ref="J97:J98"/>
+    <mergeCell ref="I97:I98"/>
+    <mergeCell ref="H97:H98"/>
+    <mergeCell ref="F97:F98"/>
+    <mergeCell ref="F102:F104"/>
+    <mergeCell ref="E97:E98"/>
+    <mergeCell ref="E102:E104"/>
+    <mergeCell ref="C102:C104"/>
+    <mergeCell ref="G94:G96"/>
+    <mergeCell ref="B94:B96"/>
+    <mergeCell ref="A94:A96"/>
+    <mergeCell ref="D94:D96"/>
+    <mergeCell ref="L94:L96"/>
+    <mergeCell ref="K94:K96"/>
+    <mergeCell ref="J94:J96"/>
+    <mergeCell ref="I94:I96"/>
+    <mergeCell ref="H94:H96"/>
+    <mergeCell ref="F94:F96"/>
+    <mergeCell ref="E94:E96"/>
+    <mergeCell ref="G83:G87"/>
+    <mergeCell ref="B83:B87"/>
+    <mergeCell ref="A83:A87"/>
+    <mergeCell ref="D83:D87"/>
+    <mergeCell ref="L88:L93"/>
+    <mergeCell ref="K88:K93"/>
+    <mergeCell ref="J88:J93"/>
+    <mergeCell ref="I88:I93"/>
+    <mergeCell ref="H88:H93"/>
+    <mergeCell ref="G88:G93"/>
+    <mergeCell ref="A88:A93"/>
+    <mergeCell ref="B88:B93"/>
+    <mergeCell ref="D88:D93"/>
+    <mergeCell ref="L83:L87"/>
+    <mergeCell ref="K83:K87"/>
+    <mergeCell ref="J83:J87"/>
+    <mergeCell ref="I83:I87"/>
+    <mergeCell ref="H83:H87"/>
+    <mergeCell ref="F83:F87"/>
+    <mergeCell ref="F88:F93"/>
+    <mergeCell ref="E83:E87"/>
+    <mergeCell ref="E88:E93"/>
+    <mergeCell ref="H78:H82"/>
+    <mergeCell ref="G78:G82"/>
+    <mergeCell ref="D78:D82"/>
+    <mergeCell ref="B78:B82"/>
+    <mergeCell ref="A78:A82"/>
+    <mergeCell ref="I72:I75"/>
+    <mergeCell ref="J72:J75"/>
+    <mergeCell ref="K72:K75"/>
+    <mergeCell ref="L72:L75"/>
+    <mergeCell ref="L78:L82"/>
+    <mergeCell ref="K78:K82"/>
+    <mergeCell ref="J78:J82"/>
+    <mergeCell ref="I78:I82"/>
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="D72:D75"/>
+    <mergeCell ref="G72:G75"/>
+    <mergeCell ref="H72:H75"/>
+    <mergeCell ref="F72:F75"/>
+    <mergeCell ref="F78:F82"/>
+    <mergeCell ref="E72:E75"/>
+    <mergeCell ref="E78:E82"/>
+    <mergeCell ref="H68:H71"/>
+    <mergeCell ref="I68:I71"/>
+    <mergeCell ref="J68:J71"/>
+    <mergeCell ref="K68:K71"/>
+    <mergeCell ref="L68:L71"/>
+    <mergeCell ref="G64:G67"/>
+    <mergeCell ref="B64:B67"/>
+    <mergeCell ref="A64:A67"/>
+    <mergeCell ref="D64:D67"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="D68:D71"/>
+    <mergeCell ref="G68:G71"/>
+    <mergeCell ref="L64:L67"/>
+    <mergeCell ref="K64:K67"/>
+    <mergeCell ref="J64:J67"/>
+    <mergeCell ref="I64:I67"/>
+    <mergeCell ref="H64:H67"/>
+    <mergeCell ref="F64:F67"/>
+    <mergeCell ref="F68:F71"/>
+    <mergeCell ref="E64:E67"/>
+    <mergeCell ref="E68:E71"/>
+    <mergeCell ref="F34:F36"/>
+    <mergeCell ref="F37:F39"/>
+    <mergeCell ref="H34:H36"/>
+    <mergeCell ref="H37:H39"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="I62:I63"/>
+    <mergeCell ref="J62:J63"/>
+    <mergeCell ref="K62:K63"/>
+    <mergeCell ref="L62:L63"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="G62:G63"/>
+    <mergeCell ref="H62:H63"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="G34:G36"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="G37:G39"/>
+    <mergeCell ref="D41:D47"/>
+    <mergeCell ref="D57:D59"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="D37:D39"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="L57:L59"/>
+    <mergeCell ref="K57:K59"/>
+    <mergeCell ref="J57:J59"/>
+    <mergeCell ref="I57:I59"/>
+    <mergeCell ref="H57:H59"/>
+    <mergeCell ref="H41:H47"/>
+    <mergeCell ref="G41:G47"/>
+    <mergeCell ref="B41:B47"/>
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="F41:F47"/>
+    <mergeCell ref="F57:F59"/>
+    <mergeCell ref="G57:G59"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="C41:C47"/>
+    <mergeCell ref="C57:C59"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="L41:L47"/>
+    <mergeCell ref="K41:K47"/>
+    <mergeCell ref="J41:J47"/>
+    <mergeCell ref="I41:I47"/>
+    <mergeCell ref="L28:L30"/>
+    <mergeCell ref="K28:K30"/>
+    <mergeCell ref="J28:J30"/>
+    <mergeCell ref="I28:I30"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="L24:L26"/>
+    <mergeCell ref="K24:K26"/>
+    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="K31:K33"/>
+    <mergeCell ref="L31:L33"/>
+    <mergeCell ref="I34:I36"/>
+    <mergeCell ref="J34:J36"/>
+    <mergeCell ref="K34:K36"/>
+    <mergeCell ref="L34:L36"/>
+    <mergeCell ref="I37:I39"/>
+    <mergeCell ref="J37:J39"/>
+    <mergeCell ref="K37:K39"/>
+    <mergeCell ref="L37:L39"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="H31:H33"/>
+    <mergeCell ref="I31:I33"/>
+    <mergeCell ref="J31:J33"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="E28:E30"/>
+    <mergeCell ref="E31:E33"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="F28:F30"/>
+    <mergeCell ref="F31:F33"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="G28:G30"/>
+    <mergeCell ref="H28:H30"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="G31:G33"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="E37:E39"/>
+    <mergeCell ref="E41:E47"/>
+    <mergeCell ref="E57:E59"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="C37:C39"/>
     <mergeCell ref="K113:K115"/>
     <mergeCell ref="L113:L115"/>
     <mergeCell ref="A116:A118"/>
@@ -5563,246 +5791,18 @@
     <mergeCell ref="J113:J115"/>
     <mergeCell ref="C113:C115"/>
     <mergeCell ref="C116:C118"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="E37:E39"/>
-    <mergeCell ref="E41:E47"/>
-    <mergeCell ref="E57:E59"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="C37:C39"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="H31:H33"/>
-    <mergeCell ref="I31:I33"/>
-    <mergeCell ref="J31:J33"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="E28:E30"/>
-    <mergeCell ref="E31:E33"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="F28:F30"/>
-    <mergeCell ref="F31:F33"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="G28:G30"/>
-    <mergeCell ref="H28:H30"/>
-    <mergeCell ref="G24:G26"/>
-    <mergeCell ref="G31:G33"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="L41:L47"/>
-    <mergeCell ref="K41:K47"/>
-    <mergeCell ref="J41:J47"/>
-    <mergeCell ref="I41:I47"/>
-    <mergeCell ref="L28:L30"/>
-    <mergeCell ref="K28:K30"/>
-    <mergeCell ref="J28:J30"/>
-    <mergeCell ref="I28:I30"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="L24:L26"/>
-    <mergeCell ref="K24:K26"/>
-    <mergeCell ref="J24:J26"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="K31:K33"/>
-    <mergeCell ref="L31:L33"/>
-    <mergeCell ref="I34:I36"/>
-    <mergeCell ref="J34:J36"/>
-    <mergeCell ref="K34:K36"/>
-    <mergeCell ref="L34:L36"/>
-    <mergeCell ref="I37:I39"/>
-    <mergeCell ref="J37:J39"/>
-    <mergeCell ref="K37:K39"/>
-    <mergeCell ref="L37:L39"/>
-    <mergeCell ref="L57:L59"/>
-    <mergeCell ref="K57:K59"/>
-    <mergeCell ref="J57:J59"/>
-    <mergeCell ref="I57:I59"/>
-    <mergeCell ref="H57:H59"/>
-    <mergeCell ref="H41:H47"/>
-    <mergeCell ref="G41:G47"/>
-    <mergeCell ref="B41:B47"/>
-    <mergeCell ref="A41:A47"/>
-    <mergeCell ref="F41:F47"/>
-    <mergeCell ref="F57:F59"/>
-    <mergeCell ref="G57:G59"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="C41:C47"/>
-    <mergeCell ref="C57:C59"/>
-    <mergeCell ref="F34:F36"/>
-    <mergeCell ref="F37:F39"/>
-    <mergeCell ref="H34:H36"/>
-    <mergeCell ref="H37:H39"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="I62:I63"/>
-    <mergeCell ref="J62:J63"/>
-    <mergeCell ref="K62:K63"/>
-    <mergeCell ref="L62:L63"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="G62:G63"/>
-    <mergeCell ref="H62:H63"/>
-    <mergeCell ref="F62:F63"/>
-    <mergeCell ref="G34:G36"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="G37:G39"/>
-    <mergeCell ref="D41:D47"/>
-    <mergeCell ref="D57:D59"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="D37:D39"/>
-    <mergeCell ref="E62:E63"/>
-    <mergeCell ref="H68:H71"/>
-    <mergeCell ref="I68:I71"/>
-    <mergeCell ref="J68:J71"/>
-    <mergeCell ref="K68:K71"/>
-    <mergeCell ref="L68:L71"/>
-    <mergeCell ref="G64:G67"/>
-    <mergeCell ref="B64:B67"/>
-    <mergeCell ref="A64:A67"/>
-    <mergeCell ref="D64:D67"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="D68:D71"/>
-    <mergeCell ref="G68:G71"/>
-    <mergeCell ref="L64:L67"/>
-    <mergeCell ref="K64:K67"/>
-    <mergeCell ref="J64:J67"/>
-    <mergeCell ref="I64:I67"/>
-    <mergeCell ref="H64:H67"/>
-    <mergeCell ref="F64:F67"/>
-    <mergeCell ref="F68:F71"/>
-    <mergeCell ref="E64:E67"/>
-    <mergeCell ref="E68:E71"/>
-    <mergeCell ref="H78:H82"/>
-    <mergeCell ref="G78:G82"/>
-    <mergeCell ref="D78:D82"/>
-    <mergeCell ref="B78:B82"/>
-    <mergeCell ref="A78:A82"/>
-    <mergeCell ref="I72:I75"/>
-    <mergeCell ref="J72:J75"/>
-    <mergeCell ref="K72:K75"/>
-    <mergeCell ref="L72:L75"/>
-    <mergeCell ref="L78:L82"/>
-    <mergeCell ref="K78:K82"/>
-    <mergeCell ref="J78:J82"/>
-    <mergeCell ref="I78:I82"/>
-    <mergeCell ref="A72:A75"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="D72:D75"/>
-    <mergeCell ref="G72:G75"/>
-    <mergeCell ref="H72:H75"/>
-    <mergeCell ref="F72:F75"/>
-    <mergeCell ref="F78:F82"/>
-    <mergeCell ref="E72:E75"/>
-    <mergeCell ref="E78:E82"/>
-    <mergeCell ref="G83:G87"/>
-    <mergeCell ref="B83:B87"/>
-    <mergeCell ref="A83:A87"/>
-    <mergeCell ref="D83:D87"/>
-    <mergeCell ref="L88:L93"/>
-    <mergeCell ref="K88:K93"/>
-    <mergeCell ref="J88:J93"/>
-    <mergeCell ref="I88:I93"/>
-    <mergeCell ref="H88:H93"/>
-    <mergeCell ref="G88:G93"/>
-    <mergeCell ref="A88:A93"/>
-    <mergeCell ref="B88:B93"/>
-    <mergeCell ref="D88:D93"/>
-    <mergeCell ref="L83:L87"/>
-    <mergeCell ref="K83:K87"/>
-    <mergeCell ref="J83:J87"/>
-    <mergeCell ref="I83:I87"/>
-    <mergeCell ref="H83:H87"/>
-    <mergeCell ref="F83:F87"/>
-    <mergeCell ref="F88:F93"/>
-    <mergeCell ref="E83:E87"/>
-    <mergeCell ref="E88:E93"/>
-    <mergeCell ref="G94:G96"/>
-    <mergeCell ref="B94:B96"/>
-    <mergeCell ref="A94:A96"/>
-    <mergeCell ref="D94:D96"/>
-    <mergeCell ref="L94:L96"/>
-    <mergeCell ref="K94:K96"/>
-    <mergeCell ref="J94:J96"/>
-    <mergeCell ref="I94:I96"/>
-    <mergeCell ref="H94:H96"/>
-    <mergeCell ref="F94:F96"/>
-    <mergeCell ref="E94:E96"/>
-    <mergeCell ref="G97:G98"/>
-    <mergeCell ref="B97:B98"/>
-    <mergeCell ref="A97:A98"/>
-    <mergeCell ref="D97:D98"/>
-    <mergeCell ref="L102:L104"/>
-    <mergeCell ref="K102:K104"/>
-    <mergeCell ref="J102:J104"/>
-    <mergeCell ref="I102:I104"/>
-    <mergeCell ref="H102:H104"/>
-    <mergeCell ref="G102:G104"/>
-    <mergeCell ref="D102:D104"/>
-    <mergeCell ref="B102:B104"/>
-    <mergeCell ref="A102:A104"/>
-    <mergeCell ref="L97:L98"/>
-    <mergeCell ref="K97:K98"/>
-    <mergeCell ref="J97:J98"/>
-    <mergeCell ref="I97:I98"/>
-    <mergeCell ref="H97:H98"/>
-    <mergeCell ref="F97:F98"/>
-    <mergeCell ref="F102:F104"/>
-    <mergeCell ref="E97:E98"/>
-    <mergeCell ref="E102:E104"/>
-    <mergeCell ref="C102:C104"/>
-    <mergeCell ref="I105:I108"/>
-    <mergeCell ref="H105:H108"/>
-    <mergeCell ref="G105:G108"/>
-    <mergeCell ref="B105:B108"/>
-    <mergeCell ref="A105:A108"/>
-    <mergeCell ref="D105:D108"/>
-    <mergeCell ref="L105:L108"/>
-    <mergeCell ref="K105:K108"/>
-    <mergeCell ref="J105:J108"/>
-    <mergeCell ref="F105:F108"/>
-    <mergeCell ref="E105:E108"/>
-    <mergeCell ref="C105:C108"/>
-    <mergeCell ref="A110:A112"/>
-    <mergeCell ref="I110:I112"/>
-    <mergeCell ref="H110:H112"/>
-    <mergeCell ref="G110:G112"/>
-    <mergeCell ref="D110:D112"/>
-    <mergeCell ref="B110:B112"/>
-    <mergeCell ref="L110:L112"/>
-    <mergeCell ref="K110:K112"/>
-    <mergeCell ref="J110:J112"/>
-    <mergeCell ref="E110:E112"/>
-    <mergeCell ref="F110:F112"/>
-    <mergeCell ref="C110:C112"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="C64:C67"/>
-    <mergeCell ref="C68:C71"/>
-    <mergeCell ref="C72:C75"/>
-    <mergeCell ref="C78:C82"/>
-    <mergeCell ref="C83:C87"/>
-    <mergeCell ref="C88:C93"/>
-    <mergeCell ref="C94:C96"/>
-    <mergeCell ref="C97:C98"/>
+    <mergeCell ref="A119:A121"/>
+    <mergeCell ref="B119:B121"/>
+    <mergeCell ref="D119:D121"/>
+    <mergeCell ref="G119:G121"/>
+    <mergeCell ref="H119:H121"/>
+    <mergeCell ref="I119:I121"/>
+    <mergeCell ref="J119:J121"/>
+    <mergeCell ref="K119:K121"/>
+    <mergeCell ref="L119:L121"/>
+    <mergeCell ref="E119:E121"/>
+    <mergeCell ref="F119:F121"/>
+    <mergeCell ref="C119:C121"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="P54" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Get Contract Available Services call to SOM API
git-tfs-id: [http://developmentvlan:8585/tfs/vanrise.collection]$/;C55395
</commit_message>
<xml_diff>
--- a/SOM/Documents/SOM/SOM APIs Mapping Sheet.xlsx
+++ b/SOM/Documents/SOM/SOM APIs Mapping Sheet.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Tables" sheetId="6" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'API Calls'!$A$1:$U$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'API Calls'!$A$1:$V$1</definedName>
   </definedNames>
   <calcPr calcId="152511" calcMode="manual"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="329">
   <si>
     <t>GetTechnicalDetails</t>
   </si>
@@ -1001,6 +1001,54 @@
   </si>
   <si>
     <t>Pending EDA</t>
+  </si>
+  <si>
+    <t>GetContractAvailableServices</t>
+  </si>
+  <si>
+    <t>Get</t>
+  </si>
+  <si>
+    <t>L2S3201</t>
+  </si>
+  <si>
+    <t>This call is used in the action of service addition for a telephony line. In the select services stage it returns all the services that are not sold yet for this customer on this contract.</t>
+  </si>
+  <si>
+    <t>http://192.168.110.185:8585/tfs/web/UI/Pages/WorkItems/WorkItemEdit.aspx?id=6621&amp;pguid=81f5a887-a9da-41fc-8c45-50b4cb40e1ea</t>
+  </si>
+  <si>
+    <t>http://94.130.97.86:8888/edit_bug.aspx?id=35</t>
+  </si>
+  <si>
+    <t>Technical Notes</t>
+  </si>
+  <si>
+    <t>ratePlanId
+contractId
+linePathId</t>
+  </si>
+  <si>
+    <t>This service should retreived the switch id from Line Path Id.
+Then Pass it to Get Rate Plan services for this call to filter them based on the switch.
+Then call contract Services Read Request in order to get the ids of the services that are already purchased
+Then filter the rate plan services by removing those that are sold.
+At the end call for each package the servicesReadRequest in order to get the name of the service in addtion to other needed fields.</t>
+  </si>
+  <si>
+    <t>MappingSheetResources\GetContractAvailableServices\GetContractAvailableServicesResponseMapping.txt</t>
+  </si>
+  <si>
+    <t>MappingSheetResources\GetContractAvailableServices\Technicallinedetailsbypathid.txt</t>
+  </si>
+  <si>
+    <t>MappingSheetResources\GetContractAvailableServices\GetRatePlanServices.txt</t>
+  </si>
+  <si>
+    <t>MappingSheetResources\GetContractAvailableServices\contractServicesReadRequest.txt</t>
+  </si>
+  <si>
+    <t>Lot of questions related to CRM and how to get subscription and access fees</t>
   </si>
 </sst>
 </file>
@@ -1123,7 +1171,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1155,6 +1203,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1167,25 +1221,22 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1653,11 +1704,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U121"/>
+  <dimension ref="A1:V124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T54" sqref="T54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A125" sqref="A125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1673,12 +1724,14 @@
     <col min="13" max="13" width="38" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="19" width="22.42578125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="19.85546875" style="12" customWidth="1"/>
-    <col min="21" max="21" width="36.7109375" style="1" customWidth="1"/>
+    <col min="16" max="17" width="22.42578125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="33.85546875" customWidth="1"/>
+    <col min="19" max="20" width="22.42578125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="19.85546875" style="12" customWidth="1"/>
+    <col min="22" max="22" width="36.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -1727,20 +1780,23 @@
       <c r="Q1" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" t="s">
+        <v>321</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="U1" s="12" t="s">
         <v>306</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>141</v>
       </c>
@@ -1772,7 +1828,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>141</v>
       </c>
@@ -1804,7 +1860,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>141</v>
       </c>
@@ -1836,7 +1892,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>141</v>
       </c>
@@ -1868,7 +1924,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>141</v>
       </c>
@@ -1900,7 +1956,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>141</v>
       </c>
@@ -1932,7 +1988,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>141</v>
       </c>
@@ -1964,7 +2020,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>141</v>
       </c>
@@ -1996,7 +2052,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>141</v>
       </c>
@@ -2028,7 +2084,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>141</v>
       </c>
@@ -2060,7 +2116,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>141</v>
       </c>
@@ -2092,7 +2148,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>141</v>
       </c>
@@ -2124,7 +2180,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>141</v>
       </c>
@@ -2156,7 +2212,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>141</v>
       </c>
@@ -2188,7 +2244,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>141</v>
       </c>
@@ -2220,7 +2276,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>141</v>
       </c>
@@ -2252,7 +2308,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>141</v>
       </c>
@@ -2284,7 +2340,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>141</v>
       </c>
@@ -2316,7 +2372,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>141</v>
       </c>
@@ -2348,7 +2404,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>141</v>
       </c>
@@ -2383,35 +2439,35 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B22" s="19" t="s">
+    <row r="22" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B22" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="15" t="s">
+      <c r="C22" s="14"/>
+      <c r="D22" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="H22" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="I22" s="19" t="s">
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="I22" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="J22" s="22" t="s">
+      <c r="J22" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="K22" s="21" t="s">
+      <c r="K22" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="L22" s="19" t="s">
+      <c r="L22" s="22" t="s">
         <v>120</v>
       </c>
       <c r="M22" t="s">
@@ -2423,23 +2479,23 @@
       <c r="O22" t="s">
         <v>67</v>
       </c>
-      <c r="U22" s="1" t="s">
+      <c r="V22" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="21"/>
-      <c r="L23" s="19"/>
+    <row r="23" spans="1:22" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="16"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="22"/>
       <c r="M23" t="s">
         <v>157</v>
       </c>
@@ -2449,36 +2505,36 @@
       <c r="O23" t="s">
         <v>27</v>
       </c>
-      <c r="U23" s="1" t="s">
+      <c r="V23" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B24" s="14" t="s">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B24" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="15" t="s">
+      <c r="C24" s="15"/>
+      <c r="D24" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I24" s="16" t="s">
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="J24" s="14" t="s">
+      <c r="J24" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="K24" s="14" t="s">
+      <c r="K24" s="16" t="s">
         <v>82</v>
       </c>
       <c r="L24" s="23" t="s">
@@ -2493,20 +2549,20 @@
       <c r="O24" t="s">
         <v>67</v>
       </c>
-      <c r="U24"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
+      <c r="V24"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
       <c r="L25" s="23"/>
       <c r="M25" t="s">
         <v>73</v>
@@ -2518,18 +2574,18 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
       <c r="L26" s="23"/>
       <c r="M26" t="s">
         <v>135</v>
@@ -2540,11 +2596,11 @@
       <c r="O26" t="s">
         <v>67</v>
       </c>
-      <c r="U26" s="1" t="s">
+      <c r="V26" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>141</v>
       </c>
@@ -2584,35 +2640,35 @@
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B28" s="14" t="s">
+    <row r="28" spans="1:22" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B28" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="15" t="s">
+      <c r="C28" s="15"/>
+      <c r="D28" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H28" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I28" s="14" t="s">
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I28" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="J28" s="16" t="s">
+      <c r="J28" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="K28" s="14" t="s">
+      <c r="K28" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L28" s="14" t="s">
+      <c r="L28" s="16" t="s">
         <v>119</v>
       </c>
       <c r="M28" t="s">
@@ -2624,23 +2680,23 @@
       <c r="O28" t="s">
         <v>67</v>
       </c>
-      <c r="U28" s="1" t="s">
+      <c r="V28" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29" s="16"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
       <c r="M29" t="s">
         <v>85</v>
       </c>
@@ -2651,19 +2707,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="16"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
+    <row r="30" spans="1:22" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="16"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
       <c r="M30" t="s">
         <v>90</v>
       </c>
@@ -2673,39 +2729,39 @@
       <c r="O30" t="s">
         <v>67</v>
       </c>
-      <c r="U30" s="1" t="s">
+      <c r="V30" s="1" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B31" s="14" t="s">
+    <row r="31" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B31" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="15" t="s">
+      <c r="C31" s="15"/>
+      <c r="D31" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H31" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I31" s="14" t="s">
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I31" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="J31" s="16" t="s">
+      <c r="J31" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="K31" s="14" t="s">
+      <c r="K31" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L31" s="14" t="s">
+      <c r="L31" s="16" t="s">
         <v>119</v>
       </c>
       <c r="M31" t="s">
@@ -2718,19 +2774,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="16"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
+    <row r="32" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="16"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="16"/>
       <c r="M32" t="s">
         <v>85</v>
       </c>
@@ -2741,19 +2797,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="16"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
+    <row r="33" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="16"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
       <c r="M33" t="s">
         <v>90</v>
       </c>
@@ -2763,39 +2819,39 @@
       <c r="O33" t="s">
         <v>67</v>
       </c>
-      <c r="U33" s="1" t="s">
+      <c r="V33" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B34" s="14" t="s">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B34" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="15" t="s">
+      <c r="C34" s="15"/>
+      <c r="D34" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H34" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I34" s="14" t="s">
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H34" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I34" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="J34" s="16" t="s">
+      <c r="J34" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="K34" s="14" t="s">
+      <c r="K34" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L34" s="14" t="s">
+      <c r="L34" s="16" t="s">
         <v>119</v>
       </c>
       <c r="M34" t="s">
@@ -2808,19 +2864,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="16"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A35" s="16"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
       <c r="M35" t="s">
         <v>85</v>
       </c>
@@ -2831,19 +2887,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="16"/>
-      <c r="K36" s="14"/>
-      <c r="L36" s="14"/>
+    <row r="36" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="16"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="16"/>
       <c r="M36" t="s">
         <v>90</v>
       </c>
@@ -2853,39 +2909,39 @@
       <c r="O36" t="s">
         <v>67</v>
       </c>
-      <c r="U36" s="1" t="s">
+      <c r="V36" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B37" s="14" t="s">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A37" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B37" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="15" t="s">
+      <c r="C37" s="15"/>
+      <c r="D37" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H37" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I37" s="14" t="s">
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H37" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I37" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="J37" s="16" t="s">
+      <c r="J37" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="K37" s="14" t="s">
+      <c r="K37" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L37" s="14" t="s">
+      <c r="L37" s="16" t="s">
         <v>119</v>
       </c>
       <c r="M37" t="s">
@@ -2898,19 +2954,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="16"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A38" s="16"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="16"/>
       <c r="M38" t="s">
         <v>85</v>
       </c>
@@ -2921,19 +2977,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="16"/>
-      <c r="K39" s="14"/>
-      <c r="L39" s="14"/>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A39" s="16"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="18"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="16"/>
       <c r="M39" t="s">
         <v>90</v>
       </c>
@@ -2944,7 +3000,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>141</v>
       </c>
@@ -2980,39 +3036,39 @@
       <c r="O40" t="s">
         <v>67</v>
       </c>
-      <c r="U40" s="1" t="s">
+      <c r="V40" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B41" s="14" t="s">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A41" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B41" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="C41" s="18"/>
-      <c r="D41" s="15" t="s">
+      <c r="C41" s="15"/>
+      <c r="D41" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H41" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I41" s="14" t="s">
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H41" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I41" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="J41" s="16" t="s">
+      <c r="J41" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="K41" s="14" t="s">
+      <c r="K41" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L41" s="14" t="s">
+      <c r="L41" s="16" t="s">
         <v>119</v>
       </c>
       <c r="M41" t="s">
@@ -3025,19 +3081,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="16"/>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A42" s="16"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="16"/>
+      <c r="J42" s="18"/>
+      <c r="K42" s="16"/>
+      <c r="L42" s="16"/>
       <c r="M42" t="s">
         <v>90</v>
       </c>
@@ -3048,19 +3104,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="17"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="16"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A43" s="16"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
+      <c r="J43" s="18"/>
+      <c r="K43" s="16"/>
+      <c r="L43" s="16"/>
       <c r="M43" t="s">
         <v>91</v>
       </c>
@@ -3070,21 +3126,21 @@
       <c r="O43" t="s">
         <v>67</v>
       </c>
-      <c r="U43"/>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
-      <c r="B44" s="14"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="16"/>
-      <c r="K44" s="14"/>
-      <c r="L44" s="14"/>
+      <c r="V43"/>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A44" s="16"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="16"/>
+      <c r="J44" s="18"/>
+      <c r="K44" s="16"/>
+      <c r="L44" s="16"/>
       <c r="M44" t="s">
         <v>93</v>
       </c>
@@ -3094,21 +3150,21 @@
       <c r="O44" t="s">
         <v>67</v>
       </c>
-      <c r="U44"/>
-    </row>
-    <row r="45" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="14"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="17"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
-      <c r="J45" s="16"/>
-      <c r="K45" s="14"/>
-      <c r="L45" s="14"/>
+      <c r="V44"/>
+    </row>
+    <row r="45" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="16"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
+      <c r="J45" s="18"/>
+      <c r="K45" s="16"/>
+      <c r="L45" s="16"/>
       <c r="M45" t="s">
         <v>81</v>
       </c>
@@ -3118,23 +3174,23 @@
       <c r="O45" t="s">
         <v>67</v>
       </c>
-      <c r="U45" s="1" t="s">
+      <c r="V45" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="16"/>
-      <c r="K46" s="14"/>
-      <c r="L46" s="14"/>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A46" s="16"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="16"/>
+      <c r="J46" s="18"/>
+      <c r="K46" s="16"/>
+      <c r="L46" s="16"/>
       <c r="M46" t="s">
         <v>126</v>
       </c>
@@ -3145,19 +3201,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
-      <c r="B47" s="14"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="14"/>
-      <c r="J47" s="16"/>
-      <c r="K47" s="14"/>
-      <c r="L47" s="14"/>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A47" s="16"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
+      <c r="J47" s="18"/>
+      <c r="K47" s="16"/>
+      <c r="L47" s="16"/>
       <c r="M47" t="s">
         <v>47</v>
       </c>
@@ -3168,7 +3224,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>141</v>
       </c>
@@ -3208,7 +3264,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>141</v>
       </c>
@@ -3248,7 +3304,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>141</v>
       </c>
@@ -3288,7 +3344,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>141</v>
       </c>
@@ -3327,11 +3383,11 @@
       <c r="O51" t="s">
         <v>67</v>
       </c>
-      <c r="U51" s="2" t="s">
+      <c r="V51" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>141</v>
       </c>
@@ -3368,9 +3424,9 @@
       <c r="O52" t="s">
         <v>67</v>
       </c>
-      <c r="U52"/>
-    </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V52"/>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>141</v>
       </c>
@@ -3405,7 +3461,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="90" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:22" ht="90" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
         <v>141</v>
       </c>
@@ -3454,20 +3510,20 @@
       <c r="Q54" s="10" t="s">
         <v>298</v>
       </c>
-      <c r="R54" s="10" t="s">
+      <c r="S54" s="10" t="s">
         <v>301</v>
       </c>
-      <c r="S54" s="10" t="s">
+      <c r="T54" s="10" t="s">
         <v>305</v>
       </c>
-      <c r="T54" s="12" t="s">
+      <c r="U54" s="12" t="s">
         <v>308</v>
       </c>
-      <c r="U54" s="1" t="s">
+      <c r="V54" s="1" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="55" spans="1:21" ht="105" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:22" ht="105" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>141</v>
       </c>
@@ -3501,11 +3557,11 @@
       <c r="O55" t="s">
         <v>67</v>
       </c>
-      <c r="U55" s="1" t="s">
+      <c r="V55" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>141</v>
       </c>
@@ -3540,30 +3596,30 @@
         <v>67</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A57" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B57" s="14" t="s">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A57" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B57" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="C57" s="18"/>
-      <c r="D57" s="16"/>
-      <c r="E57" s="20"/>
-      <c r="F57" s="20"/>
-      <c r="G57" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H57" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I57" s="14" t="s">
+      <c r="C57" s="15"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="24"/>
+      <c r="F57" s="24"/>
+      <c r="G57" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H57" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I57" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="J57" s="16" t="s">
+      <c r="J57" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="K57" s="14" t="s">
+      <c r="K57" s="16" t="s">
         <v>82</v>
       </c>
       <c r="L57" s="23" t="s">
@@ -3579,18 +3635,18 @@
         <v>67</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A58" s="14"/>
-      <c r="B58" s="14"/>
-      <c r="C58" s="18"/>
-      <c r="D58" s="16"/>
-      <c r="E58" s="20"/>
-      <c r="F58" s="20"/>
-      <c r="G58" s="14"/>
-      <c r="H58" s="14"/>
-      <c r="I58" s="14"/>
-      <c r="J58" s="16"/>
-      <c r="K58" s="14"/>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A58" s="16"/>
+      <c r="B58" s="16"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="16"/>
+      <c r="H58" s="16"/>
+      <c r="I58" s="16"/>
+      <c r="J58" s="18"/>
+      <c r="K58" s="16"/>
       <c r="L58" s="23"/>
       <c r="M58" t="s">
         <v>132</v>
@@ -3602,18 +3658,18 @@
         <v>67</v>
       </c>
     </row>
-    <row r="59" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A59" s="14"/>
-      <c r="B59" s="14"/>
-      <c r="C59" s="18"/>
-      <c r="D59" s="16"/>
-      <c r="E59" s="20"/>
-      <c r="F59" s="20"/>
-      <c r="G59" s="14"/>
-      <c r="H59" s="14"/>
-      <c r="I59" s="14"/>
-      <c r="J59" s="16"/>
-      <c r="K59" s="14"/>
+    <row r="59" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="16"/>
+      <c r="B59" s="16"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="24"/>
+      <c r="F59" s="24"/>
+      <c r="G59" s="16"/>
+      <c r="H59" s="16"/>
+      <c r="I59" s="16"/>
+      <c r="J59" s="18"/>
+      <c r="K59" s="16"/>
       <c r="L59" s="23"/>
       <c r="M59" t="s">
         <v>133</v>
@@ -3624,11 +3680,11 @@
       <c r="O59" t="s">
         <v>67</v>
       </c>
-      <c r="U59" s="2" t="s">
+      <c r="V59" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="60" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>141</v>
       </c>
@@ -3659,11 +3715,11 @@
       <c r="O60" t="s">
         <v>67</v>
       </c>
-      <c r="U60" s="1" t="s">
+      <c r="V60" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="61" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>141</v>
       </c>
@@ -3697,39 +3753,39 @@
       <c r="O61" t="s">
         <v>67</v>
       </c>
-      <c r="U61" s="1" t="s">
+      <c r="V61" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="62" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="B62" s="19" t="s">
+    <row r="62" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B62" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="C62" s="21"/>
-      <c r="D62" s="22" t="s">
+      <c r="C62" s="14"/>
+      <c r="D62" s="20" t="s">
         <v>200</v>
       </c>
-      <c r="E62" s="24"/>
-      <c r="F62" s="24"/>
-      <c r="G62" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="H62" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="I62" s="14" t="s">
+      <c r="E62" s="21"/>
+      <c r="F62" s="21"/>
+      <c r="G62" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H62" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="I62" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="J62" s="16" t="s">
+      <c r="J62" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="K62" s="14" t="s">
+      <c r="K62" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L62" s="14" t="s">
+      <c r="L62" s="16" t="s">
         <v>119</v>
       </c>
       <c r="M62" t="s">
@@ -3741,23 +3797,23 @@
       <c r="O62" t="s">
         <v>27</v>
       </c>
-      <c r="U62" s="1" t="s">
+      <c r="V62" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="63" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A63" s="19"/>
-      <c r="B63" s="19"/>
-      <c r="C63" s="21"/>
-      <c r="D63" s="22"/>
-      <c r="E63" s="24"/>
-      <c r="F63" s="24"/>
-      <c r="G63" s="19"/>
-      <c r="H63" s="19"/>
-      <c r="I63" s="14"/>
-      <c r="J63" s="16"/>
-      <c r="K63" s="14"/>
-      <c r="L63" s="14"/>
+    <row r="63" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A63" s="22"/>
+      <c r="B63" s="22"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="20"/>
+      <c r="E63" s="21"/>
+      <c r="F63" s="21"/>
+      <c r="G63" s="22"/>
+      <c r="H63" s="22"/>
+      <c r="I63" s="16"/>
+      <c r="J63" s="18"/>
+      <c r="K63" s="16"/>
+      <c r="L63" s="16"/>
       <c r="M63" t="s">
         <v>182</v>
       </c>
@@ -3767,39 +3823,39 @@
       <c r="O63" t="s">
         <v>67</v>
       </c>
-      <c r="U63" s="1" t="s">
+      <c r="V63" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="64" spans="1:21" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B64" s="14" t="s">
+    <row r="64" spans="1:22" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B64" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="C64" s="18"/>
-      <c r="D64" s="22" t="s">
+      <c r="C64" s="15"/>
+      <c r="D64" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="E64" s="24"/>
-      <c r="F64" s="24"/>
-      <c r="G64" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H64" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I64" s="14" t="s">
+      <c r="E64" s="21"/>
+      <c r="F64" s="21"/>
+      <c r="G64" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H64" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I64" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="J64" s="14" t="s">
+      <c r="J64" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="K64" s="14" t="s">
+      <c r="K64" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L64" s="14" t="s">
+      <c r="L64" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M64" t="s">
@@ -3811,23 +3867,23 @@
       <c r="O64" t="s">
         <v>67</v>
       </c>
-      <c r="U64" s="1" t="s">
+      <c r="V64" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="65" spans="1:21" ht="90" x14ac:dyDescent="0.25">
-      <c r="A65" s="14"/>
-      <c r="B65" s="14"/>
-      <c r="C65" s="18"/>
-      <c r="D65" s="22"/>
-      <c r="E65" s="24"/>
-      <c r="F65" s="24"/>
-      <c r="G65" s="14"/>
-      <c r="H65" s="14"/>
-      <c r="I65" s="14"/>
-      <c r="J65" s="14"/>
-      <c r="K65" s="14"/>
-      <c r="L65" s="14"/>
+    <row r="65" spans="1:22" ht="90" x14ac:dyDescent="0.25">
+      <c r="A65" s="16"/>
+      <c r="B65" s="16"/>
+      <c r="C65" s="15"/>
+      <c r="D65" s="20"/>
+      <c r="E65" s="21"/>
+      <c r="F65" s="21"/>
+      <c r="G65" s="16"/>
+      <c r="H65" s="16"/>
+      <c r="I65" s="16"/>
+      <c r="J65" s="16"/>
+      <c r="K65" s="16"/>
+      <c r="L65" s="16"/>
       <c r="M65" t="s">
         <v>187</v>
       </c>
@@ -3837,23 +3893,23 @@
       <c r="O65" t="s">
         <v>67</v>
       </c>
-      <c r="U65" s="1" t="s">
+      <c r="V65" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A66" s="14"/>
-      <c r="B66" s="14"/>
-      <c r="C66" s="18"/>
-      <c r="D66" s="22"/>
-      <c r="E66" s="24"/>
-      <c r="F66" s="24"/>
-      <c r="G66" s="14"/>
-      <c r="H66" s="14"/>
-      <c r="I66" s="14"/>
-      <c r="J66" s="14"/>
-      <c r="K66" s="14"/>
-      <c r="L66" s="14"/>
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A66" s="16"/>
+      <c r="B66" s="16"/>
+      <c r="C66" s="15"/>
+      <c r="D66" s="20"/>
+      <c r="E66" s="21"/>
+      <c r="F66" s="21"/>
+      <c r="G66" s="16"/>
+      <c r="H66" s="16"/>
+      <c r="I66" s="16"/>
+      <c r="J66" s="16"/>
+      <c r="K66" s="16"/>
+      <c r="L66" s="16"/>
       <c r="M66" t="s">
         <v>190</v>
       </c>
@@ -3864,19 +3920,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A67" s="14"/>
-      <c r="B67" s="14"/>
-      <c r="C67" s="18"/>
-      <c r="D67" s="22"/>
-      <c r="E67" s="24"/>
-      <c r="F67" s="24"/>
-      <c r="G67" s="14"/>
-      <c r="H67" s="14"/>
-      <c r="I67" s="14"/>
-      <c r="J67" s="14"/>
-      <c r="K67" s="14"/>
-      <c r="L67" s="14"/>
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A67" s="16"/>
+      <c r="B67" s="16"/>
+      <c r="C67" s="15"/>
+      <c r="D67" s="20"/>
+      <c r="E67" s="21"/>
+      <c r="F67" s="21"/>
+      <c r="G67" s="16"/>
+      <c r="H67" s="16"/>
+      <c r="I67" s="16"/>
+      <c r="J67" s="16"/>
+      <c r="K67" s="16"/>
+      <c r="L67" s="16"/>
       <c r="M67" t="s">
         <v>191</v>
       </c>
@@ -3887,35 +3943,35 @@
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B68" s="14" t="s">
+    <row r="68" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B68" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="C68" s="18"/>
-      <c r="D68" s="22" t="s">
+      <c r="C68" s="15"/>
+      <c r="D68" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="E68" s="24"/>
-      <c r="F68" s="24"/>
-      <c r="G68" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H68" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I68" s="14" t="s">
+      <c r="E68" s="21"/>
+      <c r="F68" s="21"/>
+      <c r="G68" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H68" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I68" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="J68" s="14" t="s">
+      <c r="J68" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="K68" s="14" t="s">
+      <c r="K68" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L68" s="14" t="s">
+      <c r="L68" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M68" t="s">
@@ -3927,23 +3983,23 @@
       <c r="O68" t="s">
         <v>67</v>
       </c>
-      <c r="U68" s="1" t="s">
+      <c r="V68" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A69" s="14"/>
-      <c r="B69" s="14"/>
-      <c r="C69" s="18"/>
-      <c r="D69" s="22"/>
-      <c r="E69" s="24"/>
-      <c r="F69" s="24"/>
-      <c r="G69" s="14"/>
-      <c r="H69" s="14"/>
-      <c r="I69" s="14"/>
-      <c r="J69" s="14"/>
-      <c r="K69" s="14"/>
-      <c r="L69" s="14"/>
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A69" s="16"/>
+      <c r="B69" s="16"/>
+      <c r="C69" s="15"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="21"/>
+      <c r="F69" s="21"/>
+      <c r="G69" s="16"/>
+      <c r="H69" s="16"/>
+      <c r="I69" s="16"/>
+      <c r="J69" s="16"/>
+      <c r="K69" s="16"/>
+      <c r="L69" s="16"/>
       <c r="M69" t="s">
         <v>187</v>
       </c>
@@ -3954,19 +4010,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A70" s="14"/>
-      <c r="B70" s="14"/>
-      <c r="C70" s="18"/>
-      <c r="D70" s="22"/>
-      <c r="E70" s="24"/>
-      <c r="F70" s="24"/>
-      <c r="G70" s="14"/>
-      <c r="H70" s="14"/>
-      <c r="I70" s="14"/>
-      <c r="J70" s="14"/>
-      <c r="K70" s="14"/>
-      <c r="L70" s="14"/>
+    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A70" s="16"/>
+      <c r="B70" s="16"/>
+      <c r="C70" s="15"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="21"/>
+      <c r="F70" s="21"/>
+      <c r="G70" s="16"/>
+      <c r="H70" s="16"/>
+      <c r="I70" s="16"/>
+      <c r="J70" s="16"/>
+      <c r="K70" s="16"/>
+      <c r="L70" s="16"/>
       <c r="M70" t="s">
         <v>190</v>
       </c>
@@ -3977,19 +4033,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A71" s="14"/>
-      <c r="B71" s="14"/>
-      <c r="C71" s="18"/>
-      <c r="D71" s="22"/>
-      <c r="E71" s="24"/>
-      <c r="F71" s="24"/>
-      <c r="G71" s="14"/>
-      <c r="H71" s="14"/>
-      <c r="I71" s="14"/>
-      <c r="J71" s="14"/>
-      <c r="K71" s="14"/>
-      <c r="L71" s="14"/>
+    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A71" s="16"/>
+      <c r="B71" s="16"/>
+      <c r="C71" s="15"/>
+      <c r="D71" s="20"/>
+      <c r="E71" s="21"/>
+      <c r="F71" s="21"/>
+      <c r="G71" s="16"/>
+      <c r="H71" s="16"/>
+      <c r="I71" s="16"/>
+      <c r="J71" s="16"/>
+      <c r="K71" s="16"/>
+      <c r="L71" s="16"/>
       <c r="M71" t="s">
         <v>191</v>
       </c>
@@ -4000,35 +4056,35 @@
         <v>67</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A72" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B72" s="14" t="s">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A72" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B72" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="C72" s="18"/>
-      <c r="D72" s="22" t="s">
+      <c r="C72" s="15"/>
+      <c r="D72" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="E72" s="24"/>
-      <c r="F72" s="24"/>
-      <c r="G72" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H72" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I72" s="14" t="s">
+      <c r="E72" s="21"/>
+      <c r="F72" s="21"/>
+      <c r="G72" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H72" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I72" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="J72" s="14" t="s">
+      <c r="J72" s="16" t="s">
         <v>198</v>
       </c>
-      <c r="K72" s="14" t="s">
+      <c r="K72" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L72" s="14" t="s">
+      <c r="L72" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M72" t="s">
@@ -4041,19 +4097,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A73" s="14"/>
-      <c r="B73" s="14"/>
-      <c r="C73" s="18"/>
-      <c r="D73" s="22"/>
-      <c r="E73" s="24"/>
-      <c r="F73" s="24"/>
-      <c r="G73" s="14"/>
-      <c r="H73" s="14"/>
-      <c r="I73" s="14"/>
-      <c r="J73" s="14"/>
-      <c r="K73" s="14"/>
-      <c r="L73" s="14"/>
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A73" s="16"/>
+      <c r="B73" s="16"/>
+      <c r="C73" s="15"/>
+      <c r="D73" s="20"/>
+      <c r="E73" s="21"/>
+      <c r="F73" s="21"/>
+      <c r="G73" s="16"/>
+      <c r="H73" s="16"/>
+      <c r="I73" s="16"/>
+      <c r="J73" s="16"/>
+      <c r="K73" s="16"/>
+      <c r="L73" s="16"/>
       <c r="M73" t="s">
         <v>187</v>
       </c>
@@ -4064,19 +4120,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A74" s="14"/>
-      <c r="B74" s="14"/>
-      <c r="C74" s="18"/>
-      <c r="D74" s="22"/>
-      <c r="E74" s="24"/>
-      <c r="F74" s="24"/>
-      <c r="G74" s="14"/>
-      <c r="H74" s="14"/>
-      <c r="I74" s="14"/>
-      <c r="J74" s="14"/>
-      <c r="K74" s="14"/>
-      <c r="L74" s="14"/>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A74" s="16"/>
+      <c r="B74" s="16"/>
+      <c r="C74" s="15"/>
+      <c r="D74" s="20"/>
+      <c r="E74" s="21"/>
+      <c r="F74" s="21"/>
+      <c r="G74" s="16"/>
+      <c r="H74" s="16"/>
+      <c r="I74" s="16"/>
+      <c r="J74" s="16"/>
+      <c r="K74" s="16"/>
+      <c r="L74" s="16"/>
       <c r="M74" t="s">
         <v>190</v>
       </c>
@@ -4087,19 +4143,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A75" s="14"/>
-      <c r="B75" s="14"/>
-      <c r="C75" s="18"/>
-      <c r="D75" s="22"/>
-      <c r="E75" s="24"/>
-      <c r="F75" s="24"/>
-      <c r="G75" s="14"/>
-      <c r="H75" s="14"/>
-      <c r="I75" s="14"/>
-      <c r="J75" s="14"/>
-      <c r="K75" s="14"/>
-      <c r="L75" s="14"/>
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A75" s="16"/>
+      <c r="B75" s="16"/>
+      <c r="C75" s="15"/>
+      <c r="D75" s="20"/>
+      <c r="E75" s="21"/>
+      <c r="F75" s="21"/>
+      <c r="G75" s="16"/>
+      <c r="H75" s="16"/>
+      <c r="I75" s="16"/>
+      <c r="J75" s="16"/>
+      <c r="K75" s="16"/>
+      <c r="L75" s="16"/>
       <c r="M75" t="s">
         <v>191</v>
       </c>
@@ -4110,7 +4166,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="76" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>141</v>
       </c>
@@ -4144,11 +4200,11 @@
       <c r="O76" t="s">
         <v>67</v>
       </c>
-      <c r="U76" s="1" t="s">
+      <c r="V76" s="1" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="77" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>141</v>
       </c>
@@ -4182,39 +4238,39 @@
       <c r="O77" t="s">
         <v>67</v>
       </c>
-      <c r="U77" s="1" t="s">
+      <c r="V77" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="78" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B78" s="14" t="s">
+    <row r="78" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B78" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="C78" s="18"/>
-      <c r="D78" s="22" t="s">
+      <c r="C78" s="15"/>
+      <c r="D78" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="E78" s="24"/>
-      <c r="F78" s="24"/>
-      <c r="G78" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H78" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I78" s="14" t="s">
+      <c r="E78" s="21"/>
+      <c r="F78" s="21"/>
+      <c r="G78" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H78" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I78" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="J78" s="14" t="s">
+      <c r="J78" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="K78" s="14" t="s">
+      <c r="K78" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L78" s="14" t="s">
+      <c r="L78" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M78" t="s">
@@ -4226,23 +4282,23 @@
       <c r="O78" t="s">
         <v>27</v>
       </c>
-      <c r="U78" s="1" t="s">
+      <c r="V78" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="79" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A79" s="14"/>
-      <c r="B79" s="14"/>
-      <c r="C79" s="18"/>
-      <c r="D79" s="22"/>
-      <c r="E79" s="24"/>
-      <c r="F79" s="24"/>
-      <c r="G79" s="14"/>
-      <c r="H79" s="14"/>
-      <c r="I79" s="14"/>
-      <c r="J79" s="14"/>
-      <c r="K79" s="14"/>
-      <c r="L79" s="14"/>
+    <row r="79" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A79" s="16"/>
+      <c r="B79" s="16"/>
+      <c r="C79" s="15"/>
+      <c r="D79" s="20"/>
+      <c r="E79" s="21"/>
+      <c r="F79" s="21"/>
+      <c r="G79" s="16"/>
+      <c r="H79" s="16"/>
+      <c r="I79" s="16"/>
+      <c r="J79" s="16"/>
+      <c r="K79" s="16"/>
+      <c r="L79" s="16"/>
       <c r="M79" t="s">
         <v>212</v>
       </c>
@@ -4252,23 +4308,23 @@
       <c r="O79" t="s">
         <v>212</v>
       </c>
-      <c r="U79" s="1" t="s">
+      <c r="V79" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="80" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="14"/>
-      <c r="B80" s="14"/>
-      <c r="C80" s="18"/>
-      <c r="D80" s="22"/>
-      <c r="E80" s="24"/>
-      <c r="F80" s="24"/>
-      <c r="G80" s="14"/>
-      <c r="H80" s="14"/>
-      <c r="I80" s="14"/>
-      <c r="J80" s="14"/>
-      <c r="K80" s="14"/>
-      <c r="L80" s="14"/>
+    <row r="80" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="16"/>
+      <c r="B80" s="16"/>
+      <c r="C80" s="15"/>
+      <c r="D80" s="20"/>
+      <c r="E80" s="21"/>
+      <c r="F80" s="21"/>
+      <c r="G80" s="16"/>
+      <c r="H80" s="16"/>
+      <c r="I80" s="16"/>
+      <c r="J80" s="16"/>
+      <c r="K80" s="16"/>
+      <c r="L80" s="16"/>
       <c r="M80" t="s">
         <v>214</v>
       </c>
@@ -4278,23 +4334,23 @@
       <c r="O80" t="s">
         <v>27</v>
       </c>
-      <c r="U80" s="1" t="s">
+      <c r="V80" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="81" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A81" s="14"/>
-      <c r="B81" s="14"/>
-      <c r="C81" s="18"/>
-      <c r="D81" s="22"/>
-      <c r="E81" s="24"/>
-      <c r="F81" s="24"/>
-      <c r="G81" s="14"/>
-      <c r="H81" s="14"/>
-      <c r="I81" s="14"/>
-      <c r="J81" s="14"/>
-      <c r="K81" s="14"/>
-      <c r="L81" s="14"/>
+    <row r="81" spans="1:22" ht="60" x14ac:dyDescent="0.25">
+      <c r="A81" s="16"/>
+      <c r="B81" s="16"/>
+      <c r="C81" s="15"/>
+      <c r="D81" s="20"/>
+      <c r="E81" s="21"/>
+      <c r="F81" s="21"/>
+      <c r="G81" s="16"/>
+      <c r="H81" s="16"/>
+      <c r="I81" s="16"/>
+      <c r="J81" s="16"/>
+      <c r="K81" s="16"/>
+      <c r="L81" s="16"/>
       <c r="M81" t="s">
         <v>132</v>
       </c>
@@ -4304,23 +4360,23 @@
       <c r="O81" t="s">
         <v>67</v>
       </c>
-      <c r="U81" s="1" t="s">
+      <c r="V81" s="1" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A82" s="14"/>
-      <c r="B82" s="14"/>
-      <c r="C82" s="18"/>
-      <c r="D82" s="22"/>
-      <c r="E82" s="24"/>
-      <c r="F82" s="24"/>
-      <c r="G82" s="14"/>
-      <c r="H82" s="14"/>
-      <c r="I82" s="14"/>
-      <c r="J82" s="14"/>
-      <c r="K82" s="14"/>
-      <c r="L82" s="14"/>
+    <row r="82" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A82" s="16"/>
+      <c r="B82" s="16"/>
+      <c r="C82" s="15"/>
+      <c r="D82" s="20"/>
+      <c r="E82" s="21"/>
+      <c r="F82" s="21"/>
+      <c r="G82" s="16"/>
+      <c r="H82" s="16"/>
+      <c r="I82" s="16"/>
+      <c r="J82" s="16"/>
+      <c r="K82" s="16"/>
+      <c r="L82" s="16"/>
       <c r="M82" t="s">
         <v>133</v>
       </c>
@@ -4331,33 +4387,33 @@
         <v>67</v>
       </c>
     </row>
-    <row r="83" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="B83" s="14" t="s">
+    <row r="83" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B83" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="C83" s="18"/>
-      <c r="D83" s="22" t="s">
+      <c r="C83" s="15"/>
+      <c r="D83" s="20" t="s">
         <v>221</v>
       </c>
-      <c r="E83" s="24"/>
-      <c r="F83" s="24"/>
-      <c r="G83" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H83" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I83" s="14"/>
-      <c r="J83" s="14" t="s">
+      <c r="E83" s="21"/>
+      <c r="F83" s="21"/>
+      <c r="G83" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H83" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I83" s="16"/>
+      <c r="J83" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="K83" s="14" t="s">
+      <c r="K83" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L83" s="14" t="s">
+      <c r="L83" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M83" t="s">
@@ -4370,19 +4426,19 @@
         <v>27</v>
       </c>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A84" s="18"/>
-      <c r="B84" s="14"/>
-      <c r="C84" s="18"/>
-      <c r="D84" s="22"/>
-      <c r="E84" s="24"/>
-      <c r="F84" s="24"/>
-      <c r="G84" s="14"/>
-      <c r="H84" s="14"/>
-      <c r="I84" s="14"/>
-      <c r="J84" s="14"/>
-      <c r="K84" s="14"/>
-      <c r="L84" s="14"/>
+    <row r="84" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A84" s="15"/>
+      <c r="B84" s="16"/>
+      <c r="C84" s="15"/>
+      <c r="D84" s="20"/>
+      <c r="E84" s="21"/>
+      <c r="F84" s="21"/>
+      <c r="G84" s="16"/>
+      <c r="H84" s="16"/>
+      <c r="I84" s="16"/>
+      <c r="J84" s="16"/>
+      <c r="K84" s="16"/>
+      <c r="L84" s="16"/>
       <c r="M84" t="s">
         <v>212</v>
       </c>
@@ -4393,19 +4449,19 @@
         <v>212</v>
       </c>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A85" s="18"/>
-      <c r="B85" s="14"/>
-      <c r="C85" s="18"/>
-      <c r="D85" s="22"/>
-      <c r="E85" s="24"/>
-      <c r="F85" s="24"/>
-      <c r="G85" s="14"/>
-      <c r="H85" s="14"/>
-      <c r="I85" s="14"/>
-      <c r="J85" s="14"/>
-      <c r="K85" s="14"/>
-      <c r="L85" s="14"/>
+    <row r="85" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A85" s="15"/>
+      <c r="B85" s="16"/>
+      <c r="C85" s="15"/>
+      <c r="D85" s="20"/>
+      <c r="E85" s="21"/>
+      <c r="F85" s="21"/>
+      <c r="G85" s="16"/>
+      <c r="H85" s="16"/>
+      <c r="I85" s="16"/>
+      <c r="J85" s="16"/>
+      <c r="K85" s="16"/>
+      <c r="L85" s="16"/>
       <c r="M85" t="s">
         <v>214</v>
       </c>
@@ -4416,19 +4472,19 @@
         <v>27</v>
       </c>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A86" s="18"/>
-      <c r="B86" s="14"/>
-      <c r="C86" s="18"/>
-      <c r="D86" s="22"/>
-      <c r="E86" s="24"/>
-      <c r="F86" s="24"/>
-      <c r="G86" s="14"/>
-      <c r="H86" s="14"/>
-      <c r="I86" s="14"/>
-      <c r="J86" s="14"/>
-      <c r="K86" s="14"/>
-      <c r="L86" s="14"/>
+    <row r="86" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A86" s="15"/>
+      <c r="B86" s="16"/>
+      <c r="C86" s="15"/>
+      <c r="D86" s="20"/>
+      <c r="E86" s="21"/>
+      <c r="F86" s="21"/>
+      <c r="G86" s="16"/>
+      <c r="H86" s="16"/>
+      <c r="I86" s="16"/>
+      <c r="J86" s="16"/>
+      <c r="K86" s="16"/>
+      <c r="L86" s="16"/>
       <c r="M86" t="s">
         <v>132</v>
       </c>
@@ -4439,19 +4495,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="87" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A87" s="18"/>
-      <c r="B87" s="14"/>
-      <c r="C87" s="18"/>
-      <c r="D87" s="22"/>
-      <c r="E87" s="24"/>
-      <c r="F87" s="24"/>
-      <c r="G87" s="14"/>
-      <c r="H87" s="14"/>
-      <c r="I87" s="14"/>
-      <c r="J87" s="14"/>
-      <c r="K87" s="14"/>
-      <c r="L87" s="14"/>
+    <row r="87" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A87" s="15"/>
+      <c r="B87" s="16"/>
+      <c r="C87" s="15"/>
+      <c r="D87" s="20"/>
+      <c r="E87" s="21"/>
+      <c r="F87" s="21"/>
+      <c r="G87" s="16"/>
+      <c r="H87" s="16"/>
+      <c r="I87" s="16"/>
+      <c r="J87" s="16"/>
+      <c r="K87" s="16"/>
+      <c r="L87" s="16"/>
       <c r="M87" t="s">
         <v>133</v>
       </c>
@@ -4461,39 +4517,39 @@
       <c r="O87" t="s">
         <v>67</v>
       </c>
-      <c r="U87" s="1" t="s">
+      <c r="V87" s="1" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="88" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B88" s="14" t="s">
+    <row r="88" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B88" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="C88" s="18"/>
-      <c r="D88" s="22" t="s">
+      <c r="C88" s="15"/>
+      <c r="D88" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="E88" s="24"/>
-      <c r="F88" s="24"/>
-      <c r="G88" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H88" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I88" s="14" t="s">
+      <c r="E88" s="21"/>
+      <c r="F88" s="21"/>
+      <c r="G88" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H88" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I88" s="16" t="s">
         <v>224</v>
       </c>
-      <c r="J88" s="14" t="s">
+      <c r="J88" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="K88" s="14" t="s">
+      <c r="K88" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L88" s="14" t="s">
+      <c r="L88" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M88" t="s">
@@ -4505,23 +4561,23 @@
       <c r="O88" t="s">
         <v>27</v>
       </c>
-      <c r="U88" s="1" t="s">
+      <c r="V88" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="89" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="14"/>
-      <c r="B89" s="14"/>
-      <c r="C89" s="18"/>
-      <c r="D89" s="22"/>
-      <c r="E89" s="24"/>
-      <c r="F89" s="24"/>
-      <c r="G89" s="14"/>
-      <c r="H89" s="14"/>
-      <c r="I89" s="14"/>
-      <c r="J89" s="14"/>
-      <c r="K89" s="14"/>
-      <c r="L89" s="14"/>
+    <row r="89" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="16"/>
+      <c r="B89" s="16"/>
+      <c r="C89" s="15"/>
+      <c r="D89" s="20"/>
+      <c r="E89" s="21"/>
+      <c r="F89" s="21"/>
+      <c r="G89" s="16"/>
+      <c r="H89" s="16"/>
+      <c r="I89" s="16"/>
+      <c r="J89" s="16"/>
+      <c r="K89" s="16"/>
+      <c r="L89" s="16"/>
       <c r="M89" t="s">
         <v>47</v>
       </c>
@@ -4531,23 +4587,23 @@
       <c r="O89" t="s">
         <v>27</v>
       </c>
-      <c r="U89" s="1" t="s">
+      <c r="V89" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="90" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="14"/>
-      <c r="B90" s="14"/>
-      <c r="C90" s="18"/>
-      <c r="D90" s="22"/>
-      <c r="E90" s="24"/>
-      <c r="F90" s="24"/>
-      <c r="G90" s="14"/>
-      <c r="H90" s="14"/>
-      <c r="I90" s="14"/>
-      <c r="J90" s="14"/>
-      <c r="K90" s="14"/>
-      <c r="L90" s="14"/>
+    <row r="90" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" s="16"/>
+      <c r="B90" s="16"/>
+      <c r="C90" s="15"/>
+      <c r="D90" s="20"/>
+      <c r="E90" s="21"/>
+      <c r="F90" s="21"/>
+      <c r="G90" s="16"/>
+      <c r="H90" s="16"/>
+      <c r="I90" s="16"/>
+      <c r="J90" s="16"/>
+      <c r="K90" s="16"/>
+      <c r="L90" s="16"/>
       <c r="M90" t="s">
         <v>180</v>
       </c>
@@ -4557,23 +4613,23 @@
       <c r="O90" t="s">
         <v>27</v>
       </c>
-      <c r="U90" s="1" t="s">
+      <c r="V90" s="1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="91" spans="1:21" ht="75" x14ac:dyDescent="0.25">
-      <c r="A91" s="14"/>
-      <c r="B91" s="14"/>
-      <c r="C91" s="18"/>
-      <c r="D91" s="22"/>
-      <c r="E91" s="24"/>
-      <c r="F91" s="24"/>
-      <c r="G91" s="14"/>
-      <c r="H91" s="14"/>
-      <c r="I91" s="14"/>
-      <c r="J91" s="14"/>
-      <c r="K91" s="14"/>
-      <c r="L91" s="14"/>
+    <row r="91" spans="1:22" ht="75" x14ac:dyDescent="0.25">
+      <c r="A91" s="16"/>
+      <c r="B91" s="16"/>
+      <c r="C91" s="15"/>
+      <c r="D91" s="20"/>
+      <c r="E91" s="21"/>
+      <c r="F91" s="21"/>
+      <c r="G91" s="16"/>
+      <c r="H91" s="16"/>
+      <c r="I91" s="16"/>
+      <c r="J91" s="16"/>
+      <c r="K91" s="16"/>
+      <c r="L91" s="16"/>
       <c r="M91" t="s">
         <v>214</v>
       </c>
@@ -4583,23 +4639,23 @@
       <c r="O91" t="s">
         <v>27</v>
       </c>
-      <c r="U91" s="1" t="s">
+      <c r="V91" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A92" s="14"/>
-      <c r="B92" s="14"/>
-      <c r="C92" s="18"/>
-      <c r="D92" s="22"/>
-      <c r="E92" s="24"/>
-      <c r="F92" s="24"/>
-      <c r="G92" s="14"/>
-      <c r="H92" s="14"/>
-      <c r="I92" s="14"/>
-      <c r="J92" s="14"/>
-      <c r="K92" s="14"/>
-      <c r="L92" s="14"/>
+    <row r="92" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A92" s="16"/>
+      <c r="B92" s="16"/>
+      <c r="C92" s="15"/>
+      <c r="D92" s="20"/>
+      <c r="E92" s="21"/>
+      <c r="F92" s="21"/>
+      <c r="G92" s="16"/>
+      <c r="H92" s="16"/>
+      <c r="I92" s="16"/>
+      <c r="J92" s="16"/>
+      <c r="K92" s="16"/>
+      <c r="L92" s="16"/>
       <c r="M92" t="s">
         <v>132</v>
       </c>
@@ -4610,19 +4666,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A93" s="14"/>
-      <c r="B93" s="14"/>
-      <c r="C93" s="18"/>
-      <c r="D93" s="22"/>
-      <c r="E93" s="24"/>
-      <c r="F93" s="24"/>
-      <c r="G93" s="14"/>
-      <c r="H93" s="14"/>
-      <c r="I93" s="14"/>
-      <c r="J93" s="14"/>
-      <c r="K93" s="14"/>
-      <c r="L93" s="14"/>
+    <row r="93" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A93" s="16"/>
+      <c r="B93" s="16"/>
+      <c r="C93" s="15"/>
+      <c r="D93" s="20"/>
+      <c r="E93" s="21"/>
+      <c r="F93" s="21"/>
+      <c r="G93" s="16"/>
+      <c r="H93" s="16"/>
+      <c r="I93" s="16"/>
+      <c r="J93" s="16"/>
+      <c r="K93" s="16"/>
+      <c r="L93" s="16"/>
       <c r="M93" t="s">
         <v>133</v>
       </c>
@@ -4633,35 +4689,35 @@
         <v>67</v>
       </c>
     </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A94" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B94" s="14" t="s">
+    <row r="94" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A94" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B94" s="16" t="s">
         <v>233</v>
       </c>
-      <c r="C94" s="18"/>
-      <c r="D94" s="22" t="s">
+      <c r="C94" s="15"/>
+      <c r="D94" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="E94" s="24"/>
-      <c r="F94" s="24"/>
-      <c r="G94" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H94" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I94" s="14" t="s">
+      <c r="E94" s="21"/>
+      <c r="F94" s="21"/>
+      <c r="G94" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H94" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I94" s="16" t="s">
         <v>232</v>
       </c>
-      <c r="J94" s="14" t="s">
+      <c r="J94" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="K94" s="14" t="s">
+      <c r="K94" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L94" s="14" t="s">
+      <c r="L94" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M94" t="s">
@@ -4674,19 +4730,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="95" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A95" s="14"/>
-      <c r="B95" s="14"/>
-      <c r="C95" s="18"/>
-      <c r="D95" s="22"/>
-      <c r="E95" s="24"/>
-      <c r="F95" s="24"/>
-      <c r="G95" s="14"/>
-      <c r="H95" s="14"/>
-      <c r="I95" s="14"/>
-      <c r="J95" s="14"/>
-      <c r="K95" s="14"/>
-      <c r="L95" s="14"/>
+    <row r="95" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A95" s="16"/>
+      <c r="B95" s="16"/>
+      <c r="C95" s="15"/>
+      <c r="D95" s="20"/>
+      <c r="E95" s="21"/>
+      <c r="F95" s="21"/>
+      <c r="G95" s="16"/>
+      <c r="H95" s="16"/>
+      <c r="I95" s="16"/>
+      <c r="J95" s="16"/>
+      <c r="K95" s="16"/>
+      <c r="L95" s="16"/>
       <c r="M95" t="s">
         <v>212</v>
       </c>
@@ -4696,23 +4752,23 @@
       <c r="O95" t="s">
         <v>212</v>
       </c>
-      <c r="U95" s="1" t="s">
+      <c r="V95" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="96" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A96" s="14"/>
-      <c r="B96" s="14"/>
-      <c r="C96" s="18"/>
-      <c r="D96" s="22"/>
-      <c r="E96" s="24"/>
-      <c r="F96" s="24"/>
-      <c r="G96" s="14"/>
-      <c r="H96" s="14"/>
-      <c r="I96" s="14"/>
-      <c r="J96" s="14"/>
-      <c r="K96" s="14"/>
-      <c r="L96" s="14"/>
+    <row r="96" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A96" s="16"/>
+      <c r="B96" s="16"/>
+      <c r="C96" s="15"/>
+      <c r="D96" s="20"/>
+      <c r="E96" s="21"/>
+      <c r="F96" s="21"/>
+      <c r="G96" s="16"/>
+      <c r="H96" s="16"/>
+      <c r="I96" s="16"/>
+      <c r="J96" s="16"/>
+      <c r="K96" s="16"/>
+      <c r="L96" s="16"/>
       <c r="M96" t="s">
         <v>212</v>
       </c>
@@ -4722,39 +4778,39 @@
       <c r="O96" t="s">
         <v>27</v>
       </c>
-      <c r="U96" s="1" t="s">
+      <c r="V96" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A97" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B97" s="14" t="s">
+    <row r="97" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A97" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B97" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="C97" s="18"/>
-      <c r="D97" s="22" t="s">
+      <c r="C97" s="15"/>
+      <c r="D97" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="E97" s="24"/>
-      <c r="F97" s="24"/>
-      <c r="G97" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H97" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I97" s="14" t="s">
+      <c r="E97" s="21"/>
+      <c r="F97" s="21"/>
+      <c r="G97" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H97" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I97" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="J97" s="14" t="s">
+      <c r="J97" s="16" t="s">
         <v>241</v>
       </c>
-      <c r="K97" s="14" t="s">
+      <c r="K97" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L97" s="14" t="s">
+      <c r="L97" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M97" t="s">
@@ -4767,19 +4823,19 @@
         <v>67</v>
       </c>
     </row>
-    <row r="98" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A98" s="14"/>
-      <c r="B98" s="14"/>
-      <c r="C98" s="18"/>
-      <c r="D98" s="22"/>
-      <c r="E98" s="24"/>
-      <c r="F98" s="24"/>
-      <c r="G98" s="14"/>
-      <c r="H98" s="14"/>
-      <c r="I98" s="14"/>
-      <c r="J98" s="14"/>
-      <c r="K98" s="14"/>
-      <c r="L98" s="14"/>
+    <row r="98" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A98" s="16"/>
+      <c r="B98" s="16"/>
+      <c r="C98" s="15"/>
+      <c r="D98" s="20"/>
+      <c r="E98" s="21"/>
+      <c r="F98" s="21"/>
+      <c r="G98" s="16"/>
+      <c r="H98" s="16"/>
+      <c r="I98" s="16"/>
+      <c r="J98" s="16"/>
+      <c r="K98" s="16"/>
+      <c r="L98" s="16"/>
       <c r="M98" t="s">
         <v>212</v>
       </c>
@@ -4789,11 +4845,11 @@
       <c r="O98" t="s">
         <v>27</v>
       </c>
-      <c r="U98" s="1" t="s">
+      <c r="V98" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>141</v>
       </c>
@@ -4813,7 +4869,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>141</v>
       </c>
@@ -4847,11 +4903,11 @@
       <c r="O100" t="s">
         <v>67</v>
       </c>
-      <c r="U100" s="1" t="s">
+      <c r="V100" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>141</v>
       </c>
@@ -4888,39 +4944,39 @@
       <c r="O101" t="s">
         <v>67</v>
       </c>
-      <c r="U101" s="1" t="s">
+      <c r="V101" s="1" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="102" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A102" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B102" s="14" t="s">
+    <row r="102" spans="1:22" ht="60" x14ac:dyDescent="0.25">
+      <c r="A102" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B102" s="16" t="s">
         <v>250</v>
       </c>
-      <c r="C102" s="18"/>
-      <c r="D102" s="22" t="s">
+      <c r="C102" s="15"/>
+      <c r="D102" s="20" t="s">
         <v>254</v>
       </c>
-      <c r="E102" s="24"/>
-      <c r="F102" s="24"/>
-      <c r="G102" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H102" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I102" s="14" t="s">
+      <c r="E102" s="21"/>
+      <c r="F102" s="21"/>
+      <c r="G102" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H102" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I102" s="16" t="s">
         <v>251</v>
       </c>
-      <c r="J102" s="14" t="s">
+      <c r="J102" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="K102" s="14" t="s">
+      <c r="K102" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L102" s="14" t="s">
+      <c r="L102" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M102" t="s">
@@ -4932,23 +4988,23 @@
       <c r="O102" t="s">
         <v>67</v>
       </c>
-      <c r="U102" s="1" t="s">
+      <c r="V102" s="1" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A103" s="14"/>
-      <c r="B103" s="14"/>
-      <c r="C103" s="18"/>
-      <c r="D103" s="22"/>
-      <c r="E103" s="24"/>
-      <c r="F103" s="24"/>
-      <c r="G103" s="14"/>
-      <c r="H103" s="14"/>
-      <c r="I103" s="14"/>
-      <c r="J103" s="14"/>
-      <c r="K103" s="14"/>
-      <c r="L103" s="14"/>
+    <row r="103" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A103" s="16"/>
+      <c r="B103" s="16"/>
+      <c r="C103" s="15"/>
+      <c r="D103" s="20"/>
+      <c r="E103" s="21"/>
+      <c r="F103" s="21"/>
+      <c r="G103" s="16"/>
+      <c r="H103" s="16"/>
+      <c r="I103" s="16"/>
+      <c r="J103" s="16"/>
+      <c r="K103" s="16"/>
+      <c r="L103" s="16"/>
       <c r="M103" t="s">
         <v>187</v>
       </c>
@@ -4958,23 +5014,23 @@
       <c r="O103" t="s">
         <v>67</v>
       </c>
-      <c r="U103" s="1" t="s">
+      <c r="V103" s="1" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="104" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A104" s="14"/>
-      <c r="B104" s="14"/>
-      <c r="C104" s="18"/>
-      <c r="D104" s="22"/>
-      <c r="E104" s="24"/>
-      <c r="F104" s="24"/>
-      <c r="G104" s="14"/>
-      <c r="H104" s="14"/>
-      <c r="I104" s="14"/>
-      <c r="J104" s="14"/>
-      <c r="K104" s="14"/>
-      <c r="L104" s="14"/>
+    <row r="104" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A104" s="16"/>
+      <c r="B104" s="16"/>
+      <c r="C104" s="15"/>
+      <c r="D104" s="20"/>
+      <c r="E104" s="21"/>
+      <c r="F104" s="21"/>
+      <c r="G104" s="16"/>
+      <c r="H104" s="16"/>
+      <c r="I104" s="16"/>
+      <c r="J104" s="16"/>
+      <c r="K104" s="16"/>
+      <c r="L104" s="16"/>
       <c r="M104" t="s">
         <v>212</v>
       </c>
@@ -4984,39 +5040,39 @@
       <c r="O104" t="s">
         <v>27</v>
       </c>
-      <c r="U104" s="1" t="s">
+      <c r="V104" s="1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="105" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A105" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B105" s="14" t="s">
+    <row r="105" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A105" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B105" s="16" t="s">
         <v>258</v>
       </c>
-      <c r="C105" s="18"/>
-      <c r="D105" s="22" t="s">
+      <c r="C105" s="15"/>
+      <c r="D105" s="20" t="s">
         <v>259</v>
       </c>
-      <c r="E105" s="24"/>
-      <c r="F105" s="24"/>
-      <c r="G105" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H105" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I105" s="14" t="s">
+      <c r="E105" s="21"/>
+      <c r="F105" s="21"/>
+      <c r="G105" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H105" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I105" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="J105" s="16" t="s">
+      <c r="J105" s="18" t="s">
         <v>265</v>
       </c>
-      <c r="K105" s="14" t="s">
+      <c r="K105" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L105" s="14" t="s">
+      <c r="L105" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M105" t="s">
@@ -5028,23 +5084,23 @@
       <c r="O105" t="s">
         <v>67</v>
       </c>
-      <c r="U105" s="1" t="s">
+      <c r="V105" s="1" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="106" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A106" s="14"/>
-      <c r="B106" s="14"/>
-      <c r="C106" s="18"/>
-      <c r="D106" s="22"/>
-      <c r="E106" s="24"/>
-      <c r="F106" s="24"/>
-      <c r="G106" s="14"/>
-      <c r="H106" s="14"/>
-      <c r="I106" s="14"/>
-      <c r="J106" s="16"/>
-      <c r="K106" s="14"/>
-      <c r="L106" s="14"/>
+    <row r="106" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A106" s="16"/>
+      <c r="B106" s="16"/>
+      <c r="C106" s="15"/>
+      <c r="D106" s="20"/>
+      <c r="E106" s="21"/>
+      <c r="F106" s="21"/>
+      <c r="G106" s="16"/>
+      <c r="H106" s="16"/>
+      <c r="I106" s="16"/>
+      <c r="J106" s="18"/>
+      <c r="K106" s="16"/>
+      <c r="L106" s="16"/>
       <c r="M106" t="s">
         <v>212</v>
       </c>
@@ -5054,23 +5110,23 @@
       <c r="O106" t="s">
         <v>67</v>
       </c>
-      <c r="U106" s="1" t="s">
+      <c r="V106" s="1" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="107" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A107" s="14"/>
-      <c r="B107" s="14"/>
-      <c r="C107" s="18"/>
-      <c r="D107" s="22"/>
-      <c r="E107" s="24"/>
-      <c r="F107" s="24"/>
-      <c r="G107" s="14"/>
-      <c r="H107" s="14"/>
-      <c r="I107" s="14"/>
-      <c r="J107" s="16"/>
-      <c r="K107" s="14"/>
-      <c r="L107" s="14"/>
+    <row r="107" spans="1:22" ht="60" x14ac:dyDescent="0.25">
+      <c r="A107" s="16"/>
+      <c r="B107" s="16"/>
+      <c r="C107" s="15"/>
+      <c r="D107" s="20"/>
+      <c r="E107" s="21"/>
+      <c r="F107" s="21"/>
+      <c r="G107" s="16"/>
+      <c r="H107" s="16"/>
+      <c r="I107" s="16"/>
+      <c r="J107" s="18"/>
+      <c r="K107" s="16"/>
+      <c r="L107" s="16"/>
       <c r="M107" t="s">
         <v>212</v>
       </c>
@@ -5080,23 +5136,23 @@
       <c r="O107" t="s">
         <v>212</v>
       </c>
-      <c r="U107" s="1" t="s">
+      <c r="V107" s="1" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="108" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A108" s="14"/>
-      <c r="B108" s="14"/>
-      <c r="C108" s="18"/>
-      <c r="D108" s="22"/>
-      <c r="E108" s="24"/>
-      <c r="F108" s="24"/>
-      <c r="G108" s="14"/>
-      <c r="H108" s="14"/>
-      <c r="I108" s="14"/>
-      <c r="J108" s="16"/>
-      <c r="K108" s="14"/>
-      <c r="L108" s="14"/>
+    <row r="108" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A108" s="16"/>
+      <c r="B108" s="16"/>
+      <c r="C108" s="15"/>
+      <c r="D108" s="20"/>
+      <c r="E108" s="21"/>
+      <c r="F108" s="21"/>
+      <c r="G108" s="16"/>
+      <c r="H108" s="16"/>
+      <c r="I108" s="16"/>
+      <c r="J108" s="18"/>
+      <c r="K108" s="16"/>
+      <c r="L108" s="16"/>
       <c r="M108" t="s">
         <v>212</v>
       </c>
@@ -5106,11 +5162,11 @@
       <c r="O108" t="s">
         <v>27</v>
       </c>
-      <c r="U108" s="1" t="s">
+      <c r="V108" s="1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="109" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>141</v>
       </c>
@@ -5144,37 +5200,37 @@
       <c r="O109" t="s">
         <v>67</v>
       </c>
-      <c r="U109" s="1" t="s">
+      <c r="V109" s="1" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="110" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A110" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B110" s="14" t="s">
+    <row r="110" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A110" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B110" s="16" t="s">
         <v>270</v>
       </c>
-      <c r="C110" s="18"/>
-      <c r="D110" s="15" t="s">
+      <c r="C110" s="15"/>
+      <c r="D110" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="E110" s="17"/>
-      <c r="F110" s="17"/>
-      <c r="G110" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H110" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I110" s="14"/>
-      <c r="J110" s="16" t="s">
+      <c r="E110" s="19"/>
+      <c r="F110" s="19"/>
+      <c r="G110" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H110" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I110" s="16"/>
+      <c r="J110" s="18" t="s">
         <v>271</v>
       </c>
-      <c r="K110" s="14" t="s">
+      <c r="K110" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L110" s="14" t="s">
+      <c r="L110" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M110" t="s">
@@ -5186,23 +5242,23 @@
       <c r="O110" t="s">
         <v>27</v>
       </c>
-      <c r="U110" s="1" t="s">
+      <c r="V110" s="1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="111" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A111" s="14"/>
-      <c r="B111" s="14"/>
-      <c r="C111" s="18"/>
-      <c r="D111" s="15"/>
-      <c r="E111" s="17"/>
-      <c r="F111" s="17"/>
-      <c r="G111" s="14"/>
-      <c r="H111" s="14"/>
-      <c r="I111" s="14"/>
-      <c r="J111" s="16"/>
-      <c r="K111" s="14"/>
-      <c r="L111" s="14"/>
+    <row r="111" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A111" s="16"/>
+      <c r="B111" s="16"/>
+      <c r="C111" s="15"/>
+      <c r="D111" s="17"/>
+      <c r="E111" s="19"/>
+      <c r="F111" s="19"/>
+      <c r="G111" s="16"/>
+      <c r="H111" s="16"/>
+      <c r="I111" s="16"/>
+      <c r="J111" s="18"/>
+      <c r="K111" s="16"/>
+      <c r="L111" s="16"/>
       <c r="M111" t="s">
         <v>212</v>
       </c>
@@ -5212,23 +5268,23 @@
       <c r="O111" t="s">
         <v>212</v>
       </c>
-      <c r="U111" s="1" t="s">
+      <c r="V111" s="1" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="112" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A112" s="14"/>
-      <c r="B112" s="14"/>
-      <c r="C112" s="18"/>
-      <c r="D112" s="15"/>
-      <c r="E112" s="17"/>
-      <c r="F112" s="17"/>
-      <c r="G112" s="14"/>
-      <c r="H112" s="14"/>
-      <c r="I112" s="14"/>
-      <c r="J112" s="16"/>
-      <c r="K112" s="14"/>
-      <c r="L112" s="14"/>
+    <row r="112" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A112" s="16"/>
+      <c r="B112" s="16"/>
+      <c r="C112" s="15"/>
+      <c r="D112" s="17"/>
+      <c r="E112" s="19"/>
+      <c r="F112" s="19"/>
+      <c r="G112" s="16"/>
+      <c r="H112" s="16"/>
+      <c r="I112" s="16"/>
+      <c r="J112" s="18"/>
+      <c r="K112" s="16"/>
+      <c r="L112" s="16"/>
       <c r="M112" t="s">
         <v>214</v>
       </c>
@@ -5238,37 +5294,37 @@
       <c r="O112" t="s">
         <v>27</v>
       </c>
-      <c r="U112" s="1" t="s">
+      <c r="V112" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="113" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A113" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B113" s="14" t="s">
+    <row r="113" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A113" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B113" s="16" t="s">
         <v>281</v>
       </c>
-      <c r="C113" s="18"/>
-      <c r="D113" s="15" t="s">
+      <c r="C113" s="15"/>
+      <c r="D113" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="E113" s="17"/>
-      <c r="F113" s="17"/>
-      <c r="G113" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H113" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I113" s="14"/>
-      <c r="J113" s="16" t="s">
+      <c r="E113" s="19"/>
+      <c r="F113" s="19"/>
+      <c r="G113" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H113" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I113" s="16"/>
+      <c r="J113" s="18" t="s">
         <v>286</v>
       </c>
-      <c r="K113" s="14" t="s">
+      <c r="K113" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L113" s="14" t="s">
+      <c r="L113" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M113" t="s">
@@ -5280,23 +5336,23 @@
       <c r="O113" t="s">
         <v>27</v>
       </c>
-      <c r="U113" s="1" t="s">
+      <c r="V113" s="1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="114" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A114" s="14"/>
-      <c r="B114" s="14"/>
-      <c r="C114" s="18"/>
-      <c r="D114" s="15"/>
-      <c r="E114" s="17"/>
-      <c r="F114" s="17"/>
-      <c r="G114" s="14"/>
-      <c r="H114" s="14"/>
-      <c r="I114" s="14"/>
-      <c r="J114" s="16"/>
-      <c r="K114" s="14"/>
-      <c r="L114" s="14"/>
+    <row r="114" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A114" s="16"/>
+      <c r="B114" s="16"/>
+      <c r="C114" s="15"/>
+      <c r="D114" s="17"/>
+      <c r="E114" s="19"/>
+      <c r="F114" s="19"/>
+      <c r="G114" s="16"/>
+      <c r="H114" s="16"/>
+      <c r="I114" s="16"/>
+      <c r="J114" s="18"/>
+      <c r="K114" s="16"/>
+      <c r="L114" s="16"/>
       <c r="M114" t="s">
         <v>212</v>
       </c>
@@ -5306,23 +5362,23 @@
       <c r="O114" t="s">
         <v>212</v>
       </c>
-      <c r="U114" s="1" t="s">
+      <c r="V114" s="1" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="115" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A115" s="14"/>
-      <c r="B115" s="14"/>
-      <c r="C115" s="18"/>
-      <c r="D115" s="15"/>
-      <c r="E115" s="17"/>
-      <c r="F115" s="17"/>
-      <c r="G115" s="14"/>
-      <c r="H115" s="14"/>
-      <c r="I115" s="14"/>
-      <c r="J115" s="16"/>
-      <c r="K115" s="14"/>
-      <c r="L115" s="14"/>
+    <row r="115" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A115" s="16"/>
+      <c r="B115" s="16"/>
+      <c r="C115" s="15"/>
+      <c r="D115" s="17"/>
+      <c r="E115" s="19"/>
+      <c r="F115" s="19"/>
+      <c r="G115" s="16"/>
+      <c r="H115" s="16"/>
+      <c r="I115" s="16"/>
+      <c r="J115" s="18"/>
+      <c r="K115" s="16"/>
+      <c r="L115" s="16"/>
       <c r="M115" t="s">
         <v>214</v>
       </c>
@@ -5332,37 +5388,37 @@
       <c r="O115" t="s">
         <v>27</v>
       </c>
-      <c r="U115" s="1" t="s">
+      <c r="V115" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="116" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A116" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B116" s="14" t="s">
+    <row r="116" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A116" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B116" s="16" t="s">
         <v>282</v>
       </c>
-      <c r="C116" s="18"/>
-      <c r="D116" s="15" t="s">
+      <c r="C116" s="15"/>
+      <c r="D116" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="E116" s="17"/>
-      <c r="F116" s="17"/>
-      <c r="G116" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H116" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I116" s="14"/>
-      <c r="J116" s="16" t="s">
+      <c r="E116" s="19"/>
+      <c r="F116" s="19"/>
+      <c r="G116" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H116" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I116" s="16"/>
+      <c r="J116" s="18" t="s">
         <v>285</v>
       </c>
-      <c r="K116" s="14" t="s">
+      <c r="K116" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L116" s="14" t="s">
+      <c r="L116" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M116" t="s">
@@ -5374,23 +5430,23 @@
       <c r="O116" t="s">
         <v>27</v>
       </c>
-      <c r="U116" s="1" t="s">
+      <c r="V116" s="1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="117" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A117" s="14"/>
-      <c r="B117" s="14"/>
-      <c r="C117" s="18"/>
-      <c r="D117" s="15"/>
-      <c r="E117" s="17"/>
-      <c r="F117" s="17"/>
-      <c r="G117" s="14"/>
-      <c r="H117" s="14"/>
-      <c r="I117" s="14"/>
-      <c r="J117" s="16"/>
-      <c r="K117" s="14"/>
-      <c r="L117" s="14"/>
+    <row r="117" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A117" s="16"/>
+      <c r="B117" s="16"/>
+      <c r="C117" s="15"/>
+      <c r="D117" s="17"/>
+      <c r="E117" s="19"/>
+      <c r="F117" s="19"/>
+      <c r="G117" s="16"/>
+      <c r="H117" s="16"/>
+      <c r="I117" s="16"/>
+      <c r="J117" s="18"/>
+      <c r="K117" s="16"/>
+      <c r="L117" s="16"/>
       <c r="M117" t="s">
         <v>212</v>
       </c>
@@ -5400,23 +5456,23 @@
       <c r="O117" t="s">
         <v>212</v>
       </c>
-      <c r="U117" s="1" t="s">
+      <c r="V117" s="1" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="118" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A118" s="14"/>
-      <c r="B118" s="14"/>
-      <c r="C118" s="18"/>
-      <c r="D118" s="15"/>
-      <c r="E118" s="17"/>
-      <c r="F118" s="17"/>
-      <c r="G118" s="14"/>
-      <c r="H118" s="14"/>
-      <c r="I118" s="14"/>
-      <c r="J118" s="16"/>
-      <c r="K118" s="14"/>
-      <c r="L118" s="14"/>
+    <row r="118" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A118" s="16"/>
+      <c r="B118" s="16"/>
+      <c r="C118" s="15"/>
+      <c r="D118" s="17"/>
+      <c r="E118" s="19"/>
+      <c r="F118" s="19"/>
+      <c r="G118" s="16"/>
+      <c r="H118" s="16"/>
+      <c r="I118" s="16"/>
+      <c r="J118" s="18"/>
+      <c r="K118" s="16"/>
+      <c r="L118" s="16"/>
       <c r="M118" t="s">
         <v>214</v>
       </c>
@@ -5426,37 +5482,37 @@
       <c r="O118" t="s">
         <v>27</v>
       </c>
-      <c r="U118" s="1" t="s">
+      <c r="V118" s="1" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="119" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A119" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B119" s="14" t="s">
+    <row r="119" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A119" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B119" s="16" t="s">
         <v>283</v>
       </c>
-      <c r="C119" s="18"/>
-      <c r="D119" s="15" t="s">
+      <c r="C119" s="15"/>
+      <c r="D119" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="E119" s="17"/>
-      <c r="F119" s="17"/>
-      <c r="G119" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H119" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I119" s="14"/>
-      <c r="J119" s="16" t="s">
+      <c r="E119" s="19"/>
+      <c r="F119" s="19"/>
+      <c r="G119" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H119" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I119" s="16"/>
+      <c r="J119" s="18" t="s">
         <v>284</v>
       </c>
-      <c r="K119" s="14" t="s">
+      <c r="K119" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L119" s="14" t="s">
+      <c r="L119" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M119" t="s">
@@ -5468,23 +5524,23 @@
       <c r="O119" t="s">
         <v>27</v>
       </c>
-      <c r="U119" s="1" t="s">
+      <c r="V119" s="1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="120" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A120" s="14"/>
-      <c r="B120" s="14"/>
-      <c r="C120" s="18"/>
-      <c r="D120" s="15"/>
-      <c r="E120" s="17"/>
-      <c r="F120" s="17"/>
-      <c r="G120" s="14"/>
-      <c r="H120" s="14"/>
-      <c r="I120" s="14"/>
-      <c r="J120" s="16"/>
-      <c r="K120" s="14"/>
-      <c r="L120" s="14"/>
+    <row r="120" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A120" s="16"/>
+      <c r="B120" s="16"/>
+      <c r="C120" s="15"/>
+      <c r="D120" s="17"/>
+      <c r="E120" s="19"/>
+      <c r="F120" s="19"/>
+      <c r="G120" s="16"/>
+      <c r="H120" s="16"/>
+      <c r="I120" s="16"/>
+      <c r="J120" s="18"/>
+      <c r="K120" s="16"/>
+      <c r="L120" s="16"/>
       <c r="M120" t="s">
         <v>212</v>
       </c>
@@ -5494,23 +5550,23 @@
       <c r="O120" t="s">
         <v>212</v>
       </c>
-      <c r="U120" s="1" t="s">
+      <c r="V120" s="1" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="121" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A121" s="14"/>
-      <c r="B121" s="14"/>
-      <c r="C121" s="18"/>
-      <c r="D121" s="15"/>
-      <c r="E121" s="17"/>
-      <c r="F121" s="17"/>
-      <c r="G121" s="14"/>
-      <c r="H121" s="14"/>
-      <c r="I121" s="14"/>
-      <c r="J121" s="16"/>
-      <c r="K121" s="14"/>
-      <c r="L121" s="14"/>
+    <row r="121" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A121" s="16"/>
+      <c r="B121" s="16"/>
+      <c r="C121" s="15"/>
+      <c r="D121" s="17"/>
+      <c r="E121" s="19"/>
+      <c r="F121" s="19"/>
+      <c r="G121" s="16"/>
+      <c r="H121" s="16"/>
+      <c r="I121" s="16"/>
+      <c r="J121" s="18"/>
+      <c r="K121" s="16"/>
+      <c r="L121" s="16"/>
       <c r="M121" t="s">
         <v>214</v>
       </c>
@@ -5520,146 +5576,278 @@
       <c r="O121" t="s">
         <v>27</v>
       </c>
-      <c r="U121" s="1" t="s">
+      <c r="V121" s="1" t="s">
         <v>280</v>
       </c>
     </row>
+    <row r="122" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B122" s="22" t="s">
+        <v>315</v>
+      </c>
+      <c r="C122" s="22" t="s">
+        <v>316</v>
+      </c>
+      <c r="D122" s="20" t="s">
+        <v>322</v>
+      </c>
+      <c r="E122" s="22"/>
+      <c r="F122" s="22"/>
+      <c r="G122" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H122" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="I122" s="22" t="s">
+        <v>317</v>
+      </c>
+      <c r="J122" s="20" t="s">
+        <v>318</v>
+      </c>
+      <c r="K122" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="L122" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="M122" t="s">
+        <v>60</v>
+      </c>
+      <c r="N122" t="s">
+        <v>26</v>
+      </c>
+      <c r="O122" t="s">
+        <v>27</v>
+      </c>
+      <c r="P122" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="Q122" s="25" t="s">
+        <v>324</v>
+      </c>
+      <c r="R122" s="20" t="s">
+        <v>323</v>
+      </c>
+      <c r="S122" s="25" t="s">
+        <v>320</v>
+      </c>
+      <c r="T122" s="25" t="s">
+        <v>319</v>
+      </c>
+      <c r="U122" s="22" t="s">
+        <v>307</v>
+      </c>
+      <c r="V122" s="20" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="123" spans="1:22" ht="60" x14ac:dyDescent="0.25">
+      <c r="A123" s="22"/>
+      <c r="B123" s="22"/>
+      <c r="C123" s="22"/>
+      <c r="D123" s="22"/>
+      <c r="E123" s="22"/>
+      <c r="F123" s="22"/>
+      <c r="G123" s="22"/>
+      <c r="H123" s="22"/>
+      <c r="I123" s="22"/>
+      <c r="J123" s="20"/>
+      <c r="K123" s="22"/>
+      <c r="L123" s="22"/>
+      <c r="M123" t="s">
+        <v>177</v>
+      </c>
+      <c r="N123" t="s">
+        <v>141</v>
+      </c>
+      <c r="O123" t="s">
+        <v>27</v>
+      </c>
+      <c r="P123" s="11" t="s">
+        <v>326</v>
+      </c>
+      <c r="Q123" s="25"/>
+      <c r="R123" s="20"/>
+      <c r="S123" s="25"/>
+      <c r="T123" s="25"/>
+      <c r="U123" s="22"/>
+      <c r="V123" s="20"/>
+    </row>
+    <row r="124" spans="1:22" ht="60" x14ac:dyDescent="0.25">
+      <c r="A124" s="22"/>
+      <c r="B124" s="22"/>
+      <c r="C124" s="22"/>
+      <c r="D124" s="22"/>
+      <c r="E124" s="22"/>
+      <c r="F124" s="22"/>
+      <c r="G124" s="22"/>
+      <c r="H124" s="22"/>
+      <c r="I124" s="22"/>
+      <c r="J124" s="20"/>
+      <c r="K124" s="22"/>
+      <c r="L124" s="22"/>
+      <c r="M124" t="s">
+        <v>111</v>
+      </c>
+      <c r="N124" t="s">
+        <v>66</v>
+      </c>
+      <c r="O124" t="s">
+        <v>67</v>
+      </c>
+      <c r="P124" s="11" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q124" s="25"/>
+      <c r="R124" s="20"/>
+      <c r="S124" s="25"/>
+      <c r="T124" s="25"/>
+      <c r="U124" s="22"/>
+      <c r="V124" s="20"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:U1"/>
-  <mergeCells count="276">
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="C64:C67"/>
-    <mergeCell ref="C68:C71"/>
-    <mergeCell ref="C72:C75"/>
-    <mergeCell ref="C78:C82"/>
-    <mergeCell ref="C83:C87"/>
-    <mergeCell ref="C88:C93"/>
-    <mergeCell ref="C94:C96"/>
-    <mergeCell ref="C97:C98"/>
-    <mergeCell ref="A110:A112"/>
-    <mergeCell ref="I110:I112"/>
-    <mergeCell ref="H110:H112"/>
-    <mergeCell ref="G110:G112"/>
-    <mergeCell ref="D110:D112"/>
-    <mergeCell ref="B110:B112"/>
-    <mergeCell ref="L110:L112"/>
-    <mergeCell ref="K110:K112"/>
-    <mergeCell ref="J110:J112"/>
-    <mergeCell ref="E110:E112"/>
-    <mergeCell ref="F110:F112"/>
-    <mergeCell ref="C110:C112"/>
-    <mergeCell ref="I105:I108"/>
-    <mergeCell ref="H105:H108"/>
-    <mergeCell ref="G105:G108"/>
-    <mergeCell ref="B105:B108"/>
-    <mergeCell ref="A105:A108"/>
-    <mergeCell ref="D105:D108"/>
-    <mergeCell ref="L105:L108"/>
-    <mergeCell ref="K105:K108"/>
-    <mergeCell ref="J105:J108"/>
-    <mergeCell ref="F105:F108"/>
-    <mergeCell ref="E105:E108"/>
-    <mergeCell ref="C105:C108"/>
-    <mergeCell ref="G97:G98"/>
-    <mergeCell ref="B97:B98"/>
-    <mergeCell ref="A97:A98"/>
-    <mergeCell ref="D97:D98"/>
-    <mergeCell ref="L102:L104"/>
-    <mergeCell ref="K102:K104"/>
-    <mergeCell ref="J102:J104"/>
-    <mergeCell ref="I102:I104"/>
-    <mergeCell ref="H102:H104"/>
-    <mergeCell ref="G102:G104"/>
-    <mergeCell ref="D102:D104"/>
-    <mergeCell ref="B102:B104"/>
-    <mergeCell ref="A102:A104"/>
-    <mergeCell ref="L97:L98"/>
-    <mergeCell ref="K97:K98"/>
-    <mergeCell ref="J97:J98"/>
-    <mergeCell ref="I97:I98"/>
-    <mergeCell ref="H97:H98"/>
-    <mergeCell ref="F97:F98"/>
-    <mergeCell ref="F102:F104"/>
-    <mergeCell ref="E97:E98"/>
-    <mergeCell ref="E102:E104"/>
-    <mergeCell ref="C102:C104"/>
-    <mergeCell ref="G94:G96"/>
-    <mergeCell ref="B94:B96"/>
-    <mergeCell ref="A94:A96"/>
-    <mergeCell ref="D94:D96"/>
-    <mergeCell ref="L94:L96"/>
-    <mergeCell ref="K94:K96"/>
-    <mergeCell ref="J94:J96"/>
-    <mergeCell ref="I94:I96"/>
-    <mergeCell ref="H94:H96"/>
-    <mergeCell ref="F94:F96"/>
-    <mergeCell ref="E94:E96"/>
-    <mergeCell ref="G83:G87"/>
-    <mergeCell ref="B83:B87"/>
-    <mergeCell ref="A83:A87"/>
-    <mergeCell ref="D83:D87"/>
-    <mergeCell ref="L88:L93"/>
-    <mergeCell ref="K88:K93"/>
-    <mergeCell ref="J88:J93"/>
-    <mergeCell ref="I88:I93"/>
-    <mergeCell ref="H88:H93"/>
-    <mergeCell ref="G88:G93"/>
-    <mergeCell ref="A88:A93"/>
-    <mergeCell ref="B88:B93"/>
-    <mergeCell ref="D88:D93"/>
-    <mergeCell ref="L83:L87"/>
-    <mergeCell ref="K83:K87"/>
-    <mergeCell ref="J83:J87"/>
-    <mergeCell ref="I83:I87"/>
-    <mergeCell ref="H83:H87"/>
-    <mergeCell ref="F83:F87"/>
-    <mergeCell ref="F88:F93"/>
-    <mergeCell ref="E83:E87"/>
-    <mergeCell ref="E88:E93"/>
-    <mergeCell ref="H78:H82"/>
-    <mergeCell ref="G78:G82"/>
-    <mergeCell ref="D78:D82"/>
-    <mergeCell ref="B78:B82"/>
-    <mergeCell ref="A78:A82"/>
-    <mergeCell ref="I72:I75"/>
-    <mergeCell ref="J72:J75"/>
-    <mergeCell ref="K72:K75"/>
-    <mergeCell ref="L72:L75"/>
-    <mergeCell ref="L78:L82"/>
-    <mergeCell ref="K78:K82"/>
-    <mergeCell ref="J78:J82"/>
-    <mergeCell ref="I78:I82"/>
-    <mergeCell ref="A72:A75"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="D72:D75"/>
-    <mergeCell ref="G72:G75"/>
-    <mergeCell ref="H72:H75"/>
-    <mergeCell ref="F72:F75"/>
-    <mergeCell ref="F78:F82"/>
-    <mergeCell ref="E72:E75"/>
-    <mergeCell ref="E78:E82"/>
-    <mergeCell ref="H68:H71"/>
-    <mergeCell ref="I68:I71"/>
-    <mergeCell ref="J68:J71"/>
-    <mergeCell ref="K68:K71"/>
-    <mergeCell ref="L68:L71"/>
-    <mergeCell ref="G64:G67"/>
-    <mergeCell ref="B64:B67"/>
-    <mergeCell ref="A64:A67"/>
-    <mergeCell ref="D64:D67"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="D68:D71"/>
-    <mergeCell ref="G68:G71"/>
-    <mergeCell ref="L64:L67"/>
-    <mergeCell ref="K64:K67"/>
-    <mergeCell ref="J64:J67"/>
-    <mergeCell ref="I64:I67"/>
-    <mergeCell ref="H64:H67"/>
-    <mergeCell ref="F64:F67"/>
-    <mergeCell ref="F68:F71"/>
-    <mergeCell ref="E64:E67"/>
-    <mergeCell ref="E68:E71"/>
+  <autoFilter ref="A1:V1"/>
+  <mergeCells count="294">
+    <mergeCell ref="L122:L124"/>
+    <mergeCell ref="J122:J124"/>
+    <mergeCell ref="I122:I124"/>
+    <mergeCell ref="H122:H124"/>
+    <mergeCell ref="G122:G124"/>
+    <mergeCell ref="F122:F124"/>
+    <mergeCell ref="R122:R124"/>
+    <mergeCell ref="Q122:Q124"/>
+    <mergeCell ref="S122:S124"/>
+    <mergeCell ref="T122:T124"/>
+    <mergeCell ref="U122:U124"/>
+    <mergeCell ref="V122:V124"/>
+    <mergeCell ref="E122:E124"/>
+    <mergeCell ref="D122:D124"/>
+    <mergeCell ref="C122:C124"/>
+    <mergeCell ref="B122:B124"/>
+    <mergeCell ref="A122:A124"/>
+    <mergeCell ref="K122:K124"/>
+    <mergeCell ref="A119:A121"/>
+    <mergeCell ref="B119:B121"/>
+    <mergeCell ref="D119:D121"/>
+    <mergeCell ref="G119:G121"/>
+    <mergeCell ref="H119:H121"/>
+    <mergeCell ref="I119:I121"/>
+    <mergeCell ref="J119:J121"/>
+    <mergeCell ref="K119:K121"/>
+    <mergeCell ref="L119:L121"/>
+    <mergeCell ref="E119:E121"/>
+    <mergeCell ref="F119:F121"/>
+    <mergeCell ref="C119:C121"/>
+    <mergeCell ref="K113:K115"/>
+    <mergeCell ref="L113:L115"/>
+    <mergeCell ref="A116:A118"/>
+    <mergeCell ref="B116:B118"/>
+    <mergeCell ref="D116:D118"/>
+    <mergeCell ref="G116:G118"/>
+    <mergeCell ref="H116:H118"/>
+    <mergeCell ref="I116:I118"/>
+    <mergeCell ref="J116:J118"/>
+    <mergeCell ref="K116:K118"/>
+    <mergeCell ref="L116:L118"/>
+    <mergeCell ref="E113:E115"/>
+    <mergeCell ref="E116:E118"/>
+    <mergeCell ref="F113:F115"/>
+    <mergeCell ref="F116:F118"/>
+    <mergeCell ref="A113:A115"/>
+    <mergeCell ref="B113:B115"/>
+    <mergeCell ref="D113:D115"/>
+    <mergeCell ref="G113:G115"/>
+    <mergeCell ref="H113:H115"/>
+    <mergeCell ref="I113:I115"/>
+    <mergeCell ref="J113:J115"/>
+    <mergeCell ref="C113:C115"/>
+    <mergeCell ref="C116:C118"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="E37:E39"/>
+    <mergeCell ref="E41:E47"/>
+    <mergeCell ref="E57:E59"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="C37:C39"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="H31:H33"/>
+    <mergeCell ref="I31:I33"/>
+    <mergeCell ref="J31:J33"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="E28:E30"/>
+    <mergeCell ref="E31:E33"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="F28:F30"/>
+    <mergeCell ref="F31:F33"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="G28:G30"/>
+    <mergeCell ref="H28:H30"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="G31:G33"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="L41:L47"/>
+    <mergeCell ref="K41:K47"/>
+    <mergeCell ref="J41:J47"/>
+    <mergeCell ref="I41:I47"/>
+    <mergeCell ref="L28:L30"/>
+    <mergeCell ref="K28:K30"/>
+    <mergeCell ref="J28:J30"/>
+    <mergeCell ref="I28:I30"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="L24:L26"/>
+    <mergeCell ref="K24:K26"/>
+    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="K31:K33"/>
+    <mergeCell ref="L31:L33"/>
+    <mergeCell ref="I34:I36"/>
+    <mergeCell ref="J34:J36"/>
+    <mergeCell ref="K34:K36"/>
+    <mergeCell ref="L34:L36"/>
+    <mergeCell ref="I37:I39"/>
+    <mergeCell ref="J37:J39"/>
+    <mergeCell ref="K37:K39"/>
+    <mergeCell ref="L37:L39"/>
+    <mergeCell ref="L57:L59"/>
+    <mergeCell ref="K57:K59"/>
+    <mergeCell ref="J57:J59"/>
+    <mergeCell ref="I57:I59"/>
+    <mergeCell ref="H57:H59"/>
+    <mergeCell ref="H41:H47"/>
+    <mergeCell ref="G41:G47"/>
+    <mergeCell ref="B41:B47"/>
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="F41:F47"/>
+    <mergeCell ref="F57:F59"/>
+    <mergeCell ref="G57:G59"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="C41:C47"/>
+    <mergeCell ref="C57:C59"/>
     <mergeCell ref="F34:F36"/>
     <mergeCell ref="F37:F39"/>
     <mergeCell ref="H34:H36"/>
@@ -5684,143 +5872,163 @@
     <mergeCell ref="D34:D36"/>
     <mergeCell ref="D37:D39"/>
     <mergeCell ref="E62:E63"/>
-    <mergeCell ref="L57:L59"/>
-    <mergeCell ref="K57:K59"/>
-    <mergeCell ref="J57:J59"/>
-    <mergeCell ref="I57:I59"/>
-    <mergeCell ref="H57:H59"/>
-    <mergeCell ref="H41:H47"/>
-    <mergeCell ref="G41:G47"/>
-    <mergeCell ref="B41:B47"/>
-    <mergeCell ref="A41:A47"/>
-    <mergeCell ref="F41:F47"/>
-    <mergeCell ref="F57:F59"/>
-    <mergeCell ref="G57:G59"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="C41:C47"/>
-    <mergeCell ref="C57:C59"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="L41:L47"/>
-    <mergeCell ref="K41:K47"/>
-    <mergeCell ref="J41:J47"/>
-    <mergeCell ref="I41:I47"/>
-    <mergeCell ref="L28:L30"/>
-    <mergeCell ref="K28:K30"/>
-    <mergeCell ref="J28:J30"/>
-    <mergeCell ref="I28:I30"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="L24:L26"/>
-    <mergeCell ref="K24:K26"/>
-    <mergeCell ref="J24:J26"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="K31:K33"/>
-    <mergeCell ref="L31:L33"/>
-    <mergeCell ref="I34:I36"/>
-    <mergeCell ref="J34:J36"/>
-    <mergeCell ref="K34:K36"/>
-    <mergeCell ref="L34:L36"/>
-    <mergeCell ref="I37:I39"/>
-    <mergeCell ref="J37:J39"/>
-    <mergeCell ref="K37:K39"/>
-    <mergeCell ref="L37:L39"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="H31:H33"/>
-    <mergeCell ref="I31:I33"/>
-    <mergeCell ref="J31:J33"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="E28:E30"/>
-    <mergeCell ref="E31:E33"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="F28:F30"/>
-    <mergeCell ref="F31:F33"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="G28:G30"/>
-    <mergeCell ref="H28:H30"/>
-    <mergeCell ref="G24:G26"/>
-    <mergeCell ref="G31:G33"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="E37:E39"/>
-    <mergeCell ref="E41:E47"/>
-    <mergeCell ref="E57:E59"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="C37:C39"/>
-    <mergeCell ref="K113:K115"/>
-    <mergeCell ref="L113:L115"/>
-    <mergeCell ref="A116:A118"/>
-    <mergeCell ref="B116:B118"/>
-    <mergeCell ref="D116:D118"/>
-    <mergeCell ref="G116:G118"/>
-    <mergeCell ref="H116:H118"/>
-    <mergeCell ref="I116:I118"/>
-    <mergeCell ref="J116:J118"/>
-    <mergeCell ref="K116:K118"/>
-    <mergeCell ref="L116:L118"/>
-    <mergeCell ref="E113:E115"/>
-    <mergeCell ref="E116:E118"/>
-    <mergeCell ref="F113:F115"/>
-    <mergeCell ref="F116:F118"/>
-    <mergeCell ref="A113:A115"/>
-    <mergeCell ref="B113:B115"/>
-    <mergeCell ref="D113:D115"/>
-    <mergeCell ref="G113:G115"/>
-    <mergeCell ref="H113:H115"/>
-    <mergeCell ref="I113:I115"/>
-    <mergeCell ref="J113:J115"/>
-    <mergeCell ref="C113:C115"/>
-    <mergeCell ref="C116:C118"/>
-    <mergeCell ref="A119:A121"/>
-    <mergeCell ref="B119:B121"/>
-    <mergeCell ref="D119:D121"/>
-    <mergeCell ref="G119:G121"/>
-    <mergeCell ref="H119:H121"/>
-    <mergeCell ref="I119:I121"/>
-    <mergeCell ref="J119:J121"/>
-    <mergeCell ref="K119:K121"/>
-    <mergeCell ref="L119:L121"/>
-    <mergeCell ref="E119:E121"/>
-    <mergeCell ref="F119:F121"/>
-    <mergeCell ref="C119:C121"/>
+    <mergeCell ref="H68:H71"/>
+    <mergeCell ref="I68:I71"/>
+    <mergeCell ref="J68:J71"/>
+    <mergeCell ref="K68:K71"/>
+    <mergeCell ref="L68:L71"/>
+    <mergeCell ref="G64:G67"/>
+    <mergeCell ref="B64:B67"/>
+    <mergeCell ref="A64:A67"/>
+    <mergeCell ref="D64:D67"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="D68:D71"/>
+    <mergeCell ref="G68:G71"/>
+    <mergeCell ref="L64:L67"/>
+    <mergeCell ref="K64:K67"/>
+    <mergeCell ref="J64:J67"/>
+    <mergeCell ref="I64:I67"/>
+    <mergeCell ref="H64:H67"/>
+    <mergeCell ref="F64:F67"/>
+    <mergeCell ref="F68:F71"/>
+    <mergeCell ref="E64:E67"/>
+    <mergeCell ref="E68:E71"/>
+    <mergeCell ref="H78:H82"/>
+    <mergeCell ref="G78:G82"/>
+    <mergeCell ref="D78:D82"/>
+    <mergeCell ref="B78:B82"/>
+    <mergeCell ref="A78:A82"/>
+    <mergeCell ref="I72:I75"/>
+    <mergeCell ref="J72:J75"/>
+    <mergeCell ref="K72:K75"/>
+    <mergeCell ref="L72:L75"/>
+    <mergeCell ref="L78:L82"/>
+    <mergeCell ref="K78:K82"/>
+    <mergeCell ref="J78:J82"/>
+    <mergeCell ref="I78:I82"/>
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="D72:D75"/>
+    <mergeCell ref="G72:G75"/>
+    <mergeCell ref="H72:H75"/>
+    <mergeCell ref="F72:F75"/>
+    <mergeCell ref="F78:F82"/>
+    <mergeCell ref="E72:E75"/>
+    <mergeCell ref="E78:E82"/>
+    <mergeCell ref="G83:G87"/>
+    <mergeCell ref="B83:B87"/>
+    <mergeCell ref="A83:A87"/>
+    <mergeCell ref="D83:D87"/>
+    <mergeCell ref="L88:L93"/>
+    <mergeCell ref="K88:K93"/>
+    <mergeCell ref="J88:J93"/>
+    <mergeCell ref="I88:I93"/>
+    <mergeCell ref="H88:H93"/>
+    <mergeCell ref="G88:G93"/>
+    <mergeCell ref="A88:A93"/>
+    <mergeCell ref="B88:B93"/>
+    <mergeCell ref="D88:D93"/>
+    <mergeCell ref="L83:L87"/>
+    <mergeCell ref="K83:K87"/>
+    <mergeCell ref="J83:J87"/>
+    <mergeCell ref="I83:I87"/>
+    <mergeCell ref="H83:H87"/>
+    <mergeCell ref="F83:F87"/>
+    <mergeCell ref="F88:F93"/>
+    <mergeCell ref="E83:E87"/>
+    <mergeCell ref="E88:E93"/>
+    <mergeCell ref="G94:G96"/>
+    <mergeCell ref="B94:B96"/>
+    <mergeCell ref="A94:A96"/>
+    <mergeCell ref="D94:D96"/>
+    <mergeCell ref="L94:L96"/>
+    <mergeCell ref="K94:K96"/>
+    <mergeCell ref="J94:J96"/>
+    <mergeCell ref="I94:I96"/>
+    <mergeCell ref="H94:H96"/>
+    <mergeCell ref="F94:F96"/>
+    <mergeCell ref="E94:E96"/>
+    <mergeCell ref="G97:G98"/>
+    <mergeCell ref="B97:B98"/>
+    <mergeCell ref="A97:A98"/>
+    <mergeCell ref="D97:D98"/>
+    <mergeCell ref="L102:L104"/>
+    <mergeCell ref="K102:K104"/>
+    <mergeCell ref="J102:J104"/>
+    <mergeCell ref="I102:I104"/>
+    <mergeCell ref="H102:H104"/>
+    <mergeCell ref="G102:G104"/>
+    <mergeCell ref="D102:D104"/>
+    <mergeCell ref="B102:B104"/>
+    <mergeCell ref="A102:A104"/>
+    <mergeCell ref="L97:L98"/>
+    <mergeCell ref="K97:K98"/>
+    <mergeCell ref="J97:J98"/>
+    <mergeCell ref="I97:I98"/>
+    <mergeCell ref="H97:H98"/>
+    <mergeCell ref="F97:F98"/>
+    <mergeCell ref="F102:F104"/>
+    <mergeCell ref="E97:E98"/>
+    <mergeCell ref="E102:E104"/>
+    <mergeCell ref="C102:C104"/>
+    <mergeCell ref="I105:I108"/>
+    <mergeCell ref="H105:H108"/>
+    <mergeCell ref="G105:G108"/>
+    <mergeCell ref="B105:B108"/>
+    <mergeCell ref="A105:A108"/>
+    <mergeCell ref="D105:D108"/>
+    <mergeCell ref="L105:L108"/>
+    <mergeCell ref="K105:K108"/>
+    <mergeCell ref="J105:J108"/>
+    <mergeCell ref="F105:F108"/>
+    <mergeCell ref="E105:E108"/>
+    <mergeCell ref="C105:C108"/>
+    <mergeCell ref="A110:A112"/>
+    <mergeCell ref="I110:I112"/>
+    <mergeCell ref="H110:H112"/>
+    <mergeCell ref="G110:G112"/>
+    <mergeCell ref="D110:D112"/>
+    <mergeCell ref="B110:B112"/>
+    <mergeCell ref="L110:L112"/>
+    <mergeCell ref="K110:K112"/>
+    <mergeCell ref="J110:J112"/>
+    <mergeCell ref="E110:E112"/>
+    <mergeCell ref="F110:F112"/>
+    <mergeCell ref="C110:C112"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="C64:C67"/>
+    <mergeCell ref="C68:C71"/>
+    <mergeCell ref="C72:C75"/>
+    <mergeCell ref="C78:C82"/>
+    <mergeCell ref="C83:C87"/>
+    <mergeCell ref="C88:C93"/>
+    <mergeCell ref="C94:C96"/>
+    <mergeCell ref="C97:C98"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="P54" r:id="rId1"/>
     <hyperlink ref="E54" r:id="rId2"/>
     <hyperlink ref="F54" r:id="rId3"/>
     <hyperlink ref="Q54" r:id="rId4"/>
-    <hyperlink ref="R54" r:id="rId5"/>
-    <hyperlink ref="S54" r:id="rId6"/>
+    <hyperlink ref="S54" r:id="rId5"/>
+    <hyperlink ref="T54" r:id="rId6"/>
+    <hyperlink ref="T122:T123" r:id="rId7" display="http://192.168.110.185:8585/tfs/web/UI/Pages/WorkItems/WorkItemEdit.aspx?id=6621&amp;pguid=81f5a887-a9da-41fc-8c45-50b4cb40e1ea"/>
+    <hyperlink ref="S122:S123" r:id="rId8" display="http://94.130.97.86:8888/edit_bug.aspx?id=35"/>
+    <hyperlink ref="Q122:Q124" r:id="rId9" display="MappingSheetResources\GetContractAvailableServices\GetContractAvailableServicesResponseMapping.txt"/>
+    <hyperlink ref="P122" r:id="rId10"/>
+    <hyperlink ref="P123" r:id="rId11"/>
+    <hyperlink ref="P124" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId7"/>
-  <drawing r:id="rId8"/>
-  <legacyDrawing r:id="rId9"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId13"/>
+  <drawing r:id="rId14"/>
+  <legacyDrawing r:id="rId15"/>
   <oleObjects>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="1025" r:id="rId10">
-          <objectPr defaultSize="0" r:id="rId11">
+        <oleObject progId="Packager Shell Object" shapeId="1025" r:id="rId16">
+          <objectPr defaultSize="0" r:id="rId17">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -5839,13 +6047,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="1025" r:id="rId10"/>
+        <oleObject progId="Packager Shell Object" shapeId="1025" r:id="rId16"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="1026" r:id="rId12">
-          <objectPr defaultSize="0" r:id="rId13">
+        <oleObject progId="Packager Shell Object" shapeId="1026" r:id="rId18">
+          <objectPr defaultSize="0" r:id="rId19">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>5</xdr:col>
@@ -5864,7 +6072,7 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="1026" r:id="rId12"/>
+        <oleObject progId="Packager Shell Object" shapeId="1026" r:id="rId18"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </oleObjects>
@@ -5875,7 +6083,7 @@
           <x14:formula1>
             <xm:f>Tables!$F$13:$F$20</xm:f>
           </x14:formula1>
-          <xm:sqref>T1:T1048576</xm:sqref>
+          <xm:sqref>U1:U122 U125:U1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Updating Get Contract Avaliable Services
git-tfs-id: [http://developmentvlan:8585/tfs/vanrise.collection]$/;C55399
</commit_message>
<xml_diff>
--- a/SOM/Documents/SOM/SOM APIs Mapping Sheet.xlsx
+++ b/SOM/Documents/SOM/SOM APIs Mapping Sheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="330">
   <si>
     <t>GetTechnicalDetails</t>
   </si>
@@ -1029,26 +1029,29 @@
 linePathId</t>
   </si>
   <si>
+    <t>MappingSheetResources\GetContractAvailableServices\GetContractAvailableServicesResponseMapping.txt</t>
+  </si>
+  <si>
+    <t>MappingSheetResources\GetContractAvailableServices\Technicallinedetailsbypathid.txt</t>
+  </si>
+  <si>
+    <t>MappingSheetResources\GetContractAvailableServices\GetRatePlanServices.txt</t>
+  </si>
+  <si>
+    <t>MappingSheetResources\GetContractAvailableServices\contractServicesReadRequest.txt</t>
+  </si>
+  <si>
+    <t>Lot of questions related to CRM and how to get subscription and access fees</t>
+  </si>
+  <si>
+    <t>MappingSheetResources\GetContractAvailableServices\GetContractAvailableServicesResponse.txt</t>
+  </si>
+  <si>
     <t>This service should retreived the switch id from Line Path Id.
-Then Pass it to Get Rate Plan services for this call to filter them based on the switch.
+Then pass it to Get Rate Plan services for this call to filter them based on the switch.
 Then call contract Services Read Request in order to get the ids of the services that are already purchased
 Then filter the rate plan services by removing those that are sold.
 At the end call for each package the servicesReadRequest in order to get the name of the service in addtion to other needed fields.</t>
-  </si>
-  <si>
-    <t>MappingSheetResources\GetContractAvailableServices\GetContractAvailableServicesResponseMapping.txt</t>
-  </si>
-  <si>
-    <t>MappingSheetResources\GetContractAvailableServices\Technicallinedetailsbypathid.txt</t>
-  </si>
-  <si>
-    <t>MappingSheetResources\GetContractAvailableServices\GetRatePlanServices.txt</t>
-  </si>
-  <si>
-    <t>MappingSheetResources\GetContractAvailableServices\contractServicesReadRequest.txt</t>
-  </si>
-  <si>
-    <t>Lot of questions related to CRM and how to get subscription and access fees</t>
   </si>
 </sst>
 </file>
@@ -1203,10 +1206,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1221,22 +1227,19 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1706,9 +1709,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A125" sqref="A125"/>
+      <selection pane="bottomLeft" activeCell="U122" sqref="U122:U124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2440,34 +2443,34 @@
       </c>
     </row>
     <row r="22" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B22" s="22" t="s">
+      <c r="A22" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B22" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="17" t="s">
+      <c r="C22" s="23"/>
+      <c r="D22" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="H22" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="I22" s="22" t="s">
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I22" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="J22" s="20" t="s">
+      <c r="J22" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="K22" s="14" t="s">
+      <c r="K22" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="L22" s="22" t="s">
+      <c r="L22" s="14" t="s">
         <v>120</v>
       </c>
       <c r="M22" t="s">
@@ -2484,18 +2487,18 @@
       </c>
     </row>
     <row r="23" spans="1:22" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="22"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="14"/>
       <c r="M23" t="s">
         <v>157</v>
       </c>
@@ -2510,34 +2513,34 @@
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A24" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B24" s="16" t="s">
+      <c r="A24" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B24" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="17" t="s">
+      <c r="C24" s="21"/>
+      <c r="D24" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H24" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I24" s="18" t="s">
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="J24" s="16" t="s">
+      <c r="J24" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="K24" s="16" t="s">
+      <c r="K24" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="L24" s="23" t="s">
+      <c r="L24" s="24" t="s">
         <v>120</v>
       </c>
       <c r="M24" t="s">
@@ -2552,18 +2555,18 @@
       <c r="V24"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16"/>
-      <c r="L25" s="23"/>
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="24"/>
       <c r="M25" t="s">
         <v>73</v>
       </c>
@@ -2575,18 +2578,18 @@
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
-      <c r="L26" s="23"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="24"/>
       <c r="M26" t="s">
         <v>135</v>
       </c>
@@ -2641,34 +2644,34 @@
       </c>
     </row>
     <row r="28" spans="1:22" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B28" s="16" t="s">
+      <c r="A28" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B28" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="17" t="s">
+      <c r="C28" s="21"/>
+      <c r="D28" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H28" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I28" s="16" t="s">
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I28" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="J28" s="18" t="s">
+      <c r="J28" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="K28" s="16" t="s">
+      <c r="K28" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="L28" s="16" t="s">
+      <c r="L28" s="17" t="s">
         <v>119</v>
       </c>
       <c r="M28" t="s">
@@ -2685,18 +2688,18 @@
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="16"/>
-      <c r="L29" s="16"/>
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
       <c r="M29" t="s">
         <v>85</v>
       </c>
@@ -2708,18 +2711,18 @@
       </c>
     </row>
     <row r="30" spans="1:22" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="16"/>
-      <c r="L30" s="16"/>
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
       <c r="M30" t="s">
         <v>90</v>
       </c>
@@ -2734,34 +2737,34 @@
       </c>
     </row>
     <row r="31" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B31" s="16" t="s">
+      <c r="A31" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B31" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="17" t="s">
+      <c r="C31" s="21"/>
+      <c r="D31" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H31" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I31" s="16" t="s">
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H31" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I31" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="J31" s="18" t="s">
+      <c r="J31" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="K31" s="16" t="s">
+      <c r="K31" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="L31" s="16" t="s">
+      <c r="L31" s="17" t="s">
         <v>119</v>
       </c>
       <c r="M31" t="s">
@@ -2775,18 +2778,18 @@
       </c>
     </row>
     <row r="32" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="16"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="16"/>
-      <c r="L32" s="16"/>
+      <c r="A32" s="17"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="17"/>
       <c r="M32" t="s">
         <v>85</v>
       </c>
@@ -2798,18 +2801,18 @@
       </c>
     </row>
     <row r="33" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="16"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="16"/>
-      <c r="L33" s="16"/>
+      <c r="A33" s="17"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="17"/>
+      <c r="L33" s="17"/>
       <c r="M33" t="s">
         <v>90</v>
       </c>
@@ -2824,34 +2827,34 @@
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A34" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B34" s="16" t="s">
+      <c r="A34" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B34" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="C34" s="15"/>
-      <c r="D34" s="17" t="s">
+      <c r="C34" s="21"/>
+      <c r="D34" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H34" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I34" s="16" t="s">
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H34" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I34" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="J34" s="18" t="s">
+      <c r="J34" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="K34" s="16" t="s">
+      <c r="K34" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="L34" s="16" t="s">
+      <c r="L34" s="17" t="s">
         <v>119</v>
       </c>
       <c r="M34" t="s">
@@ -2865,18 +2868,18 @@
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="18"/>
-      <c r="K35" s="16"/>
-      <c r="L35" s="16"/>
+      <c r="A35" s="17"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="17"/>
+      <c r="L35" s="17"/>
       <c r="M35" t="s">
         <v>85</v>
       </c>
@@ -2888,18 +2891,18 @@
       </c>
     </row>
     <row r="36" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="16"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
-      <c r="I36" s="16"/>
-      <c r="J36" s="18"/>
-      <c r="K36" s="16"/>
-      <c r="L36" s="16"/>
+      <c r="A36" s="17"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="17"/>
+      <c r="L36" s="17"/>
       <c r="M36" t="s">
         <v>90</v>
       </c>
@@ -2914,34 +2917,34 @@
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A37" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B37" s="16" t="s">
+      <c r="A37" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B37" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="C37" s="15"/>
-      <c r="D37" s="17" t="s">
+      <c r="C37" s="21"/>
+      <c r="D37" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H37" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I37" s="16" t="s">
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H37" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I37" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="J37" s="18" t="s">
+      <c r="J37" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="K37" s="16" t="s">
+      <c r="K37" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="L37" s="16" t="s">
+      <c r="L37" s="17" t="s">
         <v>119</v>
       </c>
       <c r="M37" t="s">
@@ -2955,18 +2958,18 @@
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A38" s="16"/>
-      <c r="B38" s="16"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
-      <c r="I38" s="16"/>
-      <c r="J38" s="18"/>
-      <c r="K38" s="16"/>
-      <c r="L38" s="16"/>
+      <c r="A38" s="17"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="17"/>
+      <c r="L38" s="17"/>
       <c r="M38" t="s">
         <v>85</v>
       </c>
@@ -2978,18 +2981,18 @@
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A39" s="16"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
-      <c r="I39" s="16"/>
-      <c r="J39" s="18"/>
-      <c r="K39" s="16"/>
-      <c r="L39" s="16"/>
+      <c r="A39" s="17"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="17"/>
+      <c r="L39" s="17"/>
       <c r="M39" t="s">
         <v>90</v>
       </c>
@@ -3041,34 +3044,34 @@
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A41" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B41" s="16" t="s">
+      <c r="A41" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B41" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="C41" s="15"/>
-      <c r="D41" s="17" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H41" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I41" s="16" t="s">
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H41" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I41" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="J41" s="18" t="s">
+      <c r="J41" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="K41" s="16" t="s">
+      <c r="K41" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="L41" s="16" t="s">
+      <c r="L41" s="17" t="s">
         <v>119</v>
       </c>
       <c r="M41" t="s">
@@ -3082,18 +3085,18 @@
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A42" s="16"/>
-      <c r="B42" s="16"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="16"/>
-      <c r="H42" s="16"/>
-      <c r="I42" s="16"/>
-      <c r="J42" s="18"/>
-      <c r="K42" s="16"/>
-      <c r="L42" s="16"/>
+      <c r="A42" s="17"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="17"/>
+      <c r="L42" s="17"/>
       <c r="M42" t="s">
         <v>90</v>
       </c>
@@ -3105,18 +3108,18 @@
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A43" s="16"/>
-      <c r="B43" s="16"/>
-      <c r="C43" s="15"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="16"/>
-      <c r="H43" s="16"/>
-      <c r="I43" s="16"/>
-      <c r="J43" s="18"/>
-      <c r="K43" s="16"/>
-      <c r="L43" s="16"/>
+      <c r="A43" s="17"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="17"/>
+      <c r="L43" s="17"/>
       <c r="M43" t="s">
         <v>91</v>
       </c>
@@ -3129,18 +3132,18 @@
       <c r="V43"/>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A44" s="16"/>
-      <c r="B44" s="16"/>
-      <c r="C44" s="15"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="19"/>
-      <c r="G44" s="16"/>
-      <c r="H44" s="16"/>
-      <c r="I44" s="16"/>
-      <c r="J44" s="18"/>
-      <c r="K44" s="16"/>
-      <c r="L44" s="16"/>
+      <c r="A44" s="17"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="17"/>
+      <c r="I44" s="17"/>
+      <c r="J44" s="19"/>
+      <c r="K44" s="17"/>
+      <c r="L44" s="17"/>
       <c r="M44" t="s">
         <v>93</v>
       </c>
@@ -3153,18 +3156,18 @@
       <c r="V44"/>
     </row>
     <row r="45" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="16"/>
-      <c r="B45" s="16"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="16"/>
-      <c r="H45" s="16"/>
-      <c r="I45" s="16"/>
-      <c r="J45" s="18"/>
-      <c r="K45" s="16"/>
-      <c r="L45" s="16"/>
+      <c r="A45" s="17"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="17"/>
+      <c r="I45" s="17"/>
+      <c r="J45" s="19"/>
+      <c r="K45" s="17"/>
+      <c r="L45" s="17"/>
       <c r="M45" t="s">
         <v>81</v>
       </c>
@@ -3179,18 +3182,18 @@
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A46" s="16"/>
-      <c r="B46" s="16"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="19"/>
-      <c r="G46" s="16"/>
-      <c r="H46" s="16"/>
-      <c r="I46" s="16"/>
-      <c r="J46" s="18"/>
-      <c r="K46" s="16"/>
-      <c r="L46" s="16"/>
+      <c r="A46" s="17"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="17"/>
+      <c r="J46" s="19"/>
+      <c r="K46" s="17"/>
+      <c r="L46" s="17"/>
       <c r="M46" t="s">
         <v>126</v>
       </c>
@@ -3202,18 +3205,18 @@
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A47" s="16"/>
-      <c r="B47" s="16"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="19"/>
-      <c r="G47" s="16"/>
-      <c r="H47" s="16"/>
-      <c r="I47" s="16"/>
-      <c r="J47" s="18"/>
-      <c r="K47" s="16"/>
-      <c r="L47" s="16"/>
+      <c r="A47" s="17"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="17"/>
+      <c r="J47" s="19"/>
+      <c r="K47" s="17"/>
+      <c r="L47" s="17"/>
       <c r="M47" t="s">
         <v>47</v>
       </c>
@@ -3597,32 +3600,32 @@
       </c>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A57" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B57" s="16" t="s">
+      <c r="A57" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B57" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="C57" s="15"/>
-      <c r="D57" s="18"/>
-      <c r="E57" s="24"/>
-      <c r="F57" s="24"/>
-      <c r="G57" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H57" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I57" s="16" t="s">
+      <c r="C57" s="21"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="22"/>
+      <c r="F57" s="22"/>
+      <c r="G57" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H57" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I57" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="J57" s="18" t="s">
+      <c r="J57" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="K57" s="16" t="s">
+      <c r="K57" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="L57" s="23" t="s">
+      <c r="L57" s="24" t="s">
         <v>120</v>
       </c>
       <c r="M57" t="s">
@@ -3636,18 +3639,18 @@
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A58" s="16"/>
-      <c r="B58" s="16"/>
-      <c r="C58" s="15"/>
-      <c r="D58" s="18"/>
-      <c r="E58" s="24"/>
-      <c r="F58" s="24"/>
-      <c r="G58" s="16"/>
-      <c r="H58" s="16"/>
-      <c r="I58" s="16"/>
-      <c r="J58" s="18"/>
-      <c r="K58" s="16"/>
-      <c r="L58" s="23"/>
+      <c r="A58" s="17"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="22"/>
+      <c r="F58" s="22"/>
+      <c r="G58" s="17"/>
+      <c r="H58" s="17"/>
+      <c r="I58" s="17"/>
+      <c r="J58" s="19"/>
+      <c r="K58" s="17"/>
+      <c r="L58" s="24"/>
       <c r="M58" t="s">
         <v>132</v>
       </c>
@@ -3659,18 +3662,18 @@
       </c>
     </row>
     <row r="59" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A59" s="16"/>
-      <c r="B59" s="16"/>
-      <c r="C59" s="15"/>
-      <c r="D59" s="18"/>
-      <c r="E59" s="24"/>
-      <c r="F59" s="24"/>
-      <c r="G59" s="16"/>
-      <c r="H59" s="16"/>
-      <c r="I59" s="16"/>
-      <c r="J59" s="18"/>
-      <c r="K59" s="16"/>
-      <c r="L59" s="23"/>
+      <c r="A59" s="17"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="22"/>
+      <c r="F59" s="22"/>
+      <c r="G59" s="17"/>
+      <c r="H59" s="17"/>
+      <c r="I59" s="17"/>
+      <c r="J59" s="19"/>
+      <c r="K59" s="17"/>
+      <c r="L59" s="24"/>
       <c r="M59" t="s">
         <v>133</v>
       </c>
@@ -3758,34 +3761,34 @@
       </c>
     </row>
     <row r="62" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="B62" s="22" t="s">
+      <c r="A62" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B62" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="C62" s="14"/>
-      <c r="D62" s="20" t="s">
+      <c r="C62" s="23"/>
+      <c r="D62" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="E62" s="21"/>
-      <c r="F62" s="21"/>
-      <c r="G62" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="H62" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="I62" s="16" t="s">
+      <c r="E62" s="25"/>
+      <c r="F62" s="25"/>
+      <c r="G62" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H62" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I62" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="J62" s="18" t="s">
+      <c r="J62" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="K62" s="16" t="s">
+      <c r="K62" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="L62" s="16" t="s">
+      <c r="L62" s="17" t="s">
         <v>119</v>
       </c>
       <c r="M62" t="s">
@@ -3802,18 +3805,18 @@
       </c>
     </row>
     <row r="63" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A63" s="22"/>
-      <c r="B63" s="22"/>
-      <c r="C63" s="14"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="21"/>
-      <c r="F63" s="21"/>
-      <c r="G63" s="22"/>
-      <c r="H63" s="22"/>
-      <c r="I63" s="16"/>
-      <c r="J63" s="18"/>
-      <c r="K63" s="16"/>
-      <c r="L63" s="16"/>
+      <c r="A63" s="14"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="23"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="25"/>
+      <c r="F63" s="25"/>
+      <c r="G63" s="14"/>
+      <c r="H63" s="14"/>
+      <c r="I63" s="17"/>
+      <c r="J63" s="19"/>
+      <c r="K63" s="17"/>
+      <c r="L63" s="17"/>
       <c r="M63" t="s">
         <v>182</v>
       </c>
@@ -3828,34 +3831,34 @@
       </c>
     </row>
     <row r="64" spans="1:22" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B64" s="16" t="s">
+      <c r="A64" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B64" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="C64" s="15"/>
-      <c r="D64" s="20" t="s">
+      <c r="C64" s="21"/>
+      <c r="D64" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="E64" s="21"/>
-      <c r="F64" s="21"/>
-      <c r="G64" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H64" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I64" s="16" t="s">
+      <c r="E64" s="25"/>
+      <c r="F64" s="25"/>
+      <c r="G64" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H64" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I64" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="J64" s="16" t="s">
+      <c r="J64" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="K64" s="16" t="s">
+      <c r="K64" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="L64" s="16" t="s">
+      <c r="L64" s="17" t="s">
         <v>120</v>
       </c>
       <c r="M64" t="s">
@@ -3872,18 +3875,18 @@
       </c>
     </row>
     <row r="65" spans="1:22" ht="90" x14ac:dyDescent="0.25">
-      <c r="A65" s="16"/>
-      <c r="B65" s="16"/>
-      <c r="C65" s="15"/>
-      <c r="D65" s="20"/>
-      <c r="E65" s="21"/>
-      <c r="F65" s="21"/>
-      <c r="G65" s="16"/>
-      <c r="H65" s="16"/>
-      <c r="I65" s="16"/>
-      <c r="J65" s="16"/>
-      <c r="K65" s="16"/>
-      <c r="L65" s="16"/>
+      <c r="A65" s="17"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="21"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="25"/>
+      <c r="F65" s="25"/>
+      <c r="G65" s="17"/>
+      <c r="H65" s="17"/>
+      <c r="I65" s="17"/>
+      <c r="J65" s="17"/>
+      <c r="K65" s="17"/>
+      <c r="L65" s="17"/>
       <c r="M65" t="s">
         <v>187</v>
       </c>
@@ -3898,18 +3901,18 @@
       </c>
     </row>
     <row r="66" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A66" s="16"/>
-      <c r="B66" s="16"/>
-      <c r="C66" s="15"/>
-      <c r="D66" s="20"/>
-      <c r="E66" s="21"/>
-      <c r="F66" s="21"/>
-      <c r="G66" s="16"/>
-      <c r="H66" s="16"/>
-      <c r="I66" s="16"/>
-      <c r="J66" s="16"/>
-      <c r="K66" s="16"/>
-      <c r="L66" s="16"/>
+      <c r="A66" s="17"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="21"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="25"/>
+      <c r="F66" s="25"/>
+      <c r="G66" s="17"/>
+      <c r="H66" s="17"/>
+      <c r="I66" s="17"/>
+      <c r="J66" s="17"/>
+      <c r="K66" s="17"/>
+      <c r="L66" s="17"/>
       <c r="M66" t="s">
         <v>190</v>
       </c>
@@ -3921,18 +3924,18 @@
       </c>
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A67" s="16"/>
-      <c r="B67" s="16"/>
-      <c r="C67" s="15"/>
-      <c r="D67" s="20"/>
-      <c r="E67" s="21"/>
-      <c r="F67" s="21"/>
-      <c r="G67" s="16"/>
-      <c r="H67" s="16"/>
-      <c r="I67" s="16"/>
-      <c r="J67" s="16"/>
-      <c r="K67" s="16"/>
-      <c r="L67" s="16"/>
+      <c r="A67" s="17"/>
+      <c r="B67" s="17"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="15"/>
+      <c r="E67" s="25"/>
+      <c r="F67" s="25"/>
+      <c r="G67" s="17"/>
+      <c r="H67" s="17"/>
+      <c r="I67" s="17"/>
+      <c r="J67" s="17"/>
+      <c r="K67" s="17"/>
+      <c r="L67" s="17"/>
       <c r="M67" t="s">
         <v>191</v>
       </c>
@@ -3944,34 +3947,34 @@
       </c>
     </row>
     <row r="68" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B68" s="16" t="s">
+      <c r="A68" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B68" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="C68" s="15"/>
-      <c r="D68" s="20" t="s">
+      <c r="C68" s="21"/>
+      <c r="D68" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="E68" s="21"/>
-      <c r="F68" s="21"/>
-      <c r="G68" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H68" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I68" s="16" t="s">
+      <c r="E68" s="25"/>
+      <c r="F68" s="25"/>
+      <c r="G68" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H68" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I68" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="J68" s="16" t="s">
+      <c r="J68" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="K68" s="16" t="s">
+      <c r="K68" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="L68" s="16" t="s">
+      <c r="L68" s="17" t="s">
         <v>120</v>
       </c>
       <c r="M68" t="s">
@@ -3988,18 +3991,18 @@
       </c>
     </row>
     <row r="69" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A69" s="16"/>
-      <c r="B69" s="16"/>
-      <c r="C69" s="15"/>
-      <c r="D69" s="20"/>
-      <c r="E69" s="21"/>
-      <c r="F69" s="21"/>
-      <c r="G69" s="16"/>
-      <c r="H69" s="16"/>
-      <c r="I69" s="16"/>
-      <c r="J69" s="16"/>
-      <c r="K69" s="16"/>
-      <c r="L69" s="16"/>
+      <c r="A69" s="17"/>
+      <c r="B69" s="17"/>
+      <c r="C69" s="21"/>
+      <c r="D69" s="15"/>
+      <c r="E69" s="25"/>
+      <c r="F69" s="25"/>
+      <c r="G69" s="17"/>
+      <c r="H69" s="17"/>
+      <c r="I69" s="17"/>
+      <c r="J69" s="17"/>
+      <c r="K69" s="17"/>
+      <c r="L69" s="17"/>
       <c r="M69" t="s">
         <v>187</v>
       </c>
@@ -4011,18 +4014,18 @@
       </c>
     </row>
     <row r="70" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A70" s="16"/>
-      <c r="B70" s="16"/>
-      <c r="C70" s="15"/>
-      <c r="D70" s="20"/>
-      <c r="E70" s="21"/>
-      <c r="F70" s="21"/>
-      <c r="G70" s="16"/>
-      <c r="H70" s="16"/>
-      <c r="I70" s="16"/>
-      <c r="J70" s="16"/>
-      <c r="K70" s="16"/>
-      <c r="L70" s="16"/>
+      <c r="A70" s="17"/>
+      <c r="B70" s="17"/>
+      <c r="C70" s="21"/>
+      <c r="D70" s="15"/>
+      <c r="E70" s="25"/>
+      <c r="F70" s="25"/>
+      <c r="G70" s="17"/>
+      <c r="H70" s="17"/>
+      <c r="I70" s="17"/>
+      <c r="J70" s="17"/>
+      <c r="K70" s="17"/>
+      <c r="L70" s="17"/>
       <c r="M70" t="s">
         <v>190</v>
       </c>
@@ -4034,18 +4037,18 @@
       </c>
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A71" s="16"/>
-      <c r="B71" s="16"/>
-      <c r="C71" s="15"/>
-      <c r="D71" s="20"/>
-      <c r="E71" s="21"/>
-      <c r="F71" s="21"/>
-      <c r="G71" s="16"/>
-      <c r="H71" s="16"/>
-      <c r="I71" s="16"/>
-      <c r="J71" s="16"/>
-      <c r="K71" s="16"/>
-      <c r="L71" s="16"/>
+      <c r="A71" s="17"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="21"/>
+      <c r="D71" s="15"/>
+      <c r="E71" s="25"/>
+      <c r="F71" s="25"/>
+      <c r="G71" s="17"/>
+      <c r="H71" s="17"/>
+      <c r="I71" s="17"/>
+      <c r="J71" s="17"/>
+      <c r="K71" s="17"/>
+      <c r="L71" s="17"/>
       <c r="M71" t="s">
         <v>191</v>
       </c>
@@ -4057,34 +4060,34 @@
       </c>
     </row>
     <row r="72" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A72" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B72" s="16" t="s">
+      <c r="A72" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B72" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="C72" s="15"/>
-      <c r="D72" s="20" t="s">
+      <c r="C72" s="21"/>
+      <c r="D72" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="E72" s="21"/>
-      <c r="F72" s="21"/>
-      <c r="G72" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H72" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I72" s="16" t="s">
+      <c r="E72" s="25"/>
+      <c r="F72" s="25"/>
+      <c r="G72" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H72" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I72" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="J72" s="16" t="s">
+      <c r="J72" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="K72" s="16" t="s">
+      <c r="K72" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="L72" s="16" t="s">
+      <c r="L72" s="17" t="s">
         <v>120</v>
       </c>
       <c r="M72" t="s">
@@ -4098,18 +4101,18 @@
       </c>
     </row>
     <row r="73" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A73" s="16"/>
-      <c r="B73" s="16"/>
-      <c r="C73" s="15"/>
-      <c r="D73" s="20"/>
-      <c r="E73" s="21"/>
-      <c r="F73" s="21"/>
-      <c r="G73" s="16"/>
-      <c r="H73" s="16"/>
-      <c r="I73" s="16"/>
-      <c r="J73" s="16"/>
-      <c r="K73" s="16"/>
-      <c r="L73" s="16"/>
+      <c r="A73" s="17"/>
+      <c r="B73" s="17"/>
+      <c r="C73" s="21"/>
+      <c r="D73" s="15"/>
+      <c r="E73" s="25"/>
+      <c r="F73" s="25"/>
+      <c r="G73" s="17"/>
+      <c r="H73" s="17"/>
+      <c r="I73" s="17"/>
+      <c r="J73" s="17"/>
+      <c r="K73" s="17"/>
+      <c r="L73" s="17"/>
       <c r="M73" t="s">
         <v>187</v>
       </c>
@@ -4121,18 +4124,18 @@
       </c>
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A74" s="16"/>
-      <c r="B74" s="16"/>
-      <c r="C74" s="15"/>
-      <c r="D74" s="20"/>
-      <c r="E74" s="21"/>
-      <c r="F74" s="21"/>
-      <c r="G74" s="16"/>
-      <c r="H74" s="16"/>
-      <c r="I74" s="16"/>
-      <c r="J74" s="16"/>
-      <c r="K74" s="16"/>
-      <c r="L74" s="16"/>
+      <c r="A74" s="17"/>
+      <c r="B74" s="17"/>
+      <c r="C74" s="21"/>
+      <c r="D74" s="15"/>
+      <c r="E74" s="25"/>
+      <c r="F74" s="25"/>
+      <c r="G74" s="17"/>
+      <c r="H74" s="17"/>
+      <c r="I74" s="17"/>
+      <c r="J74" s="17"/>
+      <c r="K74" s="17"/>
+      <c r="L74" s="17"/>
       <c r="M74" t="s">
         <v>190</v>
       </c>
@@ -4144,18 +4147,18 @@
       </c>
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A75" s="16"/>
-      <c r="B75" s="16"/>
-      <c r="C75" s="15"/>
-      <c r="D75" s="20"/>
-      <c r="E75" s="21"/>
-      <c r="F75" s="21"/>
-      <c r="G75" s="16"/>
-      <c r="H75" s="16"/>
-      <c r="I75" s="16"/>
-      <c r="J75" s="16"/>
-      <c r="K75" s="16"/>
-      <c r="L75" s="16"/>
+      <c r="A75" s="17"/>
+      <c r="B75" s="17"/>
+      <c r="C75" s="21"/>
+      <c r="D75" s="15"/>
+      <c r="E75" s="25"/>
+      <c r="F75" s="25"/>
+      <c r="G75" s="17"/>
+      <c r="H75" s="17"/>
+      <c r="I75" s="17"/>
+      <c r="J75" s="17"/>
+      <c r="K75" s="17"/>
+      <c r="L75" s="17"/>
       <c r="M75" t="s">
         <v>191</v>
       </c>
@@ -4243,34 +4246,34 @@
       </c>
     </row>
     <row r="78" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B78" s="16" t="s">
+      <c r="A78" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B78" s="17" t="s">
         <v>207</v>
       </c>
-      <c r="C78" s="15"/>
-      <c r="D78" s="20" t="s">
+      <c r="C78" s="21"/>
+      <c r="D78" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="E78" s="21"/>
-      <c r="F78" s="21"/>
-      <c r="G78" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H78" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I78" s="16" t="s">
+      <c r="E78" s="25"/>
+      <c r="F78" s="25"/>
+      <c r="G78" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H78" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I78" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="J78" s="16" t="s">
+      <c r="J78" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="K78" s="16" t="s">
+      <c r="K78" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="L78" s="16" t="s">
+      <c r="L78" s="17" t="s">
         <v>120</v>
       </c>
       <c r="M78" t="s">
@@ -4287,18 +4290,18 @@
       </c>
     </row>
     <row r="79" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A79" s="16"/>
-      <c r="B79" s="16"/>
-      <c r="C79" s="15"/>
-      <c r="D79" s="20"/>
-      <c r="E79" s="21"/>
-      <c r="F79" s="21"/>
-      <c r="G79" s="16"/>
-      <c r="H79" s="16"/>
-      <c r="I79" s="16"/>
-      <c r="J79" s="16"/>
-      <c r="K79" s="16"/>
-      <c r="L79" s="16"/>
+      <c r="A79" s="17"/>
+      <c r="B79" s="17"/>
+      <c r="C79" s="21"/>
+      <c r="D79" s="15"/>
+      <c r="E79" s="25"/>
+      <c r="F79" s="25"/>
+      <c r="G79" s="17"/>
+      <c r="H79" s="17"/>
+      <c r="I79" s="17"/>
+      <c r="J79" s="17"/>
+      <c r="K79" s="17"/>
+      <c r="L79" s="17"/>
       <c r="M79" t="s">
         <v>212</v>
       </c>
@@ -4313,18 +4316,18 @@
       </c>
     </row>
     <row r="80" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="16"/>
-      <c r="B80" s="16"/>
-      <c r="C80" s="15"/>
-      <c r="D80" s="20"/>
-      <c r="E80" s="21"/>
-      <c r="F80" s="21"/>
-      <c r="G80" s="16"/>
-      <c r="H80" s="16"/>
-      <c r="I80" s="16"/>
-      <c r="J80" s="16"/>
-      <c r="K80" s="16"/>
-      <c r="L80" s="16"/>
+      <c r="A80" s="17"/>
+      <c r="B80" s="17"/>
+      <c r="C80" s="21"/>
+      <c r="D80" s="15"/>
+      <c r="E80" s="25"/>
+      <c r="F80" s="25"/>
+      <c r="G80" s="17"/>
+      <c r="H80" s="17"/>
+      <c r="I80" s="17"/>
+      <c r="J80" s="17"/>
+      <c r="K80" s="17"/>
+      <c r="L80" s="17"/>
       <c r="M80" t="s">
         <v>214</v>
       </c>
@@ -4339,18 +4342,18 @@
       </c>
     </row>
     <row r="81" spans="1:22" ht="60" x14ac:dyDescent="0.25">
-      <c r="A81" s="16"/>
-      <c r="B81" s="16"/>
-      <c r="C81" s="15"/>
-      <c r="D81" s="20"/>
-      <c r="E81" s="21"/>
-      <c r="F81" s="21"/>
-      <c r="G81" s="16"/>
-      <c r="H81" s="16"/>
-      <c r="I81" s="16"/>
-      <c r="J81" s="16"/>
-      <c r="K81" s="16"/>
-      <c r="L81" s="16"/>
+      <c r="A81" s="17"/>
+      <c r="B81" s="17"/>
+      <c r="C81" s="21"/>
+      <c r="D81" s="15"/>
+      <c r="E81" s="25"/>
+      <c r="F81" s="25"/>
+      <c r="G81" s="17"/>
+      <c r="H81" s="17"/>
+      <c r="I81" s="17"/>
+      <c r="J81" s="17"/>
+      <c r="K81" s="17"/>
+      <c r="L81" s="17"/>
       <c r="M81" t="s">
         <v>132</v>
       </c>
@@ -4365,18 +4368,18 @@
       </c>
     </row>
     <row r="82" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A82" s="16"/>
-      <c r="B82" s="16"/>
-      <c r="C82" s="15"/>
-      <c r="D82" s="20"/>
-      <c r="E82" s="21"/>
-      <c r="F82" s="21"/>
-      <c r="G82" s="16"/>
-      <c r="H82" s="16"/>
-      <c r="I82" s="16"/>
-      <c r="J82" s="16"/>
-      <c r="K82" s="16"/>
-      <c r="L82" s="16"/>
+      <c r="A82" s="17"/>
+      <c r="B82" s="17"/>
+      <c r="C82" s="21"/>
+      <c r="D82" s="15"/>
+      <c r="E82" s="25"/>
+      <c r="F82" s="25"/>
+      <c r="G82" s="17"/>
+      <c r="H82" s="17"/>
+      <c r="I82" s="17"/>
+      <c r="J82" s="17"/>
+      <c r="K82" s="17"/>
+      <c r="L82" s="17"/>
       <c r="M82" t="s">
         <v>133</v>
       </c>
@@ -4388,32 +4391,32 @@
       </c>
     </row>
     <row r="83" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="B83" s="16" t="s">
+      <c r="A83" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B83" s="17" t="s">
         <v>217</v>
       </c>
-      <c r="C83" s="15"/>
-      <c r="D83" s="20" t="s">
+      <c r="C83" s="21"/>
+      <c r="D83" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="E83" s="21"/>
-      <c r="F83" s="21"/>
-      <c r="G83" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H83" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I83" s="16"/>
-      <c r="J83" s="16" t="s">
+      <c r="E83" s="25"/>
+      <c r="F83" s="25"/>
+      <c r="G83" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H83" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I83" s="17"/>
+      <c r="J83" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="K83" s="16" t="s">
+      <c r="K83" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="L83" s="16" t="s">
+      <c r="L83" s="17" t="s">
         <v>120</v>
       </c>
       <c r="M83" t="s">
@@ -4427,18 +4430,18 @@
       </c>
     </row>
     <row r="84" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A84" s="15"/>
-      <c r="B84" s="16"/>
-      <c r="C84" s="15"/>
-      <c r="D84" s="20"/>
-      <c r="E84" s="21"/>
-      <c r="F84" s="21"/>
-      <c r="G84" s="16"/>
-      <c r="H84" s="16"/>
-      <c r="I84" s="16"/>
-      <c r="J84" s="16"/>
-      <c r="K84" s="16"/>
-      <c r="L84" s="16"/>
+      <c r="A84" s="21"/>
+      <c r="B84" s="17"/>
+      <c r="C84" s="21"/>
+      <c r="D84" s="15"/>
+      <c r="E84" s="25"/>
+      <c r="F84" s="25"/>
+      <c r="G84" s="17"/>
+      <c r="H84" s="17"/>
+      <c r="I84" s="17"/>
+      <c r="J84" s="17"/>
+      <c r="K84" s="17"/>
+      <c r="L84" s="17"/>
       <c r="M84" t="s">
         <v>212</v>
       </c>
@@ -4450,18 +4453,18 @@
       </c>
     </row>
     <row r="85" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A85" s="15"/>
-      <c r="B85" s="16"/>
-      <c r="C85" s="15"/>
-      <c r="D85" s="20"/>
-      <c r="E85" s="21"/>
-      <c r="F85" s="21"/>
-      <c r="G85" s="16"/>
-      <c r="H85" s="16"/>
-      <c r="I85" s="16"/>
-      <c r="J85" s="16"/>
-      <c r="K85" s="16"/>
-      <c r="L85" s="16"/>
+      <c r="A85" s="21"/>
+      <c r="B85" s="17"/>
+      <c r="C85" s="21"/>
+      <c r="D85" s="15"/>
+      <c r="E85" s="25"/>
+      <c r="F85" s="25"/>
+      <c r="G85" s="17"/>
+      <c r="H85" s="17"/>
+      <c r="I85" s="17"/>
+      <c r="J85" s="17"/>
+      <c r="K85" s="17"/>
+      <c r="L85" s="17"/>
       <c r="M85" t="s">
         <v>214</v>
       </c>
@@ -4473,18 +4476,18 @@
       </c>
     </row>
     <row r="86" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A86" s="15"/>
-      <c r="B86" s="16"/>
-      <c r="C86" s="15"/>
-      <c r="D86" s="20"/>
-      <c r="E86" s="21"/>
-      <c r="F86" s="21"/>
-      <c r="G86" s="16"/>
-      <c r="H86" s="16"/>
-      <c r="I86" s="16"/>
-      <c r="J86" s="16"/>
-      <c r="K86" s="16"/>
-      <c r="L86" s="16"/>
+      <c r="A86" s="21"/>
+      <c r="B86" s="17"/>
+      <c r="C86" s="21"/>
+      <c r="D86" s="15"/>
+      <c r="E86" s="25"/>
+      <c r="F86" s="25"/>
+      <c r="G86" s="17"/>
+      <c r="H86" s="17"/>
+      <c r="I86" s="17"/>
+      <c r="J86" s="17"/>
+      <c r="K86" s="17"/>
+      <c r="L86" s="17"/>
       <c r="M86" t="s">
         <v>132</v>
       </c>
@@ -4496,18 +4499,18 @@
       </c>
     </row>
     <row r="87" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A87" s="15"/>
-      <c r="B87" s="16"/>
-      <c r="C87" s="15"/>
-      <c r="D87" s="20"/>
-      <c r="E87" s="21"/>
-      <c r="F87" s="21"/>
-      <c r="G87" s="16"/>
-      <c r="H87" s="16"/>
-      <c r="I87" s="16"/>
-      <c r="J87" s="16"/>
-      <c r="K87" s="16"/>
-      <c r="L87" s="16"/>
+      <c r="A87" s="21"/>
+      <c r="B87" s="17"/>
+      <c r="C87" s="21"/>
+      <c r="D87" s="15"/>
+      <c r="E87" s="25"/>
+      <c r="F87" s="25"/>
+      <c r="G87" s="17"/>
+      <c r="H87" s="17"/>
+      <c r="I87" s="17"/>
+      <c r="J87" s="17"/>
+      <c r="K87" s="17"/>
+      <c r="L87" s="17"/>
       <c r="M87" t="s">
         <v>133</v>
       </c>
@@ -4522,34 +4525,34 @@
       </c>
     </row>
     <row r="88" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B88" s="16" t="s">
+      <c r="A88" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B88" s="17" t="s">
         <v>223</v>
       </c>
-      <c r="C88" s="15"/>
-      <c r="D88" s="20" t="s">
+      <c r="C88" s="21"/>
+      <c r="D88" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="E88" s="21"/>
-      <c r="F88" s="21"/>
-      <c r="G88" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H88" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I88" s="16" t="s">
+      <c r="E88" s="25"/>
+      <c r="F88" s="25"/>
+      <c r="G88" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H88" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I88" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="J88" s="16" t="s">
+      <c r="J88" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="K88" s="16" t="s">
+      <c r="K88" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="L88" s="16" t="s">
+      <c r="L88" s="17" t="s">
         <v>120</v>
       </c>
       <c r="M88" t="s">
@@ -4566,18 +4569,18 @@
       </c>
     </row>
     <row r="89" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="16"/>
-      <c r="B89" s="16"/>
-      <c r="C89" s="15"/>
-      <c r="D89" s="20"/>
-      <c r="E89" s="21"/>
-      <c r="F89" s="21"/>
-      <c r="G89" s="16"/>
-      <c r="H89" s="16"/>
-      <c r="I89" s="16"/>
-      <c r="J89" s="16"/>
-      <c r="K89" s="16"/>
-      <c r="L89" s="16"/>
+      <c r="A89" s="17"/>
+      <c r="B89" s="17"/>
+      <c r="C89" s="21"/>
+      <c r="D89" s="15"/>
+      <c r="E89" s="25"/>
+      <c r="F89" s="25"/>
+      <c r="G89" s="17"/>
+      <c r="H89" s="17"/>
+      <c r="I89" s="17"/>
+      <c r="J89" s="17"/>
+      <c r="K89" s="17"/>
+      <c r="L89" s="17"/>
       <c r="M89" t="s">
         <v>47</v>
       </c>
@@ -4592,18 +4595,18 @@
       </c>
     </row>
     <row r="90" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="16"/>
-      <c r="B90" s="16"/>
-      <c r="C90" s="15"/>
-      <c r="D90" s="20"/>
-      <c r="E90" s="21"/>
-      <c r="F90" s="21"/>
-      <c r="G90" s="16"/>
-      <c r="H90" s="16"/>
-      <c r="I90" s="16"/>
-      <c r="J90" s="16"/>
-      <c r="K90" s="16"/>
-      <c r="L90" s="16"/>
+      <c r="A90" s="17"/>
+      <c r="B90" s="17"/>
+      <c r="C90" s="21"/>
+      <c r="D90" s="15"/>
+      <c r="E90" s="25"/>
+      <c r="F90" s="25"/>
+      <c r="G90" s="17"/>
+      <c r="H90" s="17"/>
+      <c r="I90" s="17"/>
+      <c r="J90" s="17"/>
+      <c r="K90" s="17"/>
+      <c r="L90" s="17"/>
       <c r="M90" t="s">
         <v>180</v>
       </c>
@@ -4618,18 +4621,18 @@
       </c>
     </row>
     <row r="91" spans="1:22" ht="75" x14ac:dyDescent="0.25">
-      <c r="A91" s="16"/>
-      <c r="B91" s="16"/>
-      <c r="C91" s="15"/>
-      <c r="D91" s="20"/>
-      <c r="E91" s="21"/>
-      <c r="F91" s="21"/>
-      <c r="G91" s="16"/>
-      <c r="H91" s="16"/>
-      <c r="I91" s="16"/>
-      <c r="J91" s="16"/>
-      <c r="K91" s="16"/>
-      <c r="L91" s="16"/>
+      <c r="A91" s="17"/>
+      <c r="B91" s="17"/>
+      <c r="C91" s="21"/>
+      <c r="D91" s="15"/>
+      <c r="E91" s="25"/>
+      <c r="F91" s="25"/>
+      <c r="G91" s="17"/>
+      <c r="H91" s="17"/>
+      <c r="I91" s="17"/>
+      <c r="J91" s="17"/>
+      <c r="K91" s="17"/>
+      <c r="L91" s="17"/>
       <c r="M91" t="s">
         <v>214</v>
       </c>
@@ -4644,18 +4647,18 @@
       </c>
     </row>
     <row r="92" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A92" s="16"/>
-      <c r="B92" s="16"/>
-      <c r="C92" s="15"/>
-      <c r="D92" s="20"/>
-      <c r="E92" s="21"/>
-      <c r="F92" s="21"/>
-      <c r="G92" s="16"/>
-      <c r="H92" s="16"/>
-      <c r="I92" s="16"/>
-      <c r="J92" s="16"/>
-      <c r="K92" s="16"/>
-      <c r="L92" s="16"/>
+      <c r="A92" s="17"/>
+      <c r="B92" s="17"/>
+      <c r="C92" s="21"/>
+      <c r="D92" s="15"/>
+      <c r="E92" s="25"/>
+      <c r="F92" s="25"/>
+      <c r="G92" s="17"/>
+      <c r="H92" s="17"/>
+      <c r="I92" s="17"/>
+      <c r="J92" s="17"/>
+      <c r="K92" s="17"/>
+      <c r="L92" s="17"/>
       <c r="M92" t="s">
         <v>132</v>
       </c>
@@ -4667,18 +4670,18 @@
       </c>
     </row>
     <row r="93" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A93" s="16"/>
-      <c r="B93" s="16"/>
-      <c r="C93" s="15"/>
-      <c r="D93" s="20"/>
-      <c r="E93" s="21"/>
-      <c r="F93" s="21"/>
-      <c r="G93" s="16"/>
-      <c r="H93" s="16"/>
-      <c r="I93" s="16"/>
-      <c r="J93" s="16"/>
-      <c r="K93" s="16"/>
-      <c r="L93" s="16"/>
+      <c r="A93" s="17"/>
+      <c r="B93" s="17"/>
+      <c r="C93" s="21"/>
+      <c r="D93" s="15"/>
+      <c r="E93" s="25"/>
+      <c r="F93" s="25"/>
+      <c r="G93" s="17"/>
+      <c r="H93" s="17"/>
+      <c r="I93" s="17"/>
+      <c r="J93" s="17"/>
+      <c r="K93" s="17"/>
+      <c r="L93" s="17"/>
       <c r="M93" t="s">
         <v>133</v>
       </c>
@@ -4690,34 +4693,34 @@
       </c>
     </row>
     <row r="94" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A94" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B94" s="16" t="s">
+      <c r="A94" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B94" s="17" t="s">
         <v>233</v>
       </c>
-      <c r="C94" s="15"/>
-      <c r="D94" s="20" t="s">
+      <c r="C94" s="21"/>
+      <c r="D94" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="E94" s="21"/>
-      <c r="F94" s="21"/>
-      <c r="G94" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H94" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I94" s="16" t="s">
+      <c r="E94" s="25"/>
+      <c r="F94" s="25"/>
+      <c r="G94" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H94" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I94" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="J94" s="16" t="s">
+      <c r="J94" s="17" t="s">
         <v>234</v>
       </c>
-      <c r="K94" s="16" t="s">
+      <c r="K94" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="L94" s="16" t="s">
+      <c r="L94" s="17" t="s">
         <v>120</v>
       </c>
       <c r="M94" t="s">
@@ -4731,18 +4734,18 @@
       </c>
     </row>
     <row r="95" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A95" s="16"/>
-      <c r="B95" s="16"/>
-      <c r="C95" s="15"/>
-      <c r="D95" s="20"/>
-      <c r="E95" s="21"/>
-      <c r="F95" s="21"/>
-      <c r="G95" s="16"/>
-      <c r="H95" s="16"/>
-      <c r="I95" s="16"/>
-      <c r="J95" s="16"/>
-      <c r="K95" s="16"/>
-      <c r="L95" s="16"/>
+      <c r="A95" s="17"/>
+      <c r="B95" s="17"/>
+      <c r="C95" s="21"/>
+      <c r="D95" s="15"/>
+      <c r="E95" s="25"/>
+      <c r="F95" s="25"/>
+      <c r="G95" s="17"/>
+      <c r="H95" s="17"/>
+      <c r="I95" s="17"/>
+      <c r="J95" s="17"/>
+      <c r="K95" s="17"/>
+      <c r="L95" s="17"/>
       <c r="M95" t="s">
         <v>212</v>
       </c>
@@ -4757,18 +4760,18 @@
       </c>
     </row>
     <row r="96" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A96" s="16"/>
-      <c r="B96" s="16"/>
-      <c r="C96" s="15"/>
-      <c r="D96" s="20"/>
-      <c r="E96" s="21"/>
-      <c r="F96" s="21"/>
-      <c r="G96" s="16"/>
-      <c r="H96" s="16"/>
-      <c r="I96" s="16"/>
-      <c r="J96" s="16"/>
-      <c r="K96" s="16"/>
-      <c r="L96" s="16"/>
+      <c r="A96" s="17"/>
+      <c r="B96" s="17"/>
+      <c r="C96" s="21"/>
+      <c r="D96" s="15"/>
+      <c r="E96" s="25"/>
+      <c r="F96" s="25"/>
+      <c r="G96" s="17"/>
+      <c r="H96" s="17"/>
+      <c r="I96" s="17"/>
+      <c r="J96" s="17"/>
+      <c r="K96" s="17"/>
+      <c r="L96" s="17"/>
       <c r="M96" t="s">
         <v>212</v>
       </c>
@@ -4783,34 +4786,34 @@
       </c>
     </row>
     <row r="97" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A97" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B97" s="16" t="s">
+      <c r="A97" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B97" s="17" t="s">
         <v>239</v>
       </c>
-      <c r="C97" s="15"/>
-      <c r="D97" s="20" t="s">
+      <c r="C97" s="21"/>
+      <c r="D97" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="E97" s="21"/>
-      <c r="F97" s="21"/>
-      <c r="G97" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H97" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I97" s="16" t="s">
+      <c r="E97" s="25"/>
+      <c r="F97" s="25"/>
+      <c r="G97" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H97" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I97" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="J97" s="16" t="s">
+      <c r="J97" s="17" t="s">
         <v>241</v>
       </c>
-      <c r="K97" s="16" t="s">
+      <c r="K97" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="L97" s="16" t="s">
+      <c r="L97" s="17" t="s">
         <v>120</v>
       </c>
       <c r="M97" t="s">
@@ -4824,18 +4827,18 @@
       </c>
     </row>
     <row r="98" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A98" s="16"/>
-      <c r="B98" s="16"/>
-      <c r="C98" s="15"/>
-      <c r="D98" s="20"/>
-      <c r="E98" s="21"/>
-      <c r="F98" s="21"/>
-      <c r="G98" s="16"/>
-      <c r="H98" s="16"/>
-      <c r="I98" s="16"/>
-      <c r="J98" s="16"/>
-      <c r="K98" s="16"/>
-      <c r="L98" s="16"/>
+      <c r="A98" s="17"/>
+      <c r="B98" s="17"/>
+      <c r="C98" s="21"/>
+      <c r="D98" s="15"/>
+      <c r="E98" s="25"/>
+      <c r="F98" s="25"/>
+      <c r="G98" s="17"/>
+      <c r="H98" s="17"/>
+      <c r="I98" s="17"/>
+      <c r="J98" s="17"/>
+      <c r="K98" s="17"/>
+      <c r="L98" s="17"/>
       <c r="M98" t="s">
         <v>212</v>
       </c>
@@ -4949,34 +4952,34 @@
       </c>
     </row>
     <row r="102" spans="1:22" ht="60" x14ac:dyDescent="0.25">
-      <c r="A102" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B102" s="16" t="s">
+      <c r="A102" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B102" s="17" t="s">
         <v>250</v>
       </c>
-      <c r="C102" s="15"/>
-      <c r="D102" s="20" t="s">
+      <c r="C102" s="21"/>
+      <c r="D102" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="E102" s="21"/>
-      <c r="F102" s="21"/>
-      <c r="G102" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H102" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I102" s="16" t="s">
+      <c r="E102" s="25"/>
+      <c r="F102" s="25"/>
+      <c r="G102" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H102" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I102" s="17" t="s">
         <v>251</v>
       </c>
-      <c r="J102" s="16" t="s">
+      <c r="J102" s="17" t="s">
         <v>252</v>
       </c>
-      <c r="K102" s="16" t="s">
+      <c r="K102" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="L102" s="16" t="s">
+      <c r="L102" s="17" t="s">
         <v>120</v>
       </c>
       <c r="M102" t="s">
@@ -4993,18 +4996,18 @@
       </c>
     </row>
     <row r="103" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A103" s="16"/>
-      <c r="B103" s="16"/>
-      <c r="C103" s="15"/>
-      <c r="D103" s="20"/>
-      <c r="E103" s="21"/>
-      <c r="F103" s="21"/>
-      <c r="G103" s="16"/>
-      <c r="H103" s="16"/>
-      <c r="I103" s="16"/>
-      <c r="J103" s="16"/>
-      <c r="K103" s="16"/>
-      <c r="L103" s="16"/>
+      <c r="A103" s="17"/>
+      <c r="B103" s="17"/>
+      <c r="C103" s="21"/>
+      <c r="D103" s="15"/>
+      <c r="E103" s="25"/>
+      <c r="F103" s="25"/>
+      <c r="G103" s="17"/>
+      <c r="H103" s="17"/>
+      <c r="I103" s="17"/>
+      <c r="J103" s="17"/>
+      <c r="K103" s="17"/>
+      <c r="L103" s="17"/>
       <c r="M103" t="s">
         <v>187</v>
       </c>
@@ -5019,18 +5022,18 @@
       </c>
     </row>
     <row r="104" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A104" s="16"/>
-      <c r="B104" s="16"/>
-      <c r="C104" s="15"/>
-      <c r="D104" s="20"/>
-      <c r="E104" s="21"/>
-      <c r="F104" s="21"/>
-      <c r="G104" s="16"/>
-      <c r="H104" s="16"/>
-      <c r="I104" s="16"/>
-      <c r="J104" s="16"/>
-      <c r="K104" s="16"/>
-      <c r="L104" s="16"/>
+      <c r="A104" s="17"/>
+      <c r="B104" s="17"/>
+      <c r="C104" s="21"/>
+      <c r="D104" s="15"/>
+      <c r="E104" s="25"/>
+      <c r="F104" s="25"/>
+      <c r="G104" s="17"/>
+      <c r="H104" s="17"/>
+      <c r="I104" s="17"/>
+      <c r="J104" s="17"/>
+      <c r="K104" s="17"/>
+      <c r="L104" s="17"/>
       <c r="M104" t="s">
         <v>212</v>
       </c>
@@ -5045,34 +5048,34 @@
       </c>
     </row>
     <row r="105" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A105" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B105" s="16" t="s">
+      <c r="A105" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B105" s="17" t="s">
         <v>258</v>
       </c>
-      <c r="C105" s="15"/>
-      <c r="D105" s="20" t="s">
+      <c r="C105" s="21"/>
+      <c r="D105" s="15" t="s">
         <v>259</v>
       </c>
-      <c r="E105" s="21"/>
-      <c r="F105" s="21"/>
-      <c r="G105" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H105" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I105" s="16" t="s">
+      <c r="E105" s="25"/>
+      <c r="F105" s="25"/>
+      <c r="G105" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H105" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I105" s="17" t="s">
         <v>260</v>
       </c>
-      <c r="J105" s="18" t="s">
+      <c r="J105" s="19" t="s">
         <v>265</v>
       </c>
-      <c r="K105" s="16" t="s">
+      <c r="K105" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="L105" s="16" t="s">
+      <c r="L105" s="17" t="s">
         <v>120</v>
       </c>
       <c r="M105" t="s">
@@ -5089,18 +5092,18 @@
       </c>
     </row>
     <row r="106" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A106" s="16"/>
-      <c r="B106" s="16"/>
-      <c r="C106" s="15"/>
-      <c r="D106" s="20"/>
-      <c r="E106" s="21"/>
-      <c r="F106" s="21"/>
-      <c r="G106" s="16"/>
-      <c r="H106" s="16"/>
-      <c r="I106" s="16"/>
-      <c r="J106" s="18"/>
-      <c r="K106" s="16"/>
-      <c r="L106" s="16"/>
+      <c r="A106" s="17"/>
+      <c r="B106" s="17"/>
+      <c r="C106" s="21"/>
+      <c r="D106" s="15"/>
+      <c r="E106" s="25"/>
+      <c r="F106" s="25"/>
+      <c r="G106" s="17"/>
+      <c r="H106" s="17"/>
+      <c r="I106" s="17"/>
+      <c r="J106" s="19"/>
+      <c r="K106" s="17"/>
+      <c r="L106" s="17"/>
       <c r="M106" t="s">
         <v>212</v>
       </c>
@@ -5115,18 +5118,18 @@
       </c>
     </row>
     <row r="107" spans="1:22" ht="60" x14ac:dyDescent="0.25">
-      <c r="A107" s="16"/>
-      <c r="B107" s="16"/>
-      <c r="C107" s="15"/>
-      <c r="D107" s="20"/>
-      <c r="E107" s="21"/>
-      <c r="F107" s="21"/>
-      <c r="G107" s="16"/>
-      <c r="H107" s="16"/>
-      <c r="I107" s="16"/>
-      <c r="J107" s="18"/>
-      <c r="K107" s="16"/>
-      <c r="L107" s="16"/>
+      <c r="A107" s="17"/>
+      <c r="B107" s="17"/>
+      <c r="C107" s="21"/>
+      <c r="D107" s="15"/>
+      <c r="E107" s="25"/>
+      <c r="F107" s="25"/>
+      <c r="G107" s="17"/>
+      <c r="H107" s="17"/>
+      <c r="I107" s="17"/>
+      <c r="J107" s="19"/>
+      <c r="K107" s="17"/>
+      <c r="L107" s="17"/>
       <c r="M107" t="s">
         <v>212</v>
       </c>
@@ -5141,18 +5144,18 @@
       </c>
     </row>
     <row r="108" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A108" s="16"/>
-      <c r="B108" s="16"/>
-      <c r="C108" s="15"/>
-      <c r="D108" s="20"/>
-      <c r="E108" s="21"/>
-      <c r="F108" s="21"/>
-      <c r="G108" s="16"/>
-      <c r="H108" s="16"/>
-      <c r="I108" s="16"/>
-      <c r="J108" s="18"/>
-      <c r="K108" s="16"/>
-      <c r="L108" s="16"/>
+      <c r="A108" s="17"/>
+      <c r="B108" s="17"/>
+      <c r="C108" s="21"/>
+      <c r="D108" s="15"/>
+      <c r="E108" s="25"/>
+      <c r="F108" s="25"/>
+      <c r="G108" s="17"/>
+      <c r="H108" s="17"/>
+      <c r="I108" s="17"/>
+      <c r="J108" s="19"/>
+      <c r="K108" s="17"/>
+      <c r="L108" s="17"/>
       <c r="M108" t="s">
         <v>212</v>
       </c>
@@ -5205,32 +5208,32 @@
       </c>
     </row>
     <row r="110" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A110" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B110" s="16" t="s">
+      <c r="A110" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B110" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="C110" s="15"/>
-      <c r="D110" s="17" t="s">
+      <c r="C110" s="21"/>
+      <c r="D110" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="E110" s="19"/>
-      <c r="F110" s="19"/>
-      <c r="G110" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H110" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I110" s="16"/>
-      <c r="J110" s="18" t="s">
+      <c r="E110" s="20"/>
+      <c r="F110" s="20"/>
+      <c r="G110" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H110" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I110" s="17"/>
+      <c r="J110" s="19" t="s">
         <v>271</v>
       </c>
-      <c r="K110" s="16" t="s">
+      <c r="K110" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="L110" s="16" t="s">
+      <c r="L110" s="17" t="s">
         <v>120</v>
       </c>
       <c r="M110" t="s">
@@ -5247,18 +5250,18 @@
       </c>
     </row>
     <row r="111" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A111" s="16"/>
-      <c r="B111" s="16"/>
-      <c r="C111" s="15"/>
-      <c r="D111" s="17"/>
-      <c r="E111" s="19"/>
-      <c r="F111" s="19"/>
-      <c r="G111" s="16"/>
-      <c r="H111" s="16"/>
-      <c r="I111" s="16"/>
-      <c r="J111" s="18"/>
-      <c r="K111" s="16"/>
-      <c r="L111" s="16"/>
+      <c r="A111" s="17"/>
+      <c r="B111" s="17"/>
+      <c r="C111" s="21"/>
+      <c r="D111" s="18"/>
+      <c r="E111" s="20"/>
+      <c r="F111" s="20"/>
+      <c r="G111" s="17"/>
+      <c r="H111" s="17"/>
+      <c r="I111" s="17"/>
+      <c r="J111" s="19"/>
+      <c r="K111" s="17"/>
+      <c r="L111" s="17"/>
       <c r="M111" t="s">
         <v>212</v>
       </c>
@@ -5273,18 +5276,18 @@
       </c>
     </row>
     <row r="112" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A112" s="16"/>
-      <c r="B112" s="16"/>
-      <c r="C112" s="15"/>
-      <c r="D112" s="17"/>
-      <c r="E112" s="19"/>
-      <c r="F112" s="19"/>
-      <c r="G112" s="16"/>
-      <c r="H112" s="16"/>
-      <c r="I112" s="16"/>
-      <c r="J112" s="18"/>
-      <c r="K112" s="16"/>
-      <c r="L112" s="16"/>
+      <c r="A112" s="17"/>
+      <c r="B112" s="17"/>
+      <c r="C112" s="21"/>
+      <c r="D112" s="18"/>
+      <c r="E112" s="20"/>
+      <c r="F112" s="20"/>
+      <c r="G112" s="17"/>
+      <c r="H112" s="17"/>
+      <c r="I112" s="17"/>
+      <c r="J112" s="19"/>
+      <c r="K112" s="17"/>
+      <c r="L112" s="17"/>
       <c r="M112" t="s">
         <v>214</v>
       </c>
@@ -5299,32 +5302,32 @@
       </c>
     </row>
     <row r="113" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A113" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B113" s="16" t="s">
+      <c r="A113" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B113" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="C113" s="15"/>
-      <c r="D113" s="17" t="s">
+      <c r="C113" s="21"/>
+      <c r="D113" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="E113" s="19"/>
-      <c r="F113" s="19"/>
-      <c r="G113" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H113" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I113" s="16"/>
-      <c r="J113" s="18" t="s">
+      <c r="E113" s="20"/>
+      <c r="F113" s="20"/>
+      <c r="G113" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H113" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I113" s="17"/>
+      <c r="J113" s="19" t="s">
         <v>286</v>
       </c>
-      <c r="K113" s="16" t="s">
+      <c r="K113" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="L113" s="16" t="s">
+      <c r="L113" s="17" t="s">
         <v>120</v>
       </c>
       <c r="M113" t="s">
@@ -5341,18 +5344,18 @@
       </c>
     </row>
     <row r="114" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A114" s="16"/>
-      <c r="B114" s="16"/>
-      <c r="C114" s="15"/>
-      <c r="D114" s="17"/>
-      <c r="E114" s="19"/>
-      <c r="F114" s="19"/>
-      <c r="G114" s="16"/>
-      <c r="H114" s="16"/>
-      <c r="I114" s="16"/>
-      <c r="J114" s="18"/>
-      <c r="K114" s="16"/>
-      <c r="L114" s="16"/>
+      <c r="A114" s="17"/>
+      <c r="B114" s="17"/>
+      <c r="C114" s="21"/>
+      <c r="D114" s="18"/>
+      <c r="E114" s="20"/>
+      <c r="F114" s="20"/>
+      <c r="G114" s="17"/>
+      <c r="H114" s="17"/>
+      <c r="I114" s="17"/>
+      <c r="J114" s="19"/>
+      <c r="K114" s="17"/>
+      <c r="L114" s="17"/>
       <c r="M114" t="s">
         <v>212</v>
       </c>
@@ -5367,18 +5370,18 @@
       </c>
     </row>
     <row r="115" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A115" s="16"/>
-      <c r="B115" s="16"/>
-      <c r="C115" s="15"/>
-      <c r="D115" s="17"/>
-      <c r="E115" s="19"/>
-      <c r="F115" s="19"/>
-      <c r="G115" s="16"/>
-      <c r="H115" s="16"/>
-      <c r="I115" s="16"/>
-      <c r="J115" s="18"/>
-      <c r="K115" s="16"/>
-      <c r="L115" s="16"/>
+      <c r="A115" s="17"/>
+      <c r="B115" s="17"/>
+      <c r="C115" s="21"/>
+      <c r="D115" s="18"/>
+      <c r="E115" s="20"/>
+      <c r="F115" s="20"/>
+      <c r="G115" s="17"/>
+      <c r="H115" s="17"/>
+      <c r="I115" s="17"/>
+      <c r="J115" s="19"/>
+      <c r="K115" s="17"/>
+      <c r="L115" s="17"/>
       <c r="M115" t="s">
         <v>214</v>
       </c>
@@ -5393,32 +5396,32 @@
       </c>
     </row>
     <row r="116" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A116" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B116" s="16" t="s">
+      <c r="A116" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B116" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="C116" s="15"/>
-      <c r="D116" s="17" t="s">
+      <c r="C116" s="21"/>
+      <c r="D116" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="E116" s="19"/>
-      <c r="F116" s="19"/>
-      <c r="G116" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H116" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I116" s="16"/>
-      <c r="J116" s="18" t="s">
+      <c r="E116" s="20"/>
+      <c r="F116" s="20"/>
+      <c r="G116" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H116" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I116" s="17"/>
+      <c r="J116" s="19" t="s">
         <v>285</v>
       </c>
-      <c r="K116" s="16" t="s">
+      <c r="K116" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="L116" s="16" t="s">
+      <c r="L116" s="17" t="s">
         <v>120</v>
       </c>
       <c r="M116" t="s">
@@ -5435,18 +5438,18 @@
       </c>
     </row>
     <row r="117" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A117" s="16"/>
-      <c r="B117" s="16"/>
-      <c r="C117" s="15"/>
-      <c r="D117" s="17"/>
-      <c r="E117" s="19"/>
-      <c r="F117" s="19"/>
-      <c r="G117" s="16"/>
-      <c r="H117" s="16"/>
-      <c r="I117" s="16"/>
-      <c r="J117" s="18"/>
-      <c r="K117" s="16"/>
-      <c r="L117" s="16"/>
+      <c r="A117" s="17"/>
+      <c r="B117" s="17"/>
+      <c r="C117" s="21"/>
+      <c r="D117" s="18"/>
+      <c r="E117" s="20"/>
+      <c r="F117" s="20"/>
+      <c r="G117" s="17"/>
+      <c r="H117" s="17"/>
+      <c r="I117" s="17"/>
+      <c r="J117" s="19"/>
+      <c r="K117" s="17"/>
+      <c r="L117" s="17"/>
       <c r="M117" t="s">
         <v>212</v>
       </c>
@@ -5461,18 +5464,18 @@
       </c>
     </row>
     <row r="118" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A118" s="16"/>
-      <c r="B118" s="16"/>
-      <c r="C118" s="15"/>
-      <c r="D118" s="17"/>
-      <c r="E118" s="19"/>
-      <c r="F118" s="19"/>
-      <c r="G118" s="16"/>
-      <c r="H118" s="16"/>
-      <c r="I118" s="16"/>
-      <c r="J118" s="18"/>
-      <c r="K118" s="16"/>
-      <c r="L118" s="16"/>
+      <c r="A118" s="17"/>
+      <c r="B118" s="17"/>
+      <c r="C118" s="21"/>
+      <c r="D118" s="18"/>
+      <c r="E118" s="20"/>
+      <c r="F118" s="20"/>
+      <c r="G118" s="17"/>
+      <c r="H118" s="17"/>
+      <c r="I118" s="17"/>
+      <c r="J118" s="19"/>
+      <c r="K118" s="17"/>
+      <c r="L118" s="17"/>
       <c r="M118" t="s">
         <v>214</v>
       </c>
@@ -5487,32 +5490,32 @@
       </c>
     </row>
     <row r="119" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A119" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B119" s="16" t="s">
+      <c r="A119" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B119" s="17" t="s">
         <v>283</v>
       </c>
-      <c r="C119" s="15"/>
-      <c r="D119" s="17" t="s">
+      <c r="C119" s="21"/>
+      <c r="D119" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="E119" s="19"/>
-      <c r="F119" s="19"/>
-      <c r="G119" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H119" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I119" s="16"/>
-      <c r="J119" s="18" t="s">
+      <c r="E119" s="20"/>
+      <c r="F119" s="20"/>
+      <c r="G119" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H119" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I119" s="17"/>
+      <c r="J119" s="19" t="s">
         <v>284</v>
       </c>
-      <c r="K119" s="16" t="s">
+      <c r="K119" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="L119" s="16" t="s">
+      <c r="L119" s="17" t="s">
         <v>120</v>
       </c>
       <c r="M119" t="s">
@@ -5529,18 +5532,18 @@
       </c>
     </row>
     <row r="120" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A120" s="16"/>
-      <c r="B120" s="16"/>
-      <c r="C120" s="15"/>
-      <c r="D120" s="17"/>
-      <c r="E120" s="19"/>
-      <c r="F120" s="19"/>
-      <c r="G120" s="16"/>
-      <c r="H120" s="16"/>
-      <c r="I120" s="16"/>
-      <c r="J120" s="18"/>
-      <c r="K120" s="16"/>
-      <c r="L120" s="16"/>
+      <c r="A120" s="17"/>
+      <c r="B120" s="17"/>
+      <c r="C120" s="21"/>
+      <c r="D120" s="18"/>
+      <c r="E120" s="20"/>
+      <c r="F120" s="20"/>
+      <c r="G120" s="17"/>
+      <c r="H120" s="17"/>
+      <c r="I120" s="17"/>
+      <c r="J120" s="19"/>
+      <c r="K120" s="17"/>
+      <c r="L120" s="17"/>
       <c r="M120" t="s">
         <v>212</v>
       </c>
@@ -5555,18 +5558,18 @@
       </c>
     </row>
     <row r="121" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A121" s="16"/>
-      <c r="B121" s="16"/>
-      <c r="C121" s="15"/>
-      <c r="D121" s="17"/>
-      <c r="E121" s="19"/>
-      <c r="F121" s="19"/>
-      <c r="G121" s="16"/>
-      <c r="H121" s="16"/>
-      <c r="I121" s="16"/>
-      <c r="J121" s="18"/>
-      <c r="K121" s="16"/>
-      <c r="L121" s="16"/>
+      <c r="A121" s="17"/>
+      <c r="B121" s="17"/>
+      <c r="C121" s="21"/>
+      <c r="D121" s="18"/>
+      <c r="E121" s="20"/>
+      <c r="F121" s="20"/>
+      <c r="G121" s="17"/>
+      <c r="H121" s="17"/>
+      <c r="I121" s="17"/>
+      <c r="J121" s="19"/>
+      <c r="K121" s="17"/>
+      <c r="L121" s="17"/>
       <c r="M121" t="s">
         <v>214</v>
       </c>
@@ -5581,36 +5584,38 @@
       </c>
     </row>
     <row r="122" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="B122" s="22" t="s">
+      <c r="A122" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B122" s="14" t="s">
         <v>315</v>
       </c>
-      <c r="C122" s="22" t="s">
+      <c r="C122" s="14" t="s">
         <v>316</v>
       </c>
-      <c r="D122" s="20" t="s">
+      <c r="D122" s="15" t="s">
         <v>322</v>
       </c>
-      <c r="E122" s="22"/>
-      <c r="F122" s="22"/>
-      <c r="G122" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="H122" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="I122" s="22" t="s">
+      <c r="E122" s="14"/>
+      <c r="F122" s="16" t="s">
+        <v>328</v>
+      </c>
+      <c r="G122" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H122" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I122" s="14" t="s">
         <v>317</v>
       </c>
-      <c r="J122" s="20" t="s">
+      <c r="J122" s="15" t="s">
         <v>318</v>
       </c>
-      <c r="K122" s="22" t="s">
+      <c r="K122" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="L122" s="22" t="s">
+      <c r="L122" s="14" t="s">
         <v>119</v>
       </c>
       <c r="M122" t="s">
@@ -5623,40 +5628,40 @@
         <v>27</v>
       </c>
       <c r="P122" s="11" t="s">
-        <v>325</v>
-      </c>
-      <c r="Q122" s="25" t="s">
         <v>324</v>
       </c>
-      <c r="R122" s="20" t="s">
+      <c r="Q122" s="16" t="s">
         <v>323</v>
       </c>
-      <c r="S122" s="25" t="s">
+      <c r="R122" s="15" t="s">
+        <v>329</v>
+      </c>
+      <c r="S122" s="16" t="s">
         <v>320</v>
       </c>
-      <c r="T122" s="25" t="s">
+      <c r="T122" s="16" t="s">
         <v>319</v>
       </c>
-      <c r="U122" s="22" t="s">
-        <v>307</v>
-      </c>
-      <c r="V122" s="20" t="s">
-        <v>328</v>
+      <c r="U122" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="V122" s="15" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="123" spans="1:22" ht="60" x14ac:dyDescent="0.25">
-      <c r="A123" s="22"/>
-      <c r="B123" s="22"/>
-      <c r="C123" s="22"/>
-      <c r="D123" s="22"/>
-      <c r="E123" s="22"/>
-      <c r="F123" s="22"/>
-      <c r="G123" s="22"/>
-      <c r="H123" s="22"/>
-      <c r="I123" s="22"/>
-      <c r="J123" s="20"/>
-      <c r="K123" s="22"/>
-      <c r="L123" s="22"/>
+      <c r="A123" s="14"/>
+      <c r="B123" s="14"/>
+      <c r="C123" s="14"/>
+      <c r="D123" s="14"/>
+      <c r="E123" s="14"/>
+      <c r="F123" s="16"/>
+      <c r="G123" s="14"/>
+      <c r="H123" s="14"/>
+      <c r="I123" s="14"/>
+      <c r="J123" s="15"/>
+      <c r="K123" s="14"/>
+      <c r="L123" s="14"/>
       <c r="M123" t="s">
         <v>177</v>
       </c>
@@ -5667,28 +5672,28 @@
         <v>27</v>
       </c>
       <c r="P123" s="11" t="s">
-        <v>326</v>
-      </c>
-      <c r="Q123" s="25"/>
-      <c r="R123" s="20"/>
-      <c r="S123" s="25"/>
-      <c r="T123" s="25"/>
-      <c r="U123" s="22"/>
-      <c r="V123" s="20"/>
+        <v>325</v>
+      </c>
+      <c r="Q123" s="16"/>
+      <c r="R123" s="15"/>
+      <c r="S123" s="16"/>
+      <c r="T123" s="16"/>
+      <c r="U123" s="14"/>
+      <c r="V123" s="15"/>
     </row>
     <row r="124" spans="1:22" ht="60" x14ac:dyDescent="0.25">
-      <c r="A124" s="22"/>
-      <c r="B124" s="22"/>
-      <c r="C124" s="22"/>
-      <c r="D124" s="22"/>
-      <c r="E124" s="22"/>
-      <c r="F124" s="22"/>
-      <c r="G124" s="22"/>
-      <c r="H124" s="22"/>
-      <c r="I124" s="22"/>
-      <c r="J124" s="20"/>
-      <c r="K124" s="22"/>
-      <c r="L124" s="22"/>
+      <c r="A124" s="14"/>
+      <c r="B124" s="14"/>
+      <c r="C124" s="14"/>
+      <c r="D124" s="14"/>
+      <c r="E124" s="14"/>
+      <c r="F124" s="16"/>
+      <c r="G124" s="14"/>
+      <c r="H124" s="14"/>
+      <c r="I124" s="14"/>
+      <c r="J124" s="15"/>
+      <c r="K124" s="14"/>
+      <c r="L124" s="14"/>
       <c r="M124" t="s">
         <v>111</v>
       </c>
@@ -5699,48 +5704,258 @@
         <v>67</v>
       </c>
       <c r="P124" s="11" t="s">
-        <v>327</v>
-      </c>
-      <c r="Q124" s="25"/>
-      <c r="R124" s="20"/>
-      <c r="S124" s="25"/>
-      <c r="T124" s="25"/>
-      <c r="U124" s="22"/>
-      <c r="V124" s="20"/>
+        <v>326</v>
+      </c>
+      <c r="Q124" s="16"/>
+      <c r="R124" s="15"/>
+      <c r="S124" s="16"/>
+      <c r="T124" s="16"/>
+      <c r="U124" s="14"/>
+      <c r="V124" s="15"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:V1"/>
   <mergeCells count="294">
-    <mergeCell ref="L122:L124"/>
-    <mergeCell ref="J122:J124"/>
-    <mergeCell ref="I122:I124"/>
-    <mergeCell ref="H122:H124"/>
-    <mergeCell ref="G122:G124"/>
-    <mergeCell ref="F122:F124"/>
-    <mergeCell ref="R122:R124"/>
-    <mergeCell ref="Q122:Q124"/>
-    <mergeCell ref="S122:S124"/>
-    <mergeCell ref="T122:T124"/>
-    <mergeCell ref="U122:U124"/>
-    <mergeCell ref="V122:V124"/>
-    <mergeCell ref="E122:E124"/>
-    <mergeCell ref="D122:D124"/>
-    <mergeCell ref="C122:C124"/>
-    <mergeCell ref="B122:B124"/>
-    <mergeCell ref="A122:A124"/>
-    <mergeCell ref="K122:K124"/>
-    <mergeCell ref="A119:A121"/>
-    <mergeCell ref="B119:B121"/>
-    <mergeCell ref="D119:D121"/>
-    <mergeCell ref="G119:G121"/>
-    <mergeCell ref="H119:H121"/>
-    <mergeCell ref="I119:I121"/>
-    <mergeCell ref="J119:J121"/>
-    <mergeCell ref="K119:K121"/>
-    <mergeCell ref="L119:L121"/>
-    <mergeCell ref="E119:E121"/>
-    <mergeCell ref="F119:F121"/>
-    <mergeCell ref="C119:C121"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="C64:C67"/>
+    <mergeCell ref="C68:C71"/>
+    <mergeCell ref="C72:C75"/>
+    <mergeCell ref="C78:C82"/>
+    <mergeCell ref="C83:C87"/>
+    <mergeCell ref="C88:C93"/>
+    <mergeCell ref="C94:C96"/>
+    <mergeCell ref="C97:C98"/>
+    <mergeCell ref="A110:A112"/>
+    <mergeCell ref="I110:I112"/>
+    <mergeCell ref="H110:H112"/>
+    <mergeCell ref="G110:G112"/>
+    <mergeCell ref="D110:D112"/>
+    <mergeCell ref="B110:B112"/>
+    <mergeCell ref="L110:L112"/>
+    <mergeCell ref="K110:K112"/>
+    <mergeCell ref="J110:J112"/>
+    <mergeCell ref="E110:E112"/>
+    <mergeCell ref="F110:F112"/>
+    <mergeCell ref="C110:C112"/>
+    <mergeCell ref="I105:I108"/>
+    <mergeCell ref="H105:H108"/>
+    <mergeCell ref="G105:G108"/>
+    <mergeCell ref="B105:B108"/>
+    <mergeCell ref="A105:A108"/>
+    <mergeCell ref="D105:D108"/>
+    <mergeCell ref="L105:L108"/>
+    <mergeCell ref="K105:K108"/>
+    <mergeCell ref="J105:J108"/>
+    <mergeCell ref="F105:F108"/>
+    <mergeCell ref="E105:E108"/>
+    <mergeCell ref="C105:C108"/>
+    <mergeCell ref="G97:G98"/>
+    <mergeCell ref="B97:B98"/>
+    <mergeCell ref="A97:A98"/>
+    <mergeCell ref="D97:D98"/>
+    <mergeCell ref="L102:L104"/>
+    <mergeCell ref="K102:K104"/>
+    <mergeCell ref="J102:J104"/>
+    <mergeCell ref="I102:I104"/>
+    <mergeCell ref="H102:H104"/>
+    <mergeCell ref="G102:G104"/>
+    <mergeCell ref="D102:D104"/>
+    <mergeCell ref="B102:B104"/>
+    <mergeCell ref="A102:A104"/>
+    <mergeCell ref="L97:L98"/>
+    <mergeCell ref="K97:K98"/>
+    <mergeCell ref="J97:J98"/>
+    <mergeCell ref="I97:I98"/>
+    <mergeCell ref="H97:H98"/>
+    <mergeCell ref="F97:F98"/>
+    <mergeCell ref="F102:F104"/>
+    <mergeCell ref="E97:E98"/>
+    <mergeCell ref="E102:E104"/>
+    <mergeCell ref="C102:C104"/>
+    <mergeCell ref="G94:G96"/>
+    <mergeCell ref="B94:B96"/>
+    <mergeCell ref="A94:A96"/>
+    <mergeCell ref="D94:D96"/>
+    <mergeCell ref="L94:L96"/>
+    <mergeCell ref="K94:K96"/>
+    <mergeCell ref="J94:J96"/>
+    <mergeCell ref="I94:I96"/>
+    <mergeCell ref="H94:H96"/>
+    <mergeCell ref="F94:F96"/>
+    <mergeCell ref="E94:E96"/>
+    <mergeCell ref="G83:G87"/>
+    <mergeCell ref="B83:B87"/>
+    <mergeCell ref="A83:A87"/>
+    <mergeCell ref="D83:D87"/>
+    <mergeCell ref="L88:L93"/>
+    <mergeCell ref="K88:K93"/>
+    <mergeCell ref="J88:J93"/>
+    <mergeCell ref="I88:I93"/>
+    <mergeCell ref="H88:H93"/>
+    <mergeCell ref="G88:G93"/>
+    <mergeCell ref="A88:A93"/>
+    <mergeCell ref="B88:B93"/>
+    <mergeCell ref="D88:D93"/>
+    <mergeCell ref="L83:L87"/>
+    <mergeCell ref="K83:K87"/>
+    <mergeCell ref="J83:J87"/>
+    <mergeCell ref="I83:I87"/>
+    <mergeCell ref="H83:H87"/>
+    <mergeCell ref="F83:F87"/>
+    <mergeCell ref="F88:F93"/>
+    <mergeCell ref="E83:E87"/>
+    <mergeCell ref="E88:E93"/>
+    <mergeCell ref="H78:H82"/>
+    <mergeCell ref="G78:G82"/>
+    <mergeCell ref="D78:D82"/>
+    <mergeCell ref="B78:B82"/>
+    <mergeCell ref="A78:A82"/>
+    <mergeCell ref="I72:I75"/>
+    <mergeCell ref="J72:J75"/>
+    <mergeCell ref="K72:K75"/>
+    <mergeCell ref="L72:L75"/>
+    <mergeCell ref="L78:L82"/>
+    <mergeCell ref="K78:K82"/>
+    <mergeCell ref="J78:J82"/>
+    <mergeCell ref="I78:I82"/>
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="D72:D75"/>
+    <mergeCell ref="G72:G75"/>
+    <mergeCell ref="H72:H75"/>
+    <mergeCell ref="F72:F75"/>
+    <mergeCell ref="F78:F82"/>
+    <mergeCell ref="E72:E75"/>
+    <mergeCell ref="E78:E82"/>
+    <mergeCell ref="H68:H71"/>
+    <mergeCell ref="I68:I71"/>
+    <mergeCell ref="J68:J71"/>
+    <mergeCell ref="K68:K71"/>
+    <mergeCell ref="L68:L71"/>
+    <mergeCell ref="G64:G67"/>
+    <mergeCell ref="B64:B67"/>
+    <mergeCell ref="A64:A67"/>
+    <mergeCell ref="D64:D67"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="D68:D71"/>
+    <mergeCell ref="G68:G71"/>
+    <mergeCell ref="L64:L67"/>
+    <mergeCell ref="K64:K67"/>
+    <mergeCell ref="J64:J67"/>
+    <mergeCell ref="I64:I67"/>
+    <mergeCell ref="H64:H67"/>
+    <mergeCell ref="F64:F67"/>
+    <mergeCell ref="F68:F71"/>
+    <mergeCell ref="E64:E67"/>
+    <mergeCell ref="E68:E71"/>
+    <mergeCell ref="F34:F36"/>
+    <mergeCell ref="F37:F39"/>
+    <mergeCell ref="H34:H36"/>
+    <mergeCell ref="H37:H39"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="I62:I63"/>
+    <mergeCell ref="J62:J63"/>
+    <mergeCell ref="K62:K63"/>
+    <mergeCell ref="L62:L63"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="G62:G63"/>
+    <mergeCell ref="H62:H63"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="G34:G36"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="G37:G39"/>
+    <mergeCell ref="D41:D47"/>
+    <mergeCell ref="D57:D59"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="D37:D39"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="L57:L59"/>
+    <mergeCell ref="K57:K59"/>
+    <mergeCell ref="J57:J59"/>
+    <mergeCell ref="I57:I59"/>
+    <mergeCell ref="H57:H59"/>
+    <mergeCell ref="H41:H47"/>
+    <mergeCell ref="G41:G47"/>
+    <mergeCell ref="B41:B47"/>
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="F41:F47"/>
+    <mergeCell ref="F57:F59"/>
+    <mergeCell ref="G57:G59"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="C41:C47"/>
+    <mergeCell ref="C57:C59"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="L41:L47"/>
+    <mergeCell ref="K41:K47"/>
+    <mergeCell ref="J41:J47"/>
+    <mergeCell ref="I41:I47"/>
+    <mergeCell ref="L28:L30"/>
+    <mergeCell ref="K28:K30"/>
+    <mergeCell ref="J28:J30"/>
+    <mergeCell ref="I28:I30"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="L24:L26"/>
+    <mergeCell ref="K24:K26"/>
+    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="K31:K33"/>
+    <mergeCell ref="L31:L33"/>
+    <mergeCell ref="I34:I36"/>
+    <mergeCell ref="J34:J36"/>
+    <mergeCell ref="K34:K36"/>
+    <mergeCell ref="L34:L36"/>
+    <mergeCell ref="I37:I39"/>
+    <mergeCell ref="J37:J39"/>
+    <mergeCell ref="K37:K39"/>
+    <mergeCell ref="L37:L39"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="H31:H33"/>
+    <mergeCell ref="I31:I33"/>
+    <mergeCell ref="J31:J33"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="E28:E30"/>
+    <mergeCell ref="E31:E33"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="F28:F30"/>
+    <mergeCell ref="F31:F33"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="G28:G30"/>
+    <mergeCell ref="H28:H30"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="G31:G33"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="E37:E39"/>
+    <mergeCell ref="E41:E47"/>
+    <mergeCell ref="E57:E59"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="C37:C39"/>
     <mergeCell ref="K113:K115"/>
     <mergeCell ref="L113:L115"/>
     <mergeCell ref="A116:A118"/>
@@ -5765,246 +5980,36 @@
     <mergeCell ref="J113:J115"/>
     <mergeCell ref="C113:C115"/>
     <mergeCell ref="C116:C118"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="E37:E39"/>
-    <mergeCell ref="E41:E47"/>
-    <mergeCell ref="E57:E59"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="C37:C39"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="H31:H33"/>
-    <mergeCell ref="I31:I33"/>
-    <mergeCell ref="J31:J33"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="E28:E30"/>
-    <mergeCell ref="E31:E33"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="F28:F30"/>
-    <mergeCell ref="F31:F33"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="G28:G30"/>
-    <mergeCell ref="H28:H30"/>
-    <mergeCell ref="G24:G26"/>
-    <mergeCell ref="G31:G33"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="L41:L47"/>
-    <mergeCell ref="K41:K47"/>
-    <mergeCell ref="J41:J47"/>
-    <mergeCell ref="I41:I47"/>
-    <mergeCell ref="L28:L30"/>
-    <mergeCell ref="K28:K30"/>
-    <mergeCell ref="J28:J30"/>
-    <mergeCell ref="I28:I30"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="L24:L26"/>
-    <mergeCell ref="K24:K26"/>
-    <mergeCell ref="J24:J26"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="K31:K33"/>
-    <mergeCell ref="L31:L33"/>
-    <mergeCell ref="I34:I36"/>
-    <mergeCell ref="J34:J36"/>
-    <mergeCell ref="K34:K36"/>
-    <mergeCell ref="L34:L36"/>
-    <mergeCell ref="I37:I39"/>
-    <mergeCell ref="J37:J39"/>
-    <mergeCell ref="K37:K39"/>
-    <mergeCell ref="L37:L39"/>
-    <mergeCell ref="L57:L59"/>
-    <mergeCell ref="K57:K59"/>
-    <mergeCell ref="J57:J59"/>
-    <mergeCell ref="I57:I59"/>
-    <mergeCell ref="H57:H59"/>
-    <mergeCell ref="H41:H47"/>
-    <mergeCell ref="G41:G47"/>
-    <mergeCell ref="B41:B47"/>
-    <mergeCell ref="A41:A47"/>
-    <mergeCell ref="F41:F47"/>
-    <mergeCell ref="F57:F59"/>
-    <mergeCell ref="G57:G59"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="C41:C47"/>
-    <mergeCell ref="C57:C59"/>
-    <mergeCell ref="F34:F36"/>
-    <mergeCell ref="F37:F39"/>
-    <mergeCell ref="H34:H36"/>
-    <mergeCell ref="H37:H39"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="I62:I63"/>
-    <mergeCell ref="J62:J63"/>
-    <mergeCell ref="K62:K63"/>
-    <mergeCell ref="L62:L63"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="G62:G63"/>
-    <mergeCell ref="H62:H63"/>
-    <mergeCell ref="F62:F63"/>
-    <mergeCell ref="G34:G36"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="G37:G39"/>
-    <mergeCell ref="D41:D47"/>
-    <mergeCell ref="D57:D59"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="D37:D39"/>
-    <mergeCell ref="E62:E63"/>
-    <mergeCell ref="H68:H71"/>
-    <mergeCell ref="I68:I71"/>
-    <mergeCell ref="J68:J71"/>
-    <mergeCell ref="K68:K71"/>
-    <mergeCell ref="L68:L71"/>
-    <mergeCell ref="G64:G67"/>
-    <mergeCell ref="B64:B67"/>
-    <mergeCell ref="A64:A67"/>
-    <mergeCell ref="D64:D67"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="D68:D71"/>
-    <mergeCell ref="G68:G71"/>
-    <mergeCell ref="L64:L67"/>
-    <mergeCell ref="K64:K67"/>
-    <mergeCell ref="J64:J67"/>
-    <mergeCell ref="I64:I67"/>
-    <mergeCell ref="H64:H67"/>
-    <mergeCell ref="F64:F67"/>
-    <mergeCell ref="F68:F71"/>
-    <mergeCell ref="E64:E67"/>
-    <mergeCell ref="E68:E71"/>
-    <mergeCell ref="H78:H82"/>
-    <mergeCell ref="G78:G82"/>
-    <mergeCell ref="D78:D82"/>
-    <mergeCell ref="B78:B82"/>
-    <mergeCell ref="A78:A82"/>
-    <mergeCell ref="I72:I75"/>
-    <mergeCell ref="J72:J75"/>
-    <mergeCell ref="K72:K75"/>
-    <mergeCell ref="L72:L75"/>
-    <mergeCell ref="L78:L82"/>
-    <mergeCell ref="K78:K82"/>
-    <mergeCell ref="J78:J82"/>
-    <mergeCell ref="I78:I82"/>
-    <mergeCell ref="A72:A75"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="D72:D75"/>
-    <mergeCell ref="G72:G75"/>
-    <mergeCell ref="H72:H75"/>
-    <mergeCell ref="F72:F75"/>
-    <mergeCell ref="F78:F82"/>
-    <mergeCell ref="E72:E75"/>
-    <mergeCell ref="E78:E82"/>
-    <mergeCell ref="G83:G87"/>
-    <mergeCell ref="B83:B87"/>
-    <mergeCell ref="A83:A87"/>
-    <mergeCell ref="D83:D87"/>
-    <mergeCell ref="L88:L93"/>
-    <mergeCell ref="K88:K93"/>
-    <mergeCell ref="J88:J93"/>
-    <mergeCell ref="I88:I93"/>
-    <mergeCell ref="H88:H93"/>
-    <mergeCell ref="G88:G93"/>
-    <mergeCell ref="A88:A93"/>
-    <mergeCell ref="B88:B93"/>
-    <mergeCell ref="D88:D93"/>
-    <mergeCell ref="L83:L87"/>
-    <mergeCell ref="K83:K87"/>
-    <mergeCell ref="J83:J87"/>
-    <mergeCell ref="I83:I87"/>
-    <mergeCell ref="H83:H87"/>
-    <mergeCell ref="F83:F87"/>
-    <mergeCell ref="F88:F93"/>
-    <mergeCell ref="E83:E87"/>
-    <mergeCell ref="E88:E93"/>
-    <mergeCell ref="G94:G96"/>
-    <mergeCell ref="B94:B96"/>
-    <mergeCell ref="A94:A96"/>
-    <mergeCell ref="D94:D96"/>
-    <mergeCell ref="L94:L96"/>
-    <mergeCell ref="K94:K96"/>
-    <mergeCell ref="J94:J96"/>
-    <mergeCell ref="I94:I96"/>
-    <mergeCell ref="H94:H96"/>
-    <mergeCell ref="F94:F96"/>
-    <mergeCell ref="E94:E96"/>
-    <mergeCell ref="G97:G98"/>
-    <mergeCell ref="B97:B98"/>
-    <mergeCell ref="A97:A98"/>
-    <mergeCell ref="D97:D98"/>
-    <mergeCell ref="L102:L104"/>
-    <mergeCell ref="K102:K104"/>
-    <mergeCell ref="J102:J104"/>
-    <mergeCell ref="I102:I104"/>
-    <mergeCell ref="H102:H104"/>
-    <mergeCell ref="G102:G104"/>
-    <mergeCell ref="D102:D104"/>
-    <mergeCell ref="B102:B104"/>
-    <mergeCell ref="A102:A104"/>
-    <mergeCell ref="L97:L98"/>
-    <mergeCell ref="K97:K98"/>
-    <mergeCell ref="J97:J98"/>
-    <mergeCell ref="I97:I98"/>
-    <mergeCell ref="H97:H98"/>
-    <mergeCell ref="F97:F98"/>
-    <mergeCell ref="F102:F104"/>
-    <mergeCell ref="E97:E98"/>
-    <mergeCell ref="E102:E104"/>
-    <mergeCell ref="C102:C104"/>
-    <mergeCell ref="I105:I108"/>
-    <mergeCell ref="H105:H108"/>
-    <mergeCell ref="G105:G108"/>
-    <mergeCell ref="B105:B108"/>
-    <mergeCell ref="A105:A108"/>
-    <mergeCell ref="D105:D108"/>
-    <mergeCell ref="L105:L108"/>
-    <mergeCell ref="K105:K108"/>
-    <mergeCell ref="J105:J108"/>
-    <mergeCell ref="F105:F108"/>
-    <mergeCell ref="E105:E108"/>
-    <mergeCell ref="C105:C108"/>
-    <mergeCell ref="A110:A112"/>
-    <mergeCell ref="I110:I112"/>
-    <mergeCell ref="H110:H112"/>
-    <mergeCell ref="G110:G112"/>
-    <mergeCell ref="D110:D112"/>
-    <mergeCell ref="B110:B112"/>
-    <mergeCell ref="L110:L112"/>
-    <mergeCell ref="K110:K112"/>
-    <mergeCell ref="J110:J112"/>
-    <mergeCell ref="E110:E112"/>
-    <mergeCell ref="F110:F112"/>
-    <mergeCell ref="C110:C112"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="C64:C67"/>
-    <mergeCell ref="C68:C71"/>
-    <mergeCell ref="C72:C75"/>
-    <mergeCell ref="C78:C82"/>
-    <mergeCell ref="C83:C87"/>
-    <mergeCell ref="C88:C93"/>
-    <mergeCell ref="C94:C96"/>
-    <mergeCell ref="C97:C98"/>
+    <mergeCell ref="A119:A121"/>
+    <mergeCell ref="B119:B121"/>
+    <mergeCell ref="D119:D121"/>
+    <mergeCell ref="G119:G121"/>
+    <mergeCell ref="H119:H121"/>
+    <mergeCell ref="I119:I121"/>
+    <mergeCell ref="J119:J121"/>
+    <mergeCell ref="K119:K121"/>
+    <mergeCell ref="L119:L121"/>
+    <mergeCell ref="E119:E121"/>
+    <mergeCell ref="F119:F121"/>
+    <mergeCell ref="C119:C121"/>
+    <mergeCell ref="T122:T124"/>
+    <mergeCell ref="U122:U124"/>
+    <mergeCell ref="V122:V124"/>
+    <mergeCell ref="E122:E124"/>
+    <mergeCell ref="D122:D124"/>
+    <mergeCell ref="C122:C124"/>
+    <mergeCell ref="B122:B124"/>
+    <mergeCell ref="A122:A124"/>
+    <mergeCell ref="K122:K124"/>
+    <mergeCell ref="L122:L124"/>
+    <mergeCell ref="J122:J124"/>
+    <mergeCell ref="I122:I124"/>
+    <mergeCell ref="H122:H124"/>
+    <mergeCell ref="G122:G124"/>
+    <mergeCell ref="F122:F124"/>
+    <mergeCell ref="R122:R124"/>
+    <mergeCell ref="Q122:Q124"/>
+    <mergeCell ref="S122:S124"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="P54" r:id="rId1"/>
@@ -6019,16 +6024,17 @@
     <hyperlink ref="P122" r:id="rId10"/>
     <hyperlink ref="P123" r:id="rId11"/>
     <hyperlink ref="P124" r:id="rId12"/>
+    <hyperlink ref="F122:F124" r:id="rId13" display="MappingSheetResources\GetContractAvailableServices\GetContractAvailableServicesResponse.txt"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId13"/>
-  <drawing r:id="rId14"/>
-  <legacyDrawing r:id="rId15"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId14"/>
+  <drawing r:id="rId15"/>
+  <legacyDrawing r:id="rId16"/>
   <oleObjects>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="1025" r:id="rId16">
-          <objectPr defaultSize="0" r:id="rId17">
+        <oleObject progId="Packager Shell Object" shapeId="1025" r:id="rId17">
+          <objectPr defaultSize="0" r:id="rId18">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -6047,13 +6053,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="1025" r:id="rId16"/>
+        <oleObject progId="Packager Shell Object" shapeId="1025" r:id="rId17"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="1026" r:id="rId18">
-          <objectPr defaultSize="0" r:id="rId19">
+        <oleObject progId="Packager Shell Object" shapeId="1026" r:id="rId19">
+          <objectPr defaultSize="0" r:id="rId20">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>5</xdr:col>
@@ -6072,7 +6078,7 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="1026" r:id="rId18"/>
+        <oleObject progId="Packager Shell Object" shapeId="1026" r:id="rId19"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </oleObjects>

</xml_diff>

<commit_message>
Updated the Get Contract Available Services
git-tfs-id: [http://developmentvlan:8585/tfs/vanrise.collection]$/;C55411
</commit_message>
<xml_diff>
--- a/SOM/Documents/SOM/SOM APIs Mapping Sheet.xlsx
+++ b/SOM/Documents/SOM/SOM APIs Mapping Sheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="332">
   <si>
     <t>GetTechnicalDetails</t>
   </si>
@@ -1052,6 +1052,12 @@
 Then call contract Services Read Request in order to get the ids of the services that are already purchased
 Then filter the rate plan services by removing those that are sold.
 At the end call for each package the servicesReadRequest in order to get the name of the service in addtion to other needed fields.</t>
+  </si>
+  <si>
+    <t>ST_AddAdditionalServices</t>
+  </si>
+  <si>
+    <t>S2C3156</t>
   </si>
 </sst>
 </file>
@@ -1206,13 +1212,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1227,19 +1230,22 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1707,11 +1713,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V124"/>
+  <dimension ref="A1:V125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U122" sqref="U122:U124"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D125" sqref="D125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2443,34 +2449,34 @@
       </c>
     </row>
     <row r="22" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B22" s="14" t="s">
+      <c r="A22" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B22" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="23"/>
-      <c r="D22" s="18" t="s">
+      <c r="C22" s="14"/>
+      <c r="D22" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H22" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I22" s="14" t="s">
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="I22" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="J22" s="15" t="s">
+      <c r="J22" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="K22" s="23" t="s">
+      <c r="K22" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="L22" s="14" t="s">
+      <c r="L22" s="22" t="s">
         <v>120</v>
       </c>
       <c r="M22" t="s">
@@ -2487,18 +2493,18 @@
       </c>
     </row>
     <row r="23" spans="1:22" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="14"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="22"/>
       <c r="M23" t="s">
         <v>157</v>
       </c>
@@ -2513,34 +2519,34 @@
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A24" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B24" s="17" t="s">
+      <c r="A24" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B24" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="21"/>
-      <c r="D24" s="18" t="s">
+      <c r="C24" s="15"/>
+      <c r="D24" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="H24" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I24" s="19" t="s">
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="J24" s="17" t="s">
+      <c r="J24" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="K24" s="17" t="s">
+      <c r="K24" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L24" s="24" t="s">
+      <c r="L24" s="23" t="s">
         <v>120</v>
       </c>
       <c r="M24" t="s">
@@ -2555,18 +2561,18 @@
       <c r="V24"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="24"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="23"/>
       <c r="M25" t="s">
         <v>73</v>
       </c>
@@ -2578,18 +2584,18 @@
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="24"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="23"/>
       <c r="M26" t="s">
         <v>135</v>
       </c>
@@ -2644,34 +2650,34 @@
       </c>
     </row>
     <row r="28" spans="1:22" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B28" s="17" t="s">
+      <c r="A28" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B28" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="C28" s="21"/>
-      <c r="D28" s="18" t="s">
+      <c r="C28" s="15"/>
+      <c r="D28" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="H28" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I28" s="17" t="s">
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I28" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="J28" s="19" t="s">
+      <c r="J28" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="K28" s="17" t="s">
+      <c r="K28" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L28" s="17" t="s">
+      <c r="L28" s="16" t="s">
         <v>119</v>
       </c>
       <c r="M28" t="s">
@@ -2688,18 +2694,18 @@
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="17"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
       <c r="M29" t="s">
         <v>85</v>
       </c>
@@ -2711,18 +2717,18 @@
       </c>
     </row>
     <row r="30" spans="1:22" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
       <c r="M30" t="s">
         <v>90</v>
       </c>
@@ -2737,34 +2743,34 @@
       </c>
     </row>
     <row r="31" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B31" s="17" t="s">
+      <c r="A31" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B31" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="C31" s="21"/>
-      <c r="D31" s="18" t="s">
+      <c r="C31" s="15"/>
+      <c r="D31" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="H31" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I31" s="17" t="s">
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I31" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="J31" s="19" t="s">
+      <c r="J31" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="K31" s="17" t="s">
+      <c r="K31" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L31" s="17" t="s">
+      <c r="L31" s="16" t="s">
         <v>119</v>
       </c>
       <c r="M31" t="s">
@@ -2778,18 +2784,18 @@
       </c>
     </row>
     <row r="32" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="17"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="17"/>
-      <c r="L32" s="17"/>
+      <c r="A32" s="16"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="16"/>
       <c r="M32" t="s">
         <v>85</v>
       </c>
@@ -2801,18 +2807,18 @@
       </c>
     </row>
     <row r="33" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="17"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="17"/>
-      <c r="L33" s="17"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
       <c r="M33" t="s">
         <v>90</v>
       </c>
@@ -2827,34 +2833,34 @@
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B34" s="17" t="s">
+      <c r="A34" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B34" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="C34" s="21"/>
-      <c r="D34" s="18" t="s">
+      <c r="C34" s="15"/>
+      <c r="D34" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="H34" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I34" s="17" t="s">
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H34" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I34" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="J34" s="19" t="s">
+      <c r="J34" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="K34" s="17" t="s">
+      <c r="K34" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L34" s="17" t="s">
+      <c r="L34" s="16" t="s">
         <v>119</v>
       </c>
       <c r="M34" t="s">
@@ -2868,18 +2874,18 @@
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A35" s="17"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="17"/>
-      <c r="L35" s="17"/>
+      <c r="A35" s="16"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
       <c r="M35" t="s">
         <v>85</v>
       </c>
@@ -2891,18 +2897,18 @@
       </c>
     </row>
     <row r="36" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="17"/>
-      <c r="B36" s="17"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="17"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="17"/>
-      <c r="L36" s="17"/>
+      <c r="A36" s="16"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="16"/>
       <c r="M36" t="s">
         <v>90</v>
       </c>
@@ -2917,34 +2923,34 @@
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A37" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B37" s="17" t="s">
+      <c r="A37" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B37" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="C37" s="21"/>
-      <c r="D37" s="18" t="s">
+      <c r="C37" s="15"/>
+      <c r="D37" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="H37" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I37" s="17" t="s">
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H37" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I37" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="J37" s="19" t="s">
+      <c r="J37" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="K37" s="17" t="s">
+      <c r="K37" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L37" s="17" t="s">
+      <c r="L37" s="16" t="s">
         <v>119</v>
       </c>
       <c r="M37" t="s">
@@ -2958,18 +2964,18 @@
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A38" s="17"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17"/>
-      <c r="J38" s="19"/>
-      <c r="K38" s="17"/>
-      <c r="L38" s="17"/>
+      <c r="A38" s="16"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="16"/>
       <c r="M38" t="s">
         <v>85</v>
       </c>
@@ -2981,18 +2987,18 @@
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A39" s="17"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="17"/>
-      <c r="J39" s="19"/>
-      <c r="K39" s="17"/>
-      <c r="L39" s="17"/>
+      <c r="A39" s="16"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="18"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="16"/>
       <c r="M39" t="s">
         <v>90</v>
       </c>
@@ -3044,34 +3050,34 @@
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A41" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B41" s="17" t="s">
+      <c r="A41" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B41" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="18" t="s">
+      <c r="C41" s="15"/>
+      <c r="D41" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="H41" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I41" s="17" t="s">
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H41" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I41" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="J41" s="19" t="s">
+      <c r="J41" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="K41" s="17" t="s">
+      <c r="K41" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L41" s="17" t="s">
+      <c r="L41" s="16" t="s">
         <v>119</v>
       </c>
       <c r="M41" t="s">
@@ -3085,18 +3091,18 @@
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A42" s="17"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="17"/>
-      <c r="I42" s="17"/>
-      <c r="J42" s="19"/>
-      <c r="K42" s="17"/>
-      <c r="L42" s="17"/>
+      <c r="A42" s="16"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="16"/>
+      <c r="J42" s="18"/>
+      <c r="K42" s="16"/>
+      <c r="L42" s="16"/>
       <c r="M42" t="s">
         <v>90</v>
       </c>
@@ -3108,18 +3114,18 @@
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A43" s="17"/>
-      <c r="B43" s="17"/>
-      <c r="C43" s="21"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="17"/>
-      <c r="H43" s="17"/>
-      <c r="I43" s="17"/>
-      <c r="J43" s="19"/>
-      <c r="K43" s="17"/>
-      <c r="L43" s="17"/>
+      <c r="A43" s="16"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
+      <c r="J43" s="18"/>
+      <c r="K43" s="16"/>
+      <c r="L43" s="16"/>
       <c r="M43" t="s">
         <v>91</v>
       </c>
@@ -3132,18 +3138,18 @@
       <c r="V43"/>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A44" s="17"/>
-      <c r="B44" s="17"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="17"/>
-      <c r="I44" s="17"/>
-      <c r="J44" s="19"/>
-      <c r="K44" s="17"/>
-      <c r="L44" s="17"/>
+      <c r="A44" s="16"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="16"/>
+      <c r="J44" s="18"/>
+      <c r="K44" s="16"/>
+      <c r="L44" s="16"/>
       <c r="M44" t="s">
         <v>93</v>
       </c>
@@ -3156,18 +3162,18 @@
       <c r="V44"/>
     </row>
     <row r="45" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="17"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="21"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="17"/>
-      <c r="H45" s="17"/>
-      <c r="I45" s="17"/>
-      <c r="J45" s="19"/>
-      <c r="K45" s="17"/>
-      <c r="L45" s="17"/>
+      <c r="A45" s="16"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
+      <c r="J45" s="18"/>
+      <c r="K45" s="16"/>
+      <c r="L45" s="16"/>
       <c r="M45" t="s">
         <v>81</v>
       </c>
@@ -3182,18 +3188,18 @@
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A46" s="17"/>
-      <c r="B46" s="17"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="17"/>
-      <c r="I46" s="17"/>
-      <c r="J46" s="19"/>
-      <c r="K46" s="17"/>
-      <c r="L46" s="17"/>
+      <c r="A46" s="16"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="16"/>
+      <c r="J46" s="18"/>
+      <c r="K46" s="16"/>
+      <c r="L46" s="16"/>
       <c r="M46" t="s">
         <v>126</v>
       </c>
@@ -3205,18 +3211,18 @@
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A47" s="17"/>
-      <c r="B47" s="17"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="17"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="17"/>
-      <c r="J47" s="19"/>
-      <c r="K47" s="17"/>
-      <c r="L47" s="17"/>
+      <c r="A47" s="16"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
+      <c r="J47" s="18"/>
+      <c r="K47" s="16"/>
+      <c r="L47" s="16"/>
       <c r="M47" t="s">
         <v>47</v>
       </c>
@@ -3600,32 +3606,32 @@
       </c>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A57" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B57" s="17" t="s">
+      <c r="A57" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B57" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="C57" s="21"/>
-      <c r="D57" s="19"/>
-      <c r="E57" s="22"/>
-      <c r="F57" s="22"/>
-      <c r="G57" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="H57" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I57" s="17" t="s">
+      <c r="C57" s="15"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="24"/>
+      <c r="F57" s="24"/>
+      <c r="G57" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H57" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I57" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="J57" s="19" t="s">
+      <c r="J57" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="K57" s="17" t="s">
+      <c r="K57" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L57" s="24" t="s">
+      <c r="L57" s="23" t="s">
         <v>120</v>
       </c>
       <c r="M57" t="s">
@@ -3639,18 +3645,18 @@
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A58" s="17"/>
-      <c r="B58" s="17"/>
-      <c r="C58" s="21"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="22"/>
-      <c r="F58" s="22"/>
-      <c r="G58" s="17"/>
-      <c r="H58" s="17"/>
-      <c r="I58" s="17"/>
-      <c r="J58" s="19"/>
-      <c r="K58" s="17"/>
-      <c r="L58" s="24"/>
+      <c r="A58" s="16"/>
+      <c r="B58" s="16"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="16"/>
+      <c r="H58" s="16"/>
+      <c r="I58" s="16"/>
+      <c r="J58" s="18"/>
+      <c r="K58" s="16"/>
+      <c r="L58" s="23"/>
       <c r="M58" t="s">
         <v>132</v>
       </c>
@@ -3662,18 +3668,18 @@
       </c>
     </row>
     <row r="59" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A59" s="17"/>
-      <c r="B59" s="17"/>
-      <c r="C59" s="21"/>
-      <c r="D59" s="19"/>
-      <c r="E59" s="22"/>
-      <c r="F59" s="22"/>
-      <c r="G59" s="17"/>
-      <c r="H59" s="17"/>
-      <c r="I59" s="17"/>
-      <c r="J59" s="19"/>
-      <c r="K59" s="17"/>
-      <c r="L59" s="24"/>
+      <c r="A59" s="16"/>
+      <c r="B59" s="16"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="24"/>
+      <c r="F59" s="24"/>
+      <c r="G59" s="16"/>
+      <c r="H59" s="16"/>
+      <c r="I59" s="16"/>
+      <c r="J59" s="18"/>
+      <c r="K59" s="16"/>
+      <c r="L59" s="23"/>
       <c r="M59" t="s">
         <v>133</v>
       </c>
@@ -3761,34 +3767,34 @@
       </c>
     </row>
     <row r="62" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B62" s="14" t="s">
+      <c r="A62" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B62" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="C62" s="23"/>
-      <c r="D62" s="15" t="s">
+      <c r="C62" s="14"/>
+      <c r="D62" s="20" t="s">
         <v>200</v>
       </c>
-      <c r="E62" s="25"/>
-      <c r="F62" s="25"/>
-      <c r="G62" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H62" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I62" s="17" t="s">
+      <c r="E62" s="21"/>
+      <c r="F62" s="21"/>
+      <c r="G62" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H62" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="I62" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="J62" s="19" t="s">
+      <c r="J62" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="K62" s="17" t="s">
+      <c r="K62" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L62" s="17" t="s">
+      <c r="L62" s="16" t="s">
         <v>119</v>
       </c>
       <c r="M62" t="s">
@@ -3805,18 +3811,18 @@
       </c>
     </row>
     <row r="63" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A63" s="14"/>
-      <c r="B63" s="14"/>
-      <c r="C63" s="23"/>
-      <c r="D63" s="15"/>
-      <c r="E63" s="25"/>
-      <c r="F63" s="25"/>
-      <c r="G63" s="14"/>
-      <c r="H63" s="14"/>
-      <c r="I63" s="17"/>
-      <c r="J63" s="19"/>
-      <c r="K63" s="17"/>
-      <c r="L63" s="17"/>
+      <c r="A63" s="22"/>
+      <c r="B63" s="22"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="20"/>
+      <c r="E63" s="21"/>
+      <c r="F63" s="21"/>
+      <c r="G63" s="22"/>
+      <c r="H63" s="22"/>
+      <c r="I63" s="16"/>
+      <c r="J63" s="18"/>
+      <c r="K63" s="16"/>
+      <c r="L63" s="16"/>
       <c r="M63" t="s">
         <v>182</v>
       </c>
@@ -3831,34 +3837,34 @@
       </c>
     </row>
     <row r="64" spans="1:22" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B64" s="17" t="s">
+      <c r="A64" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B64" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="C64" s="21"/>
-      <c r="D64" s="15" t="s">
+      <c r="C64" s="15"/>
+      <c r="D64" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="E64" s="25"/>
-      <c r="F64" s="25"/>
-      <c r="G64" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="H64" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I64" s="17" t="s">
+      <c r="E64" s="21"/>
+      <c r="F64" s="21"/>
+      <c r="G64" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H64" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I64" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="J64" s="17" t="s">
+      <c r="J64" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="K64" s="17" t="s">
+      <c r="K64" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L64" s="17" t="s">
+      <c r="L64" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M64" t="s">
@@ -3875,18 +3881,18 @@
       </c>
     </row>
     <row r="65" spans="1:22" ht="90" x14ac:dyDescent="0.25">
-      <c r="A65" s="17"/>
-      <c r="B65" s="17"/>
-      <c r="C65" s="21"/>
-      <c r="D65" s="15"/>
-      <c r="E65" s="25"/>
-      <c r="F65" s="25"/>
-      <c r="G65" s="17"/>
-      <c r="H65" s="17"/>
-      <c r="I65" s="17"/>
-      <c r="J65" s="17"/>
-      <c r="K65" s="17"/>
-      <c r="L65" s="17"/>
+      <c r="A65" s="16"/>
+      <c r="B65" s="16"/>
+      <c r="C65" s="15"/>
+      <c r="D65" s="20"/>
+      <c r="E65" s="21"/>
+      <c r="F65" s="21"/>
+      <c r="G65" s="16"/>
+      <c r="H65" s="16"/>
+      <c r="I65" s="16"/>
+      <c r="J65" s="16"/>
+      <c r="K65" s="16"/>
+      <c r="L65" s="16"/>
       <c r="M65" t="s">
         <v>187</v>
       </c>
@@ -3901,18 +3907,18 @@
       </c>
     </row>
     <row r="66" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A66" s="17"/>
-      <c r="B66" s="17"/>
-      <c r="C66" s="21"/>
-      <c r="D66" s="15"/>
-      <c r="E66" s="25"/>
-      <c r="F66" s="25"/>
-      <c r="G66" s="17"/>
-      <c r="H66" s="17"/>
-      <c r="I66" s="17"/>
-      <c r="J66" s="17"/>
-      <c r="K66" s="17"/>
-      <c r="L66" s="17"/>
+      <c r="A66" s="16"/>
+      <c r="B66" s="16"/>
+      <c r="C66" s="15"/>
+      <c r="D66" s="20"/>
+      <c r="E66" s="21"/>
+      <c r="F66" s="21"/>
+      <c r="G66" s="16"/>
+      <c r="H66" s="16"/>
+      <c r="I66" s="16"/>
+      <c r="J66" s="16"/>
+      <c r="K66" s="16"/>
+      <c r="L66" s="16"/>
       <c r="M66" t="s">
         <v>190</v>
       </c>
@@ -3924,18 +3930,18 @@
       </c>
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A67" s="17"/>
-      <c r="B67" s="17"/>
-      <c r="C67" s="21"/>
-      <c r="D67" s="15"/>
-      <c r="E67" s="25"/>
-      <c r="F67" s="25"/>
-      <c r="G67" s="17"/>
-      <c r="H67" s="17"/>
-      <c r="I67" s="17"/>
-      <c r="J67" s="17"/>
-      <c r="K67" s="17"/>
-      <c r="L67" s="17"/>
+      <c r="A67" s="16"/>
+      <c r="B67" s="16"/>
+      <c r="C67" s="15"/>
+      <c r="D67" s="20"/>
+      <c r="E67" s="21"/>
+      <c r="F67" s="21"/>
+      <c r="G67" s="16"/>
+      <c r="H67" s="16"/>
+      <c r="I67" s="16"/>
+      <c r="J67" s="16"/>
+      <c r="K67" s="16"/>
+      <c r="L67" s="16"/>
       <c r="M67" t="s">
         <v>191</v>
       </c>
@@ -3947,34 +3953,34 @@
       </c>
     </row>
     <row r="68" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B68" s="17" t="s">
+      <c r="A68" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B68" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="C68" s="21"/>
-      <c r="D68" s="15" t="s">
+      <c r="C68" s="15"/>
+      <c r="D68" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="E68" s="25"/>
-      <c r="F68" s="25"/>
-      <c r="G68" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="H68" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I68" s="17" t="s">
+      <c r="E68" s="21"/>
+      <c r="F68" s="21"/>
+      <c r="G68" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H68" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I68" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="J68" s="17" t="s">
+      <c r="J68" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="K68" s="17" t="s">
+      <c r="K68" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L68" s="17" t="s">
+      <c r="L68" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M68" t="s">
@@ -3991,18 +3997,18 @@
       </c>
     </row>
     <row r="69" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A69" s="17"/>
-      <c r="B69" s="17"/>
-      <c r="C69" s="21"/>
-      <c r="D69" s="15"/>
-      <c r="E69" s="25"/>
-      <c r="F69" s="25"/>
-      <c r="G69" s="17"/>
-      <c r="H69" s="17"/>
-      <c r="I69" s="17"/>
-      <c r="J69" s="17"/>
-      <c r="K69" s="17"/>
-      <c r="L69" s="17"/>
+      <c r="A69" s="16"/>
+      <c r="B69" s="16"/>
+      <c r="C69" s="15"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="21"/>
+      <c r="F69" s="21"/>
+      <c r="G69" s="16"/>
+      <c r="H69" s="16"/>
+      <c r="I69" s="16"/>
+      <c r="J69" s="16"/>
+      <c r="K69" s="16"/>
+      <c r="L69" s="16"/>
       <c r="M69" t="s">
         <v>187</v>
       </c>
@@ -4014,18 +4020,18 @@
       </c>
     </row>
     <row r="70" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A70" s="17"/>
-      <c r="B70" s="17"/>
-      <c r="C70" s="21"/>
-      <c r="D70" s="15"/>
-      <c r="E70" s="25"/>
-      <c r="F70" s="25"/>
-      <c r="G70" s="17"/>
-      <c r="H70" s="17"/>
-      <c r="I70" s="17"/>
-      <c r="J70" s="17"/>
-      <c r="K70" s="17"/>
-      <c r="L70" s="17"/>
+      <c r="A70" s="16"/>
+      <c r="B70" s="16"/>
+      <c r="C70" s="15"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="21"/>
+      <c r="F70" s="21"/>
+      <c r="G70" s="16"/>
+      <c r="H70" s="16"/>
+      <c r="I70" s="16"/>
+      <c r="J70" s="16"/>
+      <c r="K70" s="16"/>
+      <c r="L70" s="16"/>
       <c r="M70" t="s">
         <v>190</v>
       </c>
@@ -4037,18 +4043,18 @@
       </c>
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A71" s="17"/>
-      <c r="B71" s="17"/>
-      <c r="C71" s="21"/>
-      <c r="D71" s="15"/>
-      <c r="E71" s="25"/>
-      <c r="F71" s="25"/>
-      <c r="G71" s="17"/>
-      <c r="H71" s="17"/>
-      <c r="I71" s="17"/>
-      <c r="J71" s="17"/>
-      <c r="K71" s="17"/>
-      <c r="L71" s="17"/>
+      <c r="A71" s="16"/>
+      <c r="B71" s="16"/>
+      <c r="C71" s="15"/>
+      <c r="D71" s="20"/>
+      <c r="E71" s="21"/>
+      <c r="F71" s="21"/>
+      <c r="G71" s="16"/>
+      <c r="H71" s="16"/>
+      <c r="I71" s="16"/>
+      <c r="J71" s="16"/>
+      <c r="K71" s="16"/>
+      <c r="L71" s="16"/>
       <c r="M71" t="s">
         <v>191</v>
       </c>
@@ -4060,34 +4066,34 @@
       </c>
     </row>
     <row r="72" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A72" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B72" s="17" t="s">
+      <c r="A72" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B72" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="C72" s="21"/>
-      <c r="D72" s="15" t="s">
+      <c r="C72" s="15"/>
+      <c r="D72" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="E72" s="25"/>
-      <c r="F72" s="25"/>
-      <c r="G72" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="H72" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I72" s="17" t="s">
+      <c r="E72" s="21"/>
+      <c r="F72" s="21"/>
+      <c r="G72" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H72" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I72" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="J72" s="17" t="s">
+      <c r="J72" s="16" t="s">
         <v>198</v>
       </c>
-      <c r="K72" s="17" t="s">
+      <c r="K72" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L72" s="17" t="s">
+      <c r="L72" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M72" t="s">
@@ -4101,18 +4107,18 @@
       </c>
     </row>
     <row r="73" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A73" s="17"/>
-      <c r="B73" s="17"/>
-      <c r="C73" s="21"/>
-      <c r="D73" s="15"/>
-      <c r="E73" s="25"/>
-      <c r="F73" s="25"/>
-      <c r="G73" s="17"/>
-      <c r="H73" s="17"/>
-      <c r="I73" s="17"/>
-      <c r="J73" s="17"/>
-      <c r="K73" s="17"/>
-      <c r="L73" s="17"/>
+      <c r="A73" s="16"/>
+      <c r="B73" s="16"/>
+      <c r="C73" s="15"/>
+      <c r="D73" s="20"/>
+      <c r="E73" s="21"/>
+      <c r="F73" s="21"/>
+      <c r="G73" s="16"/>
+      <c r="H73" s="16"/>
+      <c r="I73" s="16"/>
+      <c r="J73" s="16"/>
+      <c r="K73" s="16"/>
+      <c r="L73" s="16"/>
       <c r="M73" t="s">
         <v>187</v>
       </c>
@@ -4124,18 +4130,18 @@
       </c>
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A74" s="17"/>
-      <c r="B74" s="17"/>
-      <c r="C74" s="21"/>
-      <c r="D74" s="15"/>
-      <c r="E74" s="25"/>
-      <c r="F74" s="25"/>
-      <c r="G74" s="17"/>
-      <c r="H74" s="17"/>
-      <c r="I74" s="17"/>
-      <c r="J74" s="17"/>
-      <c r="K74" s="17"/>
-      <c r="L74" s="17"/>
+      <c r="A74" s="16"/>
+      <c r="B74" s="16"/>
+      <c r="C74" s="15"/>
+      <c r="D74" s="20"/>
+      <c r="E74" s="21"/>
+      <c r="F74" s="21"/>
+      <c r="G74" s="16"/>
+      <c r="H74" s="16"/>
+      <c r="I74" s="16"/>
+      <c r="J74" s="16"/>
+      <c r="K74" s="16"/>
+      <c r="L74" s="16"/>
       <c r="M74" t="s">
         <v>190</v>
       </c>
@@ -4147,18 +4153,18 @@
       </c>
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A75" s="17"/>
-      <c r="B75" s="17"/>
-      <c r="C75" s="21"/>
-      <c r="D75" s="15"/>
-      <c r="E75" s="25"/>
-      <c r="F75" s="25"/>
-      <c r="G75" s="17"/>
-      <c r="H75" s="17"/>
-      <c r="I75" s="17"/>
-      <c r="J75" s="17"/>
-      <c r="K75" s="17"/>
-      <c r="L75" s="17"/>
+      <c r="A75" s="16"/>
+      <c r="B75" s="16"/>
+      <c r="C75" s="15"/>
+      <c r="D75" s="20"/>
+      <c r="E75" s="21"/>
+      <c r="F75" s="21"/>
+      <c r="G75" s="16"/>
+      <c r="H75" s="16"/>
+      <c r="I75" s="16"/>
+      <c r="J75" s="16"/>
+      <c r="K75" s="16"/>
+      <c r="L75" s="16"/>
       <c r="M75" t="s">
         <v>191</v>
       </c>
@@ -4246,34 +4252,34 @@
       </c>
     </row>
     <row r="78" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B78" s="17" t="s">
+      <c r="A78" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B78" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="C78" s="21"/>
-      <c r="D78" s="15" t="s">
+      <c r="C78" s="15"/>
+      <c r="D78" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="E78" s="25"/>
-      <c r="F78" s="25"/>
-      <c r="G78" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="H78" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I78" s="17" t="s">
+      <c r="E78" s="21"/>
+      <c r="F78" s="21"/>
+      <c r="G78" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H78" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I78" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="J78" s="17" t="s">
+      <c r="J78" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="K78" s="17" t="s">
+      <c r="K78" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L78" s="17" t="s">
+      <c r="L78" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M78" t="s">
@@ -4290,18 +4296,18 @@
       </c>
     </row>
     <row r="79" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A79" s="17"/>
-      <c r="B79" s="17"/>
-      <c r="C79" s="21"/>
-      <c r="D79" s="15"/>
-      <c r="E79" s="25"/>
-      <c r="F79" s="25"/>
-      <c r="G79" s="17"/>
-      <c r="H79" s="17"/>
-      <c r="I79" s="17"/>
-      <c r="J79" s="17"/>
-      <c r="K79" s="17"/>
-      <c r="L79" s="17"/>
+      <c r="A79" s="16"/>
+      <c r="B79" s="16"/>
+      <c r="C79" s="15"/>
+      <c r="D79" s="20"/>
+      <c r="E79" s="21"/>
+      <c r="F79" s="21"/>
+      <c r="G79" s="16"/>
+      <c r="H79" s="16"/>
+      <c r="I79" s="16"/>
+      <c r="J79" s="16"/>
+      <c r="K79" s="16"/>
+      <c r="L79" s="16"/>
       <c r="M79" t="s">
         <v>212</v>
       </c>
@@ -4316,18 +4322,18 @@
       </c>
     </row>
     <row r="80" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="17"/>
-      <c r="B80" s="17"/>
-      <c r="C80" s="21"/>
-      <c r="D80" s="15"/>
-      <c r="E80" s="25"/>
-      <c r="F80" s="25"/>
-      <c r="G80" s="17"/>
-      <c r="H80" s="17"/>
-      <c r="I80" s="17"/>
-      <c r="J80" s="17"/>
-      <c r="K80" s="17"/>
-      <c r="L80" s="17"/>
+      <c r="A80" s="16"/>
+      <c r="B80" s="16"/>
+      <c r="C80" s="15"/>
+      <c r="D80" s="20"/>
+      <c r="E80" s="21"/>
+      <c r="F80" s="21"/>
+      <c r="G80" s="16"/>
+      <c r="H80" s="16"/>
+      <c r="I80" s="16"/>
+      <c r="J80" s="16"/>
+      <c r="K80" s="16"/>
+      <c r="L80" s="16"/>
       <c r="M80" t="s">
         <v>214</v>
       </c>
@@ -4342,18 +4348,18 @@
       </c>
     </row>
     <row r="81" spans="1:22" ht="60" x14ac:dyDescent="0.25">
-      <c r="A81" s="17"/>
-      <c r="B81" s="17"/>
-      <c r="C81" s="21"/>
-      <c r="D81" s="15"/>
-      <c r="E81" s="25"/>
-      <c r="F81" s="25"/>
-      <c r="G81" s="17"/>
-      <c r="H81" s="17"/>
-      <c r="I81" s="17"/>
-      <c r="J81" s="17"/>
-      <c r="K81" s="17"/>
-      <c r="L81" s="17"/>
+      <c r="A81" s="16"/>
+      <c r="B81" s="16"/>
+      <c r="C81" s="15"/>
+      <c r="D81" s="20"/>
+      <c r="E81" s="21"/>
+      <c r="F81" s="21"/>
+      <c r="G81" s="16"/>
+      <c r="H81" s="16"/>
+      <c r="I81" s="16"/>
+      <c r="J81" s="16"/>
+      <c r="K81" s="16"/>
+      <c r="L81" s="16"/>
       <c r="M81" t="s">
         <v>132</v>
       </c>
@@ -4368,18 +4374,18 @@
       </c>
     </row>
     <row r="82" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A82" s="17"/>
-      <c r="B82" s="17"/>
-      <c r="C82" s="21"/>
-      <c r="D82" s="15"/>
-      <c r="E82" s="25"/>
-      <c r="F82" s="25"/>
-      <c r="G82" s="17"/>
-      <c r="H82" s="17"/>
-      <c r="I82" s="17"/>
-      <c r="J82" s="17"/>
-      <c r="K82" s="17"/>
-      <c r="L82" s="17"/>
+      <c r="A82" s="16"/>
+      <c r="B82" s="16"/>
+      <c r="C82" s="15"/>
+      <c r="D82" s="20"/>
+      <c r="E82" s="21"/>
+      <c r="F82" s="21"/>
+      <c r="G82" s="16"/>
+      <c r="H82" s="16"/>
+      <c r="I82" s="16"/>
+      <c r="J82" s="16"/>
+      <c r="K82" s="16"/>
+      <c r="L82" s="16"/>
       <c r="M82" t="s">
         <v>133</v>
       </c>
@@ -4391,32 +4397,32 @@
       </c>
     </row>
     <row r="83" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="B83" s="17" t="s">
+      <c r="A83" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B83" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="C83" s="21"/>
-      <c r="D83" s="15" t="s">
+      <c r="C83" s="15"/>
+      <c r="D83" s="20" t="s">
         <v>221</v>
       </c>
-      <c r="E83" s="25"/>
-      <c r="F83" s="25"/>
-      <c r="G83" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="H83" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I83" s="17"/>
-      <c r="J83" s="17" t="s">
+      <c r="E83" s="21"/>
+      <c r="F83" s="21"/>
+      <c r="G83" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H83" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I83" s="16"/>
+      <c r="J83" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="K83" s="17" t="s">
+      <c r="K83" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L83" s="17" t="s">
+      <c r="L83" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M83" t="s">
@@ -4430,18 +4436,18 @@
       </c>
     </row>
     <row r="84" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A84" s="21"/>
-      <c r="B84" s="17"/>
-      <c r="C84" s="21"/>
-      <c r="D84" s="15"/>
-      <c r="E84" s="25"/>
-      <c r="F84" s="25"/>
-      <c r="G84" s="17"/>
-      <c r="H84" s="17"/>
-      <c r="I84" s="17"/>
-      <c r="J84" s="17"/>
-      <c r="K84" s="17"/>
-      <c r="L84" s="17"/>
+      <c r="A84" s="15"/>
+      <c r="B84" s="16"/>
+      <c r="C84" s="15"/>
+      <c r="D84" s="20"/>
+      <c r="E84" s="21"/>
+      <c r="F84" s="21"/>
+      <c r="G84" s="16"/>
+      <c r="H84" s="16"/>
+      <c r="I84" s="16"/>
+      <c r="J84" s="16"/>
+      <c r="K84" s="16"/>
+      <c r="L84" s="16"/>
       <c r="M84" t="s">
         <v>212</v>
       </c>
@@ -4453,18 +4459,18 @@
       </c>
     </row>
     <row r="85" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A85" s="21"/>
-      <c r="B85" s="17"/>
-      <c r="C85" s="21"/>
-      <c r="D85" s="15"/>
-      <c r="E85" s="25"/>
-      <c r="F85" s="25"/>
-      <c r="G85" s="17"/>
-      <c r="H85" s="17"/>
-      <c r="I85" s="17"/>
-      <c r="J85" s="17"/>
-      <c r="K85" s="17"/>
-      <c r="L85" s="17"/>
+      <c r="A85" s="15"/>
+      <c r="B85" s="16"/>
+      <c r="C85" s="15"/>
+      <c r="D85" s="20"/>
+      <c r="E85" s="21"/>
+      <c r="F85" s="21"/>
+      <c r="G85" s="16"/>
+      <c r="H85" s="16"/>
+      <c r="I85" s="16"/>
+      <c r="J85" s="16"/>
+      <c r="K85" s="16"/>
+      <c r="L85" s="16"/>
       <c r="M85" t="s">
         <v>214</v>
       </c>
@@ -4476,18 +4482,18 @@
       </c>
     </row>
     <row r="86" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A86" s="21"/>
-      <c r="B86" s="17"/>
-      <c r="C86" s="21"/>
-      <c r="D86" s="15"/>
-      <c r="E86" s="25"/>
-      <c r="F86" s="25"/>
-      <c r="G86" s="17"/>
-      <c r="H86" s="17"/>
-      <c r="I86" s="17"/>
-      <c r="J86" s="17"/>
-      <c r="K86" s="17"/>
-      <c r="L86" s="17"/>
+      <c r="A86" s="15"/>
+      <c r="B86" s="16"/>
+      <c r="C86" s="15"/>
+      <c r="D86" s="20"/>
+      <c r="E86" s="21"/>
+      <c r="F86" s="21"/>
+      <c r="G86" s="16"/>
+      <c r="H86" s="16"/>
+      <c r="I86" s="16"/>
+      <c r="J86" s="16"/>
+      <c r="K86" s="16"/>
+      <c r="L86" s="16"/>
       <c r="M86" t="s">
         <v>132</v>
       </c>
@@ -4499,18 +4505,18 @@
       </c>
     </row>
     <row r="87" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A87" s="21"/>
-      <c r="B87" s="17"/>
-      <c r="C87" s="21"/>
-      <c r="D87" s="15"/>
-      <c r="E87" s="25"/>
-      <c r="F87" s="25"/>
-      <c r="G87" s="17"/>
-      <c r="H87" s="17"/>
-      <c r="I87" s="17"/>
-      <c r="J87" s="17"/>
-      <c r="K87" s="17"/>
-      <c r="L87" s="17"/>
+      <c r="A87" s="15"/>
+      <c r="B87" s="16"/>
+      <c r="C87" s="15"/>
+      <c r="D87" s="20"/>
+      <c r="E87" s="21"/>
+      <c r="F87" s="21"/>
+      <c r="G87" s="16"/>
+      <c r="H87" s="16"/>
+      <c r="I87" s="16"/>
+      <c r="J87" s="16"/>
+      <c r="K87" s="16"/>
+      <c r="L87" s="16"/>
       <c r="M87" t="s">
         <v>133</v>
       </c>
@@ -4525,34 +4531,34 @@
       </c>
     </row>
     <row r="88" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B88" s="17" t="s">
+      <c r="A88" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B88" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="C88" s="21"/>
-      <c r="D88" s="15" t="s">
+      <c r="C88" s="15"/>
+      <c r="D88" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="E88" s="25"/>
-      <c r="F88" s="25"/>
-      <c r="G88" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="H88" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I88" s="17" t="s">
+      <c r="E88" s="21"/>
+      <c r="F88" s="21"/>
+      <c r="G88" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H88" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I88" s="16" t="s">
         <v>224</v>
       </c>
-      <c r="J88" s="17" t="s">
+      <c r="J88" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="K88" s="17" t="s">
+      <c r="K88" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L88" s="17" t="s">
+      <c r="L88" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M88" t="s">
@@ -4569,18 +4575,18 @@
       </c>
     </row>
     <row r="89" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="17"/>
-      <c r="B89" s="17"/>
-      <c r="C89" s="21"/>
-      <c r="D89" s="15"/>
-      <c r="E89" s="25"/>
-      <c r="F89" s="25"/>
-      <c r="G89" s="17"/>
-      <c r="H89" s="17"/>
-      <c r="I89" s="17"/>
-      <c r="J89" s="17"/>
-      <c r="K89" s="17"/>
-      <c r="L89" s="17"/>
+      <c r="A89" s="16"/>
+      <c r="B89" s="16"/>
+      <c r="C89" s="15"/>
+      <c r="D89" s="20"/>
+      <c r="E89" s="21"/>
+      <c r="F89" s="21"/>
+      <c r="G89" s="16"/>
+      <c r="H89" s="16"/>
+      <c r="I89" s="16"/>
+      <c r="J89" s="16"/>
+      <c r="K89" s="16"/>
+      <c r="L89" s="16"/>
       <c r="M89" t="s">
         <v>47</v>
       </c>
@@ -4595,18 +4601,18 @@
       </c>
     </row>
     <row r="90" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="17"/>
-      <c r="B90" s="17"/>
-      <c r="C90" s="21"/>
-      <c r="D90" s="15"/>
-      <c r="E90" s="25"/>
-      <c r="F90" s="25"/>
-      <c r="G90" s="17"/>
-      <c r="H90" s="17"/>
-      <c r="I90" s="17"/>
-      <c r="J90" s="17"/>
-      <c r="K90" s="17"/>
-      <c r="L90" s="17"/>
+      <c r="A90" s="16"/>
+      <c r="B90" s="16"/>
+      <c r="C90" s="15"/>
+      <c r="D90" s="20"/>
+      <c r="E90" s="21"/>
+      <c r="F90" s="21"/>
+      <c r="G90" s="16"/>
+      <c r="H90" s="16"/>
+      <c r="I90" s="16"/>
+      <c r="J90" s="16"/>
+      <c r="K90" s="16"/>
+      <c r="L90" s="16"/>
       <c r="M90" t="s">
         <v>180</v>
       </c>
@@ -4621,18 +4627,18 @@
       </c>
     </row>
     <row r="91" spans="1:22" ht="75" x14ac:dyDescent="0.25">
-      <c r="A91" s="17"/>
-      <c r="B91" s="17"/>
-      <c r="C91" s="21"/>
-      <c r="D91" s="15"/>
-      <c r="E91" s="25"/>
-      <c r="F91" s="25"/>
-      <c r="G91" s="17"/>
-      <c r="H91" s="17"/>
-      <c r="I91" s="17"/>
-      <c r="J91" s="17"/>
-      <c r="K91" s="17"/>
-      <c r="L91" s="17"/>
+      <c r="A91" s="16"/>
+      <c r="B91" s="16"/>
+      <c r="C91" s="15"/>
+      <c r="D91" s="20"/>
+      <c r="E91" s="21"/>
+      <c r="F91" s="21"/>
+      <c r="G91" s="16"/>
+      <c r="H91" s="16"/>
+      <c r="I91" s="16"/>
+      <c r="J91" s="16"/>
+      <c r="K91" s="16"/>
+      <c r="L91" s="16"/>
       <c r="M91" t="s">
         <v>214</v>
       </c>
@@ -4647,18 +4653,18 @@
       </c>
     </row>
     <row r="92" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A92" s="17"/>
-      <c r="B92" s="17"/>
-      <c r="C92" s="21"/>
-      <c r="D92" s="15"/>
-      <c r="E92" s="25"/>
-      <c r="F92" s="25"/>
-      <c r="G92" s="17"/>
-      <c r="H92" s="17"/>
-      <c r="I92" s="17"/>
-      <c r="J92" s="17"/>
-      <c r="K92" s="17"/>
-      <c r="L92" s="17"/>
+      <c r="A92" s="16"/>
+      <c r="B92" s="16"/>
+      <c r="C92" s="15"/>
+      <c r="D92" s="20"/>
+      <c r="E92" s="21"/>
+      <c r="F92" s="21"/>
+      <c r="G92" s="16"/>
+      <c r="H92" s="16"/>
+      <c r="I92" s="16"/>
+      <c r="J92" s="16"/>
+      <c r="K92" s="16"/>
+      <c r="L92" s="16"/>
       <c r="M92" t="s">
         <v>132</v>
       </c>
@@ -4670,18 +4676,18 @@
       </c>
     </row>
     <row r="93" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A93" s="17"/>
-      <c r="B93" s="17"/>
-      <c r="C93" s="21"/>
-      <c r="D93" s="15"/>
-      <c r="E93" s="25"/>
-      <c r="F93" s="25"/>
-      <c r="G93" s="17"/>
-      <c r="H93" s="17"/>
-      <c r="I93" s="17"/>
-      <c r="J93" s="17"/>
-      <c r="K93" s="17"/>
-      <c r="L93" s="17"/>
+      <c r="A93" s="16"/>
+      <c r="B93" s="16"/>
+      <c r="C93" s="15"/>
+      <c r="D93" s="20"/>
+      <c r="E93" s="21"/>
+      <c r="F93" s="21"/>
+      <c r="G93" s="16"/>
+      <c r="H93" s="16"/>
+      <c r="I93" s="16"/>
+      <c r="J93" s="16"/>
+      <c r="K93" s="16"/>
+      <c r="L93" s="16"/>
       <c r="M93" t="s">
         <v>133</v>
       </c>
@@ -4693,34 +4699,34 @@
       </c>
     </row>
     <row r="94" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A94" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B94" s="17" t="s">
+      <c r="A94" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B94" s="16" t="s">
         <v>233</v>
       </c>
-      <c r="C94" s="21"/>
-      <c r="D94" s="15" t="s">
+      <c r="C94" s="15"/>
+      <c r="D94" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="E94" s="25"/>
-      <c r="F94" s="25"/>
-      <c r="G94" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="H94" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I94" s="17" t="s">
+      <c r="E94" s="21"/>
+      <c r="F94" s="21"/>
+      <c r="G94" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H94" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I94" s="16" t="s">
         <v>232</v>
       </c>
-      <c r="J94" s="17" t="s">
+      <c r="J94" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="K94" s="17" t="s">
+      <c r="K94" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L94" s="17" t="s">
+      <c r="L94" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M94" t="s">
@@ -4734,18 +4740,18 @@
       </c>
     </row>
     <row r="95" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A95" s="17"/>
-      <c r="B95" s="17"/>
-      <c r="C95" s="21"/>
-      <c r="D95" s="15"/>
-      <c r="E95" s="25"/>
-      <c r="F95" s="25"/>
-      <c r="G95" s="17"/>
-      <c r="H95" s="17"/>
-      <c r="I95" s="17"/>
-      <c r="J95" s="17"/>
-      <c r="K95" s="17"/>
-      <c r="L95" s="17"/>
+      <c r="A95" s="16"/>
+      <c r="B95" s="16"/>
+      <c r="C95" s="15"/>
+      <c r="D95" s="20"/>
+      <c r="E95" s="21"/>
+      <c r="F95" s="21"/>
+      <c r="G95" s="16"/>
+      <c r="H95" s="16"/>
+      <c r="I95" s="16"/>
+      <c r="J95" s="16"/>
+      <c r="K95" s="16"/>
+      <c r="L95" s="16"/>
       <c r="M95" t="s">
         <v>212</v>
       </c>
@@ -4760,18 +4766,18 @@
       </c>
     </row>
     <row r="96" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A96" s="17"/>
-      <c r="B96" s="17"/>
-      <c r="C96" s="21"/>
-      <c r="D96" s="15"/>
-      <c r="E96" s="25"/>
-      <c r="F96" s="25"/>
-      <c r="G96" s="17"/>
-      <c r="H96" s="17"/>
-      <c r="I96" s="17"/>
-      <c r="J96" s="17"/>
-      <c r="K96" s="17"/>
-      <c r="L96" s="17"/>
+      <c r="A96" s="16"/>
+      <c r="B96" s="16"/>
+      <c r="C96" s="15"/>
+      <c r="D96" s="20"/>
+      <c r="E96" s="21"/>
+      <c r="F96" s="21"/>
+      <c r="G96" s="16"/>
+      <c r="H96" s="16"/>
+      <c r="I96" s="16"/>
+      <c r="J96" s="16"/>
+      <c r="K96" s="16"/>
+      <c r="L96" s="16"/>
       <c r="M96" t="s">
         <v>212</v>
       </c>
@@ -4786,34 +4792,34 @@
       </c>
     </row>
     <row r="97" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A97" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B97" s="17" t="s">
+      <c r="A97" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B97" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="C97" s="21"/>
-      <c r="D97" s="15" t="s">
+      <c r="C97" s="15"/>
+      <c r="D97" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="E97" s="25"/>
-      <c r="F97" s="25"/>
-      <c r="G97" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="H97" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I97" s="17" t="s">
+      <c r="E97" s="21"/>
+      <c r="F97" s="21"/>
+      <c r="G97" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H97" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I97" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="J97" s="17" t="s">
+      <c r="J97" s="16" t="s">
         <v>241</v>
       </c>
-      <c r="K97" s="17" t="s">
+      <c r="K97" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L97" s="17" t="s">
+      <c r="L97" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M97" t="s">
@@ -4827,18 +4833,18 @@
       </c>
     </row>
     <row r="98" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A98" s="17"/>
-      <c r="B98" s="17"/>
-      <c r="C98" s="21"/>
-      <c r="D98" s="15"/>
-      <c r="E98" s="25"/>
-      <c r="F98" s="25"/>
-      <c r="G98" s="17"/>
-      <c r="H98" s="17"/>
-      <c r="I98" s="17"/>
-      <c r="J98" s="17"/>
-      <c r="K98" s="17"/>
-      <c r="L98" s="17"/>
+      <c r="A98" s="16"/>
+      <c r="B98" s="16"/>
+      <c r="C98" s="15"/>
+      <c r="D98" s="20"/>
+      <c r="E98" s="21"/>
+      <c r="F98" s="21"/>
+      <c r="G98" s="16"/>
+      <c r="H98" s="16"/>
+      <c r="I98" s="16"/>
+      <c r="J98" s="16"/>
+      <c r="K98" s="16"/>
+      <c r="L98" s="16"/>
       <c r="M98" t="s">
         <v>212</v>
       </c>
@@ -4952,34 +4958,34 @@
       </c>
     </row>
     <row r="102" spans="1:22" ht="60" x14ac:dyDescent="0.25">
-      <c r="A102" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B102" s="17" t="s">
+      <c r="A102" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B102" s="16" t="s">
         <v>250</v>
       </c>
-      <c r="C102" s="21"/>
-      <c r="D102" s="15" t="s">
+      <c r="C102" s="15"/>
+      <c r="D102" s="20" t="s">
         <v>254</v>
       </c>
-      <c r="E102" s="25"/>
-      <c r="F102" s="25"/>
-      <c r="G102" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="H102" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I102" s="17" t="s">
+      <c r="E102" s="21"/>
+      <c r="F102" s="21"/>
+      <c r="G102" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H102" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I102" s="16" t="s">
         <v>251</v>
       </c>
-      <c r="J102" s="17" t="s">
+      <c r="J102" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="K102" s="17" t="s">
+      <c r="K102" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L102" s="17" t="s">
+      <c r="L102" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M102" t="s">
@@ -4996,18 +5002,18 @@
       </c>
     </row>
     <row r="103" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A103" s="17"/>
-      <c r="B103" s="17"/>
-      <c r="C103" s="21"/>
-      <c r="D103" s="15"/>
-      <c r="E103" s="25"/>
-      <c r="F103" s="25"/>
-      <c r="G103" s="17"/>
-      <c r="H103" s="17"/>
-      <c r="I103" s="17"/>
-      <c r="J103" s="17"/>
-      <c r="K103" s="17"/>
-      <c r="L103" s="17"/>
+      <c r="A103" s="16"/>
+      <c r="B103" s="16"/>
+      <c r="C103" s="15"/>
+      <c r="D103" s="20"/>
+      <c r="E103" s="21"/>
+      <c r="F103" s="21"/>
+      <c r="G103" s="16"/>
+      <c r="H103" s="16"/>
+      <c r="I103" s="16"/>
+      <c r="J103" s="16"/>
+      <c r="K103" s="16"/>
+      <c r="L103" s="16"/>
       <c r="M103" t="s">
         <v>187</v>
       </c>
@@ -5022,18 +5028,18 @@
       </c>
     </row>
     <row r="104" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A104" s="17"/>
-      <c r="B104" s="17"/>
-      <c r="C104" s="21"/>
-      <c r="D104" s="15"/>
-      <c r="E104" s="25"/>
-      <c r="F104" s="25"/>
-      <c r="G104" s="17"/>
-      <c r="H104" s="17"/>
-      <c r="I104" s="17"/>
-      <c r="J104" s="17"/>
-      <c r="K104" s="17"/>
-      <c r="L104" s="17"/>
+      <c r="A104" s="16"/>
+      <c r="B104" s="16"/>
+      <c r="C104" s="15"/>
+      <c r="D104" s="20"/>
+      <c r="E104" s="21"/>
+      <c r="F104" s="21"/>
+      <c r="G104" s="16"/>
+      <c r="H104" s="16"/>
+      <c r="I104" s="16"/>
+      <c r="J104" s="16"/>
+      <c r="K104" s="16"/>
+      <c r="L104" s="16"/>
       <c r="M104" t="s">
         <v>212</v>
       </c>
@@ -5048,34 +5054,34 @@
       </c>
     </row>
     <row r="105" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A105" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B105" s="17" t="s">
+      <c r="A105" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B105" s="16" t="s">
         <v>258</v>
       </c>
-      <c r="C105" s="21"/>
-      <c r="D105" s="15" t="s">
+      <c r="C105" s="15"/>
+      <c r="D105" s="20" t="s">
         <v>259</v>
       </c>
-      <c r="E105" s="25"/>
-      <c r="F105" s="25"/>
-      <c r="G105" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="H105" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I105" s="17" t="s">
+      <c r="E105" s="21"/>
+      <c r="F105" s="21"/>
+      <c r="G105" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H105" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I105" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="J105" s="19" t="s">
+      <c r="J105" s="18" t="s">
         <v>265</v>
       </c>
-      <c r="K105" s="17" t="s">
+      <c r="K105" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L105" s="17" t="s">
+      <c r="L105" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M105" t="s">
@@ -5092,18 +5098,18 @@
       </c>
     </row>
     <row r="106" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A106" s="17"/>
-      <c r="B106" s="17"/>
-      <c r="C106" s="21"/>
-      <c r="D106" s="15"/>
-      <c r="E106" s="25"/>
-      <c r="F106" s="25"/>
-      <c r="G106" s="17"/>
-      <c r="H106" s="17"/>
-      <c r="I106" s="17"/>
-      <c r="J106" s="19"/>
-      <c r="K106" s="17"/>
-      <c r="L106" s="17"/>
+      <c r="A106" s="16"/>
+      <c r="B106" s="16"/>
+      <c r="C106" s="15"/>
+      <c r="D106" s="20"/>
+      <c r="E106" s="21"/>
+      <c r="F106" s="21"/>
+      <c r="G106" s="16"/>
+      <c r="H106" s="16"/>
+      <c r="I106" s="16"/>
+      <c r="J106" s="18"/>
+      <c r="K106" s="16"/>
+      <c r="L106" s="16"/>
       <c r="M106" t="s">
         <v>212</v>
       </c>
@@ -5118,18 +5124,18 @@
       </c>
     </row>
     <row r="107" spans="1:22" ht="60" x14ac:dyDescent="0.25">
-      <c r="A107" s="17"/>
-      <c r="B107" s="17"/>
-      <c r="C107" s="21"/>
-      <c r="D107" s="15"/>
-      <c r="E107" s="25"/>
-      <c r="F107" s="25"/>
-      <c r="G107" s="17"/>
-      <c r="H107" s="17"/>
-      <c r="I107" s="17"/>
-      <c r="J107" s="19"/>
-      <c r="K107" s="17"/>
-      <c r="L107" s="17"/>
+      <c r="A107" s="16"/>
+      <c r="B107" s="16"/>
+      <c r="C107" s="15"/>
+      <c r="D107" s="20"/>
+      <c r="E107" s="21"/>
+      <c r="F107" s="21"/>
+      <c r="G107" s="16"/>
+      <c r="H107" s="16"/>
+      <c r="I107" s="16"/>
+      <c r="J107" s="18"/>
+      <c r="K107" s="16"/>
+      <c r="L107" s="16"/>
       <c r="M107" t="s">
         <v>212</v>
       </c>
@@ -5144,18 +5150,18 @@
       </c>
     </row>
     <row r="108" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A108" s="17"/>
-      <c r="B108" s="17"/>
-      <c r="C108" s="21"/>
-      <c r="D108" s="15"/>
-      <c r="E108" s="25"/>
-      <c r="F108" s="25"/>
-      <c r="G108" s="17"/>
-      <c r="H108" s="17"/>
-      <c r="I108" s="17"/>
-      <c r="J108" s="19"/>
-      <c r="K108" s="17"/>
-      <c r="L108" s="17"/>
+      <c r="A108" s="16"/>
+      <c r="B108" s="16"/>
+      <c r="C108" s="15"/>
+      <c r="D108" s="20"/>
+      <c r="E108" s="21"/>
+      <c r="F108" s="21"/>
+      <c r="G108" s="16"/>
+      <c r="H108" s="16"/>
+      <c r="I108" s="16"/>
+      <c r="J108" s="18"/>
+      <c r="K108" s="16"/>
+      <c r="L108" s="16"/>
       <c r="M108" t="s">
         <v>212</v>
       </c>
@@ -5208,32 +5214,32 @@
       </c>
     </row>
     <row r="110" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A110" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B110" s="17" t="s">
+      <c r="A110" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B110" s="16" t="s">
         <v>270</v>
       </c>
-      <c r="C110" s="21"/>
-      <c r="D110" s="18" t="s">
+      <c r="C110" s="15"/>
+      <c r="D110" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="E110" s="20"/>
-      <c r="F110" s="20"/>
-      <c r="G110" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="H110" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I110" s="17"/>
-      <c r="J110" s="19" t="s">
+      <c r="E110" s="19"/>
+      <c r="F110" s="19"/>
+      <c r="G110" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H110" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I110" s="16"/>
+      <c r="J110" s="18" t="s">
         <v>271</v>
       </c>
-      <c r="K110" s="17" t="s">
+      <c r="K110" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L110" s="17" t="s">
+      <c r="L110" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M110" t="s">
@@ -5250,18 +5256,18 @@
       </c>
     </row>
     <row r="111" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A111" s="17"/>
-      <c r="B111" s="17"/>
-      <c r="C111" s="21"/>
-      <c r="D111" s="18"/>
-      <c r="E111" s="20"/>
-      <c r="F111" s="20"/>
-      <c r="G111" s="17"/>
-      <c r="H111" s="17"/>
-      <c r="I111" s="17"/>
-      <c r="J111" s="19"/>
-      <c r="K111" s="17"/>
-      <c r="L111" s="17"/>
+      <c r="A111" s="16"/>
+      <c r="B111" s="16"/>
+      <c r="C111" s="15"/>
+      <c r="D111" s="17"/>
+      <c r="E111" s="19"/>
+      <c r="F111" s="19"/>
+      <c r="G111" s="16"/>
+      <c r="H111" s="16"/>
+      <c r="I111" s="16"/>
+      <c r="J111" s="18"/>
+      <c r="K111" s="16"/>
+      <c r="L111" s="16"/>
       <c r="M111" t="s">
         <v>212</v>
       </c>
@@ -5276,18 +5282,18 @@
       </c>
     </row>
     <row r="112" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A112" s="17"/>
-      <c r="B112" s="17"/>
-      <c r="C112" s="21"/>
-      <c r="D112" s="18"/>
-      <c r="E112" s="20"/>
-      <c r="F112" s="20"/>
-      <c r="G112" s="17"/>
-      <c r="H112" s="17"/>
-      <c r="I112" s="17"/>
-      <c r="J112" s="19"/>
-      <c r="K112" s="17"/>
-      <c r="L112" s="17"/>
+      <c r="A112" s="16"/>
+      <c r="B112" s="16"/>
+      <c r="C112" s="15"/>
+      <c r="D112" s="17"/>
+      <c r="E112" s="19"/>
+      <c r="F112" s="19"/>
+      <c r="G112" s="16"/>
+      <c r="H112" s="16"/>
+      <c r="I112" s="16"/>
+      <c r="J112" s="18"/>
+      <c r="K112" s="16"/>
+      <c r="L112" s="16"/>
       <c r="M112" t="s">
         <v>214</v>
       </c>
@@ -5302,32 +5308,32 @@
       </c>
     </row>
     <row r="113" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A113" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B113" s="17" t="s">
+      <c r="A113" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B113" s="16" t="s">
         <v>281</v>
       </c>
-      <c r="C113" s="21"/>
-      <c r="D113" s="18" t="s">
+      <c r="C113" s="15"/>
+      <c r="D113" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="E113" s="20"/>
-      <c r="F113" s="20"/>
-      <c r="G113" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="H113" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I113" s="17"/>
-      <c r="J113" s="19" t="s">
+      <c r="E113" s="19"/>
+      <c r="F113" s="19"/>
+      <c r="G113" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H113" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I113" s="16"/>
+      <c r="J113" s="18" t="s">
         <v>286</v>
       </c>
-      <c r="K113" s="17" t="s">
+      <c r="K113" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L113" s="17" t="s">
+      <c r="L113" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M113" t="s">
@@ -5344,18 +5350,18 @@
       </c>
     </row>
     <row r="114" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A114" s="17"/>
-      <c r="B114" s="17"/>
-      <c r="C114" s="21"/>
-      <c r="D114" s="18"/>
-      <c r="E114" s="20"/>
-      <c r="F114" s="20"/>
-      <c r="G114" s="17"/>
-      <c r="H114" s="17"/>
-      <c r="I114" s="17"/>
-      <c r="J114" s="19"/>
-      <c r="K114" s="17"/>
-      <c r="L114" s="17"/>
+      <c r="A114" s="16"/>
+      <c r="B114" s="16"/>
+      <c r="C114" s="15"/>
+      <c r="D114" s="17"/>
+      <c r="E114" s="19"/>
+      <c r="F114" s="19"/>
+      <c r="G114" s="16"/>
+      <c r="H114" s="16"/>
+      <c r="I114" s="16"/>
+      <c r="J114" s="18"/>
+      <c r="K114" s="16"/>
+      <c r="L114" s="16"/>
       <c r="M114" t="s">
         <v>212</v>
       </c>
@@ -5370,18 +5376,18 @@
       </c>
     </row>
     <row r="115" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A115" s="17"/>
-      <c r="B115" s="17"/>
-      <c r="C115" s="21"/>
-      <c r="D115" s="18"/>
-      <c r="E115" s="20"/>
-      <c r="F115" s="20"/>
-      <c r="G115" s="17"/>
-      <c r="H115" s="17"/>
-      <c r="I115" s="17"/>
-      <c r="J115" s="19"/>
-      <c r="K115" s="17"/>
-      <c r="L115" s="17"/>
+      <c r="A115" s="16"/>
+      <c r="B115" s="16"/>
+      <c r="C115" s="15"/>
+      <c r="D115" s="17"/>
+      <c r="E115" s="19"/>
+      <c r="F115" s="19"/>
+      <c r="G115" s="16"/>
+      <c r="H115" s="16"/>
+      <c r="I115" s="16"/>
+      <c r="J115" s="18"/>
+      <c r="K115" s="16"/>
+      <c r="L115" s="16"/>
       <c r="M115" t="s">
         <v>214</v>
       </c>
@@ -5396,32 +5402,32 @@
       </c>
     </row>
     <row r="116" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A116" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B116" s="17" t="s">
+      <c r="A116" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B116" s="16" t="s">
         <v>282</v>
       </c>
-      <c r="C116" s="21"/>
-      <c r="D116" s="18" t="s">
+      <c r="C116" s="15"/>
+      <c r="D116" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="E116" s="20"/>
-      <c r="F116" s="20"/>
-      <c r="G116" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="H116" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I116" s="17"/>
-      <c r="J116" s="19" t="s">
+      <c r="E116" s="19"/>
+      <c r="F116" s="19"/>
+      <c r="G116" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H116" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I116" s="16"/>
+      <c r="J116" s="18" t="s">
         <v>285</v>
       </c>
-      <c r="K116" s="17" t="s">
+      <c r="K116" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L116" s="17" t="s">
+      <c r="L116" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M116" t="s">
@@ -5438,18 +5444,18 @@
       </c>
     </row>
     <row r="117" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A117" s="17"/>
-      <c r="B117" s="17"/>
-      <c r="C117" s="21"/>
-      <c r="D117" s="18"/>
-      <c r="E117" s="20"/>
-      <c r="F117" s="20"/>
-      <c r="G117" s="17"/>
-      <c r="H117" s="17"/>
-      <c r="I117" s="17"/>
-      <c r="J117" s="19"/>
-      <c r="K117" s="17"/>
-      <c r="L117" s="17"/>
+      <c r="A117" s="16"/>
+      <c r="B117" s="16"/>
+      <c r="C117" s="15"/>
+      <c r="D117" s="17"/>
+      <c r="E117" s="19"/>
+      <c r="F117" s="19"/>
+      <c r="G117" s="16"/>
+      <c r="H117" s="16"/>
+      <c r="I117" s="16"/>
+      <c r="J117" s="18"/>
+      <c r="K117" s="16"/>
+      <c r="L117" s="16"/>
       <c r="M117" t="s">
         <v>212</v>
       </c>
@@ -5464,18 +5470,18 @@
       </c>
     </row>
     <row r="118" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A118" s="17"/>
-      <c r="B118" s="17"/>
-      <c r="C118" s="21"/>
-      <c r="D118" s="18"/>
-      <c r="E118" s="20"/>
-      <c r="F118" s="20"/>
-      <c r="G118" s="17"/>
-      <c r="H118" s="17"/>
-      <c r="I118" s="17"/>
-      <c r="J118" s="19"/>
-      <c r="K118" s="17"/>
-      <c r="L118" s="17"/>
+      <c r="A118" s="16"/>
+      <c r="B118" s="16"/>
+      <c r="C118" s="15"/>
+      <c r="D118" s="17"/>
+      <c r="E118" s="19"/>
+      <c r="F118" s="19"/>
+      <c r="G118" s="16"/>
+      <c r="H118" s="16"/>
+      <c r="I118" s="16"/>
+      <c r="J118" s="18"/>
+      <c r="K118" s="16"/>
+      <c r="L118" s="16"/>
       <c r="M118" t="s">
         <v>214</v>
       </c>
@@ -5490,32 +5496,32 @@
       </c>
     </row>
     <row r="119" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A119" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B119" s="17" t="s">
+      <c r="A119" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B119" s="16" t="s">
         <v>283</v>
       </c>
-      <c r="C119" s="21"/>
-      <c r="D119" s="18" t="s">
+      <c r="C119" s="15"/>
+      <c r="D119" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="E119" s="20"/>
-      <c r="F119" s="20"/>
-      <c r="G119" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="H119" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I119" s="17"/>
-      <c r="J119" s="19" t="s">
+      <c r="E119" s="19"/>
+      <c r="F119" s="19"/>
+      <c r="G119" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H119" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I119" s="16"/>
+      <c r="J119" s="18" t="s">
         <v>284</v>
       </c>
-      <c r="K119" s="17" t="s">
+      <c r="K119" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L119" s="17" t="s">
+      <c r="L119" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M119" t="s">
@@ -5532,18 +5538,18 @@
       </c>
     </row>
     <row r="120" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A120" s="17"/>
-      <c r="B120" s="17"/>
-      <c r="C120" s="21"/>
-      <c r="D120" s="18"/>
-      <c r="E120" s="20"/>
-      <c r="F120" s="20"/>
-      <c r="G120" s="17"/>
-      <c r="H120" s="17"/>
-      <c r="I120" s="17"/>
-      <c r="J120" s="19"/>
-      <c r="K120" s="17"/>
-      <c r="L120" s="17"/>
+      <c r="A120" s="16"/>
+      <c r="B120" s="16"/>
+      <c r="C120" s="15"/>
+      <c r="D120" s="17"/>
+      <c r="E120" s="19"/>
+      <c r="F120" s="19"/>
+      <c r="G120" s="16"/>
+      <c r="H120" s="16"/>
+      <c r="I120" s="16"/>
+      <c r="J120" s="18"/>
+      <c r="K120" s="16"/>
+      <c r="L120" s="16"/>
       <c r="M120" t="s">
         <v>212</v>
       </c>
@@ -5558,18 +5564,18 @@
       </c>
     </row>
     <row r="121" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A121" s="17"/>
-      <c r="B121" s="17"/>
-      <c r="C121" s="21"/>
-      <c r="D121" s="18"/>
-      <c r="E121" s="20"/>
-      <c r="F121" s="20"/>
-      <c r="G121" s="17"/>
-      <c r="H121" s="17"/>
-      <c r="I121" s="17"/>
-      <c r="J121" s="19"/>
-      <c r="K121" s="17"/>
-      <c r="L121" s="17"/>
+      <c r="A121" s="16"/>
+      <c r="B121" s="16"/>
+      <c r="C121" s="15"/>
+      <c r="D121" s="17"/>
+      <c r="E121" s="19"/>
+      <c r="F121" s="19"/>
+      <c r="G121" s="16"/>
+      <c r="H121" s="16"/>
+      <c r="I121" s="16"/>
+      <c r="J121" s="18"/>
+      <c r="K121" s="16"/>
+      <c r="L121" s="16"/>
       <c r="M121" t="s">
         <v>214</v>
       </c>
@@ -5584,38 +5590,38 @@
       </c>
     </row>
     <row r="122" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B122" s="14" t="s">
+      <c r="A122" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B122" s="22" t="s">
         <v>315</v>
       </c>
-      <c r="C122" s="14" t="s">
+      <c r="C122" s="22" t="s">
         <v>316</v>
       </c>
-      <c r="D122" s="15" t="s">
+      <c r="D122" s="20" t="s">
         <v>322</v>
       </c>
-      <c r="E122" s="14"/>
-      <c r="F122" s="16" t="s">
+      <c r="E122" s="22"/>
+      <c r="F122" s="25" t="s">
         <v>328</v>
       </c>
-      <c r="G122" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H122" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I122" s="14" t="s">
+      <c r="G122" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H122" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="I122" s="22" t="s">
         <v>317</v>
       </c>
-      <c r="J122" s="15" t="s">
+      <c r="J122" s="20" t="s">
         <v>318</v>
       </c>
-      <c r="K122" s="14" t="s">
+      <c r="K122" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="L122" s="14" t="s">
+      <c r="L122" s="22" t="s">
         <v>119</v>
       </c>
       <c r="M122" t="s">
@@ -5630,38 +5636,38 @@
       <c r="P122" s="11" t="s">
         <v>324</v>
       </c>
-      <c r="Q122" s="16" t="s">
+      <c r="Q122" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="R122" s="15" t="s">
+      <c r="R122" s="20" t="s">
         <v>329</v>
       </c>
-      <c r="S122" s="16" t="s">
+      <c r="S122" s="25" t="s">
         <v>320</v>
       </c>
-      <c r="T122" s="16" t="s">
+      <c r="T122" s="25" t="s">
         <v>319</v>
       </c>
-      <c r="U122" s="14" t="s">
+      <c r="U122" s="22" t="s">
         <v>308</v>
       </c>
-      <c r="V122" s="15" t="s">
+      <c r="V122" s="20" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="123" spans="1:22" ht="60" x14ac:dyDescent="0.25">
-      <c r="A123" s="14"/>
-      <c r="B123" s="14"/>
-      <c r="C123" s="14"/>
-      <c r="D123" s="14"/>
-      <c r="E123" s="14"/>
-      <c r="F123" s="16"/>
-      <c r="G123" s="14"/>
-      <c r="H123" s="14"/>
-      <c r="I123" s="14"/>
-      <c r="J123" s="15"/>
-      <c r="K123" s="14"/>
-      <c r="L123" s="14"/>
+      <c r="A123" s="22"/>
+      <c r="B123" s="22"/>
+      <c r="C123" s="22"/>
+      <c r="D123" s="22"/>
+      <c r="E123" s="22"/>
+      <c r="F123" s="25"/>
+      <c r="G123" s="22"/>
+      <c r="H123" s="22"/>
+      <c r="I123" s="22"/>
+      <c r="J123" s="20"/>
+      <c r="K123" s="22"/>
+      <c r="L123" s="22"/>
       <c r="M123" t="s">
         <v>177</v>
       </c>
@@ -5674,26 +5680,26 @@
       <c r="P123" s="11" t="s">
         <v>325</v>
       </c>
-      <c r="Q123" s="16"/>
-      <c r="R123" s="15"/>
-      <c r="S123" s="16"/>
-      <c r="T123" s="16"/>
-      <c r="U123" s="14"/>
-      <c r="V123" s="15"/>
+      <c r="Q123" s="25"/>
+      <c r="R123" s="20"/>
+      <c r="S123" s="25"/>
+      <c r="T123" s="25"/>
+      <c r="U123" s="22"/>
+      <c r="V123" s="20"/>
     </row>
     <row r="124" spans="1:22" ht="60" x14ac:dyDescent="0.25">
-      <c r="A124" s="14"/>
-      <c r="B124" s="14"/>
-      <c r="C124" s="14"/>
-      <c r="D124" s="14"/>
-      <c r="E124" s="14"/>
-      <c r="F124" s="16"/>
-      <c r="G124" s="14"/>
-      <c r="H124" s="14"/>
-      <c r="I124" s="14"/>
-      <c r="J124" s="15"/>
-      <c r="K124" s="14"/>
-      <c r="L124" s="14"/>
+      <c r="A124" s="22"/>
+      <c r="B124" s="22"/>
+      <c r="C124" s="22"/>
+      <c r="D124" s="22"/>
+      <c r="E124" s="22"/>
+      <c r="F124" s="25"/>
+      <c r="G124" s="22"/>
+      <c r="H124" s="22"/>
+      <c r="I124" s="22"/>
+      <c r="J124" s="20"/>
+      <c r="K124" s="22"/>
+      <c r="L124" s="22"/>
       <c r="M124" t="s">
         <v>111</v>
       </c>
@@ -5706,149 +5712,173 @@
       <c r="P124" s="11" t="s">
         <v>326</v>
       </c>
-      <c r="Q124" s="16"/>
-      <c r="R124" s="15"/>
-      <c r="S124" s="16"/>
-      <c r="T124" s="16"/>
-      <c r="U124" s="14"/>
-      <c r="V124" s="15"/>
+      <c r="Q124" s="25"/>
+      <c r="R124" s="20"/>
+      <c r="S124" s="25"/>
+      <c r="T124" s="25"/>
+      <c r="U124" s="22"/>
+      <c r="V124" s="20"/>
+    </row>
+    <row r="125" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>141</v>
+      </c>
+      <c r="B125" t="s">
+        <v>330</v>
+      </c>
+      <c r="C125" t="s">
+        <v>303</v>
+      </c>
+      <c r="G125" t="s">
+        <v>25</v>
+      </c>
+      <c r="H125" t="s">
+        <v>27</v>
+      </c>
+      <c r="I125" t="s">
+        <v>331</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:V1"/>
   <mergeCells count="294">
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="C64:C67"/>
-    <mergeCell ref="C68:C71"/>
-    <mergeCell ref="C72:C75"/>
-    <mergeCell ref="C78:C82"/>
-    <mergeCell ref="C83:C87"/>
-    <mergeCell ref="C88:C93"/>
-    <mergeCell ref="C94:C96"/>
-    <mergeCell ref="C97:C98"/>
-    <mergeCell ref="A110:A112"/>
-    <mergeCell ref="I110:I112"/>
-    <mergeCell ref="H110:H112"/>
-    <mergeCell ref="G110:G112"/>
-    <mergeCell ref="D110:D112"/>
-    <mergeCell ref="B110:B112"/>
-    <mergeCell ref="L110:L112"/>
-    <mergeCell ref="K110:K112"/>
-    <mergeCell ref="J110:J112"/>
-    <mergeCell ref="E110:E112"/>
-    <mergeCell ref="F110:F112"/>
-    <mergeCell ref="C110:C112"/>
-    <mergeCell ref="I105:I108"/>
-    <mergeCell ref="H105:H108"/>
-    <mergeCell ref="G105:G108"/>
-    <mergeCell ref="B105:B108"/>
-    <mergeCell ref="A105:A108"/>
-    <mergeCell ref="D105:D108"/>
-    <mergeCell ref="L105:L108"/>
-    <mergeCell ref="K105:K108"/>
-    <mergeCell ref="J105:J108"/>
-    <mergeCell ref="F105:F108"/>
-    <mergeCell ref="E105:E108"/>
-    <mergeCell ref="C105:C108"/>
-    <mergeCell ref="G97:G98"/>
-    <mergeCell ref="B97:B98"/>
-    <mergeCell ref="A97:A98"/>
-    <mergeCell ref="D97:D98"/>
-    <mergeCell ref="L102:L104"/>
-    <mergeCell ref="K102:K104"/>
-    <mergeCell ref="J102:J104"/>
-    <mergeCell ref="I102:I104"/>
-    <mergeCell ref="H102:H104"/>
-    <mergeCell ref="G102:G104"/>
-    <mergeCell ref="D102:D104"/>
-    <mergeCell ref="B102:B104"/>
-    <mergeCell ref="A102:A104"/>
-    <mergeCell ref="L97:L98"/>
-    <mergeCell ref="K97:K98"/>
-    <mergeCell ref="J97:J98"/>
-    <mergeCell ref="I97:I98"/>
-    <mergeCell ref="H97:H98"/>
-    <mergeCell ref="F97:F98"/>
-    <mergeCell ref="F102:F104"/>
-    <mergeCell ref="E97:E98"/>
-    <mergeCell ref="E102:E104"/>
-    <mergeCell ref="C102:C104"/>
-    <mergeCell ref="G94:G96"/>
-    <mergeCell ref="B94:B96"/>
-    <mergeCell ref="A94:A96"/>
-    <mergeCell ref="D94:D96"/>
-    <mergeCell ref="L94:L96"/>
-    <mergeCell ref="K94:K96"/>
-    <mergeCell ref="J94:J96"/>
-    <mergeCell ref="I94:I96"/>
-    <mergeCell ref="H94:H96"/>
-    <mergeCell ref="F94:F96"/>
-    <mergeCell ref="E94:E96"/>
-    <mergeCell ref="G83:G87"/>
-    <mergeCell ref="B83:B87"/>
-    <mergeCell ref="A83:A87"/>
-    <mergeCell ref="D83:D87"/>
-    <mergeCell ref="L88:L93"/>
-    <mergeCell ref="K88:K93"/>
-    <mergeCell ref="J88:J93"/>
-    <mergeCell ref="I88:I93"/>
-    <mergeCell ref="H88:H93"/>
-    <mergeCell ref="G88:G93"/>
-    <mergeCell ref="A88:A93"/>
-    <mergeCell ref="B88:B93"/>
-    <mergeCell ref="D88:D93"/>
-    <mergeCell ref="L83:L87"/>
-    <mergeCell ref="K83:K87"/>
-    <mergeCell ref="J83:J87"/>
-    <mergeCell ref="I83:I87"/>
-    <mergeCell ref="H83:H87"/>
-    <mergeCell ref="F83:F87"/>
-    <mergeCell ref="F88:F93"/>
-    <mergeCell ref="E83:E87"/>
-    <mergeCell ref="E88:E93"/>
-    <mergeCell ref="H78:H82"/>
-    <mergeCell ref="G78:G82"/>
-    <mergeCell ref="D78:D82"/>
-    <mergeCell ref="B78:B82"/>
-    <mergeCell ref="A78:A82"/>
-    <mergeCell ref="I72:I75"/>
-    <mergeCell ref="J72:J75"/>
-    <mergeCell ref="K72:K75"/>
-    <mergeCell ref="L72:L75"/>
-    <mergeCell ref="L78:L82"/>
-    <mergeCell ref="K78:K82"/>
-    <mergeCell ref="J78:J82"/>
-    <mergeCell ref="I78:I82"/>
-    <mergeCell ref="A72:A75"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="D72:D75"/>
-    <mergeCell ref="G72:G75"/>
-    <mergeCell ref="H72:H75"/>
-    <mergeCell ref="F72:F75"/>
-    <mergeCell ref="F78:F82"/>
-    <mergeCell ref="E72:E75"/>
-    <mergeCell ref="E78:E82"/>
-    <mergeCell ref="H68:H71"/>
-    <mergeCell ref="I68:I71"/>
-    <mergeCell ref="J68:J71"/>
-    <mergeCell ref="K68:K71"/>
-    <mergeCell ref="L68:L71"/>
-    <mergeCell ref="G64:G67"/>
-    <mergeCell ref="B64:B67"/>
-    <mergeCell ref="A64:A67"/>
-    <mergeCell ref="D64:D67"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="D68:D71"/>
-    <mergeCell ref="G68:G71"/>
-    <mergeCell ref="L64:L67"/>
-    <mergeCell ref="K64:K67"/>
-    <mergeCell ref="J64:J67"/>
-    <mergeCell ref="I64:I67"/>
-    <mergeCell ref="H64:H67"/>
-    <mergeCell ref="F64:F67"/>
-    <mergeCell ref="F68:F71"/>
-    <mergeCell ref="E64:E67"/>
-    <mergeCell ref="E68:E71"/>
+    <mergeCell ref="T122:T124"/>
+    <mergeCell ref="U122:U124"/>
+    <mergeCell ref="V122:V124"/>
+    <mergeCell ref="E122:E124"/>
+    <mergeCell ref="D122:D124"/>
+    <mergeCell ref="C122:C124"/>
+    <mergeCell ref="B122:B124"/>
+    <mergeCell ref="A122:A124"/>
+    <mergeCell ref="K122:K124"/>
+    <mergeCell ref="L122:L124"/>
+    <mergeCell ref="J122:J124"/>
+    <mergeCell ref="I122:I124"/>
+    <mergeCell ref="H122:H124"/>
+    <mergeCell ref="G122:G124"/>
+    <mergeCell ref="F122:F124"/>
+    <mergeCell ref="R122:R124"/>
+    <mergeCell ref="Q122:Q124"/>
+    <mergeCell ref="S122:S124"/>
+    <mergeCell ref="A119:A121"/>
+    <mergeCell ref="B119:B121"/>
+    <mergeCell ref="D119:D121"/>
+    <mergeCell ref="G119:G121"/>
+    <mergeCell ref="H119:H121"/>
+    <mergeCell ref="I119:I121"/>
+    <mergeCell ref="J119:J121"/>
+    <mergeCell ref="K119:K121"/>
+    <mergeCell ref="L119:L121"/>
+    <mergeCell ref="E119:E121"/>
+    <mergeCell ref="F119:F121"/>
+    <mergeCell ref="C119:C121"/>
+    <mergeCell ref="K113:K115"/>
+    <mergeCell ref="L113:L115"/>
+    <mergeCell ref="A116:A118"/>
+    <mergeCell ref="B116:B118"/>
+    <mergeCell ref="D116:D118"/>
+    <mergeCell ref="G116:G118"/>
+    <mergeCell ref="H116:H118"/>
+    <mergeCell ref="I116:I118"/>
+    <mergeCell ref="J116:J118"/>
+    <mergeCell ref="K116:K118"/>
+    <mergeCell ref="L116:L118"/>
+    <mergeCell ref="E113:E115"/>
+    <mergeCell ref="E116:E118"/>
+    <mergeCell ref="F113:F115"/>
+    <mergeCell ref="F116:F118"/>
+    <mergeCell ref="A113:A115"/>
+    <mergeCell ref="B113:B115"/>
+    <mergeCell ref="D113:D115"/>
+    <mergeCell ref="G113:G115"/>
+    <mergeCell ref="H113:H115"/>
+    <mergeCell ref="I113:I115"/>
+    <mergeCell ref="J113:J115"/>
+    <mergeCell ref="C113:C115"/>
+    <mergeCell ref="C116:C118"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="E37:E39"/>
+    <mergeCell ref="E41:E47"/>
+    <mergeCell ref="E57:E59"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="C37:C39"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="H31:H33"/>
+    <mergeCell ref="I31:I33"/>
+    <mergeCell ref="J31:J33"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="E28:E30"/>
+    <mergeCell ref="E31:E33"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="F28:F30"/>
+    <mergeCell ref="F31:F33"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="G28:G30"/>
+    <mergeCell ref="H28:H30"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="G31:G33"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="L41:L47"/>
+    <mergeCell ref="K41:K47"/>
+    <mergeCell ref="J41:J47"/>
+    <mergeCell ref="I41:I47"/>
+    <mergeCell ref="L28:L30"/>
+    <mergeCell ref="K28:K30"/>
+    <mergeCell ref="J28:J30"/>
+    <mergeCell ref="I28:I30"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="L24:L26"/>
+    <mergeCell ref="K24:K26"/>
+    <mergeCell ref="J24:J26"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="K31:K33"/>
+    <mergeCell ref="L31:L33"/>
+    <mergeCell ref="I34:I36"/>
+    <mergeCell ref="J34:J36"/>
+    <mergeCell ref="K34:K36"/>
+    <mergeCell ref="L34:L36"/>
+    <mergeCell ref="I37:I39"/>
+    <mergeCell ref="J37:J39"/>
+    <mergeCell ref="K37:K39"/>
+    <mergeCell ref="L37:L39"/>
+    <mergeCell ref="L57:L59"/>
+    <mergeCell ref="K57:K59"/>
+    <mergeCell ref="J57:J59"/>
+    <mergeCell ref="I57:I59"/>
+    <mergeCell ref="H57:H59"/>
+    <mergeCell ref="H41:H47"/>
+    <mergeCell ref="G41:G47"/>
+    <mergeCell ref="B41:B47"/>
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="F41:F47"/>
+    <mergeCell ref="F57:F59"/>
+    <mergeCell ref="G57:G59"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="C41:C47"/>
+    <mergeCell ref="C57:C59"/>
     <mergeCell ref="F34:F36"/>
     <mergeCell ref="F37:F39"/>
     <mergeCell ref="H34:H36"/>
@@ -5873,143 +5903,139 @@
     <mergeCell ref="D34:D36"/>
     <mergeCell ref="D37:D39"/>
     <mergeCell ref="E62:E63"/>
-    <mergeCell ref="L57:L59"/>
-    <mergeCell ref="K57:K59"/>
-    <mergeCell ref="J57:J59"/>
-    <mergeCell ref="I57:I59"/>
-    <mergeCell ref="H57:H59"/>
-    <mergeCell ref="H41:H47"/>
-    <mergeCell ref="G41:G47"/>
-    <mergeCell ref="B41:B47"/>
-    <mergeCell ref="A41:A47"/>
-    <mergeCell ref="F41:F47"/>
-    <mergeCell ref="F57:F59"/>
-    <mergeCell ref="G57:G59"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="C41:C47"/>
-    <mergeCell ref="C57:C59"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="L41:L47"/>
-    <mergeCell ref="K41:K47"/>
-    <mergeCell ref="J41:J47"/>
-    <mergeCell ref="I41:I47"/>
-    <mergeCell ref="L28:L30"/>
-    <mergeCell ref="K28:K30"/>
-    <mergeCell ref="J28:J30"/>
-    <mergeCell ref="I28:I30"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="L24:L26"/>
-    <mergeCell ref="K24:K26"/>
-    <mergeCell ref="J24:J26"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="K31:K33"/>
-    <mergeCell ref="L31:L33"/>
-    <mergeCell ref="I34:I36"/>
-    <mergeCell ref="J34:J36"/>
-    <mergeCell ref="K34:K36"/>
-    <mergeCell ref="L34:L36"/>
-    <mergeCell ref="I37:I39"/>
-    <mergeCell ref="J37:J39"/>
-    <mergeCell ref="K37:K39"/>
-    <mergeCell ref="L37:L39"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="H31:H33"/>
-    <mergeCell ref="I31:I33"/>
-    <mergeCell ref="J31:J33"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="E28:E30"/>
-    <mergeCell ref="E31:E33"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="F28:F30"/>
-    <mergeCell ref="F31:F33"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="G28:G30"/>
-    <mergeCell ref="H28:H30"/>
-    <mergeCell ref="G24:G26"/>
-    <mergeCell ref="G31:G33"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="E37:E39"/>
-    <mergeCell ref="E41:E47"/>
-    <mergeCell ref="E57:E59"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="C37:C39"/>
-    <mergeCell ref="K113:K115"/>
-    <mergeCell ref="L113:L115"/>
-    <mergeCell ref="A116:A118"/>
-    <mergeCell ref="B116:B118"/>
-    <mergeCell ref="D116:D118"/>
-    <mergeCell ref="G116:G118"/>
-    <mergeCell ref="H116:H118"/>
-    <mergeCell ref="I116:I118"/>
-    <mergeCell ref="J116:J118"/>
-    <mergeCell ref="K116:K118"/>
-    <mergeCell ref="L116:L118"/>
-    <mergeCell ref="E113:E115"/>
-    <mergeCell ref="E116:E118"/>
-    <mergeCell ref="F113:F115"/>
-    <mergeCell ref="F116:F118"/>
-    <mergeCell ref="A113:A115"/>
-    <mergeCell ref="B113:B115"/>
-    <mergeCell ref="D113:D115"/>
-    <mergeCell ref="G113:G115"/>
-    <mergeCell ref="H113:H115"/>
-    <mergeCell ref="I113:I115"/>
-    <mergeCell ref="J113:J115"/>
-    <mergeCell ref="C113:C115"/>
-    <mergeCell ref="C116:C118"/>
-    <mergeCell ref="A119:A121"/>
-    <mergeCell ref="B119:B121"/>
-    <mergeCell ref="D119:D121"/>
-    <mergeCell ref="G119:G121"/>
-    <mergeCell ref="H119:H121"/>
-    <mergeCell ref="I119:I121"/>
-    <mergeCell ref="J119:J121"/>
-    <mergeCell ref="K119:K121"/>
-    <mergeCell ref="L119:L121"/>
-    <mergeCell ref="E119:E121"/>
-    <mergeCell ref="F119:F121"/>
-    <mergeCell ref="C119:C121"/>
-    <mergeCell ref="T122:T124"/>
-    <mergeCell ref="U122:U124"/>
-    <mergeCell ref="V122:V124"/>
-    <mergeCell ref="E122:E124"/>
-    <mergeCell ref="D122:D124"/>
-    <mergeCell ref="C122:C124"/>
-    <mergeCell ref="B122:B124"/>
-    <mergeCell ref="A122:A124"/>
-    <mergeCell ref="K122:K124"/>
-    <mergeCell ref="L122:L124"/>
-    <mergeCell ref="J122:J124"/>
-    <mergeCell ref="I122:I124"/>
-    <mergeCell ref="H122:H124"/>
-    <mergeCell ref="G122:G124"/>
-    <mergeCell ref="F122:F124"/>
-    <mergeCell ref="R122:R124"/>
-    <mergeCell ref="Q122:Q124"/>
-    <mergeCell ref="S122:S124"/>
+    <mergeCell ref="H68:H71"/>
+    <mergeCell ref="I68:I71"/>
+    <mergeCell ref="J68:J71"/>
+    <mergeCell ref="K68:K71"/>
+    <mergeCell ref="L68:L71"/>
+    <mergeCell ref="G64:G67"/>
+    <mergeCell ref="B64:B67"/>
+    <mergeCell ref="A64:A67"/>
+    <mergeCell ref="D64:D67"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="D68:D71"/>
+    <mergeCell ref="G68:G71"/>
+    <mergeCell ref="L64:L67"/>
+    <mergeCell ref="K64:K67"/>
+    <mergeCell ref="J64:J67"/>
+    <mergeCell ref="I64:I67"/>
+    <mergeCell ref="H64:H67"/>
+    <mergeCell ref="F64:F67"/>
+    <mergeCell ref="F68:F71"/>
+    <mergeCell ref="E64:E67"/>
+    <mergeCell ref="E68:E71"/>
+    <mergeCell ref="H78:H82"/>
+    <mergeCell ref="G78:G82"/>
+    <mergeCell ref="D78:D82"/>
+    <mergeCell ref="B78:B82"/>
+    <mergeCell ref="A78:A82"/>
+    <mergeCell ref="I72:I75"/>
+    <mergeCell ref="J72:J75"/>
+    <mergeCell ref="K72:K75"/>
+    <mergeCell ref="L72:L75"/>
+    <mergeCell ref="L78:L82"/>
+    <mergeCell ref="K78:K82"/>
+    <mergeCell ref="J78:J82"/>
+    <mergeCell ref="I78:I82"/>
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="D72:D75"/>
+    <mergeCell ref="G72:G75"/>
+    <mergeCell ref="H72:H75"/>
+    <mergeCell ref="F72:F75"/>
+    <mergeCell ref="F78:F82"/>
+    <mergeCell ref="E72:E75"/>
+    <mergeCell ref="E78:E82"/>
+    <mergeCell ref="G83:G87"/>
+    <mergeCell ref="B83:B87"/>
+    <mergeCell ref="A83:A87"/>
+    <mergeCell ref="D83:D87"/>
+    <mergeCell ref="L88:L93"/>
+    <mergeCell ref="K88:K93"/>
+    <mergeCell ref="J88:J93"/>
+    <mergeCell ref="I88:I93"/>
+    <mergeCell ref="H88:H93"/>
+    <mergeCell ref="G88:G93"/>
+    <mergeCell ref="A88:A93"/>
+    <mergeCell ref="B88:B93"/>
+    <mergeCell ref="D88:D93"/>
+    <mergeCell ref="L83:L87"/>
+    <mergeCell ref="K83:K87"/>
+    <mergeCell ref="J83:J87"/>
+    <mergeCell ref="I83:I87"/>
+    <mergeCell ref="H83:H87"/>
+    <mergeCell ref="F83:F87"/>
+    <mergeCell ref="F88:F93"/>
+    <mergeCell ref="E83:E87"/>
+    <mergeCell ref="E88:E93"/>
+    <mergeCell ref="G94:G96"/>
+    <mergeCell ref="B94:B96"/>
+    <mergeCell ref="A94:A96"/>
+    <mergeCell ref="D94:D96"/>
+    <mergeCell ref="L94:L96"/>
+    <mergeCell ref="K94:K96"/>
+    <mergeCell ref="J94:J96"/>
+    <mergeCell ref="I94:I96"/>
+    <mergeCell ref="H94:H96"/>
+    <mergeCell ref="F94:F96"/>
+    <mergeCell ref="E94:E96"/>
+    <mergeCell ref="G97:G98"/>
+    <mergeCell ref="B97:B98"/>
+    <mergeCell ref="A97:A98"/>
+    <mergeCell ref="D97:D98"/>
+    <mergeCell ref="L102:L104"/>
+    <mergeCell ref="K102:K104"/>
+    <mergeCell ref="J102:J104"/>
+    <mergeCell ref="I102:I104"/>
+    <mergeCell ref="H102:H104"/>
+    <mergeCell ref="G102:G104"/>
+    <mergeCell ref="D102:D104"/>
+    <mergeCell ref="B102:B104"/>
+    <mergeCell ref="A102:A104"/>
+    <mergeCell ref="L97:L98"/>
+    <mergeCell ref="K97:K98"/>
+    <mergeCell ref="J97:J98"/>
+    <mergeCell ref="I97:I98"/>
+    <mergeCell ref="H97:H98"/>
+    <mergeCell ref="F97:F98"/>
+    <mergeCell ref="F102:F104"/>
+    <mergeCell ref="E97:E98"/>
+    <mergeCell ref="E102:E104"/>
+    <mergeCell ref="C102:C104"/>
+    <mergeCell ref="I105:I108"/>
+    <mergeCell ref="H105:H108"/>
+    <mergeCell ref="G105:G108"/>
+    <mergeCell ref="B105:B108"/>
+    <mergeCell ref="A105:A108"/>
+    <mergeCell ref="D105:D108"/>
+    <mergeCell ref="L105:L108"/>
+    <mergeCell ref="K105:K108"/>
+    <mergeCell ref="J105:J108"/>
+    <mergeCell ref="F105:F108"/>
+    <mergeCell ref="E105:E108"/>
+    <mergeCell ref="C105:C108"/>
+    <mergeCell ref="A110:A112"/>
+    <mergeCell ref="I110:I112"/>
+    <mergeCell ref="H110:H112"/>
+    <mergeCell ref="G110:G112"/>
+    <mergeCell ref="D110:D112"/>
+    <mergeCell ref="B110:B112"/>
+    <mergeCell ref="L110:L112"/>
+    <mergeCell ref="K110:K112"/>
+    <mergeCell ref="J110:J112"/>
+    <mergeCell ref="E110:E112"/>
+    <mergeCell ref="F110:F112"/>
+    <mergeCell ref="C110:C112"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="C64:C67"/>
+    <mergeCell ref="C68:C71"/>
+    <mergeCell ref="C72:C75"/>
+    <mergeCell ref="C78:C82"/>
+    <mergeCell ref="C83:C87"/>
+    <mergeCell ref="C88:C93"/>
+    <mergeCell ref="C94:C96"/>
+    <mergeCell ref="C97:C98"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="P54" r:id="rId1"/>

</xml_diff>

<commit_message>
Updating the sheet with Submit Service addition workflow
git-tfs-id: [http://developmentvlan:8585/tfs/vanrise.collection]$/;C55418
</commit_message>
<xml_diff>
--- a/SOM/Documents/SOM/SOM APIs Mapping Sheet.xlsx
+++ b/SOM/Documents/SOM/SOM APIs Mapping Sheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="354">
   <si>
     <t>GetTechnicalDetails</t>
   </si>
@@ -1054,10 +1054,95 @@
 At the end call for each package the servicesReadRequest in order to get the name of the service in addtion to other needed fields.</t>
   </si>
   <si>
-    <t>ST_AddAdditionalServices</t>
-  </si>
-  <si>
     <t>S2C3156</t>
+  </si>
+  <si>
+    <t>ST_Tel_AddAdditionalServices</t>
+  </si>
+  <si>
+    <t>S2C3106</t>
+  </si>
+  <si>
+    <t>This workflow activates network services that need provisioning on EDA if switch is automatic or manually creating work orders for the respective team (Switch, OMC, MGT or SPG)</t>
+  </si>
+  <si>
+    <t>This call should accept information about the switch, with OMC or not, manual or no.
+For now pass the switch id to it in addtion to netwrok services information.
+It will create a work order on BPM for the switch team for now, considering the switch is manual.</t>
+  </si>
+  <si>
+    <t>S2C3105</t>
+  </si>
+  <si>
+    <t>ST_ActivateNetworkService</t>
+  </si>
+  <si>
+    <t>ST_ProcessNetworkServiceChange</t>
+  </si>
+  <si>
+    <t>This workflow should accept line path and get the line path description in order to pass them later on to Activate Netwrok service sub workflow.
+It also accepts the list of network services, then it loops on each either it create a workorder (for now make it for switch team) or it calls the Activate Network service workflow for provisioning handling</t>
+  </si>
+  <si>
+    <t>This workflow accepts the list of all services to add on a specific contract, we have to pass for it the contract id, line path id also.
+It should check if a service is of type network to call ST_ProcessNetworkServiceChange to pocess it.
+In all cases it will call BSCS in order to Add and Write services added on this contract</t>
+  </si>
+  <si>
+    <t>ST_SubmitServiceAdd</t>
+  </si>
+  <si>
+    <t>L2S3209</t>
+  </si>
+  <si>
+    <t>contractInfoReadRequest</t>
+  </si>
+  <si>
+    <t>This workflow is common for all LOBs activating new services on the contract, then it should accept contract id and line path id and the list of services to add with their information.
+Based on LOB type it calls the respective workflow, in case of telephony ST_Tel_AddAdditionalServices is called</t>
+  </si>
+  <si>
+    <t>This workflow processes the changes done on services of type network. Ones that need provisioning to send them for EDA or manual, and others to create a work order for them</t>
+  </si>
+  <si>
+    <t>This workflow processes the addition of services on a telephony contract</t>
+  </si>
+  <si>
+    <t>accept contract id</t>
+  </si>
+  <si>
+    <t>pass all parameters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">requestId
+contractId
+contactId
+linePathId
+list&lt;ServiceToAdd&gt;
+ServiceCode
+ServicePackage
+ServiceType
+NeedsProvisioning
+</t>
+  </si>
+  <si>
+    <t>cosPendingStatus = 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linePathId
+listofServices
+requestId
+</t>
+  </si>
+  <si>
+    <t>requestId and
+F60012C5-A0C3-4593-B7C4-B50A21988D54</t>
+  </si>
+  <si>
+    <t>SetRequestAsCompleted</t>
+  </si>
+  <si>
+    <t>Only if workorder not created</t>
   </si>
 </sst>
 </file>
@@ -1180,7 +1265,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1212,6 +1297,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1230,22 +1330,10 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1713,11 +1801,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V125"/>
+  <dimension ref="A1:V134"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D125" sqref="D125"/>
+      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M131" sqref="M131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2449,34 +2537,34 @@
       </c>
     </row>
     <row r="22" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B22" s="22" t="s">
+      <c r="A22" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B22" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="17" t="s">
+      <c r="C22" s="19"/>
+      <c r="D22" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="22" t="s">
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="H22" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="I22" s="22" t="s">
+      <c r="H22" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I22" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="J22" s="20" t="s">
+      <c r="J22" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="K22" s="14" t="s">
+      <c r="K22" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="L22" s="22" t="s">
+      <c r="L22" s="16" t="s">
         <v>120</v>
       </c>
       <c r="M22" t="s">
@@ -2493,18 +2581,18 @@
       </c>
     </row>
     <row r="23" spans="1:22" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="22"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="16"/>
       <c r="M23" t="s">
         <v>157</v>
       </c>
@@ -2519,34 +2607,34 @@
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A24" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B24" s="16" t="s">
+      <c r="A24" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B24" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="17" t="s">
+      <c r="C24" s="20"/>
+      <c r="D24" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="16" t="s">
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H24" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I24" s="18" t="s">
+      <c r="H24" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="J24" s="16" t="s">
+      <c r="J24" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="K24" s="16" t="s">
+      <c r="K24" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="L24" s="23" t="s">
+      <c r="L24" s="25" t="s">
         <v>120</v>
       </c>
       <c r="M24" t="s">
@@ -2561,18 +2649,18 @@
       <c r="V24"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16"/>
-      <c r="L25" s="23"/>
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="25"/>
       <c r="M25" t="s">
         <v>73</v>
       </c>
@@ -2584,18 +2672,18 @@
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
-      <c r="L26" s="23"/>
+      <c r="A26" s="21"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="25"/>
       <c r="M26" t="s">
         <v>135</v>
       </c>
@@ -2650,34 +2738,34 @@
       </c>
     </row>
     <row r="28" spans="1:22" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B28" s="16" t="s">
+      <c r="A28" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B28" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="17" t="s">
+      <c r="C28" s="20"/>
+      <c r="D28" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="16" t="s">
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H28" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I28" s="16" t="s">
+      <c r="H28" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="I28" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="J28" s="18" t="s">
+      <c r="J28" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="K28" s="16" t="s">
+      <c r="K28" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="L28" s="16" t="s">
+      <c r="L28" s="21" t="s">
         <v>119</v>
       </c>
       <c r="M28" t="s">
@@ -2694,18 +2782,18 @@
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="16"/>
-      <c r="L29" s="16"/>
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="21"/>
       <c r="M29" t="s">
         <v>85</v>
       </c>
@@ -2717,18 +2805,18 @@
       </c>
     </row>
     <row r="30" spans="1:22" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="16"/>
-      <c r="L30" s="16"/>
+      <c r="A30" s="21"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21"/>
       <c r="M30" t="s">
         <v>90</v>
       </c>
@@ -2743,34 +2831,34 @@
       </c>
     </row>
     <row r="31" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B31" s="16" t="s">
+      <c r="A31" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B31" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="17" t="s">
+      <c r="C31" s="20"/>
+      <c r="D31" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="16" t="s">
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H31" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I31" s="16" t="s">
+      <c r="H31" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="I31" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="J31" s="18" t="s">
+      <c r="J31" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="K31" s="16" t="s">
+      <c r="K31" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="L31" s="16" t="s">
+      <c r="L31" s="21" t="s">
         <v>119</v>
       </c>
       <c r="M31" t="s">
@@ -2784,18 +2872,18 @@
       </c>
     </row>
     <row r="32" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="16"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="16"/>
-      <c r="L32" s="16"/>
+      <c r="A32" s="21"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="21"/>
       <c r="M32" t="s">
         <v>85</v>
       </c>
@@ -2807,18 +2895,18 @@
       </c>
     </row>
     <row r="33" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="16"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="16"/>
-      <c r="L33" s="16"/>
+      <c r="A33" s="21"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="21"/>
+      <c r="L33" s="21"/>
       <c r="M33" t="s">
         <v>90</v>
       </c>
@@ -2833,34 +2921,34 @@
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A34" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B34" s="16" t="s">
+      <c r="A34" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B34" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="C34" s="15"/>
-      <c r="D34" s="17" t="s">
+      <c r="C34" s="20"/>
+      <c r="D34" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="16" t="s">
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H34" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I34" s="16" t="s">
+      <c r="H34" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="I34" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="J34" s="18" t="s">
+      <c r="J34" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="K34" s="16" t="s">
+      <c r="K34" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="L34" s="16" t="s">
+      <c r="L34" s="21" t="s">
         <v>119</v>
       </c>
       <c r="M34" t="s">
@@ -2874,18 +2962,18 @@
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="18"/>
-      <c r="K35" s="16"/>
-      <c r="L35" s="16"/>
+      <c r="A35" s="21"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="23"/>
+      <c r="K35" s="21"/>
+      <c r="L35" s="21"/>
       <c r="M35" t="s">
         <v>85</v>
       </c>
@@ -2897,18 +2985,18 @@
       </c>
     </row>
     <row r="36" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="16"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
-      <c r="I36" s="16"/>
-      <c r="J36" s="18"/>
-      <c r="K36" s="16"/>
-      <c r="L36" s="16"/>
+      <c r="A36" s="21"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="23"/>
+      <c r="K36" s="21"/>
+      <c r="L36" s="21"/>
       <c r="M36" t="s">
         <v>90</v>
       </c>
@@ -2923,34 +3011,34 @@
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A37" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B37" s="16" t="s">
+      <c r="A37" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B37" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="C37" s="15"/>
-      <c r="D37" s="17" t="s">
+      <c r="C37" s="20"/>
+      <c r="D37" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="16" t="s">
+      <c r="E37" s="24"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H37" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I37" s="16" t="s">
+      <c r="H37" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="I37" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="J37" s="18" t="s">
+      <c r="J37" s="23" t="s">
         <v>156</v>
       </c>
-      <c r="K37" s="16" t="s">
+      <c r="K37" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="L37" s="16" t="s">
+      <c r="L37" s="21" t="s">
         <v>119</v>
       </c>
       <c r="M37" t="s">
@@ -2964,18 +3052,18 @@
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A38" s="16"/>
-      <c r="B38" s="16"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
-      <c r="I38" s="16"/>
-      <c r="J38" s="18"/>
-      <c r="K38" s="16"/>
-      <c r="L38" s="16"/>
+      <c r="A38" s="21"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="23"/>
+      <c r="K38" s="21"/>
+      <c r="L38" s="21"/>
       <c r="M38" t="s">
         <v>85</v>
       </c>
@@ -2987,18 +3075,18 @@
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A39" s="16"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
-      <c r="I39" s="16"/>
-      <c r="J39" s="18"/>
-      <c r="K39" s="16"/>
-      <c r="L39" s="16"/>
+      <c r="A39" s="21"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21"/>
+      <c r="J39" s="23"/>
+      <c r="K39" s="21"/>
+      <c r="L39" s="21"/>
       <c r="M39" t="s">
         <v>90</v>
       </c>
@@ -3050,34 +3138,34 @@
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A41" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B41" s="16" t="s">
+      <c r="A41" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B41" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="C41" s="15"/>
-      <c r="D41" s="17" t="s">
+      <c r="C41" s="20"/>
+      <c r="D41" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="16" t="s">
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H41" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I41" s="16" t="s">
+      <c r="H41" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="I41" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="J41" s="18" t="s">
+      <c r="J41" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="K41" s="16" t="s">
+      <c r="K41" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="L41" s="16" t="s">
+      <c r="L41" s="21" t="s">
         <v>119</v>
       </c>
       <c r="M41" t="s">
@@ -3091,18 +3179,18 @@
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A42" s="16"/>
-      <c r="B42" s="16"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="16"/>
-      <c r="H42" s="16"/>
-      <c r="I42" s="16"/>
-      <c r="J42" s="18"/>
-      <c r="K42" s="16"/>
-      <c r="L42" s="16"/>
+      <c r="A42" s="21"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="23"/>
+      <c r="K42" s="21"/>
+      <c r="L42" s="21"/>
       <c r="M42" t="s">
         <v>90</v>
       </c>
@@ -3114,18 +3202,18 @@
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A43" s="16"/>
-      <c r="B43" s="16"/>
-      <c r="C43" s="15"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="16"/>
-      <c r="H43" s="16"/>
-      <c r="I43" s="16"/>
-      <c r="J43" s="18"/>
-      <c r="K43" s="16"/>
-      <c r="L43" s="16"/>
+      <c r="A43" s="21"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="21"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="23"/>
+      <c r="K43" s="21"/>
+      <c r="L43" s="21"/>
       <c r="M43" t="s">
         <v>91</v>
       </c>
@@ -3138,18 +3226,18 @@
       <c r="V43"/>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A44" s="16"/>
-      <c r="B44" s="16"/>
-      <c r="C44" s="15"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="19"/>
-      <c r="G44" s="16"/>
-      <c r="H44" s="16"/>
-      <c r="I44" s="16"/>
-      <c r="J44" s="18"/>
-      <c r="K44" s="16"/>
-      <c r="L44" s="16"/>
+      <c r="A44" s="21"/>
+      <c r="B44" s="21"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="21"/>
+      <c r="J44" s="23"/>
+      <c r="K44" s="21"/>
+      <c r="L44" s="21"/>
       <c r="M44" t="s">
         <v>93</v>
       </c>
@@ -3162,18 +3250,18 @@
       <c r="V44"/>
     </row>
     <row r="45" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="16"/>
-      <c r="B45" s="16"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="16"/>
-      <c r="H45" s="16"/>
-      <c r="I45" s="16"/>
-      <c r="J45" s="18"/>
-      <c r="K45" s="16"/>
-      <c r="L45" s="16"/>
+      <c r="A45" s="21"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="23"/>
+      <c r="K45" s="21"/>
+      <c r="L45" s="21"/>
       <c r="M45" t="s">
         <v>81</v>
       </c>
@@ -3188,18 +3276,18 @@
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A46" s="16"/>
-      <c r="B46" s="16"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="19"/>
-      <c r="G46" s="16"/>
-      <c r="H46" s="16"/>
-      <c r="I46" s="16"/>
-      <c r="J46" s="18"/>
-      <c r="K46" s="16"/>
-      <c r="L46" s="16"/>
+      <c r="A46" s="21"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="23"/>
+      <c r="K46" s="21"/>
+      <c r="L46" s="21"/>
       <c r="M46" t="s">
         <v>126</v>
       </c>
@@ -3211,18 +3299,18 @@
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A47" s="16"/>
-      <c r="B47" s="16"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="19"/>
-      <c r="G47" s="16"/>
-      <c r="H47" s="16"/>
-      <c r="I47" s="16"/>
-      <c r="J47" s="18"/>
-      <c r="K47" s="16"/>
-      <c r="L47" s="16"/>
+      <c r="A47" s="21"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="21"/>
+      <c r="J47" s="23"/>
+      <c r="K47" s="21"/>
+      <c r="L47" s="21"/>
       <c r="M47" t="s">
         <v>47</v>
       </c>
@@ -3606,32 +3694,32 @@
       </c>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A57" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B57" s="16" t="s">
+      <c r="A57" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B57" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="C57" s="15"/>
-      <c r="D57" s="18"/>
-      <c r="E57" s="24"/>
-      <c r="F57" s="24"/>
-      <c r="G57" s="16" t="s">
+      <c r="C57" s="20"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="26"/>
+      <c r="F57" s="26"/>
+      <c r="G57" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H57" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I57" s="16" t="s">
+      <c r="H57" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="I57" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="J57" s="18" t="s">
+      <c r="J57" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="K57" s="16" t="s">
+      <c r="K57" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="L57" s="23" t="s">
+      <c r="L57" s="25" t="s">
         <v>120</v>
       </c>
       <c r="M57" t="s">
@@ -3645,18 +3733,18 @@
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A58" s="16"/>
-      <c r="B58" s="16"/>
-      <c r="C58" s="15"/>
-      <c r="D58" s="18"/>
-      <c r="E58" s="24"/>
-      <c r="F58" s="24"/>
-      <c r="G58" s="16"/>
-      <c r="H58" s="16"/>
-      <c r="I58" s="16"/>
-      <c r="J58" s="18"/>
-      <c r="K58" s="16"/>
-      <c r="L58" s="23"/>
+      <c r="A58" s="21"/>
+      <c r="B58" s="21"/>
+      <c r="C58" s="20"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="26"/>
+      <c r="F58" s="26"/>
+      <c r="G58" s="21"/>
+      <c r="H58" s="21"/>
+      <c r="I58" s="21"/>
+      <c r="J58" s="23"/>
+      <c r="K58" s="21"/>
+      <c r="L58" s="25"/>
       <c r="M58" t="s">
         <v>132</v>
       </c>
@@ -3668,18 +3756,18 @@
       </c>
     </row>
     <row r="59" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A59" s="16"/>
-      <c r="B59" s="16"/>
-      <c r="C59" s="15"/>
-      <c r="D59" s="18"/>
-      <c r="E59" s="24"/>
-      <c r="F59" s="24"/>
-      <c r="G59" s="16"/>
-      <c r="H59" s="16"/>
-      <c r="I59" s="16"/>
-      <c r="J59" s="18"/>
-      <c r="K59" s="16"/>
-      <c r="L59" s="23"/>
+      <c r="A59" s="21"/>
+      <c r="B59" s="21"/>
+      <c r="C59" s="20"/>
+      <c r="D59" s="23"/>
+      <c r="E59" s="26"/>
+      <c r="F59" s="26"/>
+      <c r="G59" s="21"/>
+      <c r="H59" s="21"/>
+      <c r="I59" s="21"/>
+      <c r="J59" s="23"/>
+      <c r="K59" s="21"/>
+      <c r="L59" s="25"/>
       <c r="M59" t="s">
         <v>133</v>
       </c>
@@ -3767,34 +3855,34 @@
       </c>
     </row>
     <row r="62" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="B62" s="22" t="s">
+      <c r="A62" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B62" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="C62" s="14"/>
-      <c r="D62" s="20" t="s">
+      <c r="C62" s="19"/>
+      <c r="D62" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="E62" s="21"/>
-      <c r="F62" s="21"/>
-      <c r="G62" s="22" t="s">
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="H62" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="I62" s="16" t="s">
+      <c r="H62" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I62" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="J62" s="18" t="s">
+      <c r="J62" s="23" t="s">
         <v>179</v>
       </c>
-      <c r="K62" s="16" t="s">
+      <c r="K62" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="L62" s="16" t="s">
+      <c r="L62" s="21" t="s">
         <v>119</v>
       </c>
       <c r="M62" t="s">
@@ -3811,18 +3899,18 @@
       </c>
     </row>
     <row r="63" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A63" s="22"/>
-      <c r="B63" s="22"/>
-      <c r="C63" s="14"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="21"/>
-      <c r="F63" s="21"/>
-      <c r="G63" s="22"/>
-      <c r="H63" s="22"/>
-      <c r="I63" s="16"/>
-      <c r="J63" s="18"/>
-      <c r="K63" s="16"/>
-      <c r="L63" s="16"/>
+      <c r="A63" s="16"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="19"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="16"/>
+      <c r="H63" s="16"/>
+      <c r="I63" s="21"/>
+      <c r="J63" s="23"/>
+      <c r="K63" s="21"/>
+      <c r="L63" s="21"/>
       <c r="M63" t="s">
         <v>182</v>
       </c>
@@ -3837,34 +3925,34 @@
       </c>
     </row>
     <row r="64" spans="1:22" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B64" s="16" t="s">
+      <c r="A64" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B64" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="C64" s="15"/>
-      <c r="D64" s="20" t="s">
+      <c r="C64" s="20"/>
+      <c r="D64" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="E64" s="21"/>
-      <c r="F64" s="21"/>
-      <c r="G64" s="16" t="s">
+      <c r="E64" s="14"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H64" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I64" s="16" t="s">
+      <c r="H64" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="I64" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="J64" s="16" t="s">
+      <c r="J64" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="K64" s="16" t="s">
+      <c r="K64" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="L64" s="16" t="s">
+      <c r="L64" s="21" t="s">
         <v>120</v>
       </c>
       <c r="M64" t="s">
@@ -3881,18 +3969,18 @@
       </c>
     </row>
     <row r="65" spans="1:22" ht="90" x14ac:dyDescent="0.25">
-      <c r="A65" s="16"/>
-      <c r="B65" s="16"/>
-      <c r="C65" s="15"/>
-      <c r="D65" s="20"/>
-      <c r="E65" s="21"/>
-      <c r="F65" s="21"/>
-      <c r="G65" s="16"/>
-      <c r="H65" s="16"/>
-      <c r="I65" s="16"/>
-      <c r="J65" s="16"/>
-      <c r="K65" s="16"/>
-      <c r="L65" s="16"/>
+      <c r="A65" s="21"/>
+      <c r="B65" s="21"/>
+      <c r="C65" s="20"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="21"/>
+      <c r="H65" s="21"/>
+      <c r="I65" s="21"/>
+      <c r="J65" s="21"/>
+      <c r="K65" s="21"/>
+      <c r="L65" s="21"/>
       <c r="M65" t="s">
         <v>187</v>
       </c>
@@ -3907,18 +3995,18 @@
       </c>
     </row>
     <row r="66" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A66" s="16"/>
-      <c r="B66" s="16"/>
-      <c r="C66" s="15"/>
-      <c r="D66" s="20"/>
-      <c r="E66" s="21"/>
-      <c r="F66" s="21"/>
-      <c r="G66" s="16"/>
-      <c r="H66" s="16"/>
-      <c r="I66" s="16"/>
-      <c r="J66" s="16"/>
-      <c r="K66" s="16"/>
-      <c r="L66" s="16"/>
+      <c r="A66" s="21"/>
+      <c r="B66" s="21"/>
+      <c r="C66" s="20"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14"/>
+      <c r="G66" s="21"/>
+      <c r="H66" s="21"/>
+      <c r="I66" s="21"/>
+      <c r="J66" s="21"/>
+      <c r="K66" s="21"/>
+      <c r="L66" s="21"/>
       <c r="M66" t="s">
         <v>190</v>
       </c>
@@ -3930,18 +4018,18 @@
       </c>
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A67" s="16"/>
-      <c r="B67" s="16"/>
-      <c r="C67" s="15"/>
-      <c r="D67" s="20"/>
-      <c r="E67" s="21"/>
-      <c r="F67" s="21"/>
-      <c r="G67" s="16"/>
-      <c r="H67" s="16"/>
-      <c r="I67" s="16"/>
-      <c r="J67" s="16"/>
-      <c r="K67" s="16"/>
-      <c r="L67" s="16"/>
+      <c r="A67" s="21"/>
+      <c r="B67" s="21"/>
+      <c r="C67" s="20"/>
+      <c r="D67" s="15"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="14"/>
+      <c r="G67" s="21"/>
+      <c r="H67" s="21"/>
+      <c r="I67" s="21"/>
+      <c r="J67" s="21"/>
+      <c r="K67" s="21"/>
+      <c r="L67" s="21"/>
       <c r="M67" t="s">
         <v>191</v>
       </c>
@@ -3953,34 +4041,34 @@
       </c>
     </row>
     <row r="68" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B68" s="16" t="s">
+      <c r="A68" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B68" s="21" t="s">
         <v>197</v>
       </c>
-      <c r="C68" s="15"/>
-      <c r="D68" s="20" t="s">
+      <c r="C68" s="20"/>
+      <c r="D68" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="E68" s="21"/>
-      <c r="F68" s="21"/>
-      <c r="G68" s="16" t="s">
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
+      <c r="G68" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H68" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I68" s="16" t="s">
+      <c r="H68" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="I68" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="J68" s="16" t="s">
+      <c r="J68" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="K68" s="16" t="s">
+      <c r="K68" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="L68" s="16" t="s">
+      <c r="L68" s="21" t="s">
         <v>120</v>
       </c>
       <c r="M68" t="s">
@@ -3997,18 +4085,18 @@
       </c>
     </row>
     <row r="69" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A69" s="16"/>
-      <c r="B69" s="16"/>
-      <c r="C69" s="15"/>
-      <c r="D69" s="20"/>
-      <c r="E69" s="21"/>
-      <c r="F69" s="21"/>
-      <c r="G69" s="16"/>
-      <c r="H69" s="16"/>
-      <c r="I69" s="16"/>
-      <c r="J69" s="16"/>
-      <c r="K69" s="16"/>
-      <c r="L69" s="16"/>
+      <c r="A69" s="21"/>
+      <c r="B69" s="21"/>
+      <c r="C69" s="20"/>
+      <c r="D69" s="15"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="21"/>
+      <c r="H69" s="21"/>
+      <c r="I69" s="21"/>
+      <c r="J69" s="21"/>
+      <c r="K69" s="21"/>
+      <c r="L69" s="21"/>
       <c r="M69" t="s">
         <v>187</v>
       </c>
@@ -4020,18 +4108,18 @@
       </c>
     </row>
     <row r="70" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A70" s="16"/>
-      <c r="B70" s="16"/>
-      <c r="C70" s="15"/>
-      <c r="D70" s="20"/>
-      <c r="E70" s="21"/>
-      <c r="F70" s="21"/>
-      <c r="G70" s="16"/>
-      <c r="H70" s="16"/>
-      <c r="I70" s="16"/>
-      <c r="J70" s="16"/>
-      <c r="K70" s="16"/>
-      <c r="L70" s="16"/>
+      <c r="A70" s="21"/>
+      <c r="B70" s="21"/>
+      <c r="C70" s="20"/>
+      <c r="D70" s="15"/>
+      <c r="E70" s="14"/>
+      <c r="F70" s="14"/>
+      <c r="G70" s="21"/>
+      <c r="H70" s="21"/>
+      <c r="I70" s="21"/>
+      <c r="J70" s="21"/>
+      <c r="K70" s="21"/>
+      <c r="L70" s="21"/>
       <c r="M70" t="s">
         <v>190</v>
       </c>
@@ -4043,18 +4131,18 @@
       </c>
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A71" s="16"/>
-      <c r="B71" s="16"/>
-      <c r="C71" s="15"/>
-      <c r="D71" s="20"/>
-      <c r="E71" s="21"/>
-      <c r="F71" s="21"/>
-      <c r="G71" s="16"/>
-      <c r="H71" s="16"/>
-      <c r="I71" s="16"/>
-      <c r="J71" s="16"/>
-      <c r="K71" s="16"/>
-      <c r="L71" s="16"/>
+      <c r="A71" s="21"/>
+      <c r="B71" s="21"/>
+      <c r="C71" s="20"/>
+      <c r="D71" s="15"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="14"/>
+      <c r="G71" s="21"/>
+      <c r="H71" s="21"/>
+      <c r="I71" s="21"/>
+      <c r="J71" s="21"/>
+      <c r="K71" s="21"/>
+      <c r="L71" s="21"/>
       <c r="M71" t="s">
         <v>191</v>
       </c>
@@ -4066,34 +4154,34 @@
       </c>
     </row>
     <row r="72" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A72" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B72" s="16" t="s">
+      <c r="A72" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B72" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="C72" s="15"/>
-      <c r="D72" s="20" t="s">
+      <c r="C72" s="20"/>
+      <c r="D72" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="E72" s="21"/>
-      <c r="F72" s="21"/>
-      <c r="G72" s="16" t="s">
+      <c r="E72" s="14"/>
+      <c r="F72" s="14"/>
+      <c r="G72" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H72" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I72" s="16" t="s">
+      <c r="H72" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="I72" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="J72" s="16" t="s">
+      <c r="J72" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="K72" s="16" t="s">
+      <c r="K72" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="L72" s="16" t="s">
+      <c r="L72" s="21" t="s">
         <v>120</v>
       </c>
       <c r="M72" t="s">
@@ -4107,18 +4195,18 @@
       </c>
     </row>
     <row r="73" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A73" s="16"/>
-      <c r="B73" s="16"/>
-      <c r="C73" s="15"/>
-      <c r="D73" s="20"/>
-      <c r="E73" s="21"/>
-      <c r="F73" s="21"/>
-      <c r="G73" s="16"/>
-      <c r="H73" s="16"/>
-      <c r="I73" s="16"/>
-      <c r="J73" s="16"/>
-      <c r="K73" s="16"/>
-      <c r="L73" s="16"/>
+      <c r="A73" s="21"/>
+      <c r="B73" s="21"/>
+      <c r="C73" s="20"/>
+      <c r="D73" s="15"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="14"/>
+      <c r="G73" s="21"/>
+      <c r="H73" s="21"/>
+      <c r="I73" s="21"/>
+      <c r="J73" s="21"/>
+      <c r="K73" s="21"/>
+      <c r="L73" s="21"/>
       <c r="M73" t="s">
         <v>187</v>
       </c>
@@ -4130,18 +4218,18 @@
       </c>
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A74" s="16"/>
-      <c r="B74" s="16"/>
-      <c r="C74" s="15"/>
-      <c r="D74" s="20"/>
-      <c r="E74" s="21"/>
-      <c r="F74" s="21"/>
-      <c r="G74" s="16"/>
-      <c r="H74" s="16"/>
-      <c r="I74" s="16"/>
-      <c r="J74" s="16"/>
-      <c r="K74" s="16"/>
-      <c r="L74" s="16"/>
+      <c r="A74" s="21"/>
+      <c r="B74" s="21"/>
+      <c r="C74" s="20"/>
+      <c r="D74" s="15"/>
+      <c r="E74" s="14"/>
+      <c r="F74" s="14"/>
+      <c r="G74" s="21"/>
+      <c r="H74" s="21"/>
+      <c r="I74" s="21"/>
+      <c r="J74" s="21"/>
+      <c r="K74" s="21"/>
+      <c r="L74" s="21"/>
       <c r="M74" t="s">
         <v>190</v>
       </c>
@@ -4153,18 +4241,18 @@
       </c>
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A75" s="16"/>
-      <c r="B75" s="16"/>
-      <c r="C75" s="15"/>
-      <c r="D75" s="20"/>
-      <c r="E75" s="21"/>
-      <c r="F75" s="21"/>
-      <c r="G75" s="16"/>
-      <c r="H75" s="16"/>
-      <c r="I75" s="16"/>
-      <c r="J75" s="16"/>
-      <c r="K75" s="16"/>
-      <c r="L75" s="16"/>
+      <c r="A75" s="21"/>
+      <c r="B75" s="21"/>
+      <c r="C75" s="20"/>
+      <c r="D75" s="15"/>
+      <c r="E75" s="14"/>
+      <c r="F75" s="14"/>
+      <c r="G75" s="21"/>
+      <c r="H75" s="21"/>
+      <c r="I75" s="21"/>
+      <c r="J75" s="21"/>
+      <c r="K75" s="21"/>
+      <c r="L75" s="21"/>
       <c r="M75" t="s">
         <v>191</v>
       </c>
@@ -4252,34 +4340,34 @@
       </c>
     </row>
     <row r="78" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B78" s="16" t="s">
+      <c r="A78" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B78" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="C78" s="15"/>
-      <c r="D78" s="20" t="s">
+      <c r="C78" s="20"/>
+      <c r="D78" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="E78" s="21"/>
-      <c r="F78" s="21"/>
-      <c r="G78" s="16" t="s">
+      <c r="E78" s="14"/>
+      <c r="F78" s="14"/>
+      <c r="G78" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H78" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I78" s="16" t="s">
+      <c r="H78" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="I78" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="J78" s="16" t="s">
+      <c r="J78" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="K78" s="16" t="s">
+      <c r="K78" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="L78" s="16" t="s">
+      <c r="L78" s="21" t="s">
         <v>120</v>
       </c>
       <c r="M78" t="s">
@@ -4296,18 +4384,18 @@
       </c>
     </row>
     <row r="79" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A79" s="16"/>
-      <c r="B79" s="16"/>
-      <c r="C79" s="15"/>
-      <c r="D79" s="20"/>
-      <c r="E79" s="21"/>
-      <c r="F79" s="21"/>
-      <c r="G79" s="16"/>
-      <c r="H79" s="16"/>
-      <c r="I79" s="16"/>
-      <c r="J79" s="16"/>
-      <c r="K79" s="16"/>
-      <c r="L79" s="16"/>
+      <c r="A79" s="21"/>
+      <c r="B79" s="21"/>
+      <c r="C79" s="20"/>
+      <c r="D79" s="15"/>
+      <c r="E79" s="14"/>
+      <c r="F79" s="14"/>
+      <c r="G79" s="21"/>
+      <c r="H79" s="21"/>
+      <c r="I79" s="21"/>
+      <c r="J79" s="21"/>
+      <c r="K79" s="21"/>
+      <c r="L79" s="21"/>
       <c r="M79" t="s">
         <v>212</v>
       </c>
@@ -4322,18 +4410,18 @@
       </c>
     </row>
     <row r="80" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="16"/>
-      <c r="B80" s="16"/>
-      <c r="C80" s="15"/>
-      <c r="D80" s="20"/>
-      <c r="E80" s="21"/>
-      <c r="F80" s="21"/>
-      <c r="G80" s="16"/>
-      <c r="H80" s="16"/>
-      <c r="I80" s="16"/>
-      <c r="J80" s="16"/>
-      <c r="K80" s="16"/>
-      <c r="L80" s="16"/>
+      <c r="A80" s="21"/>
+      <c r="B80" s="21"/>
+      <c r="C80" s="20"/>
+      <c r="D80" s="15"/>
+      <c r="E80" s="14"/>
+      <c r="F80" s="14"/>
+      <c r="G80" s="21"/>
+      <c r="H80" s="21"/>
+      <c r="I80" s="21"/>
+      <c r="J80" s="21"/>
+      <c r="K80" s="21"/>
+      <c r="L80" s="21"/>
       <c r="M80" t="s">
         <v>214</v>
       </c>
@@ -4348,18 +4436,18 @@
       </c>
     </row>
     <row r="81" spans="1:22" ht="60" x14ac:dyDescent="0.25">
-      <c r="A81" s="16"/>
-      <c r="B81" s="16"/>
-      <c r="C81" s="15"/>
-      <c r="D81" s="20"/>
-      <c r="E81" s="21"/>
-      <c r="F81" s="21"/>
-      <c r="G81" s="16"/>
-      <c r="H81" s="16"/>
-      <c r="I81" s="16"/>
-      <c r="J81" s="16"/>
-      <c r="K81" s="16"/>
-      <c r="L81" s="16"/>
+      <c r="A81" s="21"/>
+      <c r="B81" s="21"/>
+      <c r="C81" s="20"/>
+      <c r="D81" s="15"/>
+      <c r="E81" s="14"/>
+      <c r="F81" s="14"/>
+      <c r="G81" s="21"/>
+      <c r="H81" s="21"/>
+      <c r="I81" s="21"/>
+      <c r="J81" s="21"/>
+      <c r="K81" s="21"/>
+      <c r="L81" s="21"/>
       <c r="M81" t="s">
         <v>132</v>
       </c>
@@ -4374,18 +4462,18 @@
       </c>
     </row>
     <row r="82" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A82" s="16"/>
-      <c r="B82" s="16"/>
-      <c r="C82" s="15"/>
-      <c r="D82" s="20"/>
-      <c r="E82" s="21"/>
-      <c r="F82" s="21"/>
-      <c r="G82" s="16"/>
-      <c r="H82" s="16"/>
-      <c r="I82" s="16"/>
-      <c r="J82" s="16"/>
-      <c r="K82" s="16"/>
-      <c r="L82" s="16"/>
+      <c r="A82" s="21"/>
+      <c r="B82" s="21"/>
+      <c r="C82" s="20"/>
+      <c r="D82" s="15"/>
+      <c r="E82" s="14"/>
+      <c r="F82" s="14"/>
+      <c r="G82" s="21"/>
+      <c r="H82" s="21"/>
+      <c r="I82" s="21"/>
+      <c r="J82" s="21"/>
+      <c r="K82" s="21"/>
+      <c r="L82" s="21"/>
       <c r="M82" t="s">
         <v>133</v>
       </c>
@@ -4397,32 +4485,32 @@
       </c>
     </row>
     <row r="83" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="B83" s="16" t="s">
+      <c r="A83" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="B83" s="21" t="s">
         <v>217</v>
       </c>
-      <c r="C83" s="15"/>
-      <c r="D83" s="20" t="s">
+      <c r="C83" s="20"/>
+      <c r="D83" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="E83" s="21"/>
-      <c r="F83" s="21"/>
-      <c r="G83" s="16" t="s">
+      <c r="E83" s="14"/>
+      <c r="F83" s="14"/>
+      <c r="G83" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H83" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I83" s="16"/>
-      <c r="J83" s="16" t="s">
+      <c r="H83" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="I83" s="21"/>
+      <c r="J83" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="K83" s="16" t="s">
+      <c r="K83" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="L83" s="16" t="s">
+      <c r="L83" s="21" t="s">
         <v>120</v>
       </c>
       <c r="M83" t="s">
@@ -4436,18 +4524,18 @@
       </c>
     </row>
     <row r="84" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A84" s="15"/>
-      <c r="B84" s="16"/>
-      <c r="C84" s="15"/>
-      <c r="D84" s="20"/>
-      <c r="E84" s="21"/>
-      <c r="F84" s="21"/>
-      <c r="G84" s="16"/>
-      <c r="H84" s="16"/>
-      <c r="I84" s="16"/>
-      <c r="J84" s="16"/>
-      <c r="K84" s="16"/>
-      <c r="L84" s="16"/>
+      <c r="A84" s="20"/>
+      <c r="B84" s="21"/>
+      <c r="C84" s="20"/>
+      <c r="D84" s="15"/>
+      <c r="E84" s="14"/>
+      <c r="F84" s="14"/>
+      <c r="G84" s="21"/>
+      <c r="H84" s="21"/>
+      <c r="I84" s="21"/>
+      <c r="J84" s="21"/>
+      <c r="K84" s="21"/>
+      <c r="L84" s="21"/>
       <c r="M84" t="s">
         <v>212</v>
       </c>
@@ -4459,18 +4547,18 @@
       </c>
     </row>
     <row r="85" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A85" s="15"/>
-      <c r="B85" s="16"/>
-      <c r="C85" s="15"/>
-      <c r="D85" s="20"/>
-      <c r="E85" s="21"/>
-      <c r="F85" s="21"/>
-      <c r="G85" s="16"/>
-      <c r="H85" s="16"/>
-      <c r="I85" s="16"/>
-      <c r="J85" s="16"/>
-      <c r="K85" s="16"/>
-      <c r="L85" s="16"/>
+      <c r="A85" s="20"/>
+      <c r="B85" s="21"/>
+      <c r="C85" s="20"/>
+      <c r="D85" s="15"/>
+      <c r="E85" s="14"/>
+      <c r="F85" s="14"/>
+      <c r="G85" s="21"/>
+      <c r="H85" s="21"/>
+      <c r="I85" s="21"/>
+      <c r="J85" s="21"/>
+      <c r="K85" s="21"/>
+      <c r="L85" s="21"/>
       <c r="M85" t="s">
         <v>214</v>
       </c>
@@ -4482,18 +4570,18 @@
       </c>
     </row>
     <row r="86" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A86" s="15"/>
-      <c r="B86" s="16"/>
-      <c r="C86" s="15"/>
-      <c r="D86" s="20"/>
-      <c r="E86" s="21"/>
-      <c r="F86" s="21"/>
-      <c r="G86" s="16"/>
-      <c r="H86" s="16"/>
-      <c r="I86" s="16"/>
-      <c r="J86" s="16"/>
-      <c r="K86" s="16"/>
-      <c r="L86" s="16"/>
+      <c r="A86" s="20"/>
+      <c r="B86" s="21"/>
+      <c r="C86" s="20"/>
+      <c r="D86" s="15"/>
+      <c r="E86" s="14"/>
+      <c r="F86" s="14"/>
+      <c r="G86" s="21"/>
+      <c r="H86" s="21"/>
+      <c r="I86" s="21"/>
+      <c r="J86" s="21"/>
+      <c r="K86" s="21"/>
+      <c r="L86" s="21"/>
       <c r="M86" t="s">
         <v>132</v>
       </c>
@@ -4505,18 +4593,18 @@
       </c>
     </row>
     <row r="87" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A87" s="15"/>
-      <c r="B87" s="16"/>
-      <c r="C87" s="15"/>
-      <c r="D87" s="20"/>
-      <c r="E87" s="21"/>
-      <c r="F87" s="21"/>
-      <c r="G87" s="16"/>
-      <c r="H87" s="16"/>
-      <c r="I87" s="16"/>
-      <c r="J87" s="16"/>
-      <c r="K87" s="16"/>
-      <c r="L87" s="16"/>
+      <c r="A87" s="20"/>
+      <c r="B87" s="21"/>
+      <c r="C87" s="20"/>
+      <c r="D87" s="15"/>
+      <c r="E87" s="14"/>
+      <c r="F87" s="14"/>
+      <c r="G87" s="21"/>
+      <c r="H87" s="21"/>
+      <c r="I87" s="21"/>
+      <c r="J87" s="21"/>
+      <c r="K87" s="21"/>
+      <c r="L87" s="21"/>
       <c r="M87" t="s">
         <v>133</v>
       </c>
@@ -4531,34 +4619,34 @@
       </c>
     </row>
     <row r="88" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B88" s="16" t="s">
+      <c r="A88" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B88" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="C88" s="15"/>
-      <c r="D88" s="20" t="s">
+      <c r="C88" s="20"/>
+      <c r="D88" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="E88" s="21"/>
-      <c r="F88" s="21"/>
-      <c r="G88" s="16" t="s">
+      <c r="E88" s="14"/>
+      <c r="F88" s="14"/>
+      <c r="G88" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H88" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I88" s="16" t="s">
+      <c r="H88" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="I88" s="21" t="s">
         <v>224</v>
       </c>
-      <c r="J88" s="16" t="s">
+      <c r="J88" s="21" t="s">
         <v>226</v>
       </c>
-      <c r="K88" s="16" t="s">
+      <c r="K88" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="L88" s="16" t="s">
+      <c r="L88" s="21" t="s">
         <v>120</v>
       </c>
       <c r="M88" t="s">
@@ -4575,18 +4663,18 @@
       </c>
     </row>
     <row r="89" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="16"/>
-      <c r="B89" s="16"/>
-      <c r="C89" s="15"/>
-      <c r="D89" s="20"/>
-      <c r="E89" s="21"/>
-      <c r="F89" s="21"/>
-      <c r="G89" s="16"/>
-      <c r="H89" s="16"/>
-      <c r="I89" s="16"/>
-      <c r="J89" s="16"/>
-      <c r="K89" s="16"/>
-      <c r="L89" s="16"/>
+      <c r="A89" s="21"/>
+      <c r="B89" s="21"/>
+      <c r="C89" s="20"/>
+      <c r="D89" s="15"/>
+      <c r="E89" s="14"/>
+      <c r="F89" s="14"/>
+      <c r="G89" s="21"/>
+      <c r="H89" s="21"/>
+      <c r="I89" s="21"/>
+      <c r="J89" s="21"/>
+      <c r="K89" s="21"/>
+      <c r="L89" s="21"/>
       <c r="M89" t="s">
         <v>47</v>
       </c>
@@ -4601,18 +4689,18 @@
       </c>
     </row>
     <row r="90" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="16"/>
-      <c r="B90" s="16"/>
-      <c r="C90" s="15"/>
-      <c r="D90" s="20"/>
-      <c r="E90" s="21"/>
-      <c r="F90" s="21"/>
-      <c r="G90" s="16"/>
-      <c r="H90" s="16"/>
-      <c r="I90" s="16"/>
-      <c r="J90" s="16"/>
-      <c r="K90" s="16"/>
-      <c r="L90" s="16"/>
+      <c r="A90" s="21"/>
+      <c r="B90" s="21"/>
+      <c r="C90" s="20"/>
+      <c r="D90" s="15"/>
+      <c r="E90" s="14"/>
+      <c r="F90" s="14"/>
+      <c r="G90" s="21"/>
+      <c r="H90" s="21"/>
+      <c r="I90" s="21"/>
+      <c r="J90" s="21"/>
+      <c r="K90" s="21"/>
+      <c r="L90" s="21"/>
       <c r="M90" t="s">
         <v>180</v>
       </c>
@@ -4627,18 +4715,18 @@
       </c>
     </row>
     <row r="91" spans="1:22" ht="75" x14ac:dyDescent="0.25">
-      <c r="A91" s="16"/>
-      <c r="B91" s="16"/>
-      <c r="C91" s="15"/>
-      <c r="D91" s="20"/>
-      <c r="E91" s="21"/>
-      <c r="F91" s="21"/>
-      <c r="G91" s="16"/>
-      <c r="H91" s="16"/>
-      <c r="I91" s="16"/>
-      <c r="J91" s="16"/>
-      <c r="K91" s="16"/>
-      <c r="L91" s="16"/>
+      <c r="A91" s="21"/>
+      <c r="B91" s="21"/>
+      <c r="C91" s="20"/>
+      <c r="D91" s="15"/>
+      <c r="E91" s="14"/>
+      <c r="F91" s="14"/>
+      <c r="G91" s="21"/>
+      <c r="H91" s="21"/>
+      <c r="I91" s="21"/>
+      <c r="J91" s="21"/>
+      <c r="K91" s="21"/>
+      <c r="L91" s="21"/>
       <c r="M91" t="s">
         <v>214</v>
       </c>
@@ -4653,18 +4741,18 @@
       </c>
     </row>
     <row r="92" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A92" s="16"/>
-      <c r="B92" s="16"/>
-      <c r="C92" s="15"/>
-      <c r="D92" s="20"/>
-      <c r="E92" s="21"/>
-      <c r="F92" s="21"/>
-      <c r="G92" s="16"/>
-      <c r="H92" s="16"/>
-      <c r="I92" s="16"/>
-      <c r="J92" s="16"/>
-      <c r="K92" s="16"/>
-      <c r="L92" s="16"/>
+      <c r="A92" s="21"/>
+      <c r="B92" s="21"/>
+      <c r="C92" s="20"/>
+      <c r="D92" s="15"/>
+      <c r="E92" s="14"/>
+      <c r="F92" s="14"/>
+      <c r="G92" s="21"/>
+      <c r="H92" s="21"/>
+      <c r="I92" s="21"/>
+      <c r="J92" s="21"/>
+      <c r="K92" s="21"/>
+      <c r="L92" s="21"/>
       <c r="M92" t="s">
         <v>132</v>
       </c>
@@ -4676,18 +4764,18 @@
       </c>
     </row>
     <row r="93" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A93" s="16"/>
-      <c r="B93" s="16"/>
-      <c r="C93" s="15"/>
-      <c r="D93" s="20"/>
-      <c r="E93" s="21"/>
-      <c r="F93" s="21"/>
-      <c r="G93" s="16"/>
-      <c r="H93" s="16"/>
-      <c r="I93" s="16"/>
-      <c r="J93" s="16"/>
-      <c r="K93" s="16"/>
-      <c r="L93" s="16"/>
+      <c r="A93" s="21"/>
+      <c r="B93" s="21"/>
+      <c r="C93" s="20"/>
+      <c r="D93" s="15"/>
+      <c r="E93" s="14"/>
+      <c r="F93" s="14"/>
+      <c r="G93" s="21"/>
+      <c r="H93" s="21"/>
+      <c r="I93" s="21"/>
+      <c r="J93" s="21"/>
+      <c r="K93" s="21"/>
+      <c r="L93" s="21"/>
       <c r="M93" t="s">
         <v>133</v>
       </c>
@@ -4699,34 +4787,34 @@
       </c>
     </row>
     <row r="94" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A94" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B94" s="16" t="s">
+      <c r="A94" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B94" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="C94" s="15"/>
-      <c r="D94" s="20" t="s">
+      <c r="C94" s="20"/>
+      <c r="D94" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="E94" s="21"/>
-      <c r="F94" s="21"/>
-      <c r="G94" s="16" t="s">
+      <c r="E94" s="14"/>
+      <c r="F94" s="14"/>
+      <c r="G94" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H94" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I94" s="16" t="s">
+      <c r="H94" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="I94" s="21" t="s">
         <v>232</v>
       </c>
-      <c r="J94" s="16" t="s">
+      <c r="J94" s="21" t="s">
         <v>234</v>
       </c>
-      <c r="K94" s="16" t="s">
+      <c r="K94" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="L94" s="16" t="s">
+      <c r="L94" s="21" t="s">
         <v>120</v>
       </c>
       <c r="M94" t="s">
@@ -4740,18 +4828,18 @@
       </c>
     </row>
     <row r="95" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A95" s="16"/>
-      <c r="B95" s="16"/>
-      <c r="C95" s="15"/>
-      <c r="D95" s="20"/>
-      <c r="E95" s="21"/>
-      <c r="F95" s="21"/>
-      <c r="G95" s="16"/>
-      <c r="H95" s="16"/>
-      <c r="I95" s="16"/>
-      <c r="J95" s="16"/>
-      <c r="K95" s="16"/>
-      <c r="L95" s="16"/>
+      <c r="A95" s="21"/>
+      <c r="B95" s="21"/>
+      <c r="C95" s="20"/>
+      <c r="D95" s="15"/>
+      <c r="E95" s="14"/>
+      <c r="F95" s="14"/>
+      <c r="G95" s="21"/>
+      <c r="H95" s="21"/>
+      <c r="I95" s="21"/>
+      <c r="J95" s="21"/>
+      <c r="K95" s="21"/>
+      <c r="L95" s="21"/>
       <c r="M95" t="s">
         <v>212</v>
       </c>
@@ -4766,18 +4854,18 @@
       </c>
     </row>
     <row r="96" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A96" s="16"/>
-      <c r="B96" s="16"/>
-      <c r="C96" s="15"/>
-      <c r="D96" s="20"/>
-      <c r="E96" s="21"/>
-      <c r="F96" s="21"/>
-      <c r="G96" s="16"/>
-      <c r="H96" s="16"/>
-      <c r="I96" s="16"/>
-      <c r="J96" s="16"/>
-      <c r="K96" s="16"/>
-      <c r="L96" s="16"/>
+      <c r="A96" s="21"/>
+      <c r="B96" s="21"/>
+      <c r="C96" s="20"/>
+      <c r="D96" s="15"/>
+      <c r="E96" s="14"/>
+      <c r="F96" s="14"/>
+      <c r="G96" s="21"/>
+      <c r="H96" s="21"/>
+      <c r="I96" s="21"/>
+      <c r="J96" s="21"/>
+      <c r="K96" s="21"/>
+      <c r="L96" s="21"/>
       <c r="M96" t="s">
         <v>212</v>
       </c>
@@ -4792,34 +4880,34 @@
       </c>
     </row>
     <row r="97" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A97" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B97" s="16" t="s">
+      <c r="A97" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B97" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="C97" s="15"/>
-      <c r="D97" s="20" t="s">
+      <c r="C97" s="20"/>
+      <c r="D97" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="E97" s="21"/>
-      <c r="F97" s="21"/>
-      <c r="G97" s="16" t="s">
+      <c r="E97" s="14"/>
+      <c r="F97" s="14"/>
+      <c r="G97" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H97" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I97" s="16" t="s">
+      <c r="H97" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="I97" s="21" t="s">
         <v>240</v>
       </c>
-      <c r="J97" s="16" t="s">
+      <c r="J97" s="21" t="s">
         <v>241</v>
       </c>
-      <c r="K97" s="16" t="s">
+      <c r="K97" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="L97" s="16" t="s">
+      <c r="L97" s="21" t="s">
         <v>120</v>
       </c>
       <c r="M97" t="s">
@@ -4833,18 +4921,18 @@
       </c>
     </row>
     <row r="98" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A98" s="16"/>
-      <c r="B98" s="16"/>
-      <c r="C98" s="15"/>
-      <c r="D98" s="20"/>
-      <c r="E98" s="21"/>
-      <c r="F98" s="21"/>
-      <c r="G98" s="16"/>
-      <c r="H98" s="16"/>
-      <c r="I98" s="16"/>
-      <c r="J98" s="16"/>
-      <c r="K98" s="16"/>
-      <c r="L98" s="16"/>
+      <c r="A98" s="21"/>
+      <c r="B98" s="21"/>
+      <c r="C98" s="20"/>
+      <c r="D98" s="15"/>
+      <c r="E98" s="14"/>
+      <c r="F98" s="14"/>
+      <c r="G98" s="21"/>
+      <c r="H98" s="21"/>
+      <c r="I98" s="21"/>
+      <c r="J98" s="21"/>
+      <c r="K98" s="21"/>
+      <c r="L98" s="21"/>
       <c r="M98" t="s">
         <v>212</v>
       </c>
@@ -4958,34 +5046,34 @@
       </c>
     </row>
     <row r="102" spans="1:22" ht="60" x14ac:dyDescent="0.25">
-      <c r="A102" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B102" s="16" t="s">
+      <c r="A102" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B102" s="21" t="s">
         <v>250</v>
       </c>
-      <c r="C102" s="15"/>
-      <c r="D102" s="20" t="s">
+      <c r="C102" s="20"/>
+      <c r="D102" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="E102" s="21"/>
-      <c r="F102" s="21"/>
-      <c r="G102" s="16" t="s">
+      <c r="E102" s="14"/>
+      <c r="F102" s="14"/>
+      <c r="G102" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H102" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I102" s="16" t="s">
+      <c r="H102" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="I102" s="21" t="s">
         <v>251</v>
       </c>
-      <c r="J102" s="16" t="s">
+      <c r="J102" s="21" t="s">
         <v>252</v>
       </c>
-      <c r="K102" s="16" t="s">
+      <c r="K102" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="L102" s="16" t="s">
+      <c r="L102" s="21" t="s">
         <v>120</v>
       </c>
       <c r="M102" t="s">
@@ -5002,18 +5090,18 @@
       </c>
     </row>
     <row r="103" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A103" s="16"/>
-      <c r="B103" s="16"/>
-      <c r="C103" s="15"/>
-      <c r="D103" s="20"/>
-      <c r="E103" s="21"/>
-      <c r="F103" s="21"/>
-      <c r="G103" s="16"/>
-      <c r="H103" s="16"/>
-      <c r="I103" s="16"/>
-      <c r="J103" s="16"/>
-      <c r="K103" s="16"/>
-      <c r="L103" s="16"/>
+      <c r="A103" s="21"/>
+      <c r="B103" s="21"/>
+      <c r="C103" s="20"/>
+      <c r="D103" s="15"/>
+      <c r="E103" s="14"/>
+      <c r="F103" s="14"/>
+      <c r="G103" s="21"/>
+      <c r="H103" s="21"/>
+      <c r="I103" s="21"/>
+      <c r="J103" s="21"/>
+      <c r="K103" s="21"/>
+      <c r="L103" s="21"/>
       <c r="M103" t="s">
         <v>187</v>
       </c>
@@ -5028,18 +5116,18 @@
       </c>
     </row>
     <row r="104" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A104" s="16"/>
-      <c r="B104" s="16"/>
-      <c r="C104" s="15"/>
-      <c r="D104" s="20"/>
-      <c r="E104" s="21"/>
-      <c r="F104" s="21"/>
-      <c r="G104" s="16"/>
-      <c r="H104" s="16"/>
-      <c r="I104" s="16"/>
-      <c r="J104" s="16"/>
-      <c r="K104" s="16"/>
-      <c r="L104" s="16"/>
+      <c r="A104" s="21"/>
+      <c r="B104" s="21"/>
+      <c r="C104" s="20"/>
+      <c r="D104" s="15"/>
+      <c r="E104" s="14"/>
+      <c r="F104" s="14"/>
+      <c r="G104" s="21"/>
+      <c r="H104" s="21"/>
+      <c r="I104" s="21"/>
+      <c r="J104" s="21"/>
+      <c r="K104" s="21"/>
+      <c r="L104" s="21"/>
       <c r="M104" t="s">
         <v>212</v>
       </c>
@@ -5054,34 +5142,34 @@
       </c>
     </row>
     <row r="105" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A105" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B105" s="16" t="s">
+      <c r="A105" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B105" s="21" t="s">
         <v>258</v>
       </c>
-      <c r="C105" s="15"/>
-      <c r="D105" s="20" t="s">
+      <c r="C105" s="20"/>
+      <c r="D105" s="15" t="s">
         <v>259</v>
       </c>
-      <c r="E105" s="21"/>
-      <c r="F105" s="21"/>
-      <c r="G105" s="16" t="s">
+      <c r="E105" s="14"/>
+      <c r="F105" s="14"/>
+      <c r="G105" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H105" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I105" s="16" t="s">
+      <c r="H105" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="I105" s="21" t="s">
         <v>260</v>
       </c>
-      <c r="J105" s="18" t="s">
+      <c r="J105" s="23" t="s">
         <v>265</v>
       </c>
-      <c r="K105" s="16" t="s">
+      <c r="K105" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="L105" s="16" t="s">
+      <c r="L105" s="21" t="s">
         <v>120</v>
       </c>
       <c r="M105" t="s">
@@ -5098,18 +5186,18 @@
       </c>
     </row>
     <row r="106" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A106" s="16"/>
-      <c r="B106" s="16"/>
-      <c r="C106" s="15"/>
-      <c r="D106" s="20"/>
-      <c r="E106" s="21"/>
-      <c r="F106" s="21"/>
-      <c r="G106" s="16"/>
-      <c r="H106" s="16"/>
-      <c r="I106" s="16"/>
-      <c r="J106" s="18"/>
-      <c r="K106" s="16"/>
-      <c r="L106" s="16"/>
+      <c r="A106" s="21"/>
+      <c r="B106" s="21"/>
+      <c r="C106" s="20"/>
+      <c r="D106" s="15"/>
+      <c r="E106" s="14"/>
+      <c r="F106" s="14"/>
+      <c r="G106" s="21"/>
+      <c r="H106" s="21"/>
+      <c r="I106" s="21"/>
+      <c r="J106" s="23"/>
+      <c r="K106" s="21"/>
+      <c r="L106" s="21"/>
       <c r="M106" t="s">
         <v>212</v>
       </c>
@@ -5124,18 +5212,18 @@
       </c>
     </row>
     <row r="107" spans="1:22" ht="60" x14ac:dyDescent="0.25">
-      <c r="A107" s="16"/>
-      <c r="B107" s="16"/>
-      <c r="C107" s="15"/>
-      <c r="D107" s="20"/>
-      <c r="E107" s="21"/>
-      <c r="F107" s="21"/>
-      <c r="G107" s="16"/>
-      <c r="H107" s="16"/>
-      <c r="I107" s="16"/>
-      <c r="J107" s="18"/>
-      <c r="K107" s="16"/>
-      <c r="L107" s="16"/>
+      <c r="A107" s="21"/>
+      <c r="B107" s="21"/>
+      <c r="C107" s="20"/>
+      <c r="D107" s="15"/>
+      <c r="E107" s="14"/>
+      <c r="F107" s="14"/>
+      <c r="G107" s="21"/>
+      <c r="H107" s="21"/>
+      <c r="I107" s="21"/>
+      <c r="J107" s="23"/>
+      <c r="K107" s="21"/>
+      <c r="L107" s="21"/>
       <c r="M107" t="s">
         <v>212</v>
       </c>
@@ -5150,18 +5238,18 @@
       </c>
     </row>
     <row r="108" spans="1:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="A108" s="16"/>
-      <c r="B108" s="16"/>
-      <c r="C108" s="15"/>
-      <c r="D108" s="20"/>
-      <c r="E108" s="21"/>
-      <c r="F108" s="21"/>
-      <c r="G108" s="16"/>
-      <c r="H108" s="16"/>
-      <c r="I108" s="16"/>
-      <c r="J108" s="18"/>
-      <c r="K108" s="16"/>
-      <c r="L108" s="16"/>
+      <c r="A108" s="21"/>
+      <c r="B108" s="21"/>
+      <c r="C108" s="20"/>
+      <c r="D108" s="15"/>
+      <c r="E108" s="14"/>
+      <c r="F108" s="14"/>
+      <c r="G108" s="21"/>
+      <c r="H108" s="21"/>
+      <c r="I108" s="21"/>
+      <c r="J108" s="23"/>
+      <c r="K108" s="21"/>
+      <c r="L108" s="21"/>
       <c r="M108" t="s">
         <v>212</v>
       </c>
@@ -5214,32 +5302,32 @@
       </c>
     </row>
     <row r="110" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A110" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B110" s="16" t="s">
+      <c r="A110" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B110" s="21" t="s">
         <v>270</v>
       </c>
-      <c r="C110" s="15"/>
-      <c r="D110" s="17" t="s">
+      <c r="C110" s="20"/>
+      <c r="D110" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="E110" s="19"/>
-      <c r="F110" s="19"/>
-      <c r="G110" s="16" t="s">
+      <c r="E110" s="24"/>
+      <c r="F110" s="24"/>
+      <c r="G110" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H110" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I110" s="16"/>
-      <c r="J110" s="18" t="s">
+      <c r="H110" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="I110" s="21"/>
+      <c r="J110" s="23" t="s">
         <v>271</v>
       </c>
-      <c r="K110" s="16" t="s">
+      <c r="K110" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="L110" s="16" t="s">
+      <c r="L110" s="21" t="s">
         <v>120</v>
       </c>
       <c r="M110" t="s">
@@ -5256,18 +5344,18 @@
       </c>
     </row>
     <row r="111" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A111" s="16"/>
-      <c r="B111" s="16"/>
-      <c r="C111" s="15"/>
-      <c r="D111" s="17"/>
-      <c r="E111" s="19"/>
-      <c r="F111" s="19"/>
-      <c r="G111" s="16"/>
-      <c r="H111" s="16"/>
-      <c r="I111" s="16"/>
-      <c r="J111" s="18"/>
-      <c r="K111" s="16"/>
-      <c r="L111" s="16"/>
+      <c r="A111" s="21"/>
+      <c r="B111" s="21"/>
+      <c r="C111" s="20"/>
+      <c r="D111" s="22"/>
+      <c r="E111" s="24"/>
+      <c r="F111" s="24"/>
+      <c r="G111" s="21"/>
+      <c r="H111" s="21"/>
+      <c r="I111" s="21"/>
+      <c r="J111" s="23"/>
+      <c r="K111" s="21"/>
+      <c r="L111" s="21"/>
       <c r="M111" t="s">
         <v>212</v>
       </c>
@@ -5282,18 +5370,18 @@
       </c>
     </row>
     <row r="112" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A112" s="16"/>
-      <c r="B112" s="16"/>
-      <c r="C112" s="15"/>
-      <c r="D112" s="17"/>
-      <c r="E112" s="19"/>
-      <c r="F112" s="19"/>
-      <c r="G112" s="16"/>
-      <c r="H112" s="16"/>
-      <c r="I112" s="16"/>
-      <c r="J112" s="18"/>
-      <c r="K112" s="16"/>
-      <c r="L112" s="16"/>
+      <c r="A112" s="21"/>
+      <c r="B112" s="21"/>
+      <c r="C112" s="20"/>
+      <c r="D112" s="22"/>
+      <c r="E112" s="24"/>
+      <c r="F112" s="24"/>
+      <c r="G112" s="21"/>
+      <c r="H112" s="21"/>
+      <c r="I112" s="21"/>
+      <c r="J112" s="23"/>
+      <c r="K112" s="21"/>
+      <c r="L112" s="21"/>
       <c r="M112" t="s">
         <v>214</v>
       </c>
@@ -5308,32 +5396,32 @@
       </c>
     </row>
     <row r="113" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A113" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B113" s="16" t="s">
+      <c r="A113" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B113" s="21" t="s">
         <v>281</v>
       </c>
-      <c r="C113" s="15"/>
-      <c r="D113" s="17" t="s">
+      <c r="C113" s="20"/>
+      <c r="D113" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="E113" s="19"/>
-      <c r="F113" s="19"/>
-      <c r="G113" s="16" t="s">
+      <c r="E113" s="24"/>
+      <c r="F113" s="24"/>
+      <c r="G113" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H113" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I113" s="16"/>
-      <c r="J113" s="18" t="s">
+      <c r="H113" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="I113" s="21"/>
+      <c r="J113" s="23" t="s">
         <v>286</v>
       </c>
-      <c r="K113" s="16" t="s">
+      <c r="K113" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="L113" s="16" t="s">
+      <c r="L113" s="21" t="s">
         <v>120</v>
       </c>
       <c r="M113" t="s">
@@ -5350,18 +5438,18 @@
       </c>
     </row>
     <row r="114" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A114" s="16"/>
-      <c r="B114" s="16"/>
-      <c r="C114" s="15"/>
-      <c r="D114" s="17"/>
-      <c r="E114" s="19"/>
-      <c r="F114" s="19"/>
-      <c r="G114" s="16"/>
-      <c r="H114" s="16"/>
-      <c r="I114" s="16"/>
-      <c r="J114" s="18"/>
-      <c r="K114" s="16"/>
-      <c r="L114" s="16"/>
+      <c r="A114" s="21"/>
+      <c r="B114" s="21"/>
+      <c r="C114" s="20"/>
+      <c r="D114" s="22"/>
+      <c r="E114" s="24"/>
+      <c r="F114" s="24"/>
+      <c r="G114" s="21"/>
+      <c r="H114" s="21"/>
+      <c r="I114" s="21"/>
+      <c r="J114" s="23"/>
+      <c r="K114" s="21"/>
+      <c r="L114" s="21"/>
       <c r="M114" t="s">
         <v>212</v>
       </c>
@@ -5376,18 +5464,18 @@
       </c>
     </row>
     <row r="115" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A115" s="16"/>
-      <c r="B115" s="16"/>
-      <c r="C115" s="15"/>
-      <c r="D115" s="17"/>
-      <c r="E115" s="19"/>
-      <c r="F115" s="19"/>
-      <c r="G115" s="16"/>
-      <c r="H115" s="16"/>
-      <c r="I115" s="16"/>
-      <c r="J115" s="18"/>
-      <c r="K115" s="16"/>
-      <c r="L115" s="16"/>
+      <c r="A115" s="21"/>
+      <c r="B115" s="21"/>
+      <c r="C115" s="20"/>
+      <c r="D115" s="22"/>
+      <c r="E115" s="24"/>
+      <c r="F115" s="24"/>
+      <c r="G115" s="21"/>
+      <c r="H115" s="21"/>
+      <c r="I115" s="21"/>
+      <c r="J115" s="23"/>
+      <c r="K115" s="21"/>
+      <c r="L115" s="21"/>
       <c r="M115" t="s">
         <v>214</v>
       </c>
@@ -5402,32 +5490,32 @@
       </c>
     </row>
     <row r="116" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A116" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B116" s="16" t="s">
+      <c r="A116" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B116" s="21" t="s">
         <v>282</v>
       </c>
-      <c r="C116" s="15"/>
-      <c r="D116" s="17" t="s">
+      <c r="C116" s="20"/>
+      <c r="D116" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="E116" s="19"/>
-      <c r="F116" s="19"/>
-      <c r="G116" s="16" t="s">
+      <c r="E116" s="24"/>
+      <c r="F116" s="24"/>
+      <c r="G116" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H116" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I116" s="16"/>
-      <c r="J116" s="18" t="s">
+      <c r="H116" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="I116" s="21"/>
+      <c r="J116" s="23" t="s">
         <v>285</v>
       </c>
-      <c r="K116" s="16" t="s">
+      <c r="K116" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="L116" s="16" t="s">
+      <c r="L116" s="21" t="s">
         <v>120</v>
       </c>
       <c r="M116" t="s">
@@ -5444,18 +5532,18 @@
       </c>
     </row>
     <row r="117" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A117" s="16"/>
-      <c r="B117" s="16"/>
-      <c r="C117" s="15"/>
-      <c r="D117" s="17"/>
-      <c r="E117" s="19"/>
-      <c r="F117" s="19"/>
-      <c r="G117" s="16"/>
-      <c r="H117" s="16"/>
-      <c r="I117" s="16"/>
-      <c r="J117" s="18"/>
-      <c r="K117" s="16"/>
-      <c r="L117" s="16"/>
+      <c r="A117" s="21"/>
+      <c r="B117" s="21"/>
+      <c r="C117" s="20"/>
+      <c r="D117" s="22"/>
+      <c r="E117" s="24"/>
+      <c r="F117" s="24"/>
+      <c r="G117" s="21"/>
+      <c r="H117" s="21"/>
+      <c r="I117" s="21"/>
+      <c r="J117" s="23"/>
+      <c r="K117" s="21"/>
+      <c r="L117" s="21"/>
       <c r="M117" t="s">
         <v>212</v>
       </c>
@@ -5470,18 +5558,18 @@
       </c>
     </row>
     <row r="118" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A118" s="16"/>
-      <c r="B118" s="16"/>
-      <c r="C118" s="15"/>
-      <c r="D118" s="17"/>
-      <c r="E118" s="19"/>
-      <c r="F118" s="19"/>
-      <c r="G118" s="16"/>
-      <c r="H118" s="16"/>
-      <c r="I118" s="16"/>
-      <c r="J118" s="18"/>
-      <c r="K118" s="16"/>
-      <c r="L118" s="16"/>
+      <c r="A118" s="21"/>
+      <c r="B118" s="21"/>
+      <c r="C118" s="20"/>
+      <c r="D118" s="22"/>
+      <c r="E118" s="24"/>
+      <c r="F118" s="24"/>
+      <c r="G118" s="21"/>
+      <c r="H118" s="21"/>
+      <c r="I118" s="21"/>
+      <c r="J118" s="23"/>
+      <c r="K118" s="21"/>
+      <c r="L118" s="21"/>
       <c r="M118" t="s">
         <v>214</v>
       </c>
@@ -5496,32 +5584,32 @@
       </c>
     </row>
     <row r="119" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A119" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B119" s="16" t="s">
+      <c r="A119" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B119" s="21" t="s">
         <v>283</v>
       </c>
-      <c r="C119" s="15"/>
-      <c r="D119" s="17" t="s">
+      <c r="C119" s="20"/>
+      <c r="D119" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="E119" s="19"/>
-      <c r="F119" s="19"/>
-      <c r="G119" s="16" t="s">
+      <c r="E119" s="24"/>
+      <c r="F119" s="24"/>
+      <c r="G119" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H119" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I119" s="16"/>
-      <c r="J119" s="18" t="s">
+      <c r="H119" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="I119" s="21"/>
+      <c r="J119" s="23" t="s">
         <v>284</v>
       </c>
-      <c r="K119" s="16" t="s">
+      <c r="K119" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="L119" s="16" t="s">
+      <c r="L119" s="21" t="s">
         <v>120</v>
       </c>
       <c r="M119" t="s">
@@ -5538,18 +5626,18 @@
       </c>
     </row>
     <row r="120" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A120" s="16"/>
-      <c r="B120" s="16"/>
-      <c r="C120" s="15"/>
-      <c r="D120" s="17"/>
-      <c r="E120" s="19"/>
-      <c r="F120" s="19"/>
-      <c r="G120" s="16"/>
-      <c r="H120" s="16"/>
-      <c r="I120" s="16"/>
-      <c r="J120" s="18"/>
-      <c r="K120" s="16"/>
-      <c r="L120" s="16"/>
+      <c r="A120" s="21"/>
+      <c r="B120" s="21"/>
+      <c r="C120" s="20"/>
+      <c r="D120" s="22"/>
+      <c r="E120" s="24"/>
+      <c r="F120" s="24"/>
+      <c r="G120" s="21"/>
+      <c r="H120" s="21"/>
+      <c r="I120" s="21"/>
+      <c r="J120" s="23"/>
+      <c r="K120" s="21"/>
+      <c r="L120" s="21"/>
       <c r="M120" t="s">
         <v>212</v>
       </c>
@@ -5564,18 +5652,18 @@
       </c>
     </row>
     <row r="121" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A121" s="16"/>
-      <c r="B121" s="16"/>
-      <c r="C121" s="15"/>
-      <c r="D121" s="17"/>
-      <c r="E121" s="19"/>
-      <c r="F121" s="19"/>
-      <c r="G121" s="16"/>
-      <c r="H121" s="16"/>
-      <c r="I121" s="16"/>
-      <c r="J121" s="18"/>
-      <c r="K121" s="16"/>
-      <c r="L121" s="16"/>
+      <c r="A121" s="21"/>
+      <c r="B121" s="21"/>
+      <c r="C121" s="20"/>
+      <c r="D121" s="22"/>
+      <c r="E121" s="24"/>
+      <c r="F121" s="24"/>
+      <c r="G121" s="21"/>
+      <c r="H121" s="21"/>
+      <c r="I121" s="21"/>
+      <c r="J121" s="23"/>
+      <c r="K121" s="21"/>
+      <c r="L121" s="21"/>
       <c r="M121" t="s">
         <v>214</v>
       </c>
@@ -5590,38 +5678,38 @@
       </c>
     </row>
     <row r="122" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="B122" s="22" t="s">
+      <c r="A122" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B122" s="16" t="s">
         <v>315</v>
       </c>
-      <c r="C122" s="22" t="s">
+      <c r="C122" s="16" t="s">
         <v>316</v>
       </c>
-      <c r="D122" s="20" t="s">
+      <c r="D122" s="15" t="s">
         <v>322</v>
       </c>
-      <c r="E122" s="22"/>
-      <c r="F122" s="25" t="s">
+      <c r="E122" s="16"/>
+      <c r="F122" s="18" t="s">
         <v>328</v>
       </c>
-      <c r="G122" s="22" t="s">
+      <c r="G122" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="H122" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="I122" s="22" t="s">
+      <c r="H122" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I122" s="16" t="s">
         <v>317</v>
       </c>
-      <c r="J122" s="20" t="s">
+      <c r="J122" s="15" t="s">
         <v>318</v>
       </c>
-      <c r="K122" s="22" t="s">
+      <c r="K122" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L122" s="22" t="s">
+      <c r="L122" s="16" t="s">
         <v>119</v>
       </c>
       <c r="M122" t="s">
@@ -5636,38 +5724,38 @@
       <c r="P122" s="11" t="s">
         <v>324</v>
       </c>
-      <c r="Q122" s="25" t="s">
+      <c r="Q122" s="18" t="s">
         <v>323</v>
       </c>
-      <c r="R122" s="20" t="s">
+      <c r="R122" s="15" t="s">
         <v>329</v>
       </c>
-      <c r="S122" s="25" t="s">
+      <c r="S122" s="18" t="s">
         <v>320</v>
       </c>
-      <c r="T122" s="25" t="s">
+      <c r="T122" s="18" t="s">
         <v>319</v>
       </c>
-      <c r="U122" s="22" t="s">
+      <c r="U122" s="16" t="s">
         <v>308</v>
       </c>
-      <c r="V122" s="20" t="s">
+      <c r="V122" s="15" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="123" spans="1:22" ht="60" x14ac:dyDescent="0.25">
-      <c r="A123" s="22"/>
-      <c r="B123" s="22"/>
-      <c r="C123" s="22"/>
-      <c r="D123" s="22"/>
-      <c r="E123" s="22"/>
-      <c r="F123" s="25"/>
-      <c r="G123" s="22"/>
-      <c r="H123" s="22"/>
-      <c r="I123" s="22"/>
-      <c r="J123" s="20"/>
-      <c r="K123" s="22"/>
-      <c r="L123" s="22"/>
+      <c r="A123" s="16"/>
+      <c r="B123" s="16"/>
+      <c r="C123" s="16"/>
+      <c r="D123" s="16"/>
+      <c r="E123" s="16"/>
+      <c r="F123" s="18"/>
+      <c r="G123" s="16"/>
+      <c r="H123" s="16"/>
+      <c r="I123" s="16"/>
+      <c r="J123" s="15"/>
+      <c r="K123" s="16"/>
+      <c r="L123" s="16"/>
       <c r="M123" t="s">
         <v>177</v>
       </c>
@@ -5680,26 +5768,26 @@
       <c r="P123" s="11" t="s">
         <v>325</v>
       </c>
-      <c r="Q123" s="25"/>
-      <c r="R123" s="20"/>
-      <c r="S123" s="25"/>
-      <c r="T123" s="25"/>
-      <c r="U123" s="22"/>
-      <c r="V123" s="20"/>
+      <c r="Q123" s="18"/>
+      <c r="R123" s="15"/>
+      <c r="S123" s="18"/>
+      <c r="T123" s="18"/>
+      <c r="U123" s="16"/>
+      <c r="V123" s="15"/>
     </row>
     <row r="124" spans="1:22" ht="60" x14ac:dyDescent="0.25">
-      <c r="A124" s="22"/>
-      <c r="B124" s="22"/>
-      <c r="C124" s="22"/>
-      <c r="D124" s="22"/>
-      <c r="E124" s="22"/>
-      <c r="F124" s="25"/>
-      <c r="G124" s="22"/>
-      <c r="H124" s="22"/>
-      <c r="I124" s="22"/>
-      <c r="J124" s="20"/>
-      <c r="K124" s="22"/>
-      <c r="L124" s="22"/>
+      <c r="A124" s="16"/>
+      <c r="B124" s="16"/>
+      <c r="C124" s="16"/>
+      <c r="D124" s="16"/>
+      <c r="E124" s="16"/>
+      <c r="F124" s="18"/>
+      <c r="G124" s="16"/>
+      <c r="H124" s="16"/>
+      <c r="I124" s="16"/>
+      <c r="J124" s="15"/>
+      <c r="K124" s="16"/>
+      <c r="L124" s="16"/>
       <c r="M124" t="s">
         <v>111</v>
       </c>
@@ -5712,19 +5800,19 @@
       <c r="P124" s="11" t="s">
         <v>326</v>
       </c>
-      <c r="Q124" s="25"/>
-      <c r="R124" s="20"/>
-      <c r="S124" s="25"/>
-      <c r="T124" s="25"/>
-      <c r="U124" s="22"/>
-      <c r="V124" s="20"/>
-    </row>
-    <row r="125" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Q124" s="18"/>
+      <c r="R124" s="15"/>
+      <c r="S124" s="18"/>
+      <c r="T124" s="18"/>
+      <c r="U124" s="16"/>
+      <c r="V124" s="15"/>
+    </row>
+    <row r="125" spans="1:22" ht="135" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>141</v>
       </c>
       <c r="B125" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="C125" t="s">
         <v>303</v>
@@ -5736,12 +5824,382 @@
         <v>27</v>
       </c>
       <c r="I125" t="s">
+        <v>332</v>
+      </c>
+      <c r="J125" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="K125" t="s">
+        <v>82</v>
+      </c>
+      <c r="L125" t="s">
+        <v>120</v>
+      </c>
+      <c r="M125" t="s">
+        <v>214</v>
+      </c>
+      <c r="N125" t="s">
+        <v>83</v>
+      </c>
+      <c r="O125" t="s">
+        <v>27</v>
+      </c>
+      <c r="R125" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="T125" s="11" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="126" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A126" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B126" s="16" t="s">
+        <v>337</v>
+      </c>
+      <c r="C126" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="D126" s="15" t="s">
+        <v>350</v>
+      </c>
+      <c r="E126" s="16"/>
+      <c r="F126" s="16"/>
+      <c r="G126" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H126" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I126" s="16" t="s">
+        <v>335</v>
+      </c>
+      <c r="J126" s="15" t="s">
+        <v>344</v>
+      </c>
+      <c r="K126" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="L126" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="M126" t="s">
+        <v>60</v>
+      </c>
+      <c r="N126" t="s">
+        <v>211</v>
+      </c>
+      <c r="O126" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q126" s="15"/>
+      <c r="R126" s="15" t="s">
+        <v>338</v>
+      </c>
+      <c r="S126" s="15"/>
+      <c r="T126" s="18" t="s">
+        <v>319</v>
+      </c>
+      <c r="U126" s="15"/>
+      <c r="V126" s="15"/>
+    </row>
+    <row r="127" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+      <c r="A127" s="16"/>
+      <c r="B127" s="16"/>
+      <c r="C127" s="16"/>
+      <c r="D127" s="16"/>
+      <c r="E127" s="16"/>
+      <c r="F127" s="16"/>
+      <c r="G127" s="16"/>
+      <c r="H127" s="16"/>
+      <c r="I127" s="16"/>
+      <c r="J127" s="15"/>
+      <c r="K127" s="16"/>
+      <c r="L127" s="16"/>
+      <c r="M127" t="s">
+        <v>214</v>
+      </c>
+      <c r="N127" t="s">
+        <v>83</v>
+      </c>
+      <c r="O127" t="s">
+        <v>27</v>
+      </c>
+      <c r="P127" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="Q127" s="15"/>
+      <c r="R127" s="15"/>
+      <c r="S127" s="15"/>
+      <c r="T127" s="18"/>
+      <c r="U127" s="15"/>
+      <c r="V127" s="15"/>
+    </row>
+    <row r="128" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A128" s="16"/>
+      <c r="B128" s="16"/>
+      <c r="C128" s="16"/>
+      <c r="D128" s="16"/>
+      <c r="E128" s="16"/>
+      <c r="F128" s="16"/>
+      <c r="G128" s="16"/>
+      <c r="H128" s="16"/>
+      <c r="I128" s="16"/>
+      <c r="J128" s="15"/>
+      <c r="K128" s="16"/>
+      <c r="L128" s="16"/>
+      <c r="M128" t="s">
+        <v>336</v>
+      </c>
+      <c r="N128" t="s">
+        <v>141</v>
+      </c>
+      <c r="O128" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q128" s="15"/>
+      <c r="R128" s="15"/>
+      <c r="S128" s="15"/>
+      <c r="T128" s="18"/>
+      <c r="U128" s="15"/>
+      <c r="V128" s="15"/>
+    </row>
+    <row r="129" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A129" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B129" s="16" t="s">
         <v>331</v>
       </c>
+      <c r="C129" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="D129" s="15" t="s">
+        <v>348</v>
+      </c>
+      <c r="E129" s="16"/>
+      <c r="F129" s="16"/>
+      <c r="G129" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H129" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I129" s="16" t="s">
+        <v>330</v>
+      </c>
+      <c r="J129" s="15" t="s">
+        <v>345</v>
+      </c>
+      <c r="K129" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="L129" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="M129" t="s">
+        <v>337</v>
+      </c>
+      <c r="N129" t="s">
+        <v>83</v>
+      </c>
+      <c r="O129" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q129" s="15"/>
+      <c r="R129" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="S129" s="15"/>
+      <c r="T129" s="18" t="s">
+        <v>319</v>
+      </c>
+      <c r="U129" s="15"/>
+      <c r="V129" s="15"/>
+    </row>
+    <row r="130" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A130" s="16"/>
+      <c r="B130" s="16"/>
+      <c r="C130" s="16"/>
+      <c r="D130" s="16"/>
+      <c r="E130" s="16"/>
+      <c r="F130" s="16"/>
+      <c r="G130" s="16"/>
+      <c r="H130" s="16"/>
+      <c r="I130" s="16"/>
+      <c r="J130" s="15"/>
+      <c r="K130" s="16"/>
+      <c r="L130" s="16"/>
+      <c r="M130" t="s">
+        <v>132</v>
+      </c>
+      <c r="N130" t="s">
+        <v>66</v>
+      </c>
+      <c r="O130" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q130" s="15"/>
+      <c r="R130" s="15"/>
+      <c r="S130" s="15"/>
+      <c r="T130" s="18"/>
+      <c r="U130" s="15"/>
+      <c r="V130" s="15"/>
+    </row>
+    <row r="131" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A131" s="16"/>
+      <c r="B131" s="16"/>
+      <c r="C131" s="16"/>
+      <c r="D131" s="16"/>
+      <c r="E131" s="16"/>
+      <c r="F131" s="16"/>
+      <c r="G131" s="16"/>
+      <c r="H131" s="16"/>
+      <c r="I131" s="16"/>
+      <c r="J131" s="15"/>
+      <c r="K131" s="16"/>
+      <c r="L131" s="16"/>
+      <c r="M131" t="s">
+        <v>133</v>
+      </c>
+      <c r="N131" t="s">
+        <v>66</v>
+      </c>
+      <c r="O131" t="s">
+        <v>67</v>
+      </c>
+      <c r="P131" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="Q131" s="15"/>
+      <c r="R131" s="15"/>
+      <c r="S131" s="15"/>
+      <c r="T131" s="18"/>
+      <c r="U131" s="15"/>
+      <c r="V131" s="15"/>
+    </row>
+    <row r="132" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B132" s="16" t="s">
+        <v>340</v>
+      </c>
+      <c r="C132" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="D132" s="15" t="s">
+        <v>348</v>
+      </c>
+      <c r="E132" s="16"/>
+      <c r="F132" s="16"/>
+      <c r="G132" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H132" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I132" s="16" t="s">
+        <v>341</v>
+      </c>
+      <c r="J132" s="15" t="s">
+        <v>343</v>
+      </c>
+      <c r="K132" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="L132" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="M132" t="s">
+        <v>342</v>
+      </c>
+      <c r="N132" t="s">
+        <v>66</v>
+      </c>
+      <c r="O132" t="s">
+        <v>67</v>
+      </c>
+      <c r="P132" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="Q132" s="15"/>
+      <c r="R132" s="14"/>
+      <c r="S132" s="14"/>
+      <c r="T132" s="17" t="s">
+        <v>319</v>
+      </c>
+      <c r="U132" s="14"/>
+      <c r="V132" s="14"/>
+    </row>
+    <row r="133" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A133" s="16"/>
+      <c r="B133" s="16"/>
+      <c r="C133" s="16"/>
+      <c r="D133" s="15"/>
+      <c r="E133" s="16"/>
+      <c r="F133" s="16"/>
+      <c r="G133" s="16"/>
+      <c r="H133" s="16"/>
+      <c r="I133" s="16"/>
+      <c r="J133" s="15"/>
+      <c r="K133" s="16"/>
+      <c r="L133" s="16"/>
+      <c r="M133" t="s">
+        <v>331</v>
+      </c>
+      <c r="N133" t="s">
+        <v>141</v>
+      </c>
+      <c r="O133" t="s">
+        <v>27</v>
+      </c>
+      <c r="P133" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="Q133" s="15"/>
+      <c r="R133" s="14"/>
+      <c r="S133" s="14"/>
+      <c r="T133" s="17"/>
+      <c r="U133" s="14"/>
+      <c r="V133" s="14"/>
+    </row>
+    <row r="134" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A134" s="16"/>
+      <c r="B134" s="16"/>
+      <c r="C134" s="16"/>
+      <c r="D134" s="15"/>
+      <c r="E134" s="16"/>
+      <c r="F134" s="16"/>
+      <c r="G134" s="16"/>
+      <c r="H134" s="16"/>
+      <c r="I134" s="16"/>
+      <c r="J134" s="15"/>
+      <c r="K134" s="16"/>
+      <c r="L134" s="16"/>
+      <c r="M134" t="s">
+        <v>352</v>
+      </c>
+      <c r="N134" t="s">
+        <v>83</v>
+      </c>
+      <c r="O134" t="s">
+        <v>67</v>
+      </c>
+      <c r="P134" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="Q134" s="15"/>
+      <c r="R134" s="14"/>
+      <c r="S134" s="14"/>
+      <c r="T134" s="17"/>
+      <c r="U134" s="14"/>
+      <c r="V134" s="14"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:V1"/>
-  <mergeCells count="294">
+  <mergeCells count="348">
     <mergeCell ref="T122:T124"/>
     <mergeCell ref="U122:U124"/>
     <mergeCell ref="V122:V124"/>
@@ -6027,6 +6485,8 @@
     <mergeCell ref="E110:E112"/>
     <mergeCell ref="F110:F112"/>
     <mergeCell ref="C110:C112"/>
+    <mergeCell ref="E126:E128"/>
+    <mergeCell ref="D126:D128"/>
     <mergeCell ref="C62:C63"/>
     <mergeCell ref="C64:C67"/>
     <mergeCell ref="C68:C71"/>
@@ -6036,6 +6496,58 @@
     <mergeCell ref="C88:C93"/>
     <mergeCell ref="C94:C96"/>
     <mergeCell ref="C97:C98"/>
+    <mergeCell ref="C126:C128"/>
+    <mergeCell ref="B126:B128"/>
+    <mergeCell ref="A126:A128"/>
+    <mergeCell ref="L129:L131"/>
+    <mergeCell ref="K129:K131"/>
+    <mergeCell ref="R129:R131"/>
+    <mergeCell ref="I129:I131"/>
+    <mergeCell ref="H129:H131"/>
+    <mergeCell ref="G129:G131"/>
+    <mergeCell ref="F129:F131"/>
+    <mergeCell ref="E129:E131"/>
+    <mergeCell ref="D129:D131"/>
+    <mergeCell ref="C129:C131"/>
+    <mergeCell ref="B129:B131"/>
+    <mergeCell ref="A129:A131"/>
+    <mergeCell ref="J126:J128"/>
+    <mergeCell ref="J129:J131"/>
+    <mergeCell ref="L126:L128"/>
+    <mergeCell ref="K126:K128"/>
+    <mergeCell ref="R126:R128"/>
+    <mergeCell ref="I126:I128"/>
+    <mergeCell ref="H126:H128"/>
+    <mergeCell ref="G126:G128"/>
+    <mergeCell ref="F126:F128"/>
+    <mergeCell ref="Q126:Q128"/>
+    <mergeCell ref="S126:S128"/>
+    <mergeCell ref="T126:T128"/>
+    <mergeCell ref="U126:U128"/>
+    <mergeCell ref="V126:V128"/>
+    <mergeCell ref="Q129:Q131"/>
+    <mergeCell ref="S129:S131"/>
+    <mergeCell ref="T129:T131"/>
+    <mergeCell ref="U129:U131"/>
+    <mergeCell ref="V129:V131"/>
+    <mergeCell ref="F132:F134"/>
+    <mergeCell ref="E132:E134"/>
+    <mergeCell ref="D132:D134"/>
+    <mergeCell ref="C132:C134"/>
+    <mergeCell ref="B132:B134"/>
+    <mergeCell ref="A132:A134"/>
+    <mergeCell ref="R132:R134"/>
+    <mergeCell ref="S132:S134"/>
+    <mergeCell ref="T132:T134"/>
+    <mergeCell ref="U132:U134"/>
+    <mergeCell ref="V132:V134"/>
+    <mergeCell ref="Q132:Q134"/>
+    <mergeCell ref="L132:L134"/>
+    <mergeCell ref="K132:K134"/>
+    <mergeCell ref="J132:J134"/>
+    <mergeCell ref="I132:I134"/>
+    <mergeCell ref="H132:H134"/>
+    <mergeCell ref="G132:G134"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="P54" r:id="rId1"/>
@@ -6051,16 +6563,20 @@
     <hyperlink ref="P123" r:id="rId11"/>
     <hyperlink ref="P124" r:id="rId12"/>
     <hyperlink ref="F122:F124" r:id="rId13" display="MappingSheetResources\GetContractAvailableServices\GetContractAvailableServicesResponse.txt"/>
+    <hyperlink ref="T125" r:id="rId14"/>
+    <hyperlink ref="T126:T128" r:id="rId15" display="http://192.168.110.185:8585/tfs/web/UI/Pages/WorkItems/WorkItemEdit.aspx?id=6621&amp;pguid=81f5a887-a9da-41fc-8c45-50b4cb40e1ea"/>
+    <hyperlink ref="T129:T131" r:id="rId16" display="http://192.168.110.185:8585/tfs/web/UI/Pages/WorkItems/WorkItemEdit.aspx?id=6621&amp;pguid=81f5a887-a9da-41fc-8c45-50b4cb40e1ea"/>
+    <hyperlink ref="T132:T134" r:id="rId17" display="http://192.168.110.185:8585/tfs/web/UI/Pages/WorkItems/WorkItemEdit.aspx?id=6621&amp;pguid=81f5a887-a9da-41fc-8c45-50b4cb40e1ea"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId14"/>
-  <drawing r:id="rId15"/>
-  <legacyDrawing r:id="rId16"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId18"/>
+  <drawing r:id="rId19"/>
+  <legacyDrawing r:id="rId20"/>
   <oleObjects>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="1025" r:id="rId17">
-          <objectPr defaultSize="0" r:id="rId18">
+        <oleObject progId="Packager Shell Object" shapeId="1025" r:id="rId21">
+          <objectPr defaultSize="0" r:id="rId22">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -6079,13 +6595,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="1025" r:id="rId17"/>
+        <oleObject progId="Packager Shell Object" shapeId="1025" r:id="rId21"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="1026" r:id="rId19">
-          <objectPr defaultSize="0" r:id="rId20">
+        <oleObject progId="Packager Shell Object" shapeId="1026" r:id="rId23">
+          <objectPr defaultSize="0" r:id="rId24">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>5</xdr:col>
@@ -6104,7 +6620,7 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="1026" r:id="rId19"/>
+        <oleObject progId="Packager Shell Object" shapeId="1026" r:id="rId23"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </oleObjects>

</xml_diff>